<commit_message>
Added some validation and cell highlighting to show errors
</commit_message>
<xml_diff>
--- a/input/community_cohort_inputs.xlsx
+++ b/input/community_cohort_inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14250" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23130" windowHeight="10800"/>
   </bookViews>
   <sheets>
     <sheet name="FACTORS_MUNI" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Names of columns from FACTORS sheet to be included in cohort calculations</t>
+          <t>Names of columns from FACTORS_MUNI sheet to be included in cohort calculations. If column does not also exist in FACTORS_CCA, cell will be highlighted in red. Duplicate names will be highlighted in yellow.</t>
         </r>
       </text>
     </comment>
@@ -2358,8 +2358,139 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF800000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF800000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF800000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF800000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF800000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF800000"/>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2636,9 +2767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M285"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15772,7 +15901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17563,7 +17692,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -17574,9 +17703,44 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A1048576">
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{A36205D5-D3BC-40FB-8028-6B3A6753CC9E}">
+            <xm:f>AND(ISNA(HLOOKUP(A2, FACTORS_CCA!$C$1:$XFD$1, 1, FALSE)), A2&lt;&gt;"")</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF800000"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFF7C80"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>A2:A1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FACTORS_MUNI!$C$1:$XFD$1</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add localized property tax base for CCAs
</commit_message>
<xml_diff>
--- a/input/community_cohort_inputs.xlsx
+++ b/input/community_cohort_inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23130" windowHeight="10800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25620" windowHeight="11235"/>
   </bookViews>
   <sheets>
     <sheet name="FACTORS_MUNI" sheetId="1" r:id="rId1"/>
@@ -421,6 +421,133 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>INPUT:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Total market value, calculated from 2017 county assessor data</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>INPUT:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> CCA population, from latest 5-year ACS (reported in Community Data Snapshots). Should </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <u/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>not</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> be used as a factor because population scores would </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>all</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> be artificially deflated relative to the city overall.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DERIVED:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> CCA-level EAV per capita estimate (i.e. TOT_MARKET_VAL, scaled to match city's EAV, divided by CCA_POP), plus </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>citywide</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> retail sales per capita</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t xml:space="preserve">DERIVED: </t>
         </r>
         <r>
@@ -434,16 +561,6 @@
         </r>
         <r>
           <rPr>
-            <i/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">citywide </t>
-        </r>
-        <r>
-          <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
@@ -453,7 +570,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -491,11 +608,31 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>population (i.e. LN(POP))</t>
+          <t xml:space="preserve">population (i.e. LN(POP)) -- </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <u/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>not</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> based on CCA_POP, because CCAs should not all score lower on population than the city overall.</t>
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -614,7 +751,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="382">
   <si>
     <t>GEOID</t>
   </si>
@@ -1754,6 +1891,12 @@
   </si>
   <si>
     <t>ln_MED_HH_INC</t>
+  </si>
+  <si>
+    <t>CCA_POP</t>
+  </si>
+  <si>
+    <t>TOT_MARKET_VAL</t>
   </si>
 </sst>
 </file>
@@ -1764,7 +1907,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1942,6 +2085,14 @@
     </font>
     <font>
       <i/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -2338,7 +2489,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2360,8 +2511,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -16984,9 +17140,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H67" sqref="H67"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16994,12 +17152,15 @@
     <col min="2" max="2" width="21.7109375" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="10"/>
-    <col min="7" max="7" width="15.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="26" customWidth="1"/>
+    <col min="7" max="7" width="19" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="10"/>
+    <col min="10" max="10" width="15.7109375" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>377</v>
       </c>
@@ -17012,17 +17173,26 @@
       <c r="D1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>380</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>14</v>
       </c>
@@ -17035,20 +17205,30 @@
       <c r="D2" s="22">
         <v>0.80584900000000004</v>
       </c>
-      <c r="E2" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F2" s="10">
+      <c r="E2">
+        <v>2659793284</v>
+      </c>
+      <c r="F2" s="26">
+        <v>51992</v>
+      </c>
+      <c r="G2" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E2/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F2)</f>
+        <v>26783.597043790694</v>
+      </c>
+      <c r="H2" s="10">
+        <f>LN(G2)</f>
+        <v>10.195544928514691</v>
+      </c>
+      <c r="I2" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G2" s="10">
+      <c r="J2" s="10">
         <f>LN(C2)</f>
         <v>10.97040636717122</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>57</v>
       </c>
@@ -17061,20 +17241,30 @@
       <c r="D3" s="22">
         <v>1</v>
       </c>
-      <c r="E3" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F3" s="10">
+      <c r="E3">
+        <v>754969900</v>
+      </c>
+      <c r="F3" s="26">
+        <v>13142</v>
+      </c>
+      <c r="G3" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E3/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F3)</f>
+        <v>28732.541248560938</v>
+      </c>
+      <c r="H3" s="10">
+        <f t="shared" ref="H3:H66" si="0">LN(G3)</f>
+        <v>10.265785600848284</v>
+      </c>
+      <c r="I3" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G3" s="10">
-        <f t="shared" ref="G3:G66" si="0">LN(C3)</f>
+      <c r="J3" s="10">
+        <f t="shared" ref="J3:J66" si="1">LN(C3)</f>
         <v>10.750044853062271</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>34</v>
       </c>
@@ -17087,20 +17277,30 @@
       <c r="D4" s="22">
         <v>0.99635399999999996</v>
       </c>
-      <c r="E4" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F4" s="10">
+      <c r="E4">
+        <v>944525082</v>
+      </c>
+      <c r="F4" s="26">
+        <v>13455</v>
+      </c>
+      <c r="G4" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E4/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F4)</f>
+        <v>32684.030693617187</v>
+      </c>
+      <c r="H4" s="10">
+        <f t="shared" si="0"/>
+        <v>10.394641879606384</v>
+      </c>
+      <c r="I4" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G4" s="10">
-        <f t="shared" si="0"/>
+      <c r="J4" s="10">
+        <f t="shared" si="1"/>
         <v>10.1836244818504</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>70</v>
       </c>
@@ -17113,20 +17313,30 @@
       <c r="D5" s="22">
         <v>0.68727899999999997</v>
       </c>
-      <c r="E5" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F5" s="10">
+      <c r="E5">
+        <v>2079280020</v>
+      </c>
+      <c r="F5" s="26">
+        <v>43792</v>
+      </c>
+      <c r="G5" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E5/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F5)</f>
+        <v>25644.195205065273</v>
+      </c>
+      <c r="H5" s="10">
+        <f t="shared" si="0"/>
+        <v>10.152072517192716</v>
+      </c>
+      <c r="I5" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G5" s="10">
-        <f t="shared" si="0"/>
+      <c r="J5" s="10">
+        <f t="shared" si="1"/>
         <v>11.105861028618182</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>71</v>
       </c>
@@ -17139,20 +17349,30 @@
       <c r="D6" s="22">
         <v>0.96716999999999997</v>
       </c>
-      <c r="E6" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F6" s="10">
+      <c r="E6">
+        <v>1741045138</v>
+      </c>
+      <c r="F6" s="26">
+        <v>46278</v>
+      </c>
+      <c r="G6" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E6/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F6)</f>
+        <v>22588.979507791788</v>
+      </c>
+      <c r="H6" s="10">
+        <f t="shared" si="0"/>
+        <v>10.025217433930441</v>
+      </c>
+      <c r="I6" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G6" s="10">
-        <f t="shared" si="0"/>
+      <c r="J6" s="10">
+        <f t="shared" si="1"/>
         <v>10.363888662310304</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25</v>
       </c>
@@ -17165,20 +17385,30 @@
       <c r="D7" s="22">
         <v>0.92270200000000002</v>
       </c>
-      <c r="E7" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F7" s="10">
+      <c r="E7">
+        <v>3879030006</v>
+      </c>
+      <c r="F7" s="26">
+        <v>95260</v>
+      </c>
+      <c r="G7" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E7/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F7)</f>
+        <v>23549.297184289673</v>
+      </c>
+      <c r="H7" s="10">
+        <f t="shared" si="0"/>
+        <v>10.066851255444657</v>
+      </c>
+      <c r="I7" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G7" s="10">
-        <f t="shared" si="0"/>
+      <c r="J7" s="10">
+        <f t="shared" si="1"/>
         <v>10.399495129318565</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>45</v>
       </c>
@@ -17191,20 +17421,30 @@
       <c r="D8" s="22">
         <v>0.35361599999999999</v>
       </c>
-      <c r="E8" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F8" s="10">
+      <c r="E8">
+        <v>570137718</v>
+      </c>
+      <c r="F8" s="26">
+        <v>9985</v>
+      </c>
+      <c r="G8" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E8/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F8)</f>
+        <v>28624.800094336581</v>
+      </c>
+      <c r="H8" s="10">
+        <f t="shared" si="0"/>
+        <v>10.262028757228194</v>
+      </c>
+      <c r="I8" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G8" s="10">
-        <f t="shared" si="0"/>
+      <c r="J8" s="10">
+        <f t="shared" si="1"/>
         <v>10.630896778119553</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>21</v>
       </c>
@@ -17217,20 +17457,30 @@
       <c r="D9" s="22">
         <v>0.70098700000000003</v>
       </c>
-      <c r="E9" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F9" s="10">
+      <c r="E9">
+        <v>2603323358</v>
+      </c>
+      <c r="F9" s="26">
+        <v>37368</v>
+      </c>
+      <c r="G9" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E9/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F9)</f>
+        <v>32519.288909987117</v>
+      </c>
+      <c r="H9" s="10">
+        <f t="shared" si="0"/>
+        <v>10.389588697186118</v>
+      </c>
+      <c r="I9" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G9" s="10">
-        <f t="shared" si="0"/>
+      <c r="J9" s="10">
+        <f t="shared" si="1"/>
         <v>10.853264703263591</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>19</v>
       </c>
@@ -17243,20 +17493,30 @@
       <c r="D10" s="22">
         <v>0.94839300000000004</v>
       </c>
-      <c r="E10" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F10" s="10">
+      <c r="E10">
+        <v>3634233774</v>
+      </c>
+      <c r="F10" s="26">
+        <v>79910</v>
+      </c>
+      <c r="G10" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E10/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F10)</f>
+        <v>25023.899832925606</v>
+      </c>
+      <c r="H10" s="10">
+        <f t="shared" si="0"/>
+        <v>10.127586640496776</v>
+      </c>
+      <c r="I10" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G10" s="10">
-        <f t="shared" si="0"/>
+      <c r="J10" s="10">
+        <f t="shared" si="1"/>
         <v>10.763481546279991</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>72</v>
       </c>
@@ -17269,20 +17529,30 @@
       <c r="D11" s="22">
         <v>1.812E-3</v>
       </c>
-      <c r="E11" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F11" s="10">
+      <c r="E11">
+        <v>2093954516</v>
+      </c>
+      <c r="F11" s="26">
+        <v>20822</v>
+      </c>
+      <c r="G11" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E11/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F11)</f>
+        <v>42093.732223488958</v>
+      </c>
+      <c r="H11" s="10">
+        <f t="shared" si="0"/>
+        <v>10.647654130285073</v>
+      </c>
+      <c r="I11" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G11" s="10">
-        <f t="shared" si="0"/>
+      <c r="J11" s="10">
+        <f t="shared" si="1"/>
         <v>11.428493413204896</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>60</v>
       </c>
@@ -17295,20 +17565,30 @@
       <c r="D12" s="22">
         <v>0.79158700000000004</v>
       </c>
-      <c r="E12" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F12" s="10">
+      <c r="E12">
+        <v>2404223012</v>
+      </c>
+      <c r="F12" s="26">
+        <v>33637</v>
+      </c>
+      <c r="G12" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E12/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F12)</f>
+        <v>33079.663151174842</v>
+      </c>
+      <c r="H12" s="10">
+        <f t="shared" si="0"/>
+        <v>10.406673966231333</v>
+      </c>
+      <c r="I12" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G12" s="10">
-        <f t="shared" si="0"/>
+      <c r="J12" s="10">
+        <f t="shared" si="1"/>
         <v>10.729212890286025</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>58</v>
       </c>
@@ -17321,20 +17601,30 @@
       <c r="D13" s="22">
         <v>1</v>
       </c>
-      <c r="E13" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F13" s="10">
+      <c r="E13">
+        <v>1486175062</v>
+      </c>
+      <c r="F13" s="26">
+        <v>44813</v>
+      </c>
+      <c r="G13" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E13/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F13)</f>
+        <v>21207.687950435946</v>
+      </c>
+      <c r="H13" s="10">
+        <f t="shared" si="0"/>
+        <v>9.9621190340939183</v>
+      </c>
+      <c r="I13" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G13" s="10">
-        <f t="shared" si="0"/>
+      <c r="J13" s="10">
+        <f t="shared" si="1"/>
         <v>10.609387322072662</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>47</v>
       </c>
@@ -17347,20 +17637,30 @@
       <c r="D14" s="22">
         <v>1</v>
       </c>
-      <c r="E14" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F14" s="10">
+      <c r="E14">
+        <v>148119010</v>
+      </c>
+      <c r="F14" s="26">
+        <v>2254</v>
+      </c>
+      <c r="G14" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E14/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F14)</f>
+        <v>31294.231555617636</v>
+      </c>
+      <c r="H14" s="10">
+        <f t="shared" si="0"/>
+        <v>10.35118906419609</v>
+      </c>
+      <c r="I14" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G14" s="10">
-        <f t="shared" si="0"/>
+      <c r="J14" s="10">
+        <f t="shared" si="1"/>
         <v>10.124265908980856</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>48</v>
       </c>
@@ -17373,20 +17673,30 @@
       <c r="D15" s="22">
         <v>0.32020399999999999</v>
       </c>
-      <c r="E15" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F15" s="10">
+      <c r="E15">
+        <v>750912554</v>
+      </c>
+      <c r="F15" s="26">
+        <v>13188</v>
+      </c>
+      <c r="G15" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E15/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F15)</f>
+        <v>28575.112995483159</v>
+      </c>
+      <c r="H15" s="10">
+        <f t="shared" si="0"/>
+        <v>10.26029144300281</v>
+      </c>
+      <c r="I15" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G15" s="10">
-        <f t="shared" si="0"/>
+      <c r="J15" s="10">
+        <f t="shared" si="1"/>
         <v>10.815120654472436</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>44</v>
       </c>
@@ -17399,20 +17709,30 @@
       <c r="D16" s="22">
         <v>0.68439499999999998</v>
       </c>
-      <c r="E16" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F16" s="10">
+      <c r="E16">
+        <v>1513980226</v>
+      </c>
+      <c r="F16" s="26">
+        <v>31120</v>
+      </c>
+      <c r="G16" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E16/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F16)</f>
+        <v>26006.42272950575</v>
+      </c>
+      <c r="H16" s="10">
+        <f t="shared" si="0"/>
+        <v>10.166098814555125</v>
+      </c>
+      <c r="I16" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G16" s="10">
-        <f t="shared" si="0"/>
+      <c r="J16" s="10">
+        <f t="shared" si="1"/>
         <v>10.391969403027637</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>66</v>
       </c>
@@ -17425,20 +17745,30 @@
       <c r="D17" s="22">
         <v>1</v>
       </c>
-      <c r="E17" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F17" s="10">
+      <c r="E17">
+        <v>1618153378</v>
+      </c>
+      <c r="F17" s="26">
+        <v>53098</v>
+      </c>
+      <c r="G17" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E17/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F17)</f>
+        <v>20374.397652133681</v>
+      </c>
+      <c r="H17" s="10">
+        <f t="shared" si="0"/>
+        <v>9.9220343745866035</v>
+      </c>
+      <c r="I17" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G17" s="10">
-        <f t="shared" si="0"/>
+      <c r="J17" s="10">
+        <f t="shared" si="1"/>
         <v>10.429505781994122</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>64</v>
       </c>
@@ -17451,20 +17781,30 @@
       <c r="D18" s="22">
         <v>0.29838300000000001</v>
       </c>
-      <c r="E18" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F18" s="10">
+      <c r="E18">
+        <v>1417070028</v>
+      </c>
+      <c r="F18" s="26">
+        <v>25891</v>
+      </c>
+      <c r="G18" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E18/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F18)</f>
+        <v>27891.231218524863</v>
+      </c>
+      <c r="H18" s="10">
+        <f t="shared" si="0"/>
+        <v>10.236067625166148</v>
+      </c>
+      <c r="I18" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G18" s="10">
-        <f t="shared" si="0"/>
+      <c r="J18" s="10">
+        <f t="shared" si="1"/>
         <v>11.041028203934991</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>35</v>
       </c>
@@ -17477,20 +17817,30 @@
       <c r="D19" s="22">
         <v>0.62422699999999998</v>
       </c>
-      <c r="E19" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F19" s="10">
+      <c r="E19">
+        <v>898295964</v>
+      </c>
+      <c r="F19" s="26">
+        <v>20781</v>
+      </c>
+      <c r="G19" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E19/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F19)</f>
+        <v>24325.960674676735</v>
+      </c>
+      <c r="H19" s="10">
+        <f t="shared" si="0"/>
+        <v>10.099299399580707</v>
+      </c>
+      <c r="I19" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G19" s="10">
-        <f t="shared" si="0"/>
+      <c r="J19" s="10">
+        <f t="shared" si="1"/>
         <v>10.370580073615216</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -17503,20 +17853,30 @@
       <c r="D20" s="22">
         <v>0.41344599999999998</v>
       </c>
-      <c r="E20" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F20" s="10">
+      <c r="E20">
+        <v>3351211692</v>
+      </c>
+      <c r="F20" s="26">
+        <v>43689</v>
+      </c>
+      <c r="G20" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E20/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F20)</f>
+        <v>34700.494601528771</v>
+      </c>
+      <c r="H20" s="10">
+        <f t="shared" si="0"/>
+        <v>10.45450921947973</v>
+      </c>
+      <c r="I20" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G20" s="10">
-        <f t="shared" si="0"/>
+      <c r="J20" s="10">
+        <f t="shared" si="1"/>
         <v>11.096616221184345</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>27</v>
       </c>
@@ -17529,20 +17889,30 @@
       <c r="D21" s="22">
         <v>1</v>
       </c>
-      <c r="E21" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F21" s="10">
+      <c r="E21">
+        <v>794197246</v>
+      </c>
+      <c r="F21" s="26">
+        <v>19996</v>
+      </c>
+      <c r="G21" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E21/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F21)</f>
+        <v>23238.598800575091</v>
+      </c>
+      <c r="H21" s="10">
+        <f t="shared" si="0"/>
+        <v>10.053569916573956</v>
+      </c>
+      <c r="I21" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G21" s="10">
-        <f t="shared" si="0"/>
+      <c r="J21" s="10">
+        <f t="shared" si="1"/>
         <v>10.048287219026451</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>52</v>
       </c>
@@ -17555,20 +17925,30 @@
       <c r="D22" s="22">
         <v>1</v>
       </c>
-      <c r="E22" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F22" s="10">
+      <c r="E22">
+        <v>801704354</v>
+      </c>
+      <c r="F22" s="26">
+        <v>23737</v>
+      </c>
+      <c r="G22" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E22/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F22)</f>
+        <v>21396.879390574555</v>
+      </c>
+      <c r="H22" s="10">
+        <f t="shared" si="0"/>
+        <v>9.9710003675064058</v>
+      </c>
+      <c r="I22" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G22" s="10">
-        <f t="shared" si="0"/>
+      <c r="J22" s="10">
+        <f t="shared" si="1"/>
         <v>10.674160429599166</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>77</v>
       </c>
@@ -17581,20 +17961,30 @@
       <c r="D23" s="22">
         <v>0.16884299999999999</v>
       </c>
-      <c r="E23" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F23" s="10">
+      <c r="E23">
+        <v>4436425520</v>
+      </c>
+      <c r="F23" s="26">
+        <v>55965</v>
+      </c>
+      <c r="G23" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E23/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F23)</f>
+        <v>35495.444604549441</v>
+      </c>
+      <c r="H23" s="10">
+        <f t="shared" si="0"/>
+        <v>10.477159646231057</v>
+      </c>
+      <c r="I23" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G23" s="10">
-        <f t="shared" si="0"/>
+      <c r="J23" s="10">
+        <f t="shared" si="1"/>
         <v>10.805415836467684</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>9</v>
       </c>
@@ -17607,20 +17997,30 @@
       <c r="D24" s="22">
         <v>0</v>
       </c>
-      <c r="E24" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F24" s="10">
+      <c r="E24">
+        <v>1366658654</v>
+      </c>
+      <c r="F24" s="26">
+        <v>11605</v>
+      </c>
+      <c r="G24" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E24/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F24)</f>
+        <v>47423.690949389551</v>
+      </c>
+      <c r="H24" s="10">
+        <f t="shared" si="0"/>
+        <v>10.766877191879075</v>
+      </c>
+      <c r="I24" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G24" s="10">
-        <f t="shared" si="0"/>
+      <c r="J24" s="10">
+        <f t="shared" si="1"/>
         <v>11.504834924634064</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>68</v>
       </c>
@@ -17633,20 +18033,30 @@
       <c r="D25" s="22">
         <v>1</v>
       </c>
-      <c r="E25" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F25" s="10">
+      <c r="E25">
+        <v>894960414</v>
+      </c>
+      <c r="F25" s="26">
+        <v>25075</v>
+      </c>
+      <c r="G25" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E25/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F25)</f>
+        <v>21990.881491045431</v>
+      </c>
+      <c r="H25" s="10">
+        <f t="shared" si="0"/>
+        <v>9.9983831687410838</v>
+      </c>
+      <c r="I25" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G25" s="10">
-        <f t="shared" si="0"/>
+      <c r="J25" s="10">
+        <f t="shared" si="1"/>
         <v>9.8931866802504906</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>12</v>
       </c>
@@ -17659,20 +18069,30 @@
       <c r="D26" s="22">
         <v>0</v>
       </c>
-      <c r="E26" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F26" s="10">
+      <c r="E26">
+        <v>2681457220</v>
+      </c>
+      <c r="F26" s="26">
+        <v>19019</v>
+      </c>
+      <c r="G26" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E26/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F26)</f>
+        <v>54620.232473096796</v>
+      </c>
+      <c r="H26" s="10">
+        <f t="shared" si="0"/>
+        <v>10.908159651208621</v>
+      </c>
+      <c r="I26" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G26" s="10">
-        <f t="shared" si="0"/>
+      <c r="J26" s="10">
+        <f t="shared" si="1"/>
         <v>11.611552682770766</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>37</v>
       </c>
@@ -17685,20 +18105,30 @@
       <c r="D27" s="22">
         <v>1</v>
       </c>
-      <c r="E27" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F27" s="10">
+      <c r="E27">
+        <v>118568640</v>
+      </c>
+      <c r="F27" s="26">
+        <v>2439</v>
+      </c>
+      <c r="G27" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E27/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F27)</f>
+        <v>25995.229378814405</v>
+      </c>
+      <c r="H27" s="10">
+        <f t="shared" si="0"/>
+        <v>10.165668314737893</v>
+      </c>
+      <c r="I27" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G27" s="10">
-        <f t="shared" si="0"/>
+      <c r="J27" s="10">
+        <f t="shared" si="1"/>
         <v>10.058657997939966</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>63</v>
       </c>
@@ -17711,20 +18141,30 @@
       <c r="D28" s="22">
         <v>1</v>
       </c>
-      <c r="E28" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F28" s="10">
+      <c r="E28">
+        <v>1035623032</v>
+      </c>
+      <c r="F28" s="26">
+        <v>40873</v>
+      </c>
+      <c r="G28" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E28/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F28)</f>
+        <v>18782.466594359947</v>
+      </c>
+      <c r="H28" s="10">
+        <f t="shared" si="0"/>
+        <v>9.8406790856904198</v>
+      </c>
+      <c r="I28" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G28" s="10">
-        <f t="shared" si="0"/>
+      <c r="J28" s="10">
+        <f t="shared" si="1"/>
         <v>10.624697027779037</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>56</v>
       </c>
@@ -17737,20 +18177,30 @@
       <c r="D29" s="22">
         <v>0.45426699999999998</v>
       </c>
-      <c r="E29" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F29" s="10">
+      <c r="E29">
+        <v>2437740184</v>
+      </c>
+      <c r="F29" s="26">
+        <v>36396</v>
+      </c>
+      <c r="G29" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E29/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F29)</f>
+        <v>31686.042197182069</v>
+      </c>
+      <c r="H29" s="10">
+        <f t="shared" si="0"/>
+        <v>10.363631553663637</v>
+      </c>
+      <c r="I29" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G29" s="10">
-        <f t="shared" si="0"/>
+      <c r="J29" s="10">
+        <f t="shared" si="1"/>
         <v>11.130374608617949</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>38</v>
       </c>
@@ -17763,20 +18213,30 @@
       <c r="D30" s="22">
         <v>0.89813600000000005</v>
       </c>
-      <c r="E30" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F30" s="10">
+      <c r="E30">
+        <v>1001902438</v>
+      </c>
+      <c r="F30" s="26">
+        <v>22313</v>
+      </c>
+      <c r="G30" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E30/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F30)</f>
+        <v>24845.129935497287</v>
+      </c>
+      <c r="H30" s="10">
+        <f t="shared" si="0"/>
+        <v>10.120417033867675</v>
+      </c>
+      <c r="I30" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G30" s="10">
-        <f t="shared" si="0"/>
+      <c r="J30" s="10">
+        <f t="shared" si="1"/>
         <v>10.372557308357788</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>69</v>
       </c>
@@ -17789,20 +18249,30 @@
       <c r="D31" s="22">
         <v>0.97275699999999998</v>
       </c>
-      <c r="E31" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F31" s="10">
+      <c r="E31">
+        <v>1277095082</v>
+      </c>
+      <c r="F31" s="26">
+        <v>31766</v>
+      </c>
+      <c r="G31" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E31/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F31)</f>
+        <v>23389.014608434183</v>
+      </c>
+      <c r="H31" s="10">
+        <f t="shared" si="0"/>
+        <v>10.060021729936366</v>
+      </c>
+      <c r="I31" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G31" s="10">
-        <f t="shared" si="0"/>
+      <c r="J31" s="10">
+        <f t="shared" si="1"/>
         <v>10.204903506997551</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>55</v>
       </c>
@@ -17815,20 +18285,30 @@
       <c r="D32" s="22">
         <v>1</v>
       </c>
-      <c r="E32" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F32" s="10">
+      <c r="E32">
+        <v>566863822</v>
+      </c>
+      <c r="F32" s="26">
+        <v>9418</v>
+      </c>
+      <c r="G32" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E32/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F32)</f>
+        <v>29582.322130484954</v>
+      </c>
+      <c r="H32" s="10">
+        <f t="shared" si="0"/>
+        <v>10.294932236580618</v>
+      </c>
+      <c r="I32" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G32" s="10">
-        <f t="shared" si="0"/>
+      <c r="J32" s="10">
+        <f t="shared" si="1"/>
         <v>10.922870649758847</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>20</v>
       </c>
@@ -17841,20 +18321,30 @@
       <c r="D33" s="22">
         <v>1</v>
       </c>
-      <c r="E33" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F33" s="10">
+      <c r="E33">
+        <v>1030057826</v>
+      </c>
+      <c r="F33" s="26">
+        <v>24144</v>
+      </c>
+      <c r="G33" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E33/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F33)</f>
+        <v>24151.283471277005</v>
+      </c>
+      <c r="H33" s="10">
+        <f t="shared" si="0"/>
+        <v>10.092092803477103</v>
+      </c>
+      <c r="I33" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G33" s="10">
-        <f t="shared" si="0"/>
+      <c r="J33" s="10">
+        <f t="shared" si="1"/>
         <v>10.586348005667922</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>23</v>
       </c>
@@ -17867,20 +18357,30 @@
       <c r="D34" s="22">
         <v>1</v>
       </c>
-      <c r="E34" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F34" s="10">
+      <c r="E34">
+        <v>2037895992</v>
+      </c>
+      <c r="F34" s="26">
+        <v>56427</v>
+      </c>
+      <c r="G34" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E34/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F34)</f>
+        <v>22122.355724363064</v>
+      </c>
+      <c r="H34" s="10">
+        <f t="shared" si="0"/>
+        <v>10.004343947450584</v>
+      </c>
+      <c r="I34" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G34" s="10">
-        <f t="shared" si="0"/>
+      <c r="J34" s="10">
+        <f t="shared" si="1"/>
         <v>10.489644000467457</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>41</v>
       </c>
@@ -17893,20 +18393,30 @@
       <c r="D35" s="22">
         <v>0.277254</v>
       </c>
-      <c r="E35" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F35" s="10">
+      <c r="E35">
+        <v>2075772076</v>
+      </c>
+      <c r="F35" s="26">
+        <v>26827</v>
+      </c>
+      <c r="G35" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E35/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F35)</f>
+        <v>34908.161307870818</v>
+      </c>
+      <c r="H35" s="10">
+        <f t="shared" si="0"/>
+        <v>10.460475929215313</v>
+      </c>
+      <c r="I35" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G35" s="10">
-        <f t="shared" si="0"/>
+      <c r="J35" s="10">
+        <f t="shared" si="1"/>
         <v>10.870986855208892</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>16</v>
       </c>
@@ -17919,20 +18429,30 @@
       <c r="D36" s="22">
         <v>0.60625300000000004</v>
       </c>
-      <c r="E36" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F36" s="10">
+      <c r="E36">
+        <v>3982377752</v>
+      </c>
+      <c r="F36" s="26">
+        <v>54606</v>
+      </c>
+      <c r="G36" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E36/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F36)</f>
+        <v>33530.152897002554</v>
+      </c>
+      <c r="H36" s="10">
+        <f t="shared" si="0"/>
+        <v>10.420200399455918</v>
+      </c>
+      <c r="I36" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G36" s="10">
-        <f t="shared" si="0"/>
+      <c r="J36" s="10">
+        <f t="shared" si="1"/>
         <v>10.994364500448309</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>11</v>
       </c>
@@ -17945,20 +18465,30 @@
       <c r="D37" s="22">
         <v>0.37053599999999998</v>
       </c>
-      <c r="E37" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F37" s="10">
+      <c r="E37">
+        <v>2247671506</v>
+      </c>
+      <c r="F37" s="26">
+        <v>26808</v>
+      </c>
+      <c r="G37" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E37/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F37)</f>
+        <v>36912.176133376794</v>
+      </c>
+      <c r="H37" s="10">
+        <f t="shared" si="0"/>
+        <v>10.516296752112618</v>
+      </c>
+      <c r="I37" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G37" s="10">
-        <f t="shared" si="0"/>
+      <c r="J37" s="10">
+        <f t="shared" si="1"/>
         <v>11.176881796500565</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>39</v>
       </c>
@@ -17971,20 +18501,30 @@
       <c r="D38" s="22">
         <v>0.73104400000000003</v>
       </c>
-      <c r="E38" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F38" s="10">
+      <c r="E38">
+        <v>1280660476</v>
+      </c>
+      <c r="F38" s="26">
+        <v>17189</v>
+      </c>
+      <c r="G38" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E38/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F38)</f>
+        <v>34018.319725469511</v>
+      </c>
+      <c r="H38" s="10">
+        <f t="shared" si="0"/>
+        <v>10.434654473944359</v>
+      </c>
+      <c r="I38" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G38" s="10">
-        <f t="shared" si="0"/>
+      <c r="J38" s="10">
+        <f t="shared" si="1"/>
         <v>10.69394246192479</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>6</v>
       </c>
@@ -17997,20 +18537,30 @@
       <c r="D39" s="22">
         <v>1.3212E-2</v>
       </c>
-      <c r="E39" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F39" s="10">
+      <c r="E39">
+        <v>14047386708</v>
+      </c>
+      <c r="F39" s="26">
+        <v>100470</v>
+      </c>
+      <c r="G39" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E39/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F39)</f>
+        <v>54257.174704338577</v>
+      </c>
+      <c r="H39" s="10">
+        <f t="shared" si="0"/>
+        <v>10.901490515272636</v>
+      </c>
+      <c r="I39" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G39" s="10">
-        <f t="shared" si="0"/>
+      <c r="J39" s="10">
+        <f t="shared" si="1"/>
         <v>11.363480927197566</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>7</v>
       </c>
@@ -18023,20 +18573,30 @@
       <c r="D40" s="22">
         <v>0</v>
       </c>
-      <c r="E40" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F40" s="10">
+      <c r="E40">
+        <v>14578988650</v>
+      </c>
+      <c r="F40" s="26">
+        <v>67710</v>
+      </c>
+      <c r="G40" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E40/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F40)</f>
+        <v>77652.565852034109</v>
+      </c>
+      <c r="H40" s="10">
+        <f t="shared" si="0"/>
+        <v>11.259999871843315</v>
+      </c>
+      <c r="I40" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G40" s="10">
-        <f t="shared" si="0"/>
+      <c r="J40" s="10">
+        <f t="shared" si="1"/>
         <v>11.509766179679822</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>4</v>
       </c>
@@ -18049,20 +18609,30 @@
       <c r="D41" s="22">
         <v>0.259739</v>
       </c>
-      <c r="E41" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F41" s="10">
+      <c r="E41">
+        <v>3907128224</v>
+      </c>
+      <c r="F41" s="26">
+        <v>41715</v>
+      </c>
+      <c r="G41" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E41/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F41)</f>
+        <v>39954.916446772375</v>
+      </c>
+      <c r="H41" s="10">
+        <f t="shared" si="0"/>
+        <v>10.595507008623105</v>
+      </c>
+      <c r="I41" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G41" s="10">
-        <f t="shared" si="0"/>
+      <c r="J41" s="10">
+        <f t="shared" si="1"/>
         <v>11.180760956749923</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>22</v>
       </c>
@@ -18075,20 +18645,30 @@
       <c r="D42" s="22">
         <v>0.62529599999999996</v>
       </c>
-      <c r="E42" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F42" s="10">
+      <c r="E42">
+        <v>6340183515</v>
+      </c>
+      <c r="F42" s="26">
+        <v>73046</v>
+      </c>
+      <c r="G42" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E42/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F42)</f>
+        <v>37827.504485523903</v>
+      </c>
+      <c r="H42" s="10">
+        <f t="shared" si="0"/>
+        <v>10.540791748904105</v>
+      </c>
+      <c r="I42" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G42" s="10">
-        <f t="shared" si="0"/>
+      <c r="J42" s="10">
+        <f t="shared" si="1"/>
         <v>11.161080836252781</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>31</v>
       </c>
@@ -18101,20 +18681,30 @@
       <c r="D43" s="22">
         <v>0.96367800000000003</v>
       </c>
-      <c r="E43" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F43" s="10">
+      <c r="E43">
+        <v>1797576361</v>
+      </c>
+      <c r="F43" s="26">
+        <v>32888</v>
+      </c>
+      <c r="G43" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E43/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F43)</f>
+        <v>27868.10426509337</v>
+      </c>
+      <c r="H43" s="10">
+        <f t="shared" si="0"/>
+        <v>10.235238097534333</v>
+      </c>
+      <c r="I43" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G43" s="10">
-        <f t="shared" si="0"/>
+      <c r="J43" s="10">
+        <f t="shared" si="1"/>
         <v>10.65626026775581</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>59</v>
       </c>
@@ -18127,20 +18717,30 @@
       <c r="D44" s="22">
         <v>1</v>
       </c>
-      <c r="E44" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F44" s="10">
+      <c r="E44">
+        <v>936927914</v>
+      </c>
+      <c r="F44" s="26">
+        <v>15767</v>
+      </c>
+      <c r="G44" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E44/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F44)</f>
+        <v>29344.936524643428</v>
+      </c>
+      <c r="H44" s="10">
+        <f t="shared" si="0"/>
+        <v>10.286875289917798</v>
+      </c>
+      <c r="I44" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G44" s="10">
-        <f t="shared" si="0"/>
+      <c r="J44" s="10">
+        <f t="shared" si="1"/>
         <v>10.712286833254606</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>18</v>
       </c>
@@ -18153,20 +18753,30 @@
       <c r="D45" s="22">
         <v>1</v>
       </c>
-      <c r="E45" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F45" s="10">
+      <c r="E45">
+        <v>861293526</v>
+      </c>
+      <c r="F45" s="26">
+        <v>13830</v>
+      </c>
+      <c r="G45" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E45/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F45)</f>
+        <v>30229.28286459564</v>
+      </c>
+      <c r="H45" s="10">
+        <f t="shared" si="0"/>
+        <v>10.316566364852211</v>
+      </c>
+      <c r="I45" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G45" s="10">
-        <f t="shared" si="0"/>
+      <c r="J45" s="10">
+        <f t="shared" si="1"/>
         <v>10.781501381727745</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>75</v>
       </c>
@@ -18179,20 +18789,30 @@
       <c r="D46" s="22">
         <v>0.32190200000000002</v>
       </c>
-      <c r="E46" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F46" s="10">
+      <c r="E46">
+        <v>1507879228</v>
+      </c>
+      <c r="F46" s="26">
+        <v>22394</v>
+      </c>
+      <c r="G46" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E46/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F46)</f>
+        <v>31796.306040479867</v>
+      </c>
+      <c r="H46" s="10">
+        <f t="shared" si="0"/>
+        <v>10.367105399771852</v>
+      </c>
+      <c r="I46" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G46" s="10">
-        <f t="shared" si="0"/>
+      <c r="J46" s="10">
+        <f t="shared" si="1"/>
         <v>10.982173456250395</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>74</v>
       </c>
@@ -18205,20 +18825,30 @@
       <c r="D47" s="22">
         <v>0.82890600000000003</v>
       </c>
-      <c r="E47" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F47" s="10">
+      <c r="E47">
+        <v>1514190318</v>
+      </c>
+      <c r="F47" s="26">
+        <v>19277</v>
+      </c>
+      <c r="G47" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E47/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F47)</f>
+        <v>35271.598906160376</v>
+      </c>
+      <c r="H47" s="10">
+        <f t="shared" si="0"/>
+        <v>10.470833355521552</v>
+      </c>
+      <c r="I47" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G47" s="10">
-        <f t="shared" si="0"/>
+      <c r="J47" s="10">
+        <f t="shared" si="1"/>
         <v>11.458227222425677</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>8</v>
       </c>
@@ -18231,20 +18861,30 @@
       <c r="D48" s="22">
         <v>7.0521E-2</v>
       </c>
-      <c r="E48" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F48" s="10">
+      <c r="E48">
+        <v>33135189222</v>
+      </c>
+      <c r="F48" s="26">
+        <v>88893</v>
+      </c>
+      <c r="G48" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E48/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F48)</f>
+        <v>126439.48246361231</v>
+      </c>
+      <c r="H48" s="10">
+        <f t="shared" si="0"/>
+        <v>11.747519073183026</v>
+      </c>
+      <c r="I48" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G48" s="10">
-        <f t="shared" si="0"/>
+      <c r="J48" s="10">
+        <f t="shared" si="1"/>
         <v>11.447930946548363</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>33</v>
       </c>
@@ -18257,20 +18897,30 @@
       <c r="D49" s="22">
         <v>0</v>
       </c>
-      <c r="E49" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F49" s="10">
+      <c r="E49">
+        <v>4768727942</v>
+      </c>
+      <c r="F49" s="26">
+        <v>23620</v>
+      </c>
+      <c r="G49" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E49/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F49)</f>
+        <v>73493.521706055486</v>
+      </c>
+      <c r="H49" s="10">
+        <f t="shared" si="0"/>
+        <v>11.204952541262699</v>
+      </c>
+      <c r="I49" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G49" s="10">
-        <f t="shared" si="0"/>
+      <c r="J49" s="10">
+        <f t="shared" si="1"/>
         <v>11.45266322748466</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>28</v>
       </c>
@@ -18283,20 +18933,30 @@
       <c r="D50" s="22">
         <v>0.44980900000000001</v>
       </c>
-      <c r="E50" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F50" s="10">
+      <c r="E50">
+        <v>10440604502</v>
+      </c>
+      <c r="F50" s="26">
+        <v>62872</v>
+      </c>
+      <c r="G50" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E50/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F50)</f>
+        <v>62389.814376055292</v>
+      </c>
+      <c r="H50" s="10">
+        <f t="shared" si="0"/>
+        <v>11.041157309880905</v>
+      </c>
+      <c r="I50" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G50" s="10">
-        <f t="shared" si="0"/>
+      <c r="J50" s="10">
+        <f t="shared" si="1"/>
         <v>11.298833573498596</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>61</v>
       </c>
@@ -18309,20 +18969,30 @@
       <c r="D51" s="22">
         <v>1</v>
       </c>
-      <c r="E51" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F51" s="10">
+      <c r="E51">
+        <v>1579895413</v>
+      </c>
+      <c r="F51" s="26">
+        <v>39561</v>
+      </c>
+      <c r="G51" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E51/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F51)</f>
+        <v>23306.113284522944</v>
+      </c>
+      <c r="H51" s="10">
+        <f t="shared" si="0"/>
+        <v>10.056470977866395</v>
+      </c>
+      <c r="I51" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G51" s="10">
-        <f t="shared" si="0"/>
+      <c r="J51" s="10">
+        <f t="shared" si="1"/>
         <v>10.400066167936412</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>5</v>
       </c>
@@ -18335,20 +19005,30 @@
       <c r="D52" s="22">
         <v>0</v>
       </c>
-      <c r="E52" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F52" s="10">
+      <c r="E52">
+        <v>5394259962</v>
+      </c>
+      <c r="F52" s="26">
+        <v>35789</v>
+      </c>
+      <c r="G52" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E52/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F52)</f>
+        <v>57637.100455053172</v>
+      </c>
+      <c r="H52" s="10">
+        <f t="shared" si="0"/>
+        <v>10.96192174445976</v>
+      </c>
+      <c r="I52" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G52" s="10">
-        <f t="shared" si="0"/>
+      <c r="J52" s="10">
+        <f t="shared" si="1"/>
         <v>11.555517603860098</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>29</v>
       </c>
@@ -18361,20 +19041,30 @@
       <c r="D53" s="22">
         <v>1</v>
       </c>
-      <c r="E53" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F53" s="10">
+      <c r="E53">
+        <v>1239730090</v>
+      </c>
+      <c r="F53" s="26">
+        <v>35947</v>
+      </c>
+      <c r="G53" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E53/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F53)</f>
+        <v>21617.904046535616</v>
+      </c>
+      <c r="H53" s="10">
+        <f t="shared" si="0"/>
+        <v>9.9812771413751058</v>
+      </c>
+      <c r="I53" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G53" s="10">
-        <f t="shared" si="0"/>
+      <c r="J53" s="10">
+        <f t="shared" si="1"/>
         <v>10.179675444261576</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>13</v>
       </c>
@@ -18387,20 +19077,30 @@
       <c r="D54" s="22">
         <v>0.62323300000000004</v>
       </c>
-      <c r="E54" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F54" s="10">
+      <c r="E54">
+        <v>1445636974</v>
+      </c>
+      <c r="F54" s="26">
+        <v>18842</v>
+      </c>
+      <c r="G54" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E54/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F54)</f>
+        <v>34706.104676873314</v>
+      </c>
+      <c r="H54" s="10">
+        <f t="shared" si="0"/>
+        <v>10.454670877748976</v>
+      </c>
+      <c r="I54" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G54" s="10">
-        <f t="shared" si="0"/>
+      <c r="J54" s="10">
+        <f t="shared" si="1"/>
         <v>10.934658622424207</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>10</v>
       </c>
@@ -18413,20 +19113,30 @@
       <c r="D55" s="22">
         <v>0.37513800000000003</v>
       </c>
-      <c r="E55" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F55" s="10">
+      <c r="E55">
+        <v>3766875396</v>
+      </c>
+      <c r="F55" s="26">
+        <v>37089</v>
+      </c>
+      <c r="G55" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E55/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F55)</f>
+        <v>42403.183416315922</v>
+      </c>
+      <c r="H55" s="10">
+        <f t="shared" si="0"/>
+        <v>10.654978718975133</v>
+      </c>
+      <c r="I55" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G55" s="10">
-        <f t="shared" si="0"/>
+      <c r="J55" s="10">
+        <f t="shared" si="1"/>
         <v>11.212757500511927</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>76</v>
       </c>
@@ -18439,20 +19149,30 @@
       <c r="D56" s="22">
         <v>0.48297400000000001</v>
       </c>
-      <c r="E56" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F56" s="10">
+      <c r="E56">
+        <v>1703679258</v>
+      </c>
+      <c r="F56" s="26">
+        <v>12377</v>
+      </c>
+      <c r="G56" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E56/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F56)</f>
+        <v>53585.380240825099</v>
+      </c>
+      <c r="H56" s="10">
+        <f t="shared" si="0"/>
+        <v>10.889031553152995</v>
+      </c>
+      <c r="I56" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G56" s="10">
-        <f t="shared" si="0"/>
+      <c r="J56" s="10">
+        <f t="shared" si="1"/>
         <v>10.805575297821365</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>36</v>
       </c>
@@ -18465,20 +19185,30 @@
       <c r="D57" s="22">
         <v>1</v>
       </c>
-      <c r="E57" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F57" s="10">
+      <c r="E57">
+        <v>257005596</v>
+      </c>
+      <c r="F57" s="26">
+        <v>6645</v>
+      </c>
+      <c r="G57" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E57/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F57)</f>
+        <v>22915.93157570099</v>
+      </c>
+      <c r="H57" s="10">
+        <f t="shared" si="0"/>
+        <v>10.039587649649556</v>
+      </c>
+      <c r="I57" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G57" s="10">
-        <f t="shared" si="0"/>
+      <c r="J57" s="10">
+        <f t="shared" si="1"/>
         <v>10.250315271306119</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>15</v>
       </c>
@@ -18491,20 +19221,30 @@
       <c r="D58" s="22">
         <v>0.47638200000000003</v>
       </c>
-      <c r="E58" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F58" s="10">
+      <c r="E58">
+        <v>4366334126</v>
+      </c>
+      <c r="F58" s="26">
+        <v>64307</v>
+      </c>
+      <c r="G58" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E58/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F58)</f>
+        <v>31971.139375697825</v>
+      </c>
+      <c r="H58" s="10">
+        <f t="shared" si="0"/>
+        <v>10.372588880320864</v>
+      </c>
+      <c r="I58" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G58" s="10">
-        <f t="shared" si="0"/>
+      <c r="J58" s="10">
+        <f t="shared" si="1"/>
         <v>11.025043771268599</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>50</v>
       </c>
@@ -18517,20 +19257,30 @@
       <c r="D59" s="22">
         <v>0.50225799999999998</v>
       </c>
-      <c r="E59" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F59" s="10">
+      <c r="E59">
+        <v>407871248</v>
+      </c>
+      <c r="F59" s="26">
+        <v>6613</v>
+      </c>
+      <c r="G59" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E59/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F59)</f>
+        <v>30043.355151909902</v>
+      </c>
+      <c r="H59" s="10">
+        <f t="shared" si="0"/>
+        <v>10.310396789118959</v>
+      </c>
+      <c r="I59" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G59" s="10">
-        <f t="shared" si="0"/>
+      <c r="J59" s="10">
+        <f t="shared" si="1"/>
         <v>10.613050749942245</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>54</v>
       </c>
@@ -18543,20 +19293,30 @@
       <c r="D60" s="22">
         <v>1</v>
       </c>
-      <c r="E60" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F60" s="10">
+      <c r="E60">
+        <v>108928208</v>
+      </c>
+      <c r="F60" s="26">
+        <v>7394</v>
+      </c>
+      <c r="G60" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E60/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F60)</f>
+        <v>15496.008425484353</v>
+      </c>
+      <c r="H60" s="10">
+        <f t="shared" si="0"/>
+        <v>9.6483377488066342</v>
+      </c>
+      <c r="I60" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G60" s="10">
-        <f t="shared" si="0"/>
+      <c r="J60" s="10">
+        <f t="shared" si="1"/>
         <v>9.4988753306171159</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1</v>
       </c>
@@ -18569,20 +19329,30 @@
       <c r="D61" s="22">
         <v>0.66960799999999998</v>
       </c>
-      <c r="E61" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F61" s="10">
+      <c r="E61">
+        <v>2685562288</v>
+      </c>
+      <c r="F61" s="26">
+        <v>55062</v>
+      </c>
+      <c r="G61" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E61/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F61)</f>
+        <v>26044.74676065021</v>
+      </c>
+      <c r="H61" s="10">
+        <f t="shared" si="0"/>
+        <v>10.167571366985552</v>
+      </c>
+      <c r="I61" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G61" s="10">
-        <f t="shared" si="0"/>
+      <c r="J61" s="10">
+        <f t="shared" si="1"/>
         <v>10.574035789749866</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>49</v>
       </c>
@@ -18595,20 +19365,30 @@
       <c r="D62" s="22">
         <v>0.95604299999999998</v>
       </c>
-      <c r="E62" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F62" s="10">
+      <c r="E62">
+        <v>1685199866</v>
+      </c>
+      <c r="F62" s="26">
+        <v>42433</v>
+      </c>
+      <c r="G62" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E62/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F62)</f>
+        <v>23237.534126277824</v>
+      </c>
+      <c r="H62" s="10">
+        <f t="shared" si="0"/>
+        <v>10.05352410061508</v>
+      </c>
+      <c r="I62" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G62" s="10">
-        <f t="shared" si="0"/>
+      <c r="J62" s="10">
+        <f t="shared" si="1"/>
         <v>10.563223750726763</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>46</v>
       </c>
@@ -18621,20 +19401,30 @@
       <c r="D63" s="22">
         <v>1</v>
       </c>
-      <c r="E63" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F63" s="10">
+      <c r="E63">
+        <v>1104081620</v>
+      </c>
+      <c r="F63" s="26">
+        <v>28263</v>
+      </c>
+      <c r="G63" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E63/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F63)</f>
+        <v>23036.171052973212</v>
+      </c>
+      <c r="H63" s="10">
+        <f t="shared" si="0"/>
+        <v>10.044820914062322</v>
+      </c>
+      <c r="I63" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G63" s="10">
-        <f t="shared" si="0"/>
+      <c r="J63" s="10">
+        <f t="shared" si="1"/>
         <v>10.294877062564739</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>51</v>
       </c>
@@ -18647,20 +19437,30 @@
       <c r="D64" s="22">
         <v>0.784076</v>
       </c>
-      <c r="E64" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F64" s="10">
+      <c r="E64">
+        <v>717231930</v>
+      </c>
+      <c r="F64" s="26">
+        <v>14614</v>
+      </c>
+      <c r="G64" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E64/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F64)</f>
+        <v>26139.256476460665</v>
+      </c>
+      <c r="H64" s="10">
+        <f t="shared" si="0"/>
+        <v>10.171193542873933</v>
+      </c>
+      <c r="I64" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G64" s="10">
-        <f t="shared" si="0"/>
+      <c r="J64" s="10">
+        <f t="shared" si="1"/>
         <v>10.436869362015482</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>30</v>
       </c>
@@ -18673,20 +19473,30 @@
       <c r="D65" s="22">
         <v>1</v>
       </c>
-      <c r="E65" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F65" s="10">
+      <c r="E65">
+        <v>1821836720</v>
+      </c>
+      <c r="F65" s="26">
+        <v>74851</v>
+      </c>
+      <c r="G65" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E65/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F65)</f>
+        <v>18473.184733602589</v>
+      </c>
+      <c r="H65" s="10">
+        <f t="shared" si="0"/>
+        <v>9.8240754857036556</v>
+      </c>
+      <c r="I65" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G65" s="10">
-        <f t="shared" si="0"/>
+      <c r="J65" s="10">
+        <f t="shared" si="1"/>
         <v>10.401107564767406</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>43</v>
       </c>
@@ -18699,20 +19509,30 @@
       <c r="D66" s="22">
         <v>1</v>
       </c>
-      <c r="E66" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F66" s="10">
+      <c r="E66">
+        <v>1997858988</v>
+      </c>
+      <c r="F66" s="26">
+        <v>50418</v>
+      </c>
+      <c r="G66" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E66/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F66)</f>
+        <v>23210.121307837871</v>
+      </c>
+      <c r="H66" s="10">
+        <f t="shared" si="0"/>
+        <v>10.052343725788123</v>
+      </c>
+      <c r="I66" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G66" s="10">
-        <f t="shared" si="0"/>
+      <c r="J66" s="10">
+        <f t="shared" si="1"/>
         <v>10.100066981076782</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>32</v>
       </c>
@@ -18725,20 +19545,30 @@
       <c r="D67" s="22">
         <v>0</v>
       </c>
-      <c r="E67" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F67" s="10">
+      <c r="E67">
+        <v>23772500457</v>
+      </c>
+      <c r="F67" s="26">
+        <v>35880</v>
+      </c>
+      <c r="G67" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E67/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F67)</f>
+        <v>216243.13543527765</v>
+      </c>
+      <c r="H67" s="10">
+        <f t="shared" ref="H67:H78" si="2">LN(G67)</f>
+        <v>12.28415868063839</v>
+      </c>
+      <c r="I67" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G67" s="10">
-        <f t="shared" ref="G67:G78" si="1">LN(C67)</f>
+      <c r="J67" s="10">
+        <f t="shared" ref="J67:J78" si="3">LN(C67)</f>
         <v>11.545743803515675</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>3</v>
       </c>
@@ -18751,20 +19581,30 @@
       <c r="D68" s="22">
         <v>0.24413699999999999</v>
       </c>
-      <c r="E68" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F68" s="10">
+      <c r="E68">
+        <v>4284953458</v>
+      </c>
+      <c r="F68" s="26">
+        <v>57973</v>
+      </c>
+      <c r="G68" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E68/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F68)</f>
+        <v>33834.952692314095</v>
+      </c>
+      <c r="H68" s="10">
+        <f t="shared" si="2"/>
+        <v>10.429249650477498</v>
+      </c>
+      <c r="I68" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G68" s="10">
-        <f t="shared" si="1"/>
+      <c r="J68" s="10">
+        <f t="shared" si="3"/>
         <v>10.813375832385297</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>73</v>
       </c>
@@ -18777,20 +19617,30 @@
       <c r="D69" s="22">
         <v>0.99457099999999998</v>
       </c>
-      <c r="E69" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F69" s="10">
+      <c r="E69">
+        <v>1207325418</v>
+      </c>
+      <c r="F69" s="26">
+        <v>27453</v>
+      </c>
+      <c r="G69" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E69/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F69)</f>
+        <v>24558.714902427004</v>
+      </c>
+      <c r="H69" s="10">
+        <f t="shared" si="2"/>
+        <v>10.10882205607234</v>
+      </c>
+      <c r="I69" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G69" s="10">
-        <f t="shared" si="1"/>
+      <c r="J69" s="10">
+        <f t="shared" si="3"/>
         <v>10.707876420709034</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>40</v>
       </c>
@@ -18803,20 +19653,30 @@
       <c r="D70" s="22">
         <v>1</v>
       </c>
-      <c r="E70" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F70" s="10">
+      <c r="E70">
+        <v>362904358</v>
+      </c>
+      <c r="F70" s="26">
+        <v>11502</v>
+      </c>
+      <c r="G70" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E70/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F70)</f>
+        <v>20708.003515875884</v>
+      </c>
+      <c r="H70" s="10">
+        <f t="shared" si="2"/>
+        <v>9.9382755478052367</v>
+      </c>
+      <c r="I70" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G70" s="10">
-        <f t="shared" si="1"/>
+      <c r="J70" s="10">
+        <f t="shared" si="3"/>
         <v>10.141898757799291</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>62</v>
       </c>
@@ -18829,20 +19689,30 @@
       <c r="D71" s="22">
         <v>1</v>
       </c>
-      <c r="E71" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F71" s="10">
+      <c r="E71">
+        <v>766975378</v>
+      </c>
+      <c r="F71" s="26">
+        <v>19237</v>
+      </c>
+      <c r="G71" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E71/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F71)</f>
+        <v>23285.699195768437</v>
+      </c>
+      <c r="H71" s="10">
+        <f t="shared" si="2"/>
+        <v>10.055594682698892</v>
+      </c>
+      <c r="I71" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G71" s="10">
-        <f t="shared" si="1"/>
+      <c r="J71" s="10">
+        <f t="shared" si="3"/>
         <v>10.912346526719206</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>67</v>
       </c>
@@ -18855,20 +19725,30 @@
       <c r="D72" s="22">
         <v>1</v>
       </c>
-      <c r="E72" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F72" s="10">
+      <c r="E72">
+        <v>1016982636</v>
+      </c>
+      <c r="F72" s="26">
+        <v>29929</v>
+      </c>
+      <c r="G72" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E72/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F72)</f>
+        <v>21460.522471931414</v>
+      </c>
+      <c r="H72" s="10">
+        <f t="shared" si="2"/>
+        <v>9.9739703622038594</v>
+      </c>
+      <c r="I72" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G72" s="10">
-        <f t="shared" si="1"/>
+      <c r="J72" s="10">
+        <f t="shared" si="3"/>
         <v>10.240184049723347</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>26</v>
       </c>
@@ -18881,20 +19761,30 @@
       <c r="D73" s="22">
         <v>1</v>
       </c>
-      <c r="E73" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F73" s="10">
+      <c r="E73">
+        <v>633053518</v>
+      </c>
+      <c r="F73" s="26">
+        <v>17163</v>
+      </c>
+      <c r="G73" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E73/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F73)</f>
+        <v>22360.703662421103</v>
+      </c>
+      <c r="H73" s="10">
+        <f t="shared" si="2"/>
+        <v>10.015060396470703</v>
+      </c>
+      <c r="I73" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G73" s="10">
-        <f t="shared" si="1"/>
+      <c r="J73" s="10">
+        <f t="shared" si="3"/>
         <v>10.054060411015502</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>65</v>
       </c>
@@ -18907,20 +19797,30 @@
       <c r="D74" s="22">
         <v>1</v>
       </c>
-      <c r="E74" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F74" s="10">
+      <c r="E74">
+        <v>1446745734</v>
+      </c>
+      <c r="F74" s="26">
+        <v>33108</v>
+      </c>
+      <c r="G74" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E74/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F74)</f>
+        <v>24471.906648380776</v>
+      </c>
+      <c r="H74" s="10">
+        <f t="shared" si="2"/>
+        <v>10.105281071193714</v>
+      </c>
+      <c r="I74" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G74" s="10">
-        <f t="shared" si="1"/>
+      <c r="J74" s="10">
+        <f t="shared" si="3"/>
         <v>10.829686634184238</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>53</v>
       </c>
@@ -18933,20 +19833,30 @@
       <c r="D75" s="22">
         <v>0.99952799999999997</v>
       </c>
-      <c r="E75" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F75" s="10">
+      <c r="E75">
+        <v>1093720378</v>
+      </c>
+      <c r="F75" s="26">
+        <v>27742</v>
+      </c>
+      <c r="G75" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E75/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F75)</f>
+        <v>23147.775301600788</v>
+      </c>
+      <c r="H75" s="10">
+        <f t="shared" si="2"/>
+        <v>10.049653955613644</v>
+      </c>
+      <c r="I75" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G75" s="10">
-        <f t="shared" si="1"/>
+      <c r="J75" s="10">
+        <f t="shared" si="3"/>
         <v>10.549136596399558</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2</v>
       </c>
@@ -18959,20 +19869,30 @@
       <c r="D76" s="22">
         <v>0.76276699999999997</v>
       </c>
-      <c r="E76" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F76" s="10">
+      <c r="E76">
+        <v>4150290418</v>
+      </c>
+      <c r="F76" s="26">
+        <v>76215</v>
+      </c>
+      <c r="G76" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E76/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F76)</f>
+        <v>27805.359545566072</v>
+      </c>
+      <c r="H76" s="10">
+        <f t="shared" si="2"/>
+        <v>10.23298407050609</v>
+      </c>
+      <c r="I76" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G76" s="10">
-        <f t="shared" si="1"/>
+      <c r="J76" s="10">
+        <f t="shared" si="3"/>
         <v>10.816880690436655</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>24</v>
       </c>
@@ -18985,20 +19905,30 @@
       <c r="D77" s="22">
         <v>0.28186299999999997</v>
       </c>
-      <c r="E77" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F77" s="10">
+      <c r="E77">
+        <v>10560793326</v>
+      </c>
+      <c r="F77" s="26">
+        <v>84502</v>
+      </c>
+      <c r="G77" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E77/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F77)</f>
+        <v>49658.603105971808</v>
+      </c>
+      <c r="H77" s="10">
+        <f t="shared" si="2"/>
+        <v>10.812926929507681</v>
+      </c>
+      <c r="I77" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G77" s="10">
-        <f t="shared" si="1"/>
+      <c r="J77" s="10">
+        <f t="shared" si="3"/>
         <v>11.393703206629556</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>42</v>
       </c>
@@ -19011,16 +19941,26 @@
       <c r="D78" s="22">
         <v>1</v>
       </c>
-      <c r="E78" s="10">
-        <f>FACTORS_MUNI!$L$42</f>
-        <v>10.552822172456036</v>
-      </c>
-      <c r="F78" s="10">
+      <c r="E78">
+        <v>840107106</v>
+      </c>
+      <c r="F78" s="26">
+        <v>23268</v>
+      </c>
+      <c r="G78" s="27">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E78/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F78)</f>
+        <v>22119.277976259509</v>
+      </c>
+      <c r="H78" s="10">
+        <f t="shared" si="2"/>
+        <v>10.004204813885611</v>
+      </c>
+      <c r="I78" s="10">
         <f>FACTORS_MUNI!$M$42</f>
         <v>14.810979870415512</v>
       </c>
-      <c r="G78" s="10">
-        <f t="shared" si="1"/>
+      <c r="J78" s="10">
+        <f t="shared" si="3"/>
         <v>10.131509584688109</v>
       </c>
     </row>
@@ -19146,7 +20086,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Give COVID death rate a negative weight
High death rates should yield a lower score, not higher
</commit_message>
<xml_diff>
--- a/input/community_cohort_inputs.xlsx
+++ b/input/community_cohort_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmp/Documents/GitHub/community-cohort-tool/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C619E10-CAD6-9A47-B7C8-680C7348F399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8831C94-A72C-294F-86D5-EF7D00EF5E82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1600" windowWidth="30780" windowHeight="19240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="660" windowWidth="31720" windowHeight="19840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FACTORS_MUNI" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="COHORTS" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FACTORS_MUNI!$A$1:$R$285</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FACTORS_MUNI!$A$1:$S$285</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -281,7 +281,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> Total COVID-19 deaths as of ?/?/2020, per Cook County Medical Examiner</t>
+          <t xml:space="preserve"> Total COVID-19 deaths as of 6/8/2020, per Cook County Medical Examiner</t>
         </r>
       </text>
     </comment>
@@ -484,7 +484,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -520,7 +520,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -533,7 +533,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -543,7 +543,7 @@
           <rPr>
             <i/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -552,7 +552,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1673,13 +1673,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
@@ -1709,6 +1702,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2453,7 +2453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S285"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2543,7 +2543,7 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="15">
         <v>36724</v>
@@ -2677,7 +2677,7 @@
         <v>15</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="15">
         <v>18880</v>
@@ -2744,7 +2744,7 @@
         <v>16</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="15">
         <v>14258</v>
@@ -2945,7 +2945,7 @@
         <v>19</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="15">
         <v>1602</v>
@@ -3012,7 +3012,7 @@
         <v>20</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="15">
         <v>10274</v>
@@ -3079,7 +3079,7 @@
         <v>21</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="15">
         <v>4207</v>
@@ -3146,7 +3146,7 @@
         <v>22</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="15">
         <v>40931</v>
@@ -3347,7 +3347,7 @@
         <v>25</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="15">
         <v>601</v>
@@ -3414,7 +3414,7 @@
         <v>26</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="15">
         <v>4460</v>
@@ -3481,7 +3481,7 @@
         <v>27</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="15">
         <v>18839</v>
@@ -3548,7 +3548,7 @@
         <v>28</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="15">
         <v>18226</v>
@@ -3615,7 +3615,7 @@
         <v>29</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="15">
         <v>5073</v>
@@ -3682,7 +3682,7 @@
         <v>30</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="15">
         <v>54917</v>
@@ -3749,7 +3749,7 @@
         <v>31</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="15">
         <v>1142</v>
@@ -3816,7 +3816,7 @@
         <v>32</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="15">
         <v>21894</v>
@@ -3883,7 +3883,7 @@
         <v>33</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="15">
         <v>23112</v>
@@ -4017,7 +4017,7 @@
         <v>35</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="15">
         <v>760</v>
@@ -4218,7 +4218,7 @@
         <v>38</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="15">
         <v>7692</v>
@@ -4352,7 +4352,7 @@
         <v>40</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" s="15">
         <v>40853</v>
@@ -4486,7 +4486,7 @@
         <v>42</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="15">
         <v>28534</v>
@@ -4754,7 +4754,7 @@
         <v>46</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="15">
         <v>36240</v>
@@ -4821,7 +4821,7 @@
         <v>47</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" s="15">
         <v>7672</v>
@@ -4888,7 +4888,7 @@
         <v>48</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" s="15">
         <v>11192</v>
@@ -4955,7 +4955,7 @@
         <v>49</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" s="15">
         <v>39601</v>
@@ -5156,7 +5156,7 @@
         <v>52</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" s="15">
         <v>13086</v>
@@ -5290,7 +5290,7 @@
         <v>54</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43" s="15">
         <v>29571</v>
@@ -5491,7 +5491,7 @@
         <v>57</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" s="15">
         <v>8785</v>
@@ -5558,7 +5558,7 @@
         <v>58</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47" s="15">
         <v>5368</v>
@@ -5759,7 +5759,7 @@
         <v>61</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50" s="15">
         <v>20568</v>
@@ -5826,7 +5826,7 @@
         <v>62</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51" s="15">
         <v>10770</v>
@@ -6027,7 +6027,7 @@
         <v>65</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54" s="15">
         <v>21954</v>
@@ -6228,7 +6228,7 @@
         <v>68</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57" s="15">
         <v>58959</v>
@@ -6362,7 +6362,7 @@
         <v>70</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D59" s="15">
         <v>3616</v>
@@ -6563,7 +6563,7 @@
         <v>73</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D62" s="15">
         <v>3192</v>
@@ -6697,7 +6697,7 @@
         <v>75</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D64" s="15">
         <v>5926</v>
@@ -6764,7 +6764,7 @@
         <v>76</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D65" s="15">
         <v>111683</v>
@@ -6831,7 +6831,7 @@
         <v>77</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D66" s="15">
         <v>32458</v>
@@ -6898,7 +6898,7 @@
         <v>78</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67" s="15">
         <v>46558</v>
@@ -6965,7 +6965,7 @@
         <v>79</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68" s="15">
         <v>24263</v>
@@ -7032,7 +7032,7 @@
         <v>80</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D69" s="15">
         <v>2260</v>
@@ -7099,7 +7099,7 @@
         <v>81</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70" s="15">
         <v>74106</v>
@@ -7300,7 +7300,7 @@
         <v>84</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D73" s="15">
         <v>2705</v>
@@ -7501,7 +7501,7 @@
         <v>87</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D76" s="15">
         <v>10481</v>
@@ -7836,7 +7836,7 @@
         <v>92</v>
       </c>
       <c r="C81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D81" s="15">
         <v>8097</v>
@@ -7903,7 +7903,7 @@
         <v>93</v>
       </c>
       <c r="C82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D82" s="15">
         <v>27928</v>
@@ -8238,7 +8238,7 @@
         <v>98</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D87" s="15">
         <v>737</v>
@@ -8372,7 +8372,7 @@
         <v>100</v>
       </c>
       <c r="C89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D89" s="15">
         <v>20903</v>
@@ -8506,7 +8506,7 @@
         <v>102</v>
       </c>
       <c r="C91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D91" s="15">
         <v>250</v>
@@ -8640,7 +8640,7 @@
         <v>104</v>
       </c>
       <c r="C93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D93" s="15">
         <v>3608</v>
@@ -8774,7 +8774,7 @@
         <v>106</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D95" s="15">
         <v>37747</v>
@@ -8841,7 +8841,7 @@
         <v>107</v>
       </c>
       <c r="C96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D96" s="15">
         <v>9130</v>
@@ -9511,7 +9511,7 @@
         <v>117</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D106" s="15">
         <v>17652</v>
@@ -9578,7 +9578,7 @@
         <v>118</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D107" s="15">
         <v>1885</v>
@@ -9779,7 +9779,7 @@
         <v>121</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D110" s="15">
         <v>24582</v>
@@ -10047,7 +10047,7 @@
         <v>125</v>
       </c>
       <c r="C114">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D114" s="15">
         <v>534</v>
@@ -10114,7 +10114,7 @@
         <v>126</v>
       </c>
       <c r="C115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D115" s="15">
         <v>3751</v>
@@ -10315,7 +10315,7 @@
         <v>129</v>
       </c>
       <c r="C118">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D118" s="15">
         <v>9867</v>
@@ -10382,7 +10382,7 @@
         <v>130</v>
       </c>
       <c r="C119">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D119" s="15">
         <v>6324</v>
@@ -10717,7 +10717,7 @@
         <v>135</v>
       </c>
       <c r="C124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D124" s="15">
         <v>4019</v>
@@ -10784,7 +10784,7 @@
         <v>136</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D125" s="15">
         <v>15440</v>
@@ -10851,7 +10851,7 @@
         <v>137</v>
       </c>
       <c r="C126">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D126" s="15">
         <v>13296</v>
@@ -10918,7 +10918,7 @@
         <v>138</v>
       </c>
       <c r="C127">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D127" s="15">
         <v>4879</v>
@@ -10985,7 +10985,7 @@
         <v>139</v>
       </c>
       <c r="C128">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D128" s="15">
         <v>5617</v>
@@ -11253,7 +11253,7 @@
         <v>143</v>
       </c>
       <c r="C132">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D132" s="15">
         <v>20022</v>
@@ -11320,7 +11320,7 @@
         <v>144</v>
       </c>
       <c r="C133">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D133" s="15">
         <v>6014</v>
@@ -11387,7 +11387,7 @@
         <v>145</v>
       </c>
       <c r="C134">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D134" s="15">
         <v>3985</v>
@@ -11521,7 +11521,7 @@
         <v>147</v>
       </c>
       <c r="C136">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D136" s="15">
         <v>17155</v>
@@ -11588,7 +11588,7 @@
         <v>148</v>
       </c>
       <c r="C137">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D137" s="15">
         <v>20359</v>
@@ -11655,7 +11655,7 @@
         <v>149</v>
       </c>
       <c r="C138">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D138" s="15">
         <v>1032</v>
@@ -11789,7 +11789,7 @@
         <v>151</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D140" s="15">
         <v>12349</v>
@@ -11923,7 +11923,7 @@
         <v>153</v>
       </c>
       <c r="C142">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D142" s="15">
         <v>311</v>
@@ -12124,7 +12124,7 @@
         <v>156</v>
       </c>
       <c r="C145">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D145" s="15">
         <v>44523</v>
@@ -12392,7 +12392,7 @@
         <v>160</v>
       </c>
       <c r="C149">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D149" s="15">
         <v>7999</v>
@@ -12925,7 +12925,7 @@
         <v>168</v>
       </c>
       <c r="C157">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D157" s="15">
         <v>27022</v>
@@ -13059,7 +13059,7 @@
         <v>170</v>
       </c>
       <c r="C159">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D159" s="15">
         <v>1865</v>
@@ -13193,7 +13193,7 @@
         <v>172</v>
       </c>
       <c r="C161">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D161" s="15">
         <v>14476</v>
@@ -13260,7 +13260,7 @@
         <v>173</v>
       </c>
       <c r="C162">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D162" s="15">
         <v>330</v>
@@ -13327,7 +13327,7 @@
         <v>174</v>
       </c>
       <c r="C163">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D163" s="15">
         <v>668</v>
@@ -13394,7 +13394,7 @@
         <v>175</v>
       </c>
       <c r="C164">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D164" s="15">
         <v>11352</v>
@@ -13595,7 +13595,7 @@
         <v>178</v>
       </c>
       <c r="C167">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D167" s="15">
         <v>19749</v>
@@ -13662,7 +13662,7 @@
         <v>179</v>
       </c>
       <c r="C168">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D168" s="15">
         <v>22943</v>
@@ -13863,7 +13863,7 @@
         <v>182</v>
       </c>
       <c r="C171">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D171" s="15">
         <v>148304</v>
@@ -13930,7 +13930,7 @@
         <v>183</v>
       </c>
       <c r="C172">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D172" s="15">
         <v>26780</v>
@@ -13997,7 +13997,7 @@
         <v>184</v>
       </c>
       <c r="C173">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D173" s="15">
         <v>1040</v>
@@ -14064,7 +14064,7 @@
         <v>185</v>
       </c>
       <c r="C174">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D174" s="15">
         <v>29184</v>
@@ -14131,7 +14131,7 @@
         <v>186</v>
       </c>
       <c r="C175">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D175" s="15">
         <v>14281</v>
@@ -14265,7 +14265,7 @@
         <v>188</v>
       </c>
       <c r="C177">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D177" s="15">
         <v>2970</v>
@@ -14399,7 +14399,7 @@
         <v>190</v>
       </c>
       <c r="C179">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D179" s="15">
         <v>6489</v>
@@ -14466,7 +14466,7 @@
         <v>191</v>
       </c>
       <c r="C180">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D180" s="15">
         <v>33167</v>
@@ -14533,7 +14533,7 @@
         <v>192</v>
       </c>
       <c r="C181">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D181" s="15">
         <v>5422</v>
@@ -14600,7 +14600,7 @@
         <v>193</v>
       </c>
       <c r="C182">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D182" s="15">
         <v>12235</v>
@@ -14667,7 +14667,7 @@
         <v>194</v>
       </c>
       <c r="C183">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D183" s="15">
         <v>8074</v>
@@ -14801,7 +14801,7 @@
         <v>196</v>
       </c>
       <c r="C185">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D185" s="15">
         <v>55511</v>
@@ -15002,7 +15002,7 @@
         <v>199</v>
       </c>
       <c r="C188">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D188" s="15">
         <v>2041</v>
@@ -15069,7 +15069,7 @@
         <v>200</v>
       </c>
       <c r="C189">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D189" s="15">
         <v>173</v>
@@ -15133,7 +15133,7 @@
         <v>201</v>
       </c>
       <c r="C190">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D190" s="15">
         <v>4833</v>
@@ -15334,7 +15334,7 @@
         <v>204</v>
       </c>
       <c r="C193">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D193" s="15">
         <v>35237</v>
@@ -15468,7 +15468,7 @@
         <v>206</v>
       </c>
       <c r="C195">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D195" s="15">
         <v>12626</v>
@@ -15602,7 +15602,7 @@
         <v>208</v>
       </c>
       <c r="C197">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D197" s="15">
         <v>4778</v>
@@ -15669,7 +15669,7 @@
         <v>209</v>
       </c>
       <c r="C198">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D198" s="15">
         <v>7457</v>
@@ -15870,7 +15870,7 @@
         <v>212</v>
       </c>
       <c r="C201">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D201" s="15">
         <v>4136</v>
@@ -15937,7 +15937,7 @@
         <v>213</v>
       </c>
       <c r="C202">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D202" s="15">
         <v>1925</v>
@@ -16004,7 +16004,7 @@
         <v>214</v>
       </c>
       <c r="C203">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D203" s="15">
         <v>8976</v>
@@ -16071,7 +16071,7 @@
         <v>215</v>
       </c>
       <c r="C204">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D204" s="15">
         <v>44138</v>
@@ -16269,7 +16269,7 @@
         <v>218</v>
       </c>
       <c r="C207">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D207" s="15">
         <v>1488</v>
@@ -16470,7 +16470,7 @@
         <v>221</v>
       </c>
       <c r="C210">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D210" s="15">
         <v>16014</v>
@@ -16604,7 +16604,7 @@
         <v>223</v>
       </c>
       <c r="C212">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D212" s="15">
         <v>13409</v>
@@ -16738,7 +16738,7 @@
         <v>225</v>
       </c>
       <c r="C214">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D214" s="15">
         <v>10903</v>
@@ -16805,7 +16805,7 @@
         <v>226</v>
       </c>
       <c r="C215">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D215" s="15">
         <v>9979</v>
@@ -16872,7 +16872,7 @@
         <v>227</v>
       </c>
       <c r="C216">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D216" s="15">
         <v>13205</v>
@@ -16939,7 +16939,7 @@
         <v>228</v>
       </c>
       <c r="C217">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D217" s="15">
         <v>8645</v>
@@ -17140,7 +17140,7 @@
         <v>231</v>
       </c>
       <c r="C220">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D220" s="15">
         <v>1931</v>
@@ -17274,7 +17274,7 @@
         <v>233</v>
       </c>
       <c r="C222">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D222" s="15">
         <v>39624</v>
@@ -17341,7 +17341,7 @@
         <v>234</v>
       </c>
       <c r="C223">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D223" s="15">
         <v>22656</v>
@@ -17408,7 +17408,7 @@
         <v>235</v>
       </c>
       <c r="C224">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D224" s="15">
         <v>4107</v>
@@ -17810,7 +17810,7 @@
         <v>241</v>
       </c>
       <c r="C230">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D230" s="15">
         <v>10346</v>
@@ -18212,7 +18212,7 @@
         <v>247</v>
       </c>
       <c r="C236">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D236" s="15">
         <v>4993</v>
@@ -18279,7 +18279,7 @@
         <v>248</v>
       </c>
       <c r="C237">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D237" s="15">
         <v>4042</v>
@@ -18681,7 +18681,7 @@
         <v>254</v>
       </c>
       <c r="C243">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D243" s="15">
         <v>6620</v>
@@ -18815,7 +18815,7 @@
         <v>256</v>
       </c>
       <c r="C245">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D245" s="15">
         <v>39570</v>
@@ -19016,7 +19016,7 @@
         <v>259</v>
       </c>
       <c r="C248">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D248" s="15">
         <v>94</v>
@@ -19080,7 +19080,7 @@
         <v>260</v>
       </c>
       <c r="C249">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D249" s="15">
         <v>1156</v>
@@ -19214,7 +19214,7 @@
         <v>262</v>
       </c>
       <c r="C251">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D251" s="15">
         <v>56204</v>
@@ -19415,7 +19415,7 @@
         <v>265</v>
       </c>
       <c r="C254">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D254" s="15">
         <v>556</v>
@@ -19683,7 +19683,7 @@
         <v>269</v>
       </c>
       <c r="C258">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D258" s="15">
         <v>331</v>
@@ -19817,7 +19817,7 @@
         <v>271</v>
       </c>
       <c r="C260">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D260" s="15">
         <v>3681</v>
@@ -20018,7 +20018,7 @@
         <v>274</v>
       </c>
       <c r="C263">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D263" s="15">
         <v>86792</v>
@@ -20085,7 +20085,7 @@
         <v>275</v>
       </c>
       <c r="C264">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D264" s="15">
         <v>2425</v>
@@ -20152,7 +20152,7 @@
         <v>276</v>
       </c>
       <c r="C265">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D265" s="15">
         <v>27045</v>
@@ -20286,7 +20286,7 @@
         <v>278</v>
       </c>
       <c r="C267">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D267" s="15">
         <v>16279</v>
@@ -20353,7 +20353,7 @@
         <v>279</v>
       </c>
       <c r="C268">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D268" s="15">
         <v>13404</v>
@@ -20420,7 +20420,7 @@
         <v>280</v>
       </c>
       <c r="C269">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D269" s="15">
         <v>24647</v>
@@ -20554,7 +20554,7 @@
         <v>282</v>
       </c>
       <c r="C271">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D271" s="15">
         <v>38878</v>
@@ -20621,7 +20621,7 @@
         <v>283</v>
       </c>
       <c r="C272">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D272" s="15">
         <v>5668</v>
@@ -20688,7 +20688,7 @@
         <v>284</v>
       </c>
       <c r="C273">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D273" s="15">
         <v>8493</v>
@@ -20889,7 +20889,7 @@
         <v>287</v>
       </c>
       <c r="C276">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D276" s="15">
         <v>9690</v>
@@ -20956,7 +20956,7 @@
         <v>288</v>
       </c>
       <c r="C277">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D277" s="15">
         <v>12385</v>
@@ -21090,7 +21090,7 @@
         <v>290</v>
       </c>
       <c r="C279">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D279" s="15">
         <v>3884</v>
@@ -21157,7 +21157,7 @@
         <v>291</v>
       </c>
       <c r="C280">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D280" s="15">
         <v>13717</v>
@@ -21224,7 +21224,7 @@
         <v>292</v>
       </c>
       <c r="C281">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D281" s="15">
         <v>33566</v>
@@ -21291,7 +21291,7 @@
         <v>293</v>
       </c>
       <c r="C282">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D282" s="15">
         <v>25268</v>
@@ -21358,7 +21358,7 @@
         <v>294</v>
       </c>
       <c r="C283">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D283" s="15">
         <v>10563</v>
@@ -21562,9 +21562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -21621,7 +21619,7 @@
         <v>306</v>
       </c>
       <c r="B6" s="2">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -21640,30 +21638,15 @@
   <conditionalFormatting sqref="A2:A1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A1048576">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(ISNA(HLOOKUP(A2,#REF!, 1, FALSE)), A2&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{A36205D5-D3BC-40FB-8028-6B3A6753CC9E}">
-            <xm:f>AND(ISNA(HLOOKUP(A2,#REF!, 1, FALSE)), A2&lt;&gt;"")</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF800000"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFF7C80"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A2:A1048576</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
@@ -21682,8 +21665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21705,7 +21688,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>37</v>
+        <v>37.777999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -21713,7 +21696,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>45</v>
+        <v>58.889000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -21721,7 +21704,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>65</v>
+        <v>75.555999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Reverse pop scoring, improved documentation in notes
</commit_message>
<xml_diff>
--- a/input/community_cohort_inputs.xlsx
+++ b/input/community_cohort_inputs.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmp/Documents/GitHub/community-cohort-tool/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D413E3D3-94B6-5E4A-9D49-6384545F144E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10361AB5-5001-2546-BB4B-AD97F6833D07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="660" windowWidth="31720" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="FACTORS_MUNI" sheetId="1" r:id="rId1"/>
+    <sheet name="FACTORS" sheetId="1" r:id="rId1"/>
     <sheet name="WEIGHTS" sheetId="2" r:id="rId2"/>
     <sheet name="COHORTS" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FACTORS_MUNI!$A$1:$P$285</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FACTORS!$A$1:$P$285</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +63,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Municipality name for each of the 284 munis in the CMAP region</t>
+          <t>Municipality name</t>
         </r>
       </text>
     </comment>
@@ -71,22 +71,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>INPUT:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Binary indicator of whether municipality is taxed by Cook County (1) or not (0)</t>
+          <t>Binary indicator of whether municipality is taxed by Cook County (1) or not (0)</t>
         </r>
       </text>
     </comment>
@@ -109,7 +99,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Latest population from Census Population Estimates Program.</t>
+          <t>2018 population estimate from Census Population Estimates Program (2018 vintage)</t>
         </r>
       </text>
     </comment>
@@ -132,7 +122,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Median household income, from latest 5-year ACS (reported in Community Data Snapshots)</t>
+          <t>Median household income, from 2017 5-year ACS (reported in CMAP Community Data Snapshots)</t>
         </r>
       </text>
     </comment>
@@ -155,7 +145,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Total retail sales from Community Data Snapshots</t>
+          <t>2017 total retail sales from IL Dept. of Revenue (reported in CMAP Community Data Snapshots)</t>
         </r>
       </text>
     </comment>
@@ -178,7 +168,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Total Equalized Assessed Value from Community Data Snapshots</t>
+          <t>2017 total equalized assessed value from IL Dept. of Revenue (reported in CMAP Community Data Snapshots)</t>
         </r>
       </text>
     </comment>
@@ -201,7 +191,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Percent of population living in an EDA or disinvested area, calculated from 2015 PBHI and EDA/disinvested layer</t>
+          <t>Percent of population living in an EDA or disinvested area, calculated from CMAP's 2015 parcel-level population estimates and CMAP's EDA/disinvested layer</t>
         </r>
       </text>
     </comment>
@@ -408,7 +398,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Names of columns from FACTORS_MUNI sheet to be included in cohort calculations. If column does not also exist in FACTORS_CCA, cell will be highlighted in red. Duplicate names will be highlighted in yellow.</t>
+          <t>Names of columns from FACTORS sheet to be included in cohort calculations. Duplicate names will be highlighted in yellow.</t>
         </r>
       </text>
     </comment>
@@ -417,7 +407,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1407,7 +1397,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1556,12 +1546,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1980,7 +1964,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1992,15 +1976,13 @@
     <xf numFmtId="2" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2368,7 +2350,7 @@
     <col min="13" max="13" width="8.6640625" style="10" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.83203125" style="10" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.33203125" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -2417,7 +2399,7 @@
       <c r="O1" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="P1" s="9" t="s">
         <v>303</v>
       </c>
     </row>
@@ -2473,7 +2455,7 @@
         <f t="shared" ref="O2:O65" si="5">I2/D2*100000</f>
         <v>13.615074610608866</v>
       </c>
-      <c r="P2" s="19">
+      <c r="P2" s="10">
         <f>LN(O2+1)</f>
         <v>2.6820535036209185</v>
       </c>
@@ -2530,7 +2512,7 @@
         <f t="shared" si="5"/>
         <v>3.2351989647363317</v>
       </c>
-      <c r="P3" s="19">
+      <c r="P3" s="10">
         <f t="shared" ref="P3:P66" si="6">LN(O3+1)</f>
         <v>1.4434303080479829</v>
       </c>
@@ -2587,7 +2569,7 @@
         <f t="shared" si="5"/>
         <v>15.889830508474574</v>
       </c>
-      <c r="P4" s="19">
+      <c r="P4" s="10">
         <f t="shared" si="6"/>
         <v>2.8267116957471297</v>
       </c>
@@ -2644,7 +2626,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P5" s="19">
+      <c r="P5" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2701,7 +2683,7 @@
         <f t="shared" si="5"/>
         <v>38.538718122499972</v>
       </c>
-      <c r="P6" s="19">
+      <c r="P6" s="10">
         <f t="shared" si="6"/>
         <v>3.6772803974521429</v>
       </c>
@@ -2758,7 +2740,7 @@
         <f t="shared" si="5"/>
         <v>1.5029909519944689</v>
       </c>
-      <c r="P7" s="19">
+      <c r="P7" s="10">
         <f t="shared" si="6"/>
         <v>0.91748639757872819</v>
       </c>
@@ -2815,7 +2797,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P8" s="19">
+      <c r="P8" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2872,7 +2854,7 @@
         <f t="shared" si="5"/>
         <v>29.199922133540976</v>
       </c>
-      <c r="P9" s="19">
+      <c r="P9" s="10">
         <f t="shared" si="6"/>
         <v>3.4078393460179295</v>
       </c>
@@ -2929,7 +2911,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P10" s="19">
+      <c r="P10" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2986,7 +2968,7 @@
         <f t="shared" si="5"/>
         <v>2.4431360093816421</v>
       </c>
-      <c r="P11" s="19">
+      <c r="P11" s="10">
         <f t="shared" si="6"/>
         <v>1.2363826867366692</v>
       </c>
@@ -3043,7 +3025,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P12" s="19">
+      <c r="P12" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3100,7 +3082,7 @@
         <f t="shared" si="5"/>
         <v>7.2113651114155912</v>
       </c>
-      <c r="P13" s="19">
+      <c r="P13" s="10">
         <f t="shared" si="6"/>
         <v>2.1055191838707614</v>
       </c>
@@ -3157,7 +3139,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P14" s="19">
+      <c r="P14" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3214,7 +3196,7 @@
         <f t="shared" si="5"/>
         <v>22.421524663677129</v>
       </c>
-      <c r="P15" s="19">
+      <c r="P15" s="10">
         <f t="shared" si="6"/>
         <v>3.1536554569761801</v>
       </c>
@@ -3271,7 +3253,7 @@
         <f t="shared" si="5"/>
         <v>47.773236371357292</v>
       </c>
-      <c r="P16" s="19">
+      <c r="P16" s="10">
         <f t="shared" si="6"/>
         <v>3.8871817274004403</v>
       </c>
@@ -3328,7 +3310,7 @@
         <f t="shared" si="5"/>
         <v>21.946669592889279</v>
       </c>
-      <c r="P17" s="19">
+      <c r="P17" s="10">
         <f t="shared" si="6"/>
         <v>3.1331728101979959</v>
       </c>
@@ -3385,7 +3367,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P18" s="19">
+      <c r="P18" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3442,7 +3424,7 @@
         <f t="shared" si="5"/>
         <v>63.73254183586139</v>
       </c>
-      <c r="P19" s="19">
+      <c r="P19" s="10">
         <f t="shared" si="6"/>
         <v>4.1702640400679387</v>
       </c>
@@ -3499,7 +3481,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P20" s="19">
+      <c r="P20" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3556,7 +3538,7 @@
         <f t="shared" si="5"/>
         <v>41.107152644560152</v>
       </c>
-      <c r="P21" s="19">
+      <c r="P21" s="10">
         <f t="shared" si="6"/>
         <v>3.7402176228029238</v>
       </c>
@@ -3613,7 +3595,7 @@
         <f t="shared" si="5"/>
         <v>51.921079958463132</v>
       </c>
-      <c r="P22" s="19">
+      <c r="P22" s="10">
         <f t="shared" si="6"/>
         <v>3.9688017464168932</v>
       </c>
@@ -3670,7 +3652,7 @@
         <f t="shared" si="5"/>
         <v>1.330176381388172</v>
       </c>
-      <c r="P23" s="19">
+      <c r="P23" s="10">
         <f t="shared" si="6"/>
         <v>0.84594396487909362</v>
       </c>
@@ -3727,7 +3709,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P24" s="19">
+      <c r="P24" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3784,7 +3766,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P25" s="19">
+      <c r="P25" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3841,7 +3823,7 @@
         <f t="shared" si="5"/>
         <v>160.62272193735714</v>
       </c>
-      <c r="P26" s="19">
+      <c r="P26" s="10">
         <f t="shared" si="6"/>
         <v>5.0852647422508932</v>
       </c>
@@ -3898,7 +3880,7 @@
         <f t="shared" si="5"/>
         <v>78.003120124804994</v>
       </c>
-      <c r="P27" s="19">
+      <c r="P27" s="10">
         <f t="shared" si="6"/>
         <v>4.3694873469378006</v>
       </c>
@@ -3955,7 +3937,7 @@
         <f t="shared" si="5"/>
         <v>16.221477235860277</v>
       </c>
-      <c r="P28" s="19">
+      <c r="P28" s="10">
         <f t="shared" si="6"/>
         <v>2.8461572813747753</v>
       </c>
@@ -4012,7 +3994,7 @@
         <f t="shared" si="5"/>
         <v>34.269209115609627</v>
       </c>
-      <c r="P29" s="19">
+      <c r="P29" s="10">
         <f t="shared" si="6"/>
         <v>3.5630103202826136</v>
       </c>
@@ -4069,7 +4051,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P30" s="19">
+      <c r="P30" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -4126,7 +4108,7 @@
         <f t="shared" si="5"/>
         <v>73.596411298801428</v>
       </c>
-      <c r="P31" s="19">
+      <c r="P31" s="10">
         <f t="shared" si="6"/>
         <v>4.3120924001383987</v>
       </c>
@@ -4183,7 +4165,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P32" s="19">
+      <c r="P32" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -4240,7 +4222,7 @@
         <f t="shared" si="5"/>
         <v>72.833211944646763</v>
       </c>
-      <c r="P33" s="19">
+      <c r="P33" s="10">
         <f t="shared" si="6"/>
         <v>4.3018086567251661</v>
       </c>
@@ -4297,7 +4279,7 @@
         <f t="shared" si="5"/>
         <v>18.516803999629666</v>
       </c>
-      <c r="P34" s="19">
+      <c r="P34" s="10">
         <f t="shared" si="6"/>
         <v>2.9712758380526352</v>
       </c>
@@ -4354,7 +4336,7 @@
         <f t="shared" si="5"/>
         <v>13.796909492273731</v>
       </c>
-      <c r="P35" s="19">
+      <c r="P35" s="10">
         <f t="shared" si="6"/>
         <v>2.6944183408749236</v>
       </c>
@@ -4411,7 +4393,7 @@
         <f t="shared" si="5"/>
         <v>39.103232533889468</v>
       </c>
-      <c r="P36" s="19">
+      <c r="P36" s="10">
         <f t="shared" si="6"/>
         <v>3.691456942881258</v>
       </c>
@@ -4468,7 +4450,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P37" s="19">
+      <c r="P37" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -4525,7 +4507,7 @@
         <f t="shared" si="5"/>
         <v>2.5251887578596501</v>
       </c>
-      <c r="P38" s="19">
+      <c r="P38" s="10">
         <f t="shared" si="6"/>
         <v>1.2599339831595502</v>
       </c>
@@ -4582,7 +4564,7 @@
         <f t="shared" si="5"/>
         <v>15.896566341670201</v>
       </c>
-      <c r="P39" s="19">
+      <c r="P39" s="10">
         <f t="shared" si="6"/>
         <v>2.827110426237081</v>
       </c>
@@ -4639,7 +4621,7 @@
         <f t="shared" si="5"/>
         <v>5.6217674836968747</v>
       </c>
-      <c r="P40" s="19">
+      <c r="P40" s="10">
         <f t="shared" si="6"/>
         <v>1.8903623258080267</v>
       </c>
@@ -4696,7 +4678,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P41" s="19">
+      <c r="P41" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -4753,7 +4735,7 @@
         <f t="shared" si="5"/>
         <v>81.892273227508994</v>
       </c>
-      <c r="P42" s="19">
+      <c r="P42" s="10">
         <f t="shared" si="6"/>
         <v>4.4175418518565213</v>
       </c>
@@ -4810,7 +4792,7 @@
         <f t="shared" si="5"/>
         <v>101.45074566298062</v>
       </c>
-      <c r="P43" s="19">
+      <c r="P43" s="10">
         <f t="shared" si="6"/>
         <v>4.6293821529696046</v>
       </c>
@@ -4867,7 +4849,7 @@
         <f t="shared" si="5"/>
         <v>241.9928825622776</v>
       </c>
-      <c r="P44" s="19">
+      <c r="P44" s="10">
         <f t="shared" si="6"/>
         <v>5.4930321530444219</v>
       </c>
@@ -4924,7 +4906,7 @@
         <f t="shared" si="5"/>
         <v>85.787467676507717</v>
       </c>
-      <c r="P45" s="19">
+      <c r="P45" s="10">
         <f t="shared" si="6"/>
         <v>4.4634622296352227</v>
       </c>
@@ -4981,7 +4963,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P46" s="19">
+      <c r="P46" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5038,7 +5020,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P47" s="19">
+      <c r="P47" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5095,7 +5077,7 @@
         <f t="shared" si="5"/>
         <v>175.64048210284054</v>
       </c>
-      <c r="P48" s="19">
+      <c r="P48" s="10">
         <f t="shared" si="6"/>
         <v>5.1741164923809784</v>
       </c>
@@ -5152,7 +5134,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P49" s="19">
+      <c r="P49" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5209,7 +5191,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P50" s="19">
+      <c r="P50" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5266,7 +5248,7 @@
         <f t="shared" si="5"/>
         <v>129.99071494893224</v>
       </c>
-      <c r="P51" s="19">
+      <c r="P51" s="10">
         <f t="shared" si="6"/>
         <v>4.875126442436744</v>
       </c>
@@ -5323,7 +5305,7 @@
         <f t="shared" si="5"/>
         <v>49.279290378218555</v>
       </c>
-      <c r="P52" s="19">
+      <c r="P52" s="10">
         <f t="shared" si="6"/>
         <v>3.9175932702218659</v>
       </c>
@@ -5380,7 +5362,7 @@
         <f t="shared" si="5"/>
         <v>4.9955040463582776</v>
       </c>
-      <c r="P53" s="19">
+      <c r="P53" s="10">
         <f t="shared" si="6"/>
         <v>1.7910098627363438</v>
       </c>
@@ -5437,7 +5419,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P54" s="19">
+      <c r="P54" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5494,7 +5476,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P55" s="19">
+      <c r="P55" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5551,7 +5533,7 @@
         <f t="shared" si="5"/>
         <v>42.600777464188724</v>
       </c>
-      <c r="P56" s="19">
+      <c r="P56" s="10">
         <f t="shared" si="6"/>
         <v>3.7750749819434528</v>
       </c>
@@ -5608,7 +5590,7 @@
         <f t="shared" si="5"/>
         <v>144.16798113943588</v>
       </c>
-      <c r="P57" s="19">
+      <c r="P57" s="10">
         <f t="shared" si="6"/>
         <v>4.9778915625049391</v>
       </c>
@@ -5665,7 +5647,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P58" s="19">
+      <c r="P58" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5722,7 +5704,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P59" s="19">
+      <c r="P59" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5779,7 +5761,7 @@
         <f t="shared" si="5"/>
         <v>79.833237237769993</v>
       </c>
-      <c r="P60" s="19">
+      <c r="P60" s="10">
         <f t="shared" si="6"/>
         <v>4.3923882328976287</v>
       </c>
@@ -5836,7 +5818,7 @@
         <f t="shared" si="5"/>
         <v>2.0248243464879421</v>
       </c>
-      <c r="P61" s="19">
+      <c r="P61" s="10">
         <f t="shared" si="6"/>
         <v>1.1068530225201219</v>
       </c>
@@ -5893,7 +5875,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P62" s="19">
+      <c r="P62" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5950,7 +5932,7 @@
         <f t="shared" si="5"/>
         <v>198.54401058901388</v>
       </c>
-      <c r="P63" s="19">
+      <c r="P63" s="10">
         <f t="shared" si="6"/>
         <v>5.2960348164565429</v>
       </c>
@@ -6007,7 +5989,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P64" s="19">
+      <c r="P64" s="10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -6064,7 +6046,7 @@
         <f t="shared" si="5"/>
         <v>3.58156568143764</v>
       </c>
-      <c r="P65" s="19">
+      <c r="P65" s="10">
         <f t="shared" si="6"/>
         <v>1.5220407915503451</v>
       </c>
@@ -6121,7 +6103,7 @@
         <f t="shared" ref="O66:O129" si="12">I66/D66*100000</f>
         <v>89.346232053730972</v>
       </c>
-      <c r="P66" s="19">
+      <c r="P66" s="10">
         <f t="shared" si="6"/>
         <v>4.5036493122807366</v>
       </c>
@@ -6178,7 +6160,7 @@
         <f t="shared" si="12"/>
         <v>2.1478585849907641</v>
       </c>
-      <c r="P67" s="19">
+      <c r="P67" s="10">
         <f t="shared" ref="P67:P130" si="13">LN(O67+1)</f>
         <v>1.1467224073703837</v>
       </c>
@@ -6235,7 +6217,7 @@
         <f t="shared" si="12"/>
         <v>82.430037505667059</v>
       </c>
-      <c r="P68" s="19">
+      <c r="P68" s="10">
         <f t="shared" si="13"/>
         <v>4.4240084064604126</v>
       </c>
@@ -6292,7 +6274,7 @@
         <f t="shared" si="12"/>
         <v>44.247787610619469</v>
       </c>
-      <c r="P69" s="19">
+      <c r="P69" s="10">
         <f t="shared" si="13"/>
         <v>3.8121537763676585</v>
       </c>
@@ -6349,7 +6331,7 @@
         <f t="shared" si="12"/>
         <v>76.916848838150756</v>
       </c>
-      <c r="P70" s="19">
+      <c r="P70" s="10">
         <f t="shared" si="13"/>
         <v>4.3556422175276959</v>
       </c>
@@ -6406,7 +6388,7 @@
         <f t="shared" si="12"/>
         <v>62.095730918499356</v>
       </c>
-      <c r="P71" s="19">
+      <c r="P71" s="10">
         <f t="shared" si="13"/>
         <v>4.1446531114501592</v>
       </c>
@@ -6463,7 +6445,7 @@
         <f t="shared" si="12"/>
         <v>86.608206127530579</v>
       </c>
-      <c r="P72" s="19">
+      <c r="P72" s="10">
         <f t="shared" si="13"/>
         <v>4.472874670809821</v>
       </c>
@@ -6520,7 +6502,7 @@
         <f t="shared" si="12"/>
         <v>36.968576709796672</v>
       </c>
-      <c r="P73" s="19">
+      <c r="P73" s="10">
         <f t="shared" si="13"/>
         <v>3.6367588889426909</v>
       </c>
@@ -6577,7 +6559,7 @@
         <f t="shared" si="12"/>
         <v>50.698920837256466</v>
       </c>
-      <c r="P74" s="19">
+      <c r="P74" s="10">
         <f t="shared" si="13"/>
         <v>3.9454369077424944</v>
       </c>
@@ -6634,7 +6616,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P75" s="19">
+      <c r="P75" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -6691,7 +6673,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P76" s="19">
+      <c r="P76" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -6748,7 +6730,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P77" s="19">
+      <c r="P77" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -6805,7 +6787,7 @@
         <f t="shared" si="12"/>
         <v>20.85723224528105</v>
       </c>
-      <c r="P78" s="19">
+      <c r="P78" s="10">
         <f t="shared" si="13"/>
         <v>3.0845318619821409</v>
       </c>
@@ -6862,7 +6844,7 @@
         <f t="shared" si="12"/>
         <v>56.154537286612758</v>
       </c>
-      <c r="P79" s="19">
+      <c r="P79" s="10">
         <f t="shared" si="13"/>
         <v>4.0457587796810444</v>
       </c>
@@ -6919,7 +6901,7 @@
         <f t="shared" si="12"/>
         <v>4.5743561593705691</v>
       </c>
-      <c r="P80" s="19">
+      <c r="P80" s="10">
         <f t="shared" si="13"/>
         <v>1.7181768235686148</v>
       </c>
@@ -6976,7 +6958,7 @@
         <f t="shared" si="12"/>
         <v>12.350253180190194</v>
       </c>
-      <c r="P81" s="19">
+      <c r="P81" s="10">
         <f t="shared" si="13"/>
         <v>2.5915353494746829</v>
       </c>
@@ -7033,7 +7015,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P82" s="19">
+      <c r="P82" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -7090,7 +7072,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P83" s="19">
+      <c r="P83" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -7147,7 +7129,7 @@
         <f t="shared" si="12"/>
         <v>5.8948361235557654</v>
       </c>
-      <c r="P84" s="19">
+      <c r="P84" s="10">
         <f t="shared" si="13"/>
         <v>1.9307727435307289</v>
       </c>
@@ -7204,7 +7186,7 @@
         <f t="shared" si="12"/>
         <v>86.757797621566723</v>
       </c>
-      <c r="P85" s="19">
+      <c r="P85" s="10">
         <f t="shared" si="13"/>
         <v>4.474580720182237</v>
       </c>
@@ -7261,7 +7243,7 @@
         <f t="shared" si="12"/>
         <v>45.495905368516837</v>
       </c>
-      <c r="P86" s="19">
+      <c r="P86" s="10">
         <f t="shared" si="13"/>
         <v>3.8393642521250655</v>
       </c>
@@ -7318,7 +7300,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P87" s="19">
+      <c r="P87" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -7375,7 +7357,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P88" s="19">
+      <c r="P88" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -7432,7 +7414,7 @@
         <f t="shared" si="12"/>
         <v>4.784002296321102</v>
       </c>
-      <c r="P89" s="19">
+      <c r="P89" s="10">
         <f t="shared" si="13"/>
         <v>1.7550958818690234</v>
       </c>
@@ -7489,7 +7471,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P90" s="19">
+      <c r="P90" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -7546,7 +7528,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P91" s="19">
+      <c r="P91" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -7603,7 +7585,7 @@
         <f t="shared" si="12"/>
         <v>6.5410779696493986</v>
       </c>
-      <c r="P92" s="19">
+      <c r="P92" s="10">
         <f t="shared" si="13"/>
         <v>2.0203651385980885</v>
       </c>
@@ -7660,7 +7642,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P93" s="19">
+      <c r="P93" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -7717,7 +7699,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P94" s="19">
+      <c r="P94" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -7774,7 +7756,7 @@
         <f t="shared" si="12"/>
         <v>23.842954406972737</v>
       </c>
-      <c r="P95" s="19">
+      <c r="P95" s="10">
         <f t="shared" si="13"/>
         <v>3.2125741874715503</v>
       </c>
@@ -7831,7 +7813,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P96" s="19">
+      <c r="P96" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -7888,7 +7870,7 @@
         <f t="shared" si="12"/>
         <v>81.165537112941848</v>
       </c>
-      <c r="P97" s="19">
+      <c r="P97" s="10">
         <f t="shared" si="13"/>
         <v>4.4087359576159866</v>
       </c>
@@ -7945,7 +7927,7 @@
         <f t="shared" si="12"/>
         <v>59.431831689052657</v>
       </c>
-      <c r="P98" s="19">
+      <c r="P98" s="10">
         <f t="shared" si="13"/>
         <v>4.101515980836699</v>
       </c>
@@ -8002,7 +7984,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P99" s="19">
+      <c r="P99" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -8059,7 +8041,7 @@
         <f t="shared" si="12"/>
         <v>116.83949174821089</v>
       </c>
-      <c r="P100" s="19">
+      <c r="P100" s="10">
         <f t="shared" si="13"/>
         <v>4.7693234590782954</v>
       </c>
@@ -8116,7 +8098,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P101" s="19">
+      <c r="P101" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -8173,7 +8155,7 @@
         <f t="shared" si="12"/>
         <v>21.685701893884634</v>
       </c>
-      <c r="P102" s="19">
+      <c r="P102" s="10">
         <f t="shared" si="13"/>
         <v>3.1217348535182303</v>
       </c>
@@ -8230,7 +8212,7 @@
         <f t="shared" si="12"/>
         <v>40.510431436094798</v>
       </c>
-      <c r="P103" s="19">
+      <c r="P103" s="10">
         <f t="shared" si="13"/>
         <v>3.7259447555569429</v>
       </c>
@@ -8287,7 +8269,7 @@
         <f t="shared" si="12"/>
         <v>37.936267071320181</v>
       </c>
-      <c r="P104" s="19">
+      <c r="P104" s="10">
         <f t="shared" si="13"/>
         <v>3.6619261317463843</v>
       </c>
@@ -8344,7 +8326,7 @@
         <f t="shared" si="12"/>
         <v>37.697914048755969</v>
       </c>
-      <c r="P105" s="19">
+      <c r="P105" s="10">
         <f t="shared" si="13"/>
         <v>3.6557856980341081</v>
       </c>
@@ -8401,7 +8383,7 @@
         <f t="shared" si="12"/>
         <v>28.325402220711535</v>
       </c>
-      <c r="P106" s="19">
+      <c r="P106" s="10">
         <f t="shared" si="13"/>
         <v>3.3784541104117687</v>
       </c>
@@ -8458,7 +8440,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P107" s="19">
+      <c r="P107" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -8515,7 +8497,7 @@
         <f t="shared" si="12"/>
         <v>17.579155028614959</v>
       </c>
-      <c r="P108" s="19">
+      <c r="P108" s="10">
         <f t="shared" si="13"/>
         <v>2.9220402548819679</v>
       </c>
@@ -8572,7 +8554,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P109" s="19">
+      <c r="P109" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -8629,7 +8611,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P110" s="19">
+      <c r="P110" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -8686,7 +8668,7 @@
         <f t="shared" si="12"/>
         <v>47.370914258645193</v>
       </c>
-      <c r="P111" s="19">
+      <c r="P111" s="10">
         <f t="shared" si="13"/>
         <v>3.8788986880134102</v>
       </c>
@@ -8743,7 +8725,7 @@
         <f t="shared" si="12"/>
         <v>158.85623510722795</v>
       </c>
-      <c r="P112" s="19">
+      <c r="P112" s="10">
         <f t="shared" si="13"/>
         <v>5.0742748807334257</v>
       </c>
@@ -8800,7 +8782,7 @@
         <f t="shared" si="12"/>
         <v>7.2886297376093294</v>
       </c>
-      <c r="P113" s="19">
+      <c r="P113" s="10">
         <f t="shared" si="13"/>
         <v>2.1148846644850599</v>
       </c>
@@ -8857,7 +8839,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P114" s="19">
+      <c r="P114" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -8914,7 +8896,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P115" s="19">
+      <c r="P115" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -8971,7 +8953,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P116" s="19">
+      <c r="P116" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -9028,7 +9010,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P117" s="19">
+      <c r="P117" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -9085,7 +9067,7 @@
         <f t="shared" si="12"/>
         <v>40.539170973953581</v>
       </c>
-      <c r="P118" s="19">
+      <c r="P118" s="10">
         <f t="shared" si="13"/>
         <v>3.726636860953525</v>
       </c>
@@ -9142,7 +9124,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P119" s="19">
+      <c r="P119" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -9199,7 +9181,7 @@
         <f t="shared" si="12"/>
         <v>0.67522400556384587</v>
       </c>
-      <c r="P120" s="19">
+      <c r="P120" s="10">
         <f t="shared" si="13"/>
         <v>0.51594689100032931</v>
       </c>
@@ -9256,7 +9238,7 @@
         <f t="shared" si="12"/>
         <v>31.471282454760033</v>
       </c>
-      <c r="P121" s="19">
+      <c r="P121" s="10">
         <f t="shared" si="13"/>
         <v>3.4803560819396511</v>
       </c>
@@ -9313,7 +9295,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P122" s="19">
+      <c r="P122" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -9370,7 +9352,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P123" s="19">
+      <c r="P123" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -9427,7 +9409,7 @@
         <f t="shared" si="12"/>
         <v>24.881811395869619</v>
       </c>
-      <c r="P124" s="19">
+      <c r="P124" s="10">
         <f t="shared" si="13"/>
         <v>3.2535404592957935</v>
       </c>
@@ -9484,7 +9466,7 @@
         <f t="shared" si="12"/>
         <v>77.720207253886002</v>
       </c>
-      <c r="P125" s="19">
+      <c r="P125" s="10">
         <f t="shared" si="13"/>
         <v>4.3658998855388811</v>
       </c>
@@ -9541,7 +9523,7 @@
         <f t="shared" si="12"/>
         <v>75.210589651022872</v>
       </c>
-      <c r="P126" s="19">
+      <c r="P126" s="10">
         <f t="shared" si="13"/>
         <v>4.3335004248351154</v>
       </c>
@@ -9598,7 +9580,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P127" s="19">
+      <c r="P127" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -9655,7 +9637,7 @@
         <f t="shared" si="12"/>
         <v>35.606195478013177</v>
       </c>
-      <c r="P128" s="19">
+      <c r="P128" s="10">
         <f t="shared" si="13"/>
         <v>3.6002175014374154</v>
       </c>
@@ -9712,7 +9694,7 @@
         <f t="shared" si="12"/>
         <v>10.233319688907081</v>
       </c>
-      <c r="P129" s="19">
+      <c r="P129" s="10">
         <f t="shared" si="13"/>
         <v>2.4188843340521169</v>
       </c>
@@ -9769,7 +9751,7 @@
         <f t="shared" ref="O130:O193" si="19">I130/D130*100000</f>
         <v>6.93601525923357</v>
       </c>
-      <c r="P130" s="19">
+      <c r="P130" s="10">
         <f t="shared" si="13"/>
         <v>2.0714112927672113</v>
       </c>
@@ -9826,7 +9808,7 @@
         <f t="shared" si="19"/>
         <v>11.591515011011939</v>
       </c>
-      <c r="P131" s="19">
+      <c r="P131" s="10">
         <f t="shared" ref="P131:P194" si="20">LN(O131+1)</f>
         <v>2.533023175289395</v>
       </c>
@@ -9883,7 +9865,7 @@
         <f t="shared" si="19"/>
         <v>4.9945060433523123</v>
       </c>
-      <c r="P132" s="19">
+      <c r="P132" s="10">
         <f t="shared" si="20"/>
         <v>1.7908433903145855</v>
       </c>
@@ -9940,7 +9922,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P133" s="19">
+      <c r="P133" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -9997,7 +9979,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P134" s="19">
+      <c r="P134" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -10054,7 +10036,7 @@
         <f t="shared" si="19"/>
         <v>21.69432693350689</v>
       </c>
-      <c r="P135" s="19">
+      <c r="P135" s="10">
         <f t="shared" si="20"/>
         <v>3.1221149784299587</v>
       </c>
@@ -10111,7 +10093,7 @@
         <f t="shared" si="19"/>
         <v>29.146021568055964</v>
       </c>
-      <c r="P136" s="19">
+      <c r="P136" s="10">
         <f t="shared" si="20"/>
         <v>3.4060529598414075</v>
       </c>
@@ -10168,7 +10150,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P137" s="19">
+      <c r="P137" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -10225,7 +10207,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P138" s="19">
+      <c r="P138" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -10282,7 +10264,7 @@
         <f t="shared" si="19"/>
         <v>12.618296529968456</v>
       </c>
-      <c r="P139" s="19">
+      <c r="P139" s="10">
         <f t="shared" si="20"/>
         <v>2.611414221678197</v>
       </c>
@@ -10339,7 +10321,7 @@
         <f t="shared" si="19"/>
         <v>186.24989877722894</v>
       </c>
-      <c r="P140" s="19">
+      <c r="P140" s="10">
         <f t="shared" si="20"/>
         <v>5.2324440818216367</v>
       </c>
@@ -10396,7 +10378,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P141" s="19">
+      <c r="P141" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -10453,7 +10435,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P142" s="19">
+      <c r="P142" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -10510,7 +10492,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P143" s="19">
+      <c r="P143" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -10567,7 +10549,7 @@
         <f t="shared" si="19"/>
         <v>3.9203387172651718</v>
       </c>
-      <c r="P144" s="19">
+      <c r="P144" s="10">
         <f t="shared" si="20"/>
         <v>1.5933773731071064</v>
       </c>
@@ -10624,7 +10606,7 @@
         <f t="shared" si="19"/>
         <v>6.7380904251735059</v>
       </c>
-      <c r="P145" s="19">
+      <c r="P145" s="10">
         <f t="shared" si="20"/>
         <v>2.0461549420685978</v>
       </c>
@@ -10681,7 +10663,7 @@
         <f t="shared" si="19"/>
         <v>226.24434389140274</v>
       </c>
-      <c r="P146" s="19">
+      <c r="P146" s="10">
         <f t="shared" si="20"/>
         <v>5.426025843381078</v>
       </c>
@@ -10738,7 +10720,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P147" s="19">
+      <c r="P147" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -10795,7 +10777,7 @@
         <f t="shared" si="19"/>
         <v>66.864074887763877</v>
       </c>
-      <c r="P148" s="19">
+      <c r="P148" s="10">
         <f t="shared" si="20"/>
         <v>4.217506806002465</v>
       </c>
@@ -10852,7 +10834,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P149" s="19">
+      <c r="P149" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -10909,7 +10891,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P150" s="19">
+      <c r="P150" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -10966,7 +10948,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P151" s="19">
+      <c r="P151" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -11023,7 +11005,7 @@
         <f t="shared" si="19"/>
         <v>112.73957158962796</v>
       </c>
-      <c r="P152" s="19">
+      <c r="P152" s="10">
         <f t="shared" si="20"/>
         <v>4.7339113752954036</v>
       </c>
@@ -11080,7 +11062,7 @@
         <f t="shared" si="19"/>
         <v>113.02918207973696</v>
       </c>
-      <c r="P153" s="19">
+      <c r="P153" s="10">
         <f t="shared" si="20"/>
         <v>4.7364543987919854</v>
       </c>
@@ -11137,7 +11119,7 @@
         <f t="shared" si="19"/>
         <v>42.793563847997262</v>
       </c>
-      <c r="P154" s="19">
+      <c r="P154" s="10">
         <f t="shared" si="20"/>
         <v>3.7794868624754057</v>
       </c>
@@ -11194,7 +11176,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P155" s="19">
+      <c r="P155" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -11251,7 +11233,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P156" s="19">
+      <c r="P156" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -11308,7 +11290,7 @@
         <f t="shared" si="19"/>
         <v>3.7006883280290133</v>
       </c>
-      <c r="P157" s="19">
+      <c r="P157" s="10">
         <f t="shared" si="20"/>
         <v>1.547708950764983</v>
       </c>
@@ -11365,7 +11347,7 @@
         <f t="shared" si="19"/>
         <v>56.168505516549644</v>
       </c>
-      <c r="P158" s="19">
+      <c r="P158" s="10">
         <f t="shared" si="20"/>
         <v>4.0460031438908111</v>
       </c>
@@ -11422,7 +11404,7 @@
         <f t="shared" si="19"/>
         <v>53.619302949061669</v>
       </c>
-      <c r="P159" s="19">
+      <c r="P159" s="10">
         <f t="shared" si="20"/>
         <v>4.0003873541380859</v>
       </c>
@@ -11479,7 +11461,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P160" s="19">
+      <c r="P160" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -11536,7 +11518,7 @@
         <f t="shared" si="19"/>
         <v>27.631942525559545</v>
       </c>
-      <c r="P161" s="19">
+      <c r="P161" s="10">
         <f t="shared" si="20"/>
         <v>3.3545229661118756</v>
       </c>
@@ -11593,7 +11575,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P162" s="19">
+      <c r="P162" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -11650,7 +11632,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P163" s="19">
+      <c r="P163" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -11707,7 +11689,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P164" s="19">
+      <c r="P164" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -11764,7 +11746,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P165" s="19">
+      <c r="P165" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -11821,7 +11803,7 @@
         <f t="shared" si="19"/>
         <v>39.047247169074581</v>
       </c>
-      <c r="P166" s="19">
+      <c r="P166" s="10">
         <f t="shared" si="20"/>
         <v>3.6900599362974527</v>
       </c>
@@ -11878,7 +11860,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P167" s="19">
+      <c r="P167" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -11935,7 +11917,7 @@
         <f t="shared" si="19"/>
         <v>56.66216275116593</v>
       </c>
-      <c r="P168" s="19">
+      <c r="P168" s="10">
         <f t="shared" si="20"/>
         <v>4.0546012001985661</v>
       </c>
@@ -11992,7 +11974,7 @@
         <f t="shared" si="19"/>
         <v>12.915605741909296</v>
       </c>
-      <c r="P169" s="19">
+      <c r="P169" s="10">
         <f t="shared" si="20"/>
         <v>2.633010925608485</v>
       </c>
@@ -12049,7 +12031,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P170" s="19">
+      <c r="P170" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -12106,7 +12088,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P171" s="19">
+      <c r="P171" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -12163,7 +12145,7 @@
         <f t="shared" si="19"/>
         <v>3.734129947722181</v>
       </c>
-      <c r="P172" s="19">
+      <c r="P172" s="10">
         <f t="shared" si="20"/>
         <v>1.554797960592994</v>
       </c>
@@ -12220,7 +12202,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P173" s="19">
+      <c r="P173" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -12277,7 +12259,7 @@
         <f t="shared" si="19"/>
         <v>356.35964912280701</v>
       </c>
-      <c r="P174" s="19">
+      <c r="P174" s="10">
         <f t="shared" si="20"/>
         <v>5.8787426951842114</v>
       </c>
@@ -12334,7 +12316,7 @@
         <f t="shared" si="19"/>
         <v>182.06007982634267</v>
       </c>
-      <c r="P175" s="19">
+      <c r="P175" s="10">
         <f t="shared" si="20"/>
         <v>5.2098144040230885</v>
       </c>
@@ -12391,7 +12373,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P176" s="19">
+      <c r="P176" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -12448,7 +12430,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P177" s="19">
+      <c r="P177" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -12505,7 +12487,7 @@
         <f t="shared" si="19"/>
         <v>6.7181726570372859</v>
       </c>
-      <c r="P178" s="19">
+      <c r="P178" s="10">
         <f t="shared" si="20"/>
         <v>2.0435776335619269</v>
       </c>
@@ -12562,7 +12544,7 @@
         <f t="shared" si="19"/>
         <v>30.821390044691018</v>
       </c>
-      <c r="P179" s="19">
+      <c r="P179" s="10">
         <f t="shared" si="20"/>
         <v>3.4601387065780917</v>
       </c>
@@ -12619,7 +12601,7 @@
         <f t="shared" si="19"/>
         <v>108.54162269725931</v>
       </c>
-      <c r="P180" s="19">
+      <c r="P180" s="10">
         <f t="shared" si="20"/>
         <v>4.6963045929874934</v>
       </c>
@@ -12676,7 +12658,7 @@
         <f t="shared" si="19"/>
         <v>18.443378827001109</v>
       </c>
-      <c r="P181" s="19">
+      <c r="P181" s="10">
         <f t="shared" si="20"/>
         <v>2.9675065919027452</v>
       </c>
@@ -12733,7 +12715,7 @@
         <f t="shared" si="19"/>
         <v>57.212913771965674</v>
       </c>
-      <c r="P182" s="19">
+      <c r="P182" s="10">
         <f t="shared" si="20"/>
         <v>4.0641072162405569</v>
       </c>
@@ -12790,7 +12772,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P183" s="19">
+      <c r="P183" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -12847,7 +12829,7 @@
         <f t="shared" si="19"/>
         <v>25.541852149164416</v>
       </c>
-      <c r="P184" s="19">
+      <c r="P184" s="10">
         <f t="shared" si="20"/>
         <v>3.2787228135513629</v>
       </c>
@@ -12904,7 +12886,7 @@
         <f t="shared" si="19"/>
         <v>140.51269117832501</v>
       </c>
-      <c r="P185" s="19">
+      <c r="P185" s="10">
         <f t="shared" si="20"/>
         <v>4.9523894033675413</v>
       </c>
@@ -12961,7 +12943,7 @@
         <f t="shared" si="19"/>
         <v>38.266526356070024</v>
       </c>
-      <c r="P186" s="19">
+      <c r="P186" s="10">
         <f t="shared" si="20"/>
         <v>3.6703724092680354</v>
       </c>
@@ -13018,7 +13000,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P187" s="19">
+      <c r="P187" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -13075,7 +13057,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P188" s="19">
+      <c r="P188" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -13132,7 +13114,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P189" s="19">
+      <c r="P189" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -13189,7 +13171,7 @@
         <f t="shared" si="19"/>
         <v>82.764328574384436</v>
       </c>
-      <c r="P190" s="19">
+      <c r="P190" s="10">
         <f t="shared" si="20"/>
         <v>4.4280072435267224</v>
       </c>
@@ -13246,7 +13228,7 @@
         <f t="shared" si="19"/>
         <v>28.240609997175941</v>
       </c>
-      <c r="P191" s="19">
+      <c r="P191" s="10">
         <f t="shared" si="20"/>
         <v>3.3755584964004979</v>
       </c>
@@ -13303,7 +13285,7 @@
         <f t="shared" si="19"/>
         <v>53.162299355192751</v>
       </c>
-      <c r="P192" s="19">
+      <c r="P192" s="10">
         <f t="shared" si="20"/>
         <v>3.9919850825623788</v>
       </c>
@@ -13360,7 +13342,7 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="P193" s="19">
+      <c r="P193" s="10">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -13417,7 +13399,7 @@
         <f t="shared" ref="O194:O257" si="26">I194/D194*100000</f>
         <v>19.102758144387462</v>
       </c>
-      <c r="P194" s="19">
+      <c r="P194" s="10">
         <f t="shared" si="20"/>
         <v>3.0008570267648782</v>
       </c>
@@ -13474,7 +13456,7 @@
         <f t="shared" si="26"/>
         <v>300.96626009821006</v>
       </c>
-      <c r="P195" s="19">
+      <c r="P195" s="10">
         <f t="shared" ref="P195:P258" si="27">LN(O195+1)</f>
         <v>5.7103152896044493</v>
       </c>
@@ -13531,7 +13513,7 @@
         <f t="shared" si="26"/>
         <v>81.419017156150048</v>
       </c>
-      <c r="P196" s="19">
+      <c r="P196" s="10">
         <f t="shared" si="27"/>
         <v>4.4118162010173183</v>
       </c>
@@ -13588,7 +13570,7 @@
         <f t="shared" si="26"/>
         <v>62.787777312683133</v>
       </c>
-      <c r="P197" s="19">
+      <c r="P197" s="10">
         <f t="shared" si="27"/>
         <v>4.1555615938261914</v>
       </c>
@@ -13645,7 +13627,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P198" s="19">
+      <c r="P198" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -13702,7 +13684,7 @@
         <f t="shared" si="26"/>
         <v>83.998320033599327</v>
       </c>
-      <c r="P199" s="19">
+      <c r="P199" s="10">
         <f t="shared" si="27"/>
         <v>4.4426314919844039</v>
       </c>
@@ -13759,7 +13741,7 @@
         <f t="shared" si="26"/>
         <v>102.04081632653062</v>
       </c>
-      <c r="P200" s="19">
+      <c r="P200" s="10">
         <f t="shared" si="27"/>
         <v>4.6351251847482891</v>
       </c>
@@ -13816,7 +13798,7 @@
         <f t="shared" si="26"/>
         <v>24.177949709864603</v>
       </c>
-      <c r="P201" s="19">
+      <c r="P201" s="10">
         <f t="shared" si="27"/>
         <v>3.2259685999580312</v>
       </c>
@@ -13873,7 +13855,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P202" s="19">
+      <c r="P202" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -13930,7 +13912,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P203" s="19">
+      <c r="P203" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -13987,7 +13969,7 @@
         <f t="shared" si="26"/>
         <v>2.2656214599664688</v>
       </c>
-      <c r="P204" s="19">
+      <c r="P204" s="10">
         <f t="shared" si="27"/>
         <v>1.183450084575145</v>
       </c>
@@ -14044,7 +14026,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P205" s="19">
+      <c r="P205" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -14101,7 +14083,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P206" s="19">
+      <c r="P206" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -14158,7 +14140,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P207" s="19">
+      <c r="P207" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -14215,7 +14197,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P208" s="19">
+      <c r="P208" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -14272,7 +14254,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P209" s="19">
+      <c r="P209" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -14329,7 +14311,7 @@
         <f t="shared" si="26"/>
         <v>31.222680154864491</v>
       </c>
-      <c r="P210" s="19">
+      <c r="P210" s="10">
         <f t="shared" si="27"/>
         <v>3.4726705572460062</v>
       </c>
@@ -14386,7 +14368,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P211" s="19">
+      <c r="P211" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -14443,7 +14425,7 @@
         <f t="shared" si="26"/>
         <v>89.492132150048477</v>
       </c>
-      <c r="P212" s="19">
+      <c r="P212" s="10">
         <f t="shared" si="27"/>
         <v>4.5052629093580663</v>
       </c>
@@ -14500,7 +14482,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P213" s="19">
+      <c r="P213" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -14557,7 +14539,7 @@
         <f t="shared" si="26"/>
         <v>9.1717875813996148</v>
       </c>
-      <c r="P214" s="19">
+      <c r="P214" s="10">
         <f t="shared" si="27"/>
         <v>2.3196179646638497</v>
       </c>
@@ -14614,7 +14596,7 @@
         <f t="shared" si="26"/>
         <v>30.06313257841467</v>
       </c>
-      <c r="P215" s="19">
+      <c r="P215" s="10">
         <f t="shared" si="27"/>
         <v>3.4360216683469442</v>
       </c>
@@ -14671,7 +14653,7 @@
         <f t="shared" si="26"/>
         <v>37.864445285876563</v>
       </c>
-      <c r="P216" s="19">
+      <c r="P216" s="10">
         <f t="shared" si="27"/>
         <v>3.6600798297352601</v>
       </c>
@@ -14728,7 +14710,7 @@
         <f t="shared" si="26"/>
         <v>11.56737998843262</v>
       </c>
-      <c r="P217" s="19">
+      <c r="P217" s="10">
         <f t="shared" si="27"/>
         <v>2.5311045671801451</v>
       </c>
@@ -14785,7 +14767,7 @@
         <f t="shared" si="26"/>
         <v>55.632823365785818</v>
       </c>
-      <c r="P218" s="19">
+      <c r="P218" s="10">
         <f t="shared" si="27"/>
         <v>4.0365887352450285</v>
       </c>
@@ -14842,7 +14824,7 @@
         <f t="shared" si="26"/>
         <v>73.206442166910691</v>
       </c>
-      <c r="P219" s="19">
+      <c r="P219" s="10">
         <f t="shared" si="27"/>
         <v>4.3068509680610312</v>
       </c>
@@ -14899,7 +14881,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P220" s="19">
+      <c r="P220" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -14956,7 +14938,7 @@
         <f t="shared" si="26"/>
         <v>46.319690079164559</v>
       </c>
-      <c r="P221" s="19">
+      <c r="P221" s="10">
         <f t="shared" si="27"/>
         <v>3.8569264896205335</v>
       </c>
@@ -15013,7 +14995,7 @@
         <f t="shared" si="26"/>
         <v>2.5237229961639409</v>
       </c>
-      <c r="P222" s="19">
+      <c r="P222" s="10">
         <f t="shared" si="27"/>
         <v>1.2595181000365989</v>
       </c>
@@ -15070,7 +15052,7 @@
         <f t="shared" si="26"/>
         <v>13.241525423728813</v>
       </c>
-      <c r="P223" s="19">
+      <c r="P223" s="10">
         <f t="shared" si="27"/>
         <v>2.6561620226994958</v>
       </c>
@@ -15127,7 +15109,7 @@
         <f t="shared" si="26"/>
         <v>24.348672997321646</v>
       </c>
-      <c r="P224" s="19">
+      <c r="P224" s="10">
         <f t="shared" si="27"/>
         <v>3.2327263814213327</v>
       </c>
@@ -15184,7 +15166,7 @@
         <f t="shared" si="26"/>
         <v>5.4710581026370502</v>
       </c>
-      <c r="P225" s="19">
+      <c r="P225" s="10">
         <f t="shared" si="27"/>
         <v>1.8673396349618856</v>
       </c>
@@ -15241,7 +15223,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P226" s="19">
+      <c r="P226" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -15298,7 +15280,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P227" s="19">
+      <c r="P227" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -15355,7 +15337,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P228" s="19">
+      <c r="P228" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -15412,7 +15394,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P229" s="19">
+      <c r="P229" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -15469,7 +15451,7 @@
         <f t="shared" si="26"/>
         <v>19.331142470520007</v>
       </c>
-      <c r="P230" s="19">
+      <c r="P230" s="10">
         <f t="shared" si="27"/>
         <v>3.0121538223485635</v>
       </c>
@@ -15526,7 +15508,7 @@
         <f t="shared" si="26"/>
         <v>19.045286971663334</v>
       </c>
-      <c r="P231" s="19">
+      <c r="P231" s="10">
         <f t="shared" si="27"/>
         <v>2.9979940623633232</v>
       </c>
@@ -15583,7 +15565,7 @@
         <f t="shared" si="26"/>
         <v>34.737299174989147</v>
       </c>
-      <c r="P232" s="19">
+      <c r="P232" s="10">
         <f t="shared" si="27"/>
         <v>3.5761949381849782</v>
       </c>
@@ -15640,7 +15622,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P233" s="19">
+      <c r="P233" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -15697,7 +15679,7 @@
         <f t="shared" si="26"/>
         <v>52.149178255372938</v>
       </c>
-      <c r="P234" s="19">
+      <c r="P234" s="10">
         <f t="shared" si="27"/>
         <v>3.9731026438099781</v>
       </c>
@@ -15754,7 +15736,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P235" s="19">
+      <c r="P235" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -15811,7 +15793,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P236" s="19">
+      <c r="P236" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -15868,7 +15850,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P237" s="19">
+      <c r="P237" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -15925,7 +15907,7 @@
         <f t="shared" si="26"/>
         <v>8.5298758903057958</v>
       </c>
-      <c r="P238" s="19">
+      <c r="P238" s="10">
         <f t="shared" si="27"/>
         <v>2.2544316945284031</v>
       </c>
@@ -15982,7 +15964,7 @@
         <f t="shared" si="26"/>
         <v>134.86490257173418</v>
       </c>
-      <c r="P239" s="19">
+      <c r="P239" s="10">
         <f t="shared" si="27"/>
         <v>4.9116610285804718</v>
       </c>
@@ -16039,7 +16021,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P240" s="19">
+      <c r="P240" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -16096,7 +16078,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P241" s="19">
+      <c r="P241" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -16153,7 +16135,7 @@
         <f t="shared" si="26"/>
         <v>42.867859822098382</v>
       </c>
-      <c r="P242" s="19">
+      <c r="P242" s="10">
         <f t="shared" si="27"/>
         <v>3.7811819294451134</v>
       </c>
@@ -16210,7 +16192,7 @@
         <f t="shared" si="26"/>
         <v>60.422960725075527</v>
       </c>
-      <c r="P243" s="19">
+      <c r="P243" s="10">
         <f t="shared" si="27"/>
         <v>4.1177837184271597</v>
       </c>
@@ -16267,7 +16249,7 @@
         <f t="shared" si="26"/>
         <v>123.86457473162675</v>
       </c>
-      <c r="P244" s="19">
+      <c r="P244" s="10">
         <f t="shared" si="27"/>
         <v>4.8272297478509794</v>
       </c>
@@ -16324,7 +16306,7 @@
         <f t="shared" si="26"/>
         <v>37.907505686125852</v>
       </c>
-      <c r="P245" s="19">
+      <c r="P245" s="10">
         <f t="shared" si="27"/>
         <v>3.6611871802417415</v>
       </c>
@@ -16381,7 +16363,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P246" s="19">
+      <c r="P246" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -16438,7 +16420,7 @@
         <f t="shared" si="26"/>
         <v>62.567036110117982</v>
       </c>
-      <c r="P247" s="19">
+      <c r="P247" s="10">
         <f t="shared" si="27"/>
         <v>4.1520950358267443</v>
       </c>
@@ -16495,7 +16477,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P248" s="19">
+      <c r="P248" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -16552,7 +16534,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P249" s="19">
+      <c r="P249" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -16609,7 +16591,7 @@
         <f t="shared" si="26"/>
         <v>82.678792889623807</v>
       </c>
-      <c r="P250" s="19">
+      <c r="P250" s="10">
         <f t="shared" si="27"/>
         <v>4.4269855748973637</v>
       </c>
@@ -16666,7 +16648,7 @@
         <f t="shared" si="26"/>
         <v>16.013095153369868</v>
       </c>
-      <c r="P251" s="19">
+      <c r="P251" s="10">
         <f t="shared" si="27"/>
         <v>2.8339833506644263</v>
       </c>
@@ -16723,7 +16705,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P252" s="19">
+      <c r="P252" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -16780,7 +16762,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P253" s="19">
+      <c r="P253" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -16837,7 +16819,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="P254" s="19">
+      <c r="P254" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -16894,7 +16876,7 @@
         <f t="shared" si="26"/>
         <v>57.487783845932739</v>
       </c>
-      <c r="P255" s="19">
+      <c r="P255" s="10">
         <f t="shared" si="27"/>
         <v>4.0688179092847729</v>
       </c>
@@ -16951,7 +16933,7 @@
         <f t="shared" si="26"/>
         <v>3.7536128523704062</v>
       </c>
-      <c r="P256" s="19">
+      <c r="P256" s="10">
         <f t="shared" si="27"/>
         <v>1.5589049294356119</v>
       </c>
@@ -17008,7 +16990,7 @@
         <f t="shared" si="26"/>
         <v>9.2187139893984789</v>
       </c>
-      <c r="P257" s="19">
+      <c r="P257" s="10">
         <f t="shared" si="27"/>
         <v>2.32422074411808</v>
       </c>
@@ -17065,7 +17047,7 @@
         <f t="shared" ref="O258:O285" si="33">I258/D258*100000</f>
         <v>0</v>
       </c>
-      <c r="P258" s="19">
+      <c r="P258" s="10">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -17122,7 +17104,7 @@
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="P259" s="19">
+      <c r="P259" s="10">
         <f t="shared" ref="P259:P285" si="34">LN(O259+1)</f>
         <v>0</v>
       </c>
@@ -17179,7 +17161,7 @@
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="P260" s="19">
+      <c r="P260" s="10">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
@@ -17236,7 +17218,7 @@
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="P261" s="19">
+      <c r="P261" s="10">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
@@ -17293,7 +17275,7 @@
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="P262" s="19">
+      <c r="P262" s="10">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
@@ -17350,7 +17332,7 @@
         <f t="shared" si="33"/>
         <v>8.0652594709189778</v>
       </c>
-      <c r="P263" s="19">
+      <c r="P263" s="10">
         <f t="shared" si="34"/>
         <v>2.2044494671748875</v>
       </c>
@@ -17407,7 +17389,7 @@
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="P264" s="19">
+      <c r="P264" s="10">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
@@ -17464,7 +17446,7 @@
         <f t="shared" si="33"/>
         <v>3.6975411351451286</v>
       </c>
-      <c r="P265" s="19">
+      <c r="P265" s="10">
         <f t="shared" si="34"/>
         <v>1.5470392090835616</v>
       </c>
@@ -17521,7 +17503,7 @@
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="P266" s="19">
+      <c r="P266" s="10">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
@@ -17578,7 +17560,7 @@
         <f t="shared" si="33"/>
         <v>43.000184286504087</v>
       </c>
-      <c r="P267" s="19">
+      <c r="P267" s="10">
         <f t="shared" si="34"/>
         <v>3.7841938222391285</v>
       </c>
@@ -17635,7 +17617,7 @@
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="P268" s="19">
+      <c r="P268" s="10">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
@@ -17692,7 +17674,7 @@
         <f t="shared" si="33"/>
         <v>12.171866758631882</v>
       </c>
-      <c r="P269" s="19">
+      <c r="P269" s="10">
         <f t="shared" si="34"/>
         <v>2.5780832489627952</v>
       </c>
@@ -17749,7 +17731,7 @@
         <f t="shared" si="33"/>
         <v>1.8814675446848541</v>
       </c>
-      <c r="P270" s="19">
+      <c r="P270" s="10">
         <f t="shared" si="34"/>
         <v>1.0582997284908273</v>
       </c>
@@ -17806,7 +17788,7 @@
         <f t="shared" si="33"/>
         <v>102.88595092340141</v>
       </c>
-      <c r="P271" s="19">
+      <c r="P271" s="10">
         <f t="shared" si="34"/>
         <v>4.6432936716708868</v>
       </c>
@@ -17863,7 +17845,7 @@
         <f t="shared" si="33"/>
         <v>17.642907551164434</v>
       </c>
-      <c r="P272" s="19">
+      <c r="P272" s="10">
         <f t="shared" si="34"/>
         <v>2.9254657815976568</v>
       </c>
@@ -17920,7 +17902,7 @@
         <f t="shared" si="33"/>
         <v>70.646414694454251</v>
       </c>
-      <c r="P273" s="19">
+      <c r="P273" s="10">
         <f t="shared" si="34"/>
         <v>4.2717431138659245</v>
       </c>
@@ -17977,7 +17959,7 @@
         <f t="shared" si="33"/>
         <v>22.006235099944984</v>
       </c>
-      <c r="P274" s="19">
+      <c r="P274" s="10">
         <f t="shared" si="34"/>
         <v>3.1357652704924979</v>
       </c>
@@ -18034,7 +18016,7 @@
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="P275" s="19">
+      <c r="P275" s="10">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
@@ -18091,7 +18073,7 @@
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="P276" s="19">
+      <c r="P276" s="10">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
@@ -18148,7 +18130,7 @@
         <f t="shared" si="33"/>
         <v>8.0742834073475986</v>
       </c>
-      <c r="P277" s="19">
+      <c r="P277" s="10">
         <f t="shared" si="34"/>
         <v>2.2054444136554676</v>
       </c>
@@ -18205,7 +18187,7 @@
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="P278" s="19">
+      <c r="P278" s="10">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
@@ -18262,7 +18244,7 @@
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="P279" s="19">
+      <c r="P279" s="10">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
@@ -18319,7 +18301,7 @@
         <f t="shared" si="33"/>
         <v>21.870671429612887</v>
       </c>
-      <c r="P280" s="19">
+      <c r="P280" s="10">
         <f t="shared" si="34"/>
         <v>3.1298553661351263</v>
       </c>
@@ -18376,7 +18358,7 @@
         <f t="shared" si="33"/>
         <v>2.9792051480664958</v>
       </c>
-      <c r="P281" s="19">
+      <c r="P281" s="10">
         <f t="shared" si="34"/>
         <v>1.3810820878102594</v>
       </c>
@@ -18433,7 +18415,7 @@
         <f t="shared" si="33"/>
         <v>7.915149596327371</v>
       </c>
-      <c r="P282" s="19">
+      <c r="P282" s="10">
         <f t="shared" si="34"/>
         <v>2.1877520314690297</v>
       </c>
@@ -18490,7 +18472,7 @@
         <f t="shared" si="33"/>
         <v>9.4670074789359084</v>
       </c>
-      <c r="P283" s="19">
+      <c r="P283" s="10">
         <f t="shared" si="34"/>
         <v>2.3482281653977526</v>
       </c>
@@ -18547,7 +18529,7 @@
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="P284" s="19">
+      <c r="P284" s="10">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
@@ -18604,7 +18586,7 @@
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="P285" s="19">
+      <c r="P285" s="10">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
@@ -18640,16 +18622,16 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
-        <f>FACTORS_MUNI!M1</f>
+        <f>FACTORS!M1</f>
         <v>ln_POP</v>
       </c>
       <c r="B2" s="2">
-        <v>20</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f>FACTORS_MUNI!L1</f>
+        <f>FACTORS!L1</f>
         <v>ln_TAX_BASE_PER_CAP</v>
       </c>
       <c r="B3" s="2">
@@ -18658,7 +18640,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
-        <f>FACTORS_MUNI!N1</f>
+        <f>FACTORS!N1</f>
         <v>ln_MED_HH_INC</v>
       </c>
       <c r="B4" s="2">
@@ -18667,7 +18649,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
-        <f>FACTORS_MUNI!H1</f>
+        <f>FACTORS!H1</f>
         <v>PCT_EDA_POP</v>
       </c>
       <c r="B5" s="2">
@@ -18711,7 +18693,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
-            <xm:f>FACTORS_MUNI!$D$1:$XFD$1</xm:f>
+            <xm:f>FACTORS!$D$1:$XFD$1</xm:f>
           </x14:formula1>
           <xm:sqref>A2:A1048576</xm:sqref>
         </x14:dataValidation>
@@ -18726,7 +18708,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18748,7 +18730,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>38.332999999999998</v>
+        <v>40.56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -18756,7 +18738,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>60</v>
+        <v>57.78</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -18764,7 +18746,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>75</v>
+        <v>73.34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Proposed weights for secondary allocation
Initial allocation proposed to be calculated as a flat amount per muni, plus a flat amount per capita
</commit_message>
<xml_diff>
--- a/input/community_cohort_inputs.xlsx
+++ b/input/community_cohort_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmp/Documents/GitHub/community-cohort-tool/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10361AB5-5001-2546-BB4B-AD97F6833D07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5515F4-70D9-1441-8EA5-625D726E0DB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="660" windowWidth="31720" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="660" windowWidth="31720" windowHeight="19840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FACTORS" sheetId="1" r:id="rId1"/>
@@ -2333,7 +2333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P285"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17028,11 +17028,11 @@
         <v>9465878</v>
       </c>
       <c r="K258" s="4">
-        <f t="shared" ref="K258:K321" si="29">J258/D258</f>
+        <f t="shared" ref="K258:K285" si="29">J258/D258</f>
         <v>28597.818731117826</v>
       </c>
       <c r="L258" s="10">
-        <f t="shared" ref="L258:L321" si="30">LN(K258)</f>
+        <f t="shared" ref="L258:L285" si="30">LN(K258)</f>
         <v>10.261085725756647</v>
       </c>
       <c r="M258" s="10">
@@ -18602,9 +18602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18626,7 +18624,7 @@
         <v>ln_POP</v>
       </c>
       <c r="B2" s="2">
-        <v>-20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -18635,7 +18633,7 @@
         <v>ln_TAX_BASE_PER_CAP</v>
       </c>
       <c r="B3" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -18644,7 +18642,7 @@
         <v>ln_MED_HH_INC</v>
       </c>
       <c r="B4" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -18653,7 +18651,7 @@
         <v>PCT_EDA_POP</v>
       </c>
       <c r="B5" s="2">
-        <v>-20</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
More detailed comment for CCA total market value column
</commit_message>
<xml_diff>
--- a/input/community_cohort_inputs.xlsx
+++ b/input/community_cohort_inputs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmp/Documents/GitHub/community-cohort-tool/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npeterson\Documents\GitHub\community-cohort-tool\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87AB92B-7915-A546-AF18-AACA516ED748}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24" yWindow="504" windowWidth="33600" windowHeight="20496" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FACTORS_MUNI" sheetId="1" r:id="rId1"/>
@@ -34,12 +33,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Noel M. Peterson</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{E5F6F6B7-B2A8-CC48-9797-245DA94E067C}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -88,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{D740298F-0131-A34E-81D6-4D7ABEDD6CDF}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -111,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{81990BE2-AF09-074C-812C-00B651742EE2}">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -134,7 +133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{636EBDA5-869B-824B-97BD-7DD9B9423CC5}">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -157,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -180,7 +179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -203,7 +202,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -226,7 +225,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -249,7 +248,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -272,7 +271,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -300,12 +299,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Noel M. Peterson</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -318,7 +317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -331,7 +330,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -354,7 +353,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -377,7 +376,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -396,17 +395,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> Total market value, calculated from 2019 county assessor data.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve"> Total market value, calculated from 2019 county assessor data. For each Chicago parcel, total market value is calculated by multiplying total assessed value by a factor, depending on the parcel's class. Factors are as follows: 10x for classes 100-399 &amp; 600-999; 5x for classes 400-499; and 4x for classes 500-599.
 </t>
         </r>
         <r>
@@ -432,7 +421,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -512,7 +501,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -554,7 +543,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -577,7 +566,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -639,7 +628,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -667,12 +656,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Noel M. Peterson</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -685,7 +674,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -703,12 +692,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Noel M. Peterson</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -721,7 +710,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1903,7 +1892,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
@@ -2893,27 +2882,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L285"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.77734375" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.6640625" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2951,7 +2940,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1700243</v>
       </c>
@@ -2994,7 +2983,7 @@
         <v>11.117465141678133</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1700685</v>
       </c>
@@ -3037,7 +3026,7 @@
         <v>11.541085230764084</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1701010</v>
       </c>
@@ -3080,7 +3069,7 @@
         <v>11.055830163625206</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1701595</v>
       </c>
@@ -3123,7 +3112,7 @@
         <v>11.472821962272894</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1702154</v>
       </c>
@@ -3166,7 +3155,7 @@
         <v>11.475638880184212</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1703012</v>
       </c>
@@ -3209,7 +3198,7 @@
         <v>11.180929196242513</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1703610</v>
       </c>
@@ -3252,7 +3241,7 @@
         <v>11.677736266122603</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1703844</v>
       </c>
@@ -3295,7 +3284,7 @@
         <v>11.67785498665461</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1703883</v>
       </c>
@@ -3338,7 +3327,7 @@
         <v>12.090448527732631</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1704013</v>
       </c>
@@ -3381,7 +3370,7 @@
         <v>11.595353018943539</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1704078</v>
       </c>
@@ -3424,7 +3413,7 @@
         <v>11.448802857328646</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1704303</v>
       </c>
@@ -3467,7 +3456,7 @@
         <v>11.182572467557037</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1704572</v>
       </c>
@@ -3510,7 +3499,7 @@
         <v>11.373019512226074</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1704585</v>
       </c>
@@ -3553,7 +3542,7 @@
         <v>11.317178185137777</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1704975</v>
       </c>
@@ -3596,7 +3585,7 @@
         <v>10.943004258145342</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1705248</v>
       </c>
@@ -3639,7 +3628,7 @@
         <v>11.047009469952846</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1705404</v>
       </c>
@@ -3682,7 +3671,7 @@
         <v>11.069649449465471</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1705573</v>
       </c>
@@ -3725,7 +3714,7 @@
         <v>11.047041338907707</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1705976</v>
       </c>
@@ -3768,7 +3757,7 @@
         <v>11.475939852118257</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1706587</v>
       </c>
@@ -3811,7 +3800,7 @@
         <v>11.366164083574825</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1706704</v>
       </c>
@@ -3854,7 +3843,7 @@
         <v>10.787213769536883</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1707133</v>
       </c>
@@ -3897,7 +3886,7 @@
         <v>11.421796531559126</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1707640</v>
       </c>
@@ -3940,7 +3929,7 @@
         <v>11.075396770265694</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1707770</v>
       </c>
@@ -3983,7 +3972,7 @@
         <v>11.052063919241686</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1708225</v>
       </c>
@@ -4026,7 +4015,7 @@
         <v>10.927502005497212</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1708446</v>
       </c>
@@ -4069,7 +4058,7 @@
         <v>10.900786679503748</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1708576</v>
       </c>
@@ -4112,7 +4101,7 @@
         <v>11.319765382995278</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1709447</v>
       </c>
@@ -4155,7 +4144,7 @@
         <v>11.66092296705356</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1709531</v>
       </c>
@@ -4198,7 +4187,7 @@
         <v>11.581359513678144</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1709642</v>
       </c>
@@ -4241,7 +4230,7 @@
         <v>11.044089154143165</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1709759</v>
       </c>
@@ -4284,7 +4273,7 @@
         <v>11.278556645415463</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1709798</v>
       </c>
@@ -4327,7 +4316,7 @@
         <v>10.744925419508215</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1709980</v>
       </c>
@@ -4370,7 +4359,7 @@
         <v>11.978764183001822</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1710487</v>
       </c>
@@ -4413,7 +4402,7 @@
         <v>10.702255214959758</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1710513</v>
       </c>
@@ -4456,7 +4445,7 @@
         <v>10.780871122094799</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1710906</v>
       </c>
@@ -4499,7 +4488,7 @@
         <v>11.947139986364379</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1711332</v>
       </c>
@@ -4542,7 +4531,7 @@
         <v>11.315230338109606</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1711358</v>
       </c>
@@ -4585,7 +4574,7 @@
         <v>11.14181830437332</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1711592</v>
       </c>
@@ -4628,7 +4617,7 @@
         <v>11.516309731873374</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1712476</v>
       </c>
@@ -4671,7 +4660,7 @@
         <v>11.428423663632492</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1714000</v>
       </c>
@@ -4714,7 +4703,7 @@
         <v>10.972447867955744</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>1714026</v>
       </c>
@@ -4757,7 +4746,7 @@
         <v>10.823491382322166</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1714065</v>
       </c>
@@ -4800,7 +4789,7 @@
         <v>10.797246335903196</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1714351</v>
       </c>
@@ -4843,7 +4832,7 @@
         <v>10.807037463759448</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1714572</v>
       </c>
@@ -4886,7 +4875,7 @@
         <v>11.625879079947149</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>1715170</v>
       </c>
@@ -4929,7 +4918,7 @@
         <v>11.221971378648028</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1716691</v>
       </c>
@@ -4972,7 +4961,7 @@
         <v>11.034599299294824</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1716873</v>
       </c>
@@ -5015,7 +5004,7 @@
         <v>11.015887683869506</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1717458</v>
       </c>
@@ -5058,7 +5047,7 @@
         <v>10.94404690975562</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>1717497</v>
       </c>
@@ -5101,7 +5090,7 @@
         <v>11.020790739647728</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>1717523</v>
       </c>
@@ -5144,7 +5133,7 @@
         <v>11.281938736194993</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>1717887</v>
       </c>
@@ -5187,7 +5176,7 @@
         <v>11.380285103830651</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1718628</v>
       </c>
@@ -5230,7 +5219,7 @@
         <v>11.47496395868311</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>1719083</v>
       </c>
@@ -5273,7 +5262,7 @@
         <v>12.028428134287182</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>1718992</v>
       </c>
@@ -5316,7 +5305,7 @@
         <v>11.941006233548201</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>1719642</v>
       </c>
@@ -5359,7 +5348,7 @@
         <v>11.152816058582861</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>1719837</v>
       </c>
@@ -5402,7 +5391,7 @@
         <v>11.000999235760204</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>1720149</v>
       </c>
@@ -5445,7 +5434,7 @@
         <v>10.813116141536733</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>1720292</v>
       </c>
@@ -5488,7 +5477,7 @@
         <v>10.749656204178475</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>1720591</v>
       </c>
@@ -5531,7 +5520,7 @@
         <v>11.460505220022895</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>1721696</v>
       </c>
@@ -5574,7 +5563,7 @@
         <v>11.134443028191951</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>1721904</v>
       </c>
@@ -5617,7 +5606,7 @@
         <v>10.944947309699929</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>1722931</v>
       </c>
@@ -5660,7 +5649,7 @@
         <v>11.557545039546797</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>1723074</v>
       </c>
@@ -5703,7 +5692,7 @@
         <v>11.142455810009308</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>1723256</v>
       </c>
@@ -5746,7 +5735,7 @@
         <v>11.31319321791648</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>1723620</v>
       </c>
@@ -5789,7 +5778,7 @@
         <v>11.683587647995452</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>1723724</v>
       </c>
@@ -5832,7 +5821,7 @@
         <v>11.001482984320479</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>1723945</v>
       </c>
@@ -5875,7 +5864,7 @@
         <v>11.277886442242952</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>1724582</v>
       </c>
@@ -5918,7 +5907,7 @@
         <v>11.275987202633829</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>1724634</v>
       </c>
@@ -5961,7 +5950,7 @@
         <v>11.233965246330317</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>1726571</v>
       </c>
@@ -6004,7 +5993,7 @@
         <v>11.655188624518198</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>1726710</v>
       </c>
@@ -6047,7 +6036,7 @@
         <v>10.43901554494246</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>1726935</v>
       </c>
@@ -6090,7 +6079,7 @@
         <v>11.045542399047074</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>1726987</v>
       </c>
@@ -6133,7 +6122,7 @@
         <v>11.241772694469658</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>1727442</v>
       </c>
@@ -6176,7 +6165,7 @@
         <v>11.005925846037767</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>1727533</v>
       </c>
@@ -6219,7 +6208,7 @@
         <v>11.634408314533101</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>1727624</v>
       </c>
@@ -6262,7 +6251,7 @@
         <v>11.843271833861451</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>1727702</v>
       </c>
@@ -6305,7 +6294,7 @@
         <v>11.066185134649654</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>1728872</v>
       </c>
@@ -6348,7 +6337,7 @@
         <v>11.625503868886527</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>1729171</v>
       </c>
@@ -6391,7 +6380,7 @@
         <v>11.483857042472881</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>1729756</v>
       </c>
@@ -6434,7 +6423,7 @@
         <v>11.61438036362556</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>1729652</v>
       </c>
@@ -6477,7 +6466,7 @@
         <v>12.424609602763658</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>1729730</v>
       </c>
@@ -6520,7 +6509,7 @@
         <v>11.134516028885489</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>1729938</v>
       </c>
@@ -6563,7 +6552,7 @@
         <v>11.654407665982111</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>1730029</v>
       </c>
@@ -6606,7 +6595,7 @@
         <v>11.120682557031186</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>1730120</v>
       </c>
@@ -6649,7 +6638,7 @@
         <v>10.794460476425993</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>1730328</v>
       </c>
@@ -6692,7 +6681,7 @@
         <v>12.378974980407637</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>1731121</v>
       </c>
@@ -6735,7 +6724,7 @@
         <v>11.485194491231917</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>1731446</v>
       </c>
@@ -6778,7 +6767,7 @@
         <v>12.017481475722624</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>1731667</v>
       </c>
@@ -6821,7 +6810,7 @@
         <v>11.500346682763368</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>1732018</v>
       </c>
@@ -6864,7 +6853,7 @@
         <v>11.473186217401212</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>1732200</v>
       </c>
@@ -6907,7 +6896,7 @@
         <v>11.417856256130069</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>1732525</v>
       </c>
@@ -6950,7 +6939,7 @@
         <v>11.520982916347959</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>1732746</v>
       </c>
@@ -6993,7 +6982,7 @@
         <v>11.246548159012276</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>1733331</v>
       </c>
@@ -7036,7 +7025,7 @@
         <v>10.884854161146471</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>1733383</v>
       </c>
@@ -7079,7 +7068,7 @@
         <v>10.319100991696107</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>1733435</v>
       </c>
@@ -7122,7 +7111,7 @@
         <v>11.07477702836835</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>1733630</v>
       </c>
@@ -7165,7 +7154,7 @@
         <v>12.077073822418056</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>1733695</v>
       </c>
@@ -7208,7 +7197,7 @@
         <v>10.903144693233813</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>1733851</v>
       </c>
@@ -7251,7 +7240,7 @@
         <v>11.092580194332612</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>1734514</v>
       </c>
@@ -7294,7 +7283,7 @@
         <v>11.085613441432056</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>1734722</v>
       </c>
@@ -7337,7 +7326,7 @@
         <v>11.920182300309401</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>1734865</v>
       </c>
@@ -7380,7 +7369,7 @@
         <v>11.057029848062699</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>1735086</v>
       </c>
@@ -7423,7 +7412,7 @@
         <v>10.95602099807971</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>1735307</v>
       </c>
@@ -7466,7 +7455,7 @@
         <v>12.222772424752588</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>1735385</v>
       </c>
@@ -7509,7 +7498,7 @@
         <v>10.708220829548091</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>1735411</v>
       </c>
@@ -7552,7 +7541,7 @@
         <v>11.428641274914318</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>1735515</v>
       </c>
@@ -7595,7 +7584,7 @@
         <v>11.173950098130897</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>1735835</v>
       </c>
@@ -7638,7 +7627,7 @@
         <v>11.578881730632917</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>1735866</v>
       </c>
@@ -7681,7 +7670,7 @@
         <v>10.830678658878572</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>1735879</v>
       </c>
@@ -7724,7 +7713,7 @@
         <v>11.217883038112156</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>1736750</v>
       </c>
@@ -7767,7 +7756,7 @@
         <v>11.226575837752225</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>1737218</v>
       </c>
@@ -7810,7 +7799,7 @@
         <v>11.901583454762012</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>1737257</v>
       </c>
@@ -7853,7 +7842,7 @@
         <v>11.361055515632103</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>1737608</v>
       </c>
@@ -7896,7 +7885,7 @@
         <v>12.168246159989717</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>1737894</v>
       </c>
@@ -7939,7 +7928,7 @@
         <v>11.330107785127584</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>1737907</v>
       </c>
@@ -7982,7 +7971,7 @@
         <v>11.450603152892837</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>1738479</v>
       </c>
@@ -8025,7 +8014,7 @@
         <v>11.67575834518032</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>1738570</v>
       </c>
@@ -8068,7 +8057,7 @@
         <v>11.163495640227039</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>1738830</v>
       </c>
@@ -8111,7 +8100,7 @@
         <v>10.839914189496584</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>1738895</v>
       </c>
@@ -8154,7 +8143,7 @@
         <v>11.27175795359301</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>1739519</v>
       </c>
@@ -8197,7 +8186,7 @@
         <v>12.334483450293384</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>1739883</v>
       </c>
@@ -8240,7 +8229,7 @@
         <v>12.259911946091655</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>1740767</v>
       </c>
@@ -8283,7 +8272,7 @@
         <v>11.727754546680353</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>1740793</v>
       </c>
@@ -8326,7 +8315,7 @@
         <v>11.569145104966536</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>1740884</v>
       </c>
@@ -8369,7 +8358,7 @@
         <v>11.617033196221268</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>1740910</v>
       </c>
@@ -8412,7 +8401,7 @@
         <v>12.010185490672789</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>1741105</v>
       </c>
@@ -8455,7 +8444,7 @@
         <v>12.056208598284753</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>1741183</v>
       </c>
@@ -8498,7 +8487,7 @@
         <v>11.438977480017872</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>1741586</v>
       </c>
@@ -8541,7 +8530,7 @@
         <v>11.56495798606238</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>1741742</v>
       </c>
@@ -8584,7 +8573,7 @@
         <v>11.689807253013818</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>1741326</v>
       </c>
@@ -8627,7 +8616,7 @@
         <v>11.293001724497216</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>1741651</v>
       </c>
@@ -8670,7 +8659,7 @@
         <v>11.8792338578772</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>1742028</v>
       </c>
@@ -8713,7 +8702,7 @@
         <v>10.895627596693721</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>1742795</v>
       </c>
@@ -8756,7 +8745,7 @@
         <v>11.510161649147497</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>1743250</v>
       </c>
@@ -8799,7 +8788,7 @@
         <v>11.806415637704985</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>1743406</v>
       </c>
@@ -8842,7 +8831,7 @@
         <v>11.792623247642904</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>1743666</v>
       </c>
@@ -8885,7 +8874,7 @@
         <v>11.664065904280609</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>1743744</v>
       </c>
@@ -8928,7 +8917,7 @@
         <v>11.46194791020536</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>1743770</v>
       </c>
@@ -8971,7 +8960,7 @@
         <v>11.5902938305459</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>1743900</v>
       </c>
@@ -9014,7 +9003,7 @@
         <v>11.040695358963601</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>1743939</v>
       </c>
@@ -9057,7 +9046,7 @@
         <v>11.414077032927626</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>1744225</v>
       </c>
@@ -9100,7 +9089,7 @@
         <v>11.412828848431943</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>1744407</v>
       </c>
@@ -9143,7 +9132,7 @@
         <v>11.320080733279282</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>1744524</v>
       </c>
@@ -9186,7 +9175,7 @@
         <v>12.274072357330606</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>1745421</v>
       </c>
@@ -9229,7 +9218,7 @@
         <v>11.107240332658515</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>1745434</v>
       </c>
@@ -9272,7 +9261,7 @@
         <v>11.004895928506238</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>1746357</v>
       </c>
@@ -9315,7 +9304,7 @@
         <v>11.539810793751611</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>1746604</v>
       </c>
@@ -9358,7 +9347,7 @@
         <v>11.479565146111982</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>1746786</v>
       </c>
@@ -9401,7 +9390,7 @@
         <v>11.061845645601192</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>1747007</v>
       </c>
@@ -9444,7 +9433,7 @@
         <v>10.669211175914377</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>1747540</v>
       </c>
@@ -9487,7 +9476,7 @@
         <v>11.335340671976555</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>1747774</v>
       </c>
@@ -9530,7 +9519,7 @@
         <v>10.823292103710079</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>1745564</v>
       </c>
@@ -9573,7 +9562,7 @@
         <v>11.270063782789915</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>1745616</v>
       </c>
@@ -9616,7 +9605,7 @@
         <v>11.091711999893924</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>1745694</v>
       </c>
@@ -9659,7 +9648,7 @@
         <v>11.235998679835268</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>1748242</v>
       </c>
@@ -9702,7 +9691,7 @@
         <v>10.837028637816811</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>1748554</v>
       </c>
@@ -9745,7 +9734,7 @@
         <v>10.858595069841899</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>1748671</v>
       </c>
@@ -9788,7 +9777,7 @@
         <v>11.750957628778188</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>1748892</v>
       </c>
@@ -9831,7 +9820,7 @@
         <v>11.004762958623722</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>1749100</v>
       </c>
@@ -9874,7 +9863,7 @@
         <v>11.36138138500792</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>1749308</v>
       </c>
@@ -9917,7 +9906,7 @@
         <v>11.215193056664946</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>1749607</v>
       </c>
@@ -9960,7 +9949,7 @@
         <v>11.439300453095491</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>1749854</v>
       </c>
@@ -10003,7 +9992,7 @@
         <v>11.600093496355584</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>1749945</v>
       </c>
@@ -10046,7 +10035,7 @@
         <v>11.171589419182814</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>1750218</v>
       </c>
@@ -10089,7 +10078,7 @@
         <v>11.493232831624493</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>1750647</v>
       </c>
@@ -10132,7 +10121,7 @@
         <v>11.354632885975635</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>1751089</v>
       </c>
@@ -10175,7 +10164,7 @@
         <v>11.286438831779758</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>1751349</v>
       </c>
@@ -10218,7 +10207,7 @@
         <v>11.440645052580592</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>1751622</v>
       </c>
@@ -10261,7 +10250,7 @@
         <v>11.743449711817181</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>1752584</v>
       </c>
@@ -10304,7 +10293,7 @@
         <v>11.611077058677385</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>1752103</v>
       </c>
@@ -10347,7 +10336,7 @@
         <v>11.397593173784854</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>1753000</v>
       </c>
@@ -10390,7 +10379,7 @@
         <v>11.078628690193362</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>1753377</v>
       </c>
@@ -10433,7 +10422,7 @@
         <v>11.192306892272182</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>1753442</v>
       </c>
@@ -10476,7 +10465,7 @@
         <v>11.368327347127613</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>1753455</v>
       </c>
@@ -10519,7 +10508,7 @@
         <v>12.173807684942899</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>1753559</v>
       </c>
@@ -10562,7 +10551,7 @@
         <v>10.671139055264179</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>1754144</v>
       </c>
@@ -10605,7 +10594,7 @@
         <v>10.991038893844813</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>1753481</v>
       </c>
@@ -10648,7 +10637,7 @@
         <v>11.734972415237232</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>1753663</v>
       </c>
@@ -10691,7 +10680,7 @@
         <v>11.90548768772287</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>1753871</v>
       </c>
@@ -10734,7 +10723,7 @@
         <v>10.920618599336354</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>1754534</v>
       </c>
@@ -10777,7 +10766,7 @@
         <v>11.856905164224408</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>1754638</v>
       </c>
@@ -10820,7 +10809,7 @@
         <v>11.250846159897952</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>1754820</v>
       </c>
@@ -10863,7 +10852,7 @@
         <v>11.074048340516821</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>1754885</v>
       </c>
@@ -10906,7 +10895,7 @@
         <v>11.457898894783012</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>1754560</v>
       </c>
@@ -10949,7 +10938,7 @@
         <v>11.188938956226457</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>1755041</v>
       </c>
@@ -10992,7 +10981,7 @@
         <v>11.479565146111982</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>1755639</v>
       </c>
@@ -11035,7 +11024,7 @@
         <v>11.491395346419866</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>1755938</v>
       </c>
@@ -11078,7 +11067,7 @@
         <v>11.502642778893181</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>1756627</v>
       </c>
@@ -11121,7 +11110,7 @@
         <v>11.469997086914306</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>1756640</v>
       </c>
@@ -11164,7 +11153,7 @@
         <v>11.411390954145931</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>1756887</v>
       </c>
@@ -11207,7 +11196,7 @@
         <v>11.533805942549584</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>1757225</v>
       </c>
@@ -11250,7 +11239,7 @@
         <v>11.296335392625862</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>1757381</v>
       </c>
@@ -11293,7 +11282,7 @@
         <v>11.399599979658106</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>1757394</v>
       </c>
@@ -11336,7 +11325,7 @@
         <v>11.02097066195449</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>1757407</v>
       </c>
@@ -11379,7 +11368,7 @@
         <v>11.536261059667192</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>1757654</v>
       </c>
@@ -11422,7 +11411,7 @@
         <v>10.841187463647783</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>1757732</v>
       </c>
@@ -11465,7 +11454,7 @@
         <v>10.895590517771231</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>1757875</v>
       </c>
@@ -11508,7 +11497,7 @@
         <v>11.623052602215697</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>1759052</v>
       </c>
@@ -11551,7 +11540,7 @@
         <v>11.334408660916139</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>1759572</v>
       </c>
@@ -11594,7 +11583,7 @@
         <v>10.516129418436423</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>1759988</v>
       </c>
@@ -11637,7 +11626,7 @@
         <v>11.473404706807946</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>1760287</v>
       </c>
@@ -11680,7 +11669,7 @@
         <v>11.780001687628991</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>1760352</v>
       </c>
@@ -11723,7 +11712,7 @@
         <v>11.201401418032876</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>1760391</v>
       </c>
@@ -11766,7 +11755,7 @@
         <v>11.360857614547074</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>1761216</v>
       </c>
@@ -11809,7 +11798,7 @@
         <v>11.831982650337254</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>1761314</v>
       </c>
@@ -11852,7 +11841,7 @@
         <v>10.654195843620604</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>1761678</v>
       </c>
@@ -11895,7 +11884,7 @@
         <v>11.684118663976339</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>1762016</v>
       </c>
@@ -11938,7 +11927,7 @@
         <v>11.199364743531556</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>1763641</v>
       </c>
@@ -11981,7 +11970,7 @@
         <v>10.803750523333086</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>1763706</v>
       </c>
@@ -12024,7 +12013,7 @@
         <v>11.048633493109792</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>1764135</v>
       </c>
@@ -12067,7 +12056,7 @@
         <v>11.636248681002227</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>1764304</v>
       </c>
@@ -12110,7 +12099,7 @@
         <v>11.774735729854438</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>1764343</v>
       </c>
@@ -12153,7 +12142,7 @@
         <v>10.998995026250759</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>1764278</v>
       </c>
@@ -12196,7 +12185,7 @@
         <v>10.48321404355681</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>1764421</v>
       </c>
@@ -12239,7 +12228,7 @@
         <v>11.623186951227762</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>1764538</v>
       </c>
@@ -12282,7 +12271,7 @@
         <v>12.241381872632408</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>1764616</v>
       </c>
@@ -12325,7 +12314,7 @@
         <v>10.211303079907536</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>1764902</v>
       </c>
@@ -12368,7 +12357,7 @@
         <v>10.872882937297062</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>1765338</v>
       </c>
@@ -12411,7 +12400,7 @@
         <v>11.213629545455776</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>1765442</v>
       </c>
@@ -12454,7 +12443,7 @@
         <v>11.279516908298021</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>1765806</v>
       </c>
@@ -12497,7 +12486,7 @@
         <v>11.410416435514195</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>1765819</v>
       </c>
@@ -12540,7 +12529,7 @@
         <v>11.011852132646917</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>1766027</v>
       </c>
@@ -12583,7 +12572,7 @@
         <v>11.320808085386121</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>1766040</v>
       </c>
@@ -12626,7 +12615,7 @@
         <v>11.162999126452767</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>1766053</v>
       </c>
@@ -12669,7 +12658,7 @@
         <v>11.276570019683788</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>1766066</v>
       </c>
@@ -12712,7 +12701,7 @@
         <v>10.761704157315251</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>1767548</v>
       </c>
@@ -12755,7 +12744,7 @@
         <v>11.097167567376632</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>1767769</v>
       </c>
@@ -12798,7 +12787,7 @@
         <v>10.565866199424438</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>1768003</v>
       </c>
@@ -12841,7 +12830,7 @@
         <v>11.327751844907647</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>1768081</v>
       </c>
@@ -12884,7 +12873,7 @@
         <v>10.898570980375382</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>1769758</v>
       </c>
@@ -12927,7 +12916,7 @@
         <v>11.57060929630978</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>1770122</v>
       </c>
@@ -12970,7 +12959,7 @@
         <v>11.198844658663882</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>1770161</v>
       </c>
@@ -13013,7 +13002,7 @@
         <v>11.616726765683969</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>1770564</v>
       </c>
@@ -13056,7 +13045,7 @@
         <v>11.84099103581689</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>1770629</v>
       </c>
@@ -13099,7 +13088,7 @@
         <v>10.624687547538109</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>1770720</v>
       </c>
@@ -13142,7 +13131,7 @@
         <v>11.507420339535736</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>1770850</v>
       </c>
@@ -13185,7 +13174,7 @@
         <v>11.053584783892745</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>1772052</v>
       </c>
@@ -13228,7 +13217,7 @@
         <v>11.721158403548683</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>1766703</v>
       </c>
@@ -13271,7 +13260,7 @@
         <v>11.49672494229852</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>1772520</v>
       </c>
@@ -13314,7 +13303,7 @@
         <v>10.801858683107332</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>1772676</v>
       </c>
@@ -13357,7 +13346,7 @@
         <v>11.086088599124372</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>1772923</v>
       </c>
@@ -13400,7 +13389,7 @@
         <v>10.998392979272911</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>1773157</v>
       </c>
@@ -13443,7 +13432,7 @@
         <v>11.29788648273253</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>1773391</v>
       </c>
@@ -13486,7 +13475,7 @@
         <v>11.683832118948885</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>1773638</v>
       </c>
@@ -13529,7 +13518,7 @@
         <v>10.76589215785248</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>1774275</v>
       </c>
@@ -13572,7 +13561,7 @@
         <v>11.197077086969873</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>1775081</v>
       </c>
@@ -13615,7 +13604,7 @@
         <v>11.666187178355308</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>1775185</v>
       </c>
@@ -13658,7 +13647,7 @@
         <v>11.083387926918672</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>1775484</v>
       </c>
@@ -13701,7 +13690,7 @@
         <v>11.268851901099827</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>1775874</v>
       </c>
@@ -13744,7 +13733,7 @@
         <v>11.898187865760873</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>1776160</v>
       </c>
@@ -13787,7 +13776,7 @@
         <v>11.875830958659597</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>1776706</v>
       </c>
@@ -13830,7 +13819,7 @@
         <v>11.113685937656255</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>1776935</v>
       </c>
@@ -13873,7 +13862,7 @@
         <v>10.863795169827057</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>1777694</v>
       </c>
@@ -13916,7 +13905,7 @@
         <v>11.55405781132637</v>
       </c>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>1777993</v>
       </c>
@@ -13959,7 +13948,7 @@
         <v>11.261112340932691</v>
       </c>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>1778175</v>
       </c>
@@ -13986,7 +13975,7 @@
         <v>9135366</v>
       </c>
       <c r="I258" s="4">
-        <f t="shared" ref="I258:I321" si="21">H258/C258</f>
+        <f t="shared" ref="I258:I285" si="21">H258/C258</f>
         <v>27936.899082568809</v>
       </c>
       <c r="J258" s="10">
@@ -14002,7 +13991,7 @@
         <v>11.42721505953182</v>
       </c>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>1778227</v>
       </c>
@@ -14045,7 +14034,7 @@
         <v>11.434963923500517</v>
       </c>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>1778370</v>
       </c>
@@ -14088,7 +14077,7 @@
         <v>11.522697562118932</v>
       </c>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>1778929</v>
       </c>
@@ -14131,7 +14120,7 @@
         <v>11.383625108873522</v>
       </c>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>1779267</v>
       </c>
@@ -14174,7 +14163,7 @@
         <v>11.30606118435202</v>
       </c>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>1779293</v>
       </c>
@@ -14217,7 +14206,7 @@
         <v>10.815830502162186</v>
       </c>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>1779397</v>
       </c>
@@ -14260,7 +14249,7 @@
         <v>11.810500935961494</v>
       </c>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>1780060</v>
       </c>
@@ -14303,7 +14292,7 @@
         <v>11.265950180402672</v>
       </c>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>1780125</v>
       </c>
@@ -14346,7 +14335,7 @@
         <v>11.429217715896744</v>
       </c>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>1780047</v>
       </c>
@@ -14389,7 +14378,7 @@
         <v>11.369320648202583</v>
       </c>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>1780242</v>
       </c>
@@ -14432,7 +14421,7 @@
         <v>12.071168883065372</v>
       </c>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>1780645</v>
       </c>
@@ -14475,7 +14464,7 @@
         <v>11.073117328439517</v>
       </c>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>1781048</v>
       </c>
@@ -14518,7 +14507,7 @@
         <v>11.546128105797946</v>
       </c>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>1781087</v>
       </c>
@@ -14561,7 +14550,7 @@
         <v>11.136266448703733</v>
       </c>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>1782049</v>
       </c>
@@ -14604,7 +14593,7 @@
         <v>11.336904020724754</v>
       </c>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>1781919</v>
       </c>
@@ -14647,7 +14636,7 @@
         <v>11.251521739037859</v>
       </c>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>1782075</v>
       </c>
@@ -14690,7 +14679,7 @@
         <v>12.011765548248206</v>
       </c>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>1782101</v>
       </c>
@@ -14733,7 +14722,7 @@
         <v>10.937863496628953</v>
       </c>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>1782400</v>
       </c>
@@ -14776,7 +14765,7 @@
         <v>11.640289126183502</v>
       </c>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>1782530</v>
       </c>
@@ -14819,7 +14808,7 @@
         <v>12.429220196836383</v>
       </c>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>1782686</v>
       </c>
@@ -14862,7 +14851,7 @@
         <v>11.392710725116256</v>
       </c>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>1782855</v>
       </c>
@@ -14905,7 +14894,7 @@
         <v>11.384387299697012</v>
       </c>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>1782985</v>
       </c>
@@ -14948,7 +14937,7 @@
         <v>11.164105305568016</v>
       </c>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>1783245</v>
       </c>
@@ -14991,7 +14980,7 @@
         <v>11.363195001576461</v>
       </c>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>1783349</v>
       </c>
@@ -15034,7 +15023,7 @@
         <v>11.026434666219032</v>
       </c>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>1783518</v>
       </c>
@@ -15077,7 +15066,7 @@
         <v>11.010663071864725</v>
       </c>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>1784038</v>
       </c>
@@ -15120,7 +15109,7 @@
         <v>11.488735226169011</v>
       </c>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>1784220</v>
       </c>
@@ -15171,26 +15160,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" style="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" style="19" customWidth="1"/>
     <col min="7" max="7" width="19" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.83203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" style="10"/>
+    <col min="8" max="8" width="21.77734375" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="10"/>
     <col min="10" max="10" width="15.6640625" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>375</v>
       </c>
@@ -15222,7 +15211,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>14</v>
       </c>
@@ -15258,7 +15247,7 @@
         <v>11.031002019557294</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>57</v>
       </c>
@@ -15294,7 +15283,7 @@
         <v>10.828899704034859</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>34</v>
       </c>
@@ -15330,7 +15319,7 @@
         <v>10.362913283029416</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>70</v>
       </c>
@@ -15366,7 +15355,7 @@
         <v>11.159433456203997</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>71</v>
       </c>
@@ -15402,7 +15391,7 @@
         <v>10.445709206137517</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>25</v>
       </c>
@@ -15438,7 +15427,7 @@
         <v>10.419755366577585</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>45</v>
       </c>
@@ -15474,7 +15463,7 @@
         <v>10.7052107101998</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>21</v>
       </c>
@@ -15510,7 +15499,7 @@
         <v>11.099371537808151</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>19</v>
       </c>
@@ -15546,7 +15535,7 @@
         <v>10.852996645363218</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>72</v>
       </c>
@@ -15582,7 +15571,7 @@
         <v>11.499188824048719</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>60</v>
       </c>
@@ -15618,7 +15607,7 @@
         <v>10.913546504455319</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>58</v>
       </c>
@@ -15654,7 +15643,7 @@
         <v>10.637060840167898</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>47</v>
       </c>
@@ -15690,7 +15679,7 @@
         <v>10.286172632312471</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>48</v>
       </c>
@@ -15726,7 +15715,7 @@
         <v>10.80927891415986</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>44</v>
       </c>
@@ -15762,7 +15751,7 @@
         <v>10.441186521255725</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>66</v>
       </c>
@@ -15798,7 +15787,7 @@
         <v>10.442102988774103</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>64</v>
       </c>
@@ -15834,7 +15823,7 @@
         <v>11.016652526125462</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>35</v>
       </c>
@@ -15870,7 +15859,7 @@
         <v>10.368966471251481</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>17</v>
       </c>
@@ -15906,7 +15895,7 @@
         <v>11.188188767636873</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>27</v>
       </c>
@@ -15942,7 +15931,7 @@
         <v>10.111203367622934</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>52</v>
       </c>
@@ -15978,7 +15967,7 @@
         <v>10.78083465569202</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>77</v>
       </c>
@@ -16014,7 +16003,7 @@
         <v>10.928953582167779</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>9</v>
       </c>
@@ -16050,7 +16039,7 @@
         <v>11.563929188309336</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>68</v>
       </c>
@@ -16086,7 +16075,7 @@
         <v>10.004563755714534</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>12</v>
       </c>
@@ -16122,7 +16111,7 @@
         <v>11.726871126795587</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>37</v>
       </c>
@@ -16158,7 +16147,7 @@
         <v>10.04968020856829</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>63</v>
       </c>
@@ -16194,7 +16183,7 @@
         <v>10.651995336734213</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>56</v>
       </c>
@@ -16230,7 +16219,7 @@
         <v>11.22474117429047</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>38</v>
       </c>
@@ -16266,7 +16255,7 @@
         <v>10.419402941498909</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>69</v>
       </c>
@@ -16302,7 +16291,7 @@
         <v>10.297112598242729</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>55</v>
       </c>
@@ -16338,7 +16327,7 @@
         <v>10.953452705060228</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>20</v>
       </c>
@@ -16374,7 +16363,7 @@
         <v>10.756084218436319</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>23</v>
       </c>
@@ -16410,7 +16399,7 @@
         <v>10.583852857255158</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>41</v>
       </c>
@@ -16446,7 +16435,7 @@
         <v>10.921913791121185</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>16</v>
       </c>
@@ -16482,7 +16471,7 @@
         <v>11.110619696631765</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>11</v>
       </c>
@@ -16518,7 +16507,7 @@
         <v>11.247581733844214</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>39</v>
       </c>
@@ -16554,7 +16543,7 @@
         <v>10.801904259533318</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>6</v>
       </c>
@@ -16590,7 +16579,7 @@
         <v>11.437972872207729</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>7</v>
       </c>
@@ -16626,7 +16615,7 @@
         <v>11.656061175562241</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4</v>
       </c>
@@ -16662,7 +16651,7 @@
         <v>11.304045636113189</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>22</v>
       </c>
@@ -16698,7 +16687,7 @@
         <v>11.325483293321987</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>31</v>
       </c>
@@ -16734,7 +16723,7 @@
         <v>10.86100644640474</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>59</v>
       </c>
@@ -16770,7 +16759,7 @@
         <v>10.812502811534516</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>18</v>
       </c>
@@ -16806,7 +16795,7 @@
         <v>10.883404732884975</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>75</v>
       </c>
@@ -16842,7 +16831,7 @@
         <v>11.058813994085805</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>74</v>
       </c>
@@ -16878,7 +16867,7 @@
         <v>11.535236942965653</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>8</v>
       </c>
@@ -16914,7 +16903,7 @@
         <v>11.571438648975581</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>33</v>
       </c>
@@ -16950,7 +16939,7 @@
         <v>11.60932951239965</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>28</v>
       </c>
@@ -16986,7 +16975,7 @@
         <v>11.419992599595775</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>61</v>
       </c>
@@ -17022,7 +17011,7 @@
         <v>10.460703084242111</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>5</v>
       </c>
@@ -17058,7 +17047,7 @@
         <v>11.736333998898845</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>29</v>
       </c>
@@ -17094,7 +17083,7 @@
         <v>10.251565868438577</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>13</v>
       </c>
@@ -17130,7 +17119,7 @@
         <v>10.93822116868469</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>10</v>
       </c>
@@ -17166,7 +17155,7 @@
         <v>11.338390929122015</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>76</v>
       </c>
@@ -17202,7 +17191,7 @@
         <v>10.887603686796528</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>36</v>
       </c>
@@ -17238,7 +17227,7 @@
         <v>10.399521781270227</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>15</v>
       </c>
@@ -17274,7 +17263,7 @@
         <v>11.164204798643507</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>50</v>
       </c>
@@ -17310,7 +17299,7 @@
         <v>10.68141380264416</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>54</v>
       </c>
@@ -17346,7 +17335,7 @@
         <v>9.6418743727074077</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>1</v>
       </c>
@@ -17382,7 +17371,7 @@
         <v>10.673068208964477</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>49</v>
       </c>
@@ -17418,7 +17407,7 @@
         <v>10.616089719294841</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>46</v>
       </c>
@@ -17454,7 +17443,7 @@
         <v>10.458976040221101</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>51</v>
       </c>
@@ -17490,7 +17479,7 @@
         <v>10.49997902672273</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>30</v>
       </c>
@@ -17526,7 +17515,7 @@
         <v>10.454642257781865</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>43</v>
       </c>
@@ -17562,7 +17551,7 @@
         <v>10.376396597636671</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>32</v>
       </c>
@@ -17598,7 +17587,7 @@
         <v>11.596122920978639</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>3</v>
       </c>
@@ -17634,7 +17623,7 @@
         <v>10.917067574251094</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>73</v>
       </c>
@@ -17670,7 +17659,7 @@
         <v>10.855145428033195</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>40</v>
       </c>
@@ -17706,7 +17695,7 @@
         <v>10.143412580863743</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>62</v>
       </c>
@@ -17742,7 +17731,7 @@
         <v>11.015941805644212</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>67</v>
       </c>
@@ -17778,7 +17767,7 @@
         <v>10.196927473290403</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>26</v>
       </c>
@@ -17814,7 +17803,7 @@
         <v>10.092844012001068</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>65</v>
       </c>
@@ -17850,7 +17839,7 @@
         <v>10.913660621083944</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>53</v>
       </c>
@@ -17886,7 +17875,7 @@
         <v>10.651851434609709</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2</v>
       </c>
@@ -17922,7 +17911,7 @@
         <v>10.894461906330365</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>24</v>
       </c>
@@ -17958,7 +17947,7 @@
         <v>11.558270929032696</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>42</v>
       </c>
@@ -18002,18 +17991,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="2"/>
+    <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>296</v>
       </c>
@@ -18021,7 +18010,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>FACTORS_MUNI!K1</f>
         <v>ln_POP</v>
@@ -18030,7 +18019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>FACTORS_MUNI!J1</f>
         <v>ln_TAX_BASE_PER_CAP</v>
@@ -18039,7 +18028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>FACTORS_MUNI!L1</f>
         <v>ln_MED_HH_INC</v>
@@ -18048,7 +18037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>FACTORS_MUNI!G1</f>
         <v>PCT_EDA_POP</v>
@@ -18099,7 +18088,7 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>FACTORS_MUNI!$C$1:$XFD$1</xm:f>
           </x14:formula1>
@@ -18112,18 +18101,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>297</v>
       </c>
@@ -18131,7 +18120,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="14">
         <v>4</v>
       </c>
@@ -18139,7 +18128,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="14">
         <v>3</v>
       </c>
@@ -18147,7 +18136,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="14">
         <v>2</v>
       </c>
@@ -18155,7 +18144,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="14">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Update population in EDAs with 2020 Census data
Only North Chicago saw a major change, because previous calculation used PBHI which does not include GQ pop. Much of the total pop of North Chicago is GQ (Naval Station Great Lakes)
</commit_message>
<xml_diff>
--- a/input/community_cohort_inputs.xlsx
+++ b/input/community_cohort_inputs.xlsx
@@ -17,9 +17,6 @@
     <sheet name="WEIGHTS" sheetId="2" r:id="rId3"/>
     <sheet name="COHORTS" sheetId="3" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FACTORS_CCA!$A$1:$K$78</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -178,7 +175,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Percent of population living in an EDA or disinvested area, calculated from 2015 PBHI and EDA/disinvested layer</t>
+          <t>Percent of population living in an EDA or disinvested area, calculated from 2020 Census block centroids and EDA/disinvested layer</t>
         </r>
       </text>
     </comment>
@@ -375,7 +372,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> Percent of population living in an EDA or disinvested area, calculated from 2015 PBHI and EDA/disinvested layer</t>
+          <t xml:space="preserve"> Percent of population living in an EDA or disinvested area, calculated from 2020 Census block centroids and EDA/disinvested layer</t>
         </r>
       </text>
     </comment>
@@ -2963,7 +2960,7 @@
         <v>1265737906</v>
       </c>
       <c r="G2" s="9">
-        <v>0.57489999999999997</v>
+        <v>0.5683715198028122</v>
       </c>
       <c r="H2" s="27">
         <f t="shared" ref="H2:H65" si="0">E2+F2</f>
@@ -3006,7 +3003,7 @@
         <v>982740828</v>
       </c>
       <c r="G3" s="9">
-        <v>5.1400000000000001E-2</v>
+        <v>4.4444444444444446E-2</v>
       </c>
       <c r="H3" s="27">
         <f t="shared" si="0"/>
@@ -3049,7 +3046,7 @@
         <v>569436644</v>
       </c>
       <c r="G4" s="9">
-        <v>2.18E-2</v>
+        <v>2.2556785395792898E-2</v>
       </c>
       <c r="H4" s="27">
         <f t="shared" si="0"/>
@@ -3135,7 +3132,7 @@
         <v>3366699572</v>
       </c>
       <c r="G6" s="9">
-        <v>0.17219999999999999</v>
+        <v>0.17019413976002884</v>
       </c>
       <c r="H6" s="27">
         <f t="shared" si="0"/>
@@ -3178,7 +3175,7 @@
         <v>4160197050</v>
       </c>
       <c r="G7" s="9">
-        <v>0.67459999999999998</v>
+        <v>0.62980359140809339</v>
       </c>
       <c r="H7" s="27">
         <f t="shared" si="0"/>
@@ -3307,7 +3304,7 @@
         <v>449276747</v>
       </c>
       <c r="G10" s="9">
-        <v>3.3599999999999998E-2</v>
+        <v>3.0384054448225572E-2</v>
       </c>
       <c r="H10" s="27">
         <f t="shared" si="0"/>
@@ -3350,7 +3347,7 @@
         <v>1166637184</v>
       </c>
       <c r="G11" s="9">
-        <v>0.18840000000000001</v>
+        <v>0.18829826055224425</v>
       </c>
       <c r="H11" s="27">
         <f t="shared" si="0"/>
@@ -3436,7 +3433,7 @@
         <v>225579145</v>
       </c>
       <c r="G13" s="9">
-        <v>9.9199999999999997E-2</v>
+        <v>9.1725735139308026E-2</v>
       </c>
       <c r="H13" s="27">
         <f t="shared" si="0"/>
@@ -3479,7 +3476,7 @@
         <v>398088705</v>
       </c>
       <c r="G14" s="9">
-        <v>0</v>
+        <v>2.3255813953488372E-2</v>
       </c>
       <c r="H14" s="27">
         <f t="shared" si="0"/>
@@ -3565,7 +3562,7 @@
         <v>208315798</v>
       </c>
       <c r="G16" s="9">
-        <v>0.83120000000000005</v>
+        <v>0.83186971100111773</v>
       </c>
       <c r="H16" s="27">
         <f t="shared" si="0"/>
@@ -3608,7 +3605,7 @@
         <v>623028607</v>
       </c>
       <c r="G17" s="9">
-        <v>0.25409999999999999</v>
+        <v>0.25663105299526923</v>
       </c>
       <c r="H17" s="27">
         <f t="shared" si="0"/>
@@ -3694,7 +3691,7 @@
         <v>689990767</v>
       </c>
       <c r="G19" s="9">
-        <v>0.72570000000000001</v>
+        <v>0.72496069868995638</v>
       </c>
       <c r="H19" s="27">
         <f t="shared" si="0"/>
@@ -3780,7 +3777,7 @@
         <v>897935373</v>
       </c>
       <c r="G21" s="9">
-        <v>0.125</v>
+        <v>0.12523456348851755</v>
       </c>
       <c r="H21" s="27">
         <f t="shared" si="0"/>
@@ -3866,7 +3863,7 @@
         <v>2274174440</v>
       </c>
       <c r="G23" s="9">
-        <v>0.25719999999999998</v>
+        <v>0.25710884445767163</v>
       </c>
       <c r="H23" s="27">
         <f t="shared" si="0"/>
@@ -3995,7 +3992,7 @@
         <v>433261246</v>
       </c>
       <c r="G26" s="9">
-        <v>0.29220000000000002</v>
+        <v>0.30275444881658542</v>
       </c>
       <c r="H26" s="27">
         <f t="shared" si="0"/>
@@ -4038,7 +4035,7 @@
         <v>245666345</v>
       </c>
       <c r="G27" s="9">
-        <v>0.6855</v>
+        <v>0.67529382345586397</v>
       </c>
       <c r="H27" s="27">
         <f t="shared" si="0"/>
@@ -4081,7 +4078,7 @@
         <v>393073486</v>
       </c>
       <c r="G28" s="9">
-        <v>0.7802</v>
+        <v>0.7737215033887862</v>
       </c>
       <c r="H28" s="27">
         <f t="shared" si="0"/>
@@ -4124,7 +4121,7 @@
         <v>1815545066</v>
       </c>
       <c r="G29" s="9">
-        <v>4.1000000000000003E-3</v>
+        <v>4.30435990002777E-3</v>
       </c>
       <c r="H29" s="27">
         <f t="shared" si="0"/>
@@ -4210,7 +4207,7 @@
         <v>472578911</v>
       </c>
       <c r="G31" s="9">
-        <v>0.66339999999999999</v>
+        <v>0.6628961581575461</v>
       </c>
       <c r="H31" s="27">
         <f t="shared" si="0"/>
@@ -4425,7 +4422,7 @@
         <v>76830637</v>
       </c>
       <c r="G36" s="9">
-        <v>0.55430000000000001</v>
+        <v>0.54448398576512458</v>
       </c>
       <c r="H36" s="27">
         <f t="shared" si="0"/>
@@ -4511,7 +4508,7 @@
         <v>1331716022</v>
       </c>
       <c r="G38" s="9">
-        <v>0.15939999999999999</v>
+        <v>0.16685903547950018</v>
       </c>
       <c r="H38" s="27">
         <f t="shared" si="0"/>
@@ -4554,7 +4551,7 @@
         <v>641366396</v>
       </c>
       <c r="G39" s="9">
-        <v>0.7389</v>
+        <v>0.72645657267725039</v>
       </c>
       <c r="H39" s="27">
         <f t="shared" si="0"/>
@@ -4683,7 +4680,7 @@
         <v>87825670349</v>
       </c>
       <c r="G42" s="9">
-        <v>0.64339999999999997</v>
+        <v>0.62405129937940307</v>
       </c>
       <c r="H42" s="27">
         <f t="shared" si="0"/>
@@ -4726,7 +4723,7 @@
         <v>342743426</v>
       </c>
       <c r="G43" s="9">
-        <v>0.80069999999999997</v>
+        <v>0.77678311499272201</v>
       </c>
       <c r="H43" s="27">
         <f t="shared" si="0"/>
@@ -4769,7 +4766,7 @@
         <v>318357769</v>
       </c>
       <c r="G44" s="9">
-        <v>0.55959999999999999</v>
+        <v>0.57756530173907017</v>
       </c>
       <c r="H44" s="27">
         <f t="shared" si="0"/>
@@ -4941,7 +4938,7 @@
         <v>181163680</v>
       </c>
       <c r="G48" s="9">
-        <v>0.439</v>
+        <v>0.43540983606557376</v>
       </c>
       <c r="H48" s="27">
         <f t="shared" si="0"/>
@@ -5027,7 +5024,7 @@
         <v>398393372</v>
       </c>
       <c r="G50" s="9">
-        <v>0</v>
+        <v>4.8878244293464976E-5</v>
       </c>
       <c r="H50" s="27">
         <f t="shared" si="0"/>
@@ -5070,7 +5067,7 @@
         <v>327193249</v>
       </c>
       <c r="G51" s="9">
-        <v>0.14649999999999999</v>
+        <v>0.14049510437834842</v>
       </c>
       <c r="H51" s="27">
         <f t="shared" si="0"/>
@@ -5156,7 +5153,7 @@
         <v>1199910786</v>
       </c>
       <c r="G53" s="9">
-        <v>9.5100000000000004E-2</v>
+        <v>8.9671956095259381E-2</v>
       </c>
       <c r="H53" s="27">
         <f t="shared" si="0"/>
@@ -5328,7 +5325,7 @@
         <v>2252496910</v>
       </c>
       <c r="G57" s="9">
-        <v>0.1406</v>
+        <v>0.14597445405850845</v>
       </c>
       <c r="H57" s="27">
         <f t="shared" si="0"/>
@@ -5543,7 +5540,7 @@
         <v>108311381</v>
       </c>
       <c r="G62" s="9">
-        <v>1.15E-2</v>
+        <v>6.9796954314720813E-3</v>
       </c>
       <c r="H62" s="27">
         <f t="shared" si="0"/>
@@ -5672,7 +5669,7 @@
         <v>2644524303</v>
       </c>
       <c r="G65" s="9">
-        <v>0.59970000000000001</v>
+        <v>0.5655287159072101</v>
       </c>
       <c r="H65" s="27">
         <f t="shared" si="0"/>
@@ -5715,7 +5712,7 @@
         <v>2243624199</v>
       </c>
       <c r="G66" s="9">
-        <v>1.9699999999999999E-2</v>
+        <v>2.1028891868828479E-2</v>
       </c>
       <c r="H66" s="27">
         <f t="shared" ref="H66:H129" si="5">E66+F66</f>
@@ -5801,7 +5798,7 @@
         <v>522591802</v>
       </c>
       <c r="G68" s="9">
-        <v>0.41420000000000001</v>
+        <v>0.40736511561518696</v>
       </c>
       <c r="H68" s="27">
         <f t="shared" si="5"/>
@@ -5887,7 +5884,7 @@
         <v>3432148547</v>
       </c>
       <c r="G70" s="9">
-        <v>8.5900000000000004E-2</v>
+        <v>7.9656894123671745E-2</v>
       </c>
       <c r="H70" s="27">
         <f t="shared" si="5"/>
@@ -5930,7 +5927,7 @@
         <v>412176856</v>
       </c>
       <c r="G71" s="9">
-        <v>0.25679999999999997</v>
+        <v>0.25718297146868574</v>
       </c>
       <c r="H71" s="27">
         <f t="shared" si="5"/>
@@ -6274,7 +6271,7 @@
         <v>828461628</v>
       </c>
       <c r="G79" s="9">
-        <v>8.6300000000000002E-2</v>
+        <v>7.0179238641901773E-2</v>
       </c>
       <c r="H79" s="27">
         <f t="shared" si="5"/>
@@ -6403,7 +6400,7 @@
         <v>1513681682</v>
       </c>
       <c r="G82" s="9">
-        <v>7.9699999999999993E-2</v>
+        <v>8.7741801289606874E-2</v>
       </c>
       <c r="H82" s="27">
         <f t="shared" si="5"/>
@@ -6489,7 +6486,7 @@
         <v>751406632</v>
       </c>
       <c r="G84" s="9">
-        <v>0.34200000000000003</v>
+        <v>0.32653122739329637</v>
       </c>
       <c r="H84" s="27">
         <f t="shared" si="5"/>
@@ -6532,7 +6529,7 @@
         <v>2812363119</v>
       </c>
       <c r="G85" s="9">
-        <v>6.7299999999999999E-2</v>
+        <v>7.2703007904732581E-2</v>
       </c>
       <c r="H85" s="27">
         <f t="shared" si="5"/>
@@ -6575,7 +6572,7 @@
         <v>97479482</v>
       </c>
       <c r="G86" s="9">
-        <v>0.36649999999999999</v>
+        <v>0.35407527129993072</v>
       </c>
       <c r="H86" s="27">
         <f t="shared" si="5"/>
@@ -6704,7 +6701,7 @@
         <v>599525768</v>
       </c>
       <c r="G89" s="9">
-        <v>0.17699999999999999</v>
+        <v>0.1706042921686747</v>
       </c>
       <c r="H89" s="27">
         <f t="shared" si="5"/>
@@ -6833,7 +6830,7 @@
         <v>1190068676</v>
       </c>
       <c r="G92" s="9">
-        <v>1E-3</v>
+        <v>8.7930697583534162E-4</v>
       </c>
       <c r="H92" s="27">
         <f t="shared" si="5"/>
@@ -6876,7 +6873,7 @@
         <v>73768285</v>
       </c>
       <c r="G93" s="9">
-        <v>0.40410000000000001</v>
+        <v>0.40862944162436549</v>
       </c>
       <c r="H93" s="27">
         <f t="shared" si="5"/>
@@ -6962,7 +6959,7 @@
         <v>712977924</v>
       </c>
       <c r="G95" s="9">
-        <v>0.43780000000000002</v>
+        <v>0.43509474246063518</v>
       </c>
       <c r="H95" s="27">
         <f t="shared" si="5"/>
@@ -7005,7 +7002,7 @@
         <v>127928093</v>
       </c>
       <c r="G96" s="9">
-        <v>0.81869999999999998</v>
+        <v>0.81856584644629848</v>
       </c>
       <c r="H96" s="27">
         <f t="shared" si="5"/>
@@ -7048,7 +7045,7 @@
         <v>198408405</v>
       </c>
       <c r="G97" s="9">
-        <v>0.99990000000000001</v>
+        <v>1</v>
       </c>
       <c r="H97" s="27">
         <f t="shared" si="5"/>
@@ -7177,7 +7174,7 @@
         <v>131111247</v>
       </c>
       <c r="G100" s="9">
-        <v>0.6391</v>
+        <v>0.61717232102824693</v>
       </c>
       <c r="H100" s="27">
         <f t="shared" si="5"/>
@@ -7263,7 +7260,7 @@
         <v>289749678</v>
       </c>
       <c r="G102" s="9">
-        <v>0.3357</v>
+        <v>0.34036539124439846</v>
       </c>
       <c r="H102" s="27">
         <f t="shared" si="5"/>
@@ -7306,7 +7303,7 @@
         <v>2352014644</v>
       </c>
       <c r="G103" s="9">
-        <v>2.7000000000000001E-3</v>
+        <v>1.193001060445387E-2</v>
       </c>
       <c r="H103" s="27">
         <f t="shared" si="5"/>
@@ -7349,7 +7346,7 @@
         <v>148565577</v>
       </c>
       <c r="G104" s="9">
-        <v>0.98399999999999999</v>
+        <v>0.98561292865589278</v>
       </c>
       <c r="H104" s="27">
         <f t="shared" si="5"/>
@@ -7392,7 +7389,7 @@
         <v>213154909</v>
       </c>
       <c r="G105" s="9">
-        <v>8.9999999999999998E-4</v>
+        <v>4.807692307692308E-4</v>
       </c>
       <c r="H105" s="27">
         <f t="shared" si="5"/>
@@ -7521,7 +7518,7 @@
         <v>1585481333</v>
       </c>
       <c r="G108" s="9">
-        <v>0.10100000000000001</v>
+        <v>9.9961926518180089E-2</v>
       </c>
       <c r="H108" s="27">
         <f t="shared" si="5"/>
@@ -7693,7 +7690,7 @@
         <v>358598079</v>
       </c>
       <c r="G112" s="9">
-        <v>0.3468</v>
+        <v>0.34896984020962851</v>
       </c>
       <c r="H112" s="27">
         <f t="shared" si="5"/>
@@ -8037,7 +8034,7 @@
         <v>3338556246</v>
       </c>
       <c r="G120" s="9">
-        <v>0.39510000000000001</v>
+        <v>0.38476476769396523</v>
       </c>
       <c r="H120" s="27">
         <f t="shared" si="5"/>
@@ -8080,7 +8077,7 @@
         <v>157206872</v>
       </c>
       <c r="G121" s="9">
-        <v>0.55510000000000004</v>
+        <v>0.54738095238095241</v>
       </c>
       <c r="H121" s="27">
         <f t="shared" si="5"/>
@@ -8295,7 +8292,7 @@
         <v>385485986</v>
       </c>
       <c r="G126" s="9">
-        <v>0.32229999999999998</v>
+        <v>0.33365491651205936</v>
       </c>
       <c r="H126" s="27">
         <f t="shared" si="5"/>
@@ -8682,7 +8679,7 @@
         <v>376604855</v>
       </c>
       <c r="G135" s="9">
-        <v>0.52729999999999999</v>
+        <v>0.5263103590590178</v>
       </c>
       <c r="H135" s="27">
         <f t="shared" si="10"/>
@@ -9069,7 +9066,7 @@
         <v>795598289</v>
       </c>
       <c r="G144" s="9">
-        <v>6.0000000000000001E-3</v>
+        <v>9.1591936843718868E-3</v>
       </c>
       <c r="H144" s="27">
         <f t="shared" si="10"/>
@@ -9112,7 +9109,7 @@
         <v>1664970939</v>
       </c>
       <c r="G145" s="9">
-        <v>0.31059999999999999</v>
+        <v>0.3023653206223581</v>
       </c>
       <c r="H145" s="27">
         <f t="shared" si="10"/>
@@ -9241,7 +9238,7 @@
         <v>171123356</v>
       </c>
       <c r="G148" s="9">
-        <v>0.57230000000000003</v>
+        <v>0.56891929370435423</v>
       </c>
       <c r="H148" s="27">
         <f t="shared" si="10"/>
@@ -9456,7 +9453,7 @@
         <v>395282660</v>
       </c>
       <c r="G153" s="9">
-        <v>0.16930000000000001</v>
+        <v>0.17081738583337702</v>
       </c>
       <c r="H153" s="27">
         <f t="shared" si="10"/>
@@ -9499,7 +9496,7 @@
         <v>204847370</v>
       </c>
       <c r="G154" s="9">
-        <v>0.99980000000000002</v>
+        <v>1</v>
       </c>
       <c r="H154" s="27">
         <f t="shared" si="10"/>
@@ -9671,7 +9668,7 @@
         <v>646161618</v>
       </c>
       <c r="G158" s="9">
-        <v>0.80789999999999995</v>
+        <v>0.80085497660913052</v>
       </c>
       <c r="H158" s="27">
         <f t="shared" si="10"/>
@@ -9800,7 +9797,7 @@
         <v>196157893</v>
       </c>
       <c r="G161" s="9">
-        <v>0.37509999999999999</v>
+        <v>0.38066317626527052</v>
       </c>
       <c r="H161" s="27">
         <f t="shared" si="10"/>
@@ -10058,7 +10055,7 @@
         <v>479911867</v>
       </c>
       <c r="G167" s="9">
-        <v>7.3700000000000002E-2</v>
+        <v>7.4375678610206303E-2</v>
       </c>
       <c r="H167" s="27">
         <f t="shared" si="10"/>
@@ -10101,7 +10098,7 @@
         <v>940781296</v>
       </c>
       <c r="G168" s="9">
-        <v>0.2954</v>
+        <v>0.29612206981064948</v>
       </c>
       <c r="H168" s="27">
         <f t="shared" si="10"/>
@@ -10144,7 +10141,7 @@
         <v>1971307340</v>
       </c>
       <c r="G169" s="9">
-        <v>0.32369999999999999</v>
+        <v>0.32104411454302401</v>
       </c>
       <c r="H169" s="27">
         <f t="shared" si="10"/>
@@ -10187,7 +10184,7 @@
         <v>931954514</v>
       </c>
       <c r="G170" s="9">
-        <v>0.1903</v>
+        <v>0.17908745247148289</v>
       </c>
       <c r="H170" s="27">
         <f t="shared" si="10"/>
@@ -10230,7 +10227,7 @@
         <v>7451453141</v>
       </c>
       <c r="G171" s="9">
-        <v>0.16800000000000001</v>
+        <v>0.16067272970442692</v>
       </c>
       <c r="H171" s="27">
         <f t="shared" si="10"/>
@@ -10273,7 +10270,7 @@
         <v>927982302</v>
       </c>
       <c r="G172" s="9">
-        <v>8.4699999999999998E-2</v>
+        <v>7.4924671125156175E-2</v>
       </c>
       <c r="H172" s="27">
         <f t="shared" si="10"/>
@@ -10359,7 +10356,7 @@
         <v>1391070617</v>
       </c>
       <c r="G174" s="9">
-        <v>0.33950000000000002</v>
+        <v>0.32767210144927539</v>
       </c>
       <c r="H174" s="27">
         <f t="shared" si="10"/>
@@ -10445,7 +10442,7 @@
         <v>559300173</v>
       </c>
       <c r="G176" s="9">
-        <v>4.5999999999999999E-3</v>
+        <v>1.965938338535677E-2</v>
       </c>
       <c r="H176" s="27">
         <f t="shared" si="10"/>
@@ -10531,7 +10528,7 @@
         <v>204274686</v>
       </c>
       <c r="G178" s="9">
-        <v>0.92279999999999995</v>
+        <v>0.58269124483890888</v>
       </c>
       <c r="H178" s="27">
         <f t="shared" si="10"/>
@@ -10617,7 +10614,7 @@
         <v>2866844264</v>
       </c>
       <c r="G180" s="9">
-        <v>1.4800000000000001E-2</v>
+        <v>1.371302027142127E-2</v>
       </c>
       <c r="H180" s="27">
         <f t="shared" si="10"/>
@@ -10703,7 +10700,7 @@
         <v>410394946</v>
       </c>
       <c r="G182" s="9">
-        <v>0.23</v>
+        <v>0.20973520249221184</v>
       </c>
       <c r="H182" s="27">
         <f t="shared" si="10"/>
@@ -10789,7 +10786,7 @@
         <v>438344805</v>
       </c>
       <c r="G184" s="9">
-        <v>7.2400000000000006E-2</v>
+        <v>7.4568745905815567E-2</v>
       </c>
       <c r="H184" s="27">
         <f t="shared" si="10"/>
@@ -10832,7 +10829,7 @@
         <v>1150256869</v>
       </c>
       <c r="G185" s="9">
-        <v>0.3649</v>
+        <v>0.36803056783523524</v>
       </c>
       <c r="H185" s="27">
         <f t="shared" si="10"/>
@@ -10918,7 +10915,7 @@
         <v>308469895</v>
       </c>
       <c r="G187" s="9">
-        <v>0.53900000000000003</v>
+        <v>0.5136314067611778</v>
       </c>
       <c r="H187" s="27">
         <f t="shared" si="10"/>
@@ -11176,7 +11173,7 @@
         <v>971585725</v>
       </c>
       <c r="G193" s="9">
-        <v>0.1095</v>
+        <v>0.10371548359115224</v>
       </c>
       <c r="H193" s="27">
         <f t="shared" si="10"/>
@@ -11219,7 +11216,7 @@
         <v>2033533072</v>
       </c>
       <c r="G194" s="9">
-        <v>0.19450000000000001</v>
+        <v>0.18455852035106321</v>
       </c>
       <c r="H194" s="27">
         <f t="shared" ref="H194:H257" si="15">E194+F194</f>
@@ -11305,7 +11302,7 @@
         <v>353553033</v>
       </c>
       <c r="G196" s="9">
-        <v>0.39760000000000001</v>
+        <v>0.39136535348084189</v>
       </c>
       <c r="H196" s="27">
         <f t="shared" si="15"/>
@@ -11391,7 +11388,7 @@
         <v>54452578</v>
       </c>
       <c r="G198" s="9">
-        <v>0.80710000000000004</v>
+        <v>0.79746353836398221</v>
       </c>
       <c r="H198" s="27">
         <f t="shared" si="15"/>
@@ -11434,7 +11431,7 @@
         <v>129403796</v>
       </c>
       <c r="G199" s="9">
-        <v>0.89780000000000004</v>
+        <v>0.89717342186563376</v>
       </c>
       <c r="H199" s="27">
         <f t="shared" si="15"/>
@@ -11477,7 +11474,7 @@
         <v>1801027534</v>
       </c>
       <c r="G200" s="9">
-        <v>2.0199999999999999E-2</v>
+        <v>1.7525721202340125E-2</v>
       </c>
       <c r="H200" s="27">
         <f t="shared" si="15"/>
@@ -11907,7 +11904,7 @@
         <v>435030143</v>
       </c>
       <c r="G210" s="9">
-        <v>0.28749999999999998</v>
+        <v>0.28926391829617637</v>
       </c>
       <c r="H210" s="27">
         <f t="shared" si="15"/>
@@ -11993,7 +11990,7 @@
         <v>143900332</v>
       </c>
       <c r="G212" s="9">
-        <v>0.3322</v>
+        <v>0.32790606653620352</v>
       </c>
       <c r="H212" s="27">
         <f t="shared" si="15"/>
@@ -12122,7 +12119,7 @@
         <v>231647706</v>
       </c>
       <c r="G215" s="9">
-        <v>0.63519999999999999</v>
+        <v>0.63164342254052019</v>
       </c>
       <c r="H215" s="27">
         <f t="shared" si="15"/>
@@ -12380,7 +12377,7 @@
         <v>936405983</v>
       </c>
       <c r="G221" s="9">
-        <v>6.7799999999999999E-2</v>
+        <v>5.37603305785124E-2</v>
       </c>
       <c r="H221" s="27">
         <f t="shared" si="15"/>
@@ -12423,7 +12420,7 @@
         <v>1312940380</v>
       </c>
       <c r="G222" s="9">
-        <v>0.35680000000000001</v>
+        <v>0.3603592303639967</v>
       </c>
       <c r="H222" s="27">
         <f t="shared" si="15"/>
@@ -12509,7 +12506,7 @@
         <v>546180105</v>
       </c>
       <c r="G224" s="9">
-        <v>0.38469999999999999</v>
+        <v>0.35804655870445345</v>
       </c>
       <c r="H224" s="27">
         <f t="shared" si="15"/>
@@ -12552,7 +12549,7 @@
         <v>343395644</v>
       </c>
       <c r="G225" s="9">
-        <v>0.55389999999999995</v>
+        <v>0.53351850862667594</v>
       </c>
       <c r="H225" s="27">
         <f t="shared" si="15"/>
@@ -12595,7 +12592,7 @@
         <v>396358014</v>
       </c>
       <c r="G226" s="9">
-        <v>0.6391</v>
+        <v>0.63518273888154997</v>
       </c>
       <c r="H226" s="27">
         <f t="shared" si="15"/>
@@ -12638,7 +12635,7 @@
         <v>40658464</v>
       </c>
       <c r="G227" s="9">
-        <v>0.41589999999999999</v>
+        <v>0.41952707856598015</v>
       </c>
       <c r="H227" s="27">
         <f t="shared" si="15"/>
@@ -12681,7 +12678,7 @@
         <v>76728276</v>
       </c>
       <c r="G228" s="9">
-        <v>0.73340000000000005</v>
+        <v>0.71015625000000004</v>
       </c>
       <c r="H228" s="27">
         <f t="shared" si="15"/>
@@ -12810,7 +12807,7 @@
         <v>3836141821</v>
       </c>
       <c r="G231" s="9">
-        <v>0.18859999999999999</v>
+        <v>0.18863610380701956</v>
       </c>
       <c r="H231" s="27">
         <f t="shared" si="15"/>
@@ -12939,7 +12936,7 @@
         <v>2776378150</v>
       </c>
       <c r="G234" s="9">
-        <v>9.8199999999999996E-2</v>
+        <v>9.7531847133757968E-2</v>
       </c>
       <c r="H234" s="27">
         <f t="shared" si="15"/>
@@ -13154,7 +13151,7 @@
         <v>361899570</v>
       </c>
       <c r="G239" s="9">
-        <v>0.54620000000000002</v>
+        <v>0.53640810621942703</v>
       </c>
       <c r="H239" s="27">
         <f t="shared" si="15"/>
@@ -13283,7 +13280,7 @@
         <v>110001939</v>
       </c>
       <c r="G242" s="9">
-        <v>0.2349</v>
+        <v>0.23069699499165275</v>
       </c>
       <c r="H242" s="27">
         <f t="shared" si="15"/>
@@ -13412,7 +13409,7 @@
         <v>867079916</v>
       </c>
       <c r="G245" s="9">
-        <v>0.26319999999999999</v>
+        <v>0.26090911387927329</v>
       </c>
       <c r="H245" s="27">
         <f t="shared" si="15"/>
@@ -13498,7 +13495,7 @@
         <v>152017168</v>
       </c>
       <c r="G247" s="9">
-        <v>1</v>
+        <v>0.99847683899292183</v>
       </c>
       <c r="H247" s="27">
         <f t="shared" si="15"/>
@@ -13670,7 +13667,7 @@
         <v>1514800242</v>
       </c>
       <c r="G251" s="9">
-        <v>9.0800000000000006E-2</v>
+        <v>9.1672473245073341E-2</v>
       </c>
       <c r="H251" s="27">
         <f t="shared" si="15"/>
@@ -13842,7 +13839,7 @@
         <v>126646556</v>
       </c>
       <c r="G255" s="9">
-        <v>0.4677</v>
+        <v>0.4489853044086774</v>
       </c>
       <c r="H255" s="27">
         <f t="shared" si="15"/>
@@ -13928,7 +13925,7 @@
         <v>655522290</v>
       </c>
       <c r="G257" s="9">
-        <v>0.23380000000000001</v>
+        <v>0.23321205587746485</v>
       </c>
       <c r="H257" s="27">
         <f t="shared" si="15"/>
@@ -14143,7 +14140,7 @@
         <v>395190198</v>
       </c>
       <c r="G262" s="9">
-        <v>0.17829999999999999</v>
+        <v>0.17963646691280885</v>
       </c>
       <c r="H262" s="27">
         <f t="shared" si="20"/>
@@ -14186,7 +14183,7 @@
         <v>1300583819</v>
       </c>
       <c r="G263" s="9">
-        <v>0.85199999999999998</v>
+        <v>0.84672137571231854</v>
       </c>
       <c r="H263" s="27">
         <f t="shared" si="20"/>
@@ -14272,7 +14269,7 @@
         <v>722375797</v>
       </c>
       <c r="G265" s="9">
-        <v>0.26979999999999998</v>
+        <v>0.25650035137034433</v>
       </c>
       <c r="H265" s="27">
         <f t="shared" si="20"/>
@@ -14358,7 +14355,7 @@
         <v>531380652</v>
       </c>
       <c r="G267" s="9">
-        <v>0.13900000000000001</v>
+        <v>0.13793511721524981</v>
       </c>
       <c r="H267" s="27">
         <f t="shared" si="20"/>
@@ -14530,7 +14527,7 @@
         <v>1115105481</v>
       </c>
       <c r="G271" s="9">
-        <v>0.57689999999999997</v>
+        <v>0.57822520888162099</v>
       </c>
       <c r="H271" s="27">
         <f t="shared" si="20"/>
@@ -14831,7 +14828,7 @@
         <v>131117987</v>
       </c>
       <c r="G278" s="9">
-        <v>0.43730000000000002</v>
+        <v>0.44310216256524981</v>
       </c>
       <c r="H278" s="27">
         <f t="shared" si="20"/>
@@ -14917,7 +14914,7 @@
         <v>591661527</v>
       </c>
       <c r="G280" s="9">
-        <v>5.4600000000000003E-2</v>
+        <v>5.6308878104481874E-2</v>
       </c>
       <c r="H280" s="27">
         <f t="shared" si="20"/>
@@ -15003,7 +15000,7 @@
         <v>522110432</v>
       </c>
       <c r="G282" s="9">
-        <v>0.19020000000000001</v>
+        <v>0.18306671868903629</v>
       </c>
       <c r="H282" s="27">
         <f t="shared" si="20"/>
@@ -15132,7 +15129,7 @@
         <v>322422932</v>
       </c>
       <c r="G285" s="9">
-        <v>0.47749999999999998</v>
+        <v>0.46278645305211924</v>
       </c>
       <c r="H285" s="27">
         <f t="shared" si="20"/>
@@ -15225,7 +15222,7 @@
         <v>61759.4339634633</v>
       </c>
       <c r="D2" s="15">
-        <v>0.80584900000000004</v>
+        <v>0.80810397553516822</v>
       </c>
       <c r="E2">
         <v>3074752230</v>
@@ -15297,7 +15294,7 @@
         <v>31663.291215216399</v>
       </c>
       <c r="D4" s="15">
-        <v>0.99635399999999996</v>
+        <v>0.9967602591792657</v>
       </c>
       <c r="E4">
         <v>1114516085</v>
@@ -15333,7 +15330,7 @@
         <v>70223.160426255403</v>
       </c>
       <c r="D5" s="15">
-        <v>0.68727899999999997</v>
+        <v>0.68655409022336855</v>
       </c>
       <c r="E5">
         <v>2369193464</v>
@@ -15369,7 +15366,7 @@
         <v>34396.469460680797</v>
       </c>
       <c r="D6" s="15">
-        <v>0.96716999999999997</v>
+        <v>0.96742279067694636</v>
       </c>
       <c r="E6">
         <v>1665809795</v>
@@ -15405,7 +15402,7 @@
         <v>33515.234196450197</v>
       </c>
       <c r="D7" s="15">
-        <v>0.92270200000000002</v>
+        <v>0.92424163965326178</v>
       </c>
       <c r="E7">
         <v>4184073209</v>
@@ -15441,7 +15438,7 @@
         <v>44587.583848328497</v>
       </c>
       <c r="D8" s="15">
-        <v>0.35361599999999999</v>
+        <v>0.34383590611122861</v>
       </c>
       <c r="E8">
         <v>560331876</v>
@@ -15477,7 +15474,7 @@
         <v>66129.587160920099</v>
       </c>
       <c r="D9" s="15">
-        <v>0.70098700000000003</v>
+        <v>0.70753233858289433</v>
       </c>
       <c r="E9">
         <v>3203486966</v>
@@ -15513,7 +15510,7 @@
         <v>51688.812548218899</v>
       </c>
       <c r="D10" s="15">
-        <v>0.94839300000000004</v>
+        <v>0.94340468021916124</v>
       </c>
       <c r="E10">
         <v>3801400914</v>
@@ -15549,7 +15546,7 @@
         <v>98635.727620330203</v>
       </c>
       <c r="D11" s="15">
-        <v>1.812E-3</v>
+        <v>5.192989464223299E-3</v>
       </c>
       <c r="E11">
         <v>2218940535</v>
@@ -15585,7 +15582,7 @@
         <v>54915.257564742198</v>
       </c>
       <c r="D12" s="15">
-        <v>0.79158700000000004</v>
+        <v>0.78081419500326388</v>
       </c>
       <c r="E12">
         <v>2925010709</v>
@@ -15693,7 +15690,7 @@
         <v>49477.777786994797</v>
       </c>
       <c r="D15" s="15">
-        <v>0.32020399999999999</v>
+        <v>0.31242359413202936</v>
       </c>
       <c r="E15">
         <v>758982916</v>
@@ -15729,7 +15726,7 @@
         <v>34241.256322889298</v>
       </c>
       <c r="D16" s="15">
-        <v>0.68439499999999998</v>
+        <v>0.69205298013245031</v>
       </c>
       <c r="E16">
         <v>1528169814</v>
@@ -15801,7 +15798,7 @@
         <v>60879.545446649703</v>
       </c>
       <c r="D18" s="15">
-        <v>0.29838300000000001</v>
+        <v>0.29334368487721163</v>
       </c>
       <c r="E18">
         <v>1642346506</v>
@@ -15837,7 +15834,7 @@
         <v>31855.536337622001</v>
       </c>
       <c r="D19" s="15">
-        <v>0.62422699999999998</v>
+        <v>0.58316494997782264</v>
       </c>
       <c r="E19">
         <v>1098142533</v>
@@ -15873,7 +15870,7 @@
         <v>72271.762206900297</v>
       </c>
       <c r="D20" s="15">
-        <v>0.41344599999999998</v>
+        <v>0.41284446195564001</v>
       </c>
       <c r="E20">
         <v>3618848543</v>
@@ -15981,7 +15978,7 @@
         <v>55767.892646789398</v>
       </c>
       <c r="D23" s="15">
-        <v>0.16884299999999999</v>
+        <v>0.155925820662214</v>
       </c>
       <c r="E23">
         <v>5392909908</v>
@@ -16197,7 +16194,7 @@
         <v>74962.343089686503</v>
       </c>
       <c r="D29" s="15">
-        <v>0.45426699999999998</v>
+        <v>0.44061627021078476</v>
       </c>
       <c r="E29">
         <v>2820115348</v>
@@ -16233,7 +16230,7 @@
         <v>33503.424668510801</v>
       </c>
       <c r="D30" s="15">
-        <v>0.89813600000000005</v>
+        <v>0.9041847980804425</v>
       </c>
       <c r="E30">
         <v>1238226238</v>
@@ -16269,7 +16266,7 @@
         <v>29646.892659506899</v>
       </c>
       <c r="D31" s="15">
-        <v>0.97275699999999998</v>
+        <v>0.96847891709828093</v>
       </c>
       <c r="E31">
         <v>1334281723</v>
@@ -16413,7 +16410,7 @@
         <v>55376.676989363899</v>
       </c>
       <c r="D35" s="15">
-        <v>0.277254</v>
+        <v>0.24035850081477458</v>
       </c>
       <c r="E35">
         <v>2586665620</v>
@@ -16449,7 +16446,7 @@
         <v>66877.622382902104</v>
       </c>
       <c r="D36" s="15">
-        <v>0.60625300000000004</v>
+        <v>0.60032730073161344</v>
       </c>
       <c r="E36">
         <v>4794964392</v>
@@ -16485,7 +16482,7 @@
         <v>76694.228272870096</v>
       </c>
       <c r="D37" s="15">
-        <v>0.37053599999999998</v>
+        <v>0.37648764113518463</v>
       </c>
       <c r="E37">
         <v>2558287960</v>
@@ -16521,7 +16518,7 @@
         <v>49114.238400441798</v>
       </c>
       <c r="D38" s="15">
-        <v>0.73104400000000003</v>
+        <v>0.72729650554509306</v>
       </c>
       <c r="E38">
         <v>1467645796</v>
@@ -16557,7 +16554,7 @@
         <v>92778.746912689196</v>
       </c>
       <c r="D39" s="15">
-        <v>1.3212E-2</v>
+        <v>1.3333333333333334E-2</v>
       </c>
       <c r="E39">
         <v>17020108368</v>
@@ -16629,7 +16626,7 @@
         <v>81149.274779522704</v>
       </c>
       <c r="D41" s="15">
-        <v>0.259739</v>
+        <v>0.25798883785252136</v>
       </c>
       <c r="E41">
         <v>4664155763</v>
@@ -16665,7 +16662,7 @@
         <v>82907.706095407702</v>
       </c>
       <c r="D42" s="15">
-        <v>0.62529599999999996</v>
+        <v>0.59259052536105494</v>
       </c>
       <c r="E42">
         <v>8491098449</v>
@@ -16701,7 +16698,7 @@
         <v>52104.492186009396</v>
       </c>
       <c r="D43" s="15">
-        <v>0.96367800000000003</v>
+        <v>0.95294954223578565</v>
       </c>
       <c r="E43">
         <v>2348097084</v>
@@ -16809,7 +16806,7 @@
         <v>63501.1943957517</v>
       </c>
       <c r="D46" s="15">
-        <v>0.32190200000000002</v>
+        <v>0.31365052393089776</v>
       </c>
       <c r="E46">
         <v>1562522182</v>
@@ -16845,7 +16842,7 @@
         <v>102256.22405087099</v>
       </c>
       <c r="D47" s="15">
-        <v>0.82890600000000003</v>
+        <v>0.82639038007300836</v>
       </c>
       <c r="E47">
         <v>1694398438</v>
@@ -16881,7 +16878,7 @@
         <v>106025.896406231</v>
       </c>
       <c r="D48" s="15">
-        <v>7.0521E-2</v>
+        <v>6.7775239142594396E-2</v>
       </c>
       <c r="E48">
         <v>41340193588</v>
@@ -16953,7 +16950,7 @@
         <v>91125.467498402999</v>
       </c>
       <c r="D50" s="15">
-        <v>0.44980900000000001</v>
+        <v>0.44102178812922616</v>
       </c>
       <c r="E50">
         <v>15217346858</v>
@@ -17097,7 +17094,7 @@
         <v>56287.128733088299</v>
       </c>
       <c r="D54" s="15">
-        <v>0.62323300000000004</v>
+        <v>0.63061677772082692</v>
       </c>
       <c r="E54">
         <v>1617997584</v>
@@ -17133,7 +17130,7 @@
         <v>83984.784887052097</v>
       </c>
       <c r="D55" s="15">
-        <v>0.37513800000000003</v>
+        <v>0.3766284625225178</v>
       </c>
       <c r="E55">
         <v>4482429240</v>
@@ -17169,7 +17166,7 @@
         <v>53508.92207819</v>
       </c>
       <c r="D56" s="15">
-        <v>0.48297400000000001</v>
+        <v>0.47652407214189896</v>
       </c>
       <c r="E56">
         <v>2007253376</v>
@@ -17241,7 +17238,7 @@
         <v>70559.019784666103</v>
       </c>
       <c r="D58" s="15">
-        <v>0.47638200000000003</v>
+        <v>0.48509996826404317</v>
       </c>
       <c r="E58">
         <v>4938927987</v>
@@ -17277,7 +17274,7 @@
         <v>43539.062500526998</v>
       </c>
       <c r="D59" s="15">
-        <v>0.50225799999999998</v>
+        <v>0.48020527859237538</v>
       </c>
       <c r="E59">
         <v>474600206</v>
@@ -17349,7 +17346,7 @@
         <v>43177.215191199597</v>
       </c>
       <c r="D61" s="15">
-        <v>0.66960799999999998</v>
+        <v>0.65371755231178541</v>
       </c>
       <c r="E61">
         <v>3078363644</v>
@@ -17385,7 +17382,7 @@
         <v>40785.818708368301</v>
       </c>
       <c r="D62" s="15">
-        <v>0.95604299999999998</v>
+        <v>0.94860366859027201</v>
       </c>
       <c r="E62">
         <v>1470290440</v>
@@ -17457,7 +17454,7 @@
         <v>36314.741027126998</v>
       </c>
       <c r="D64" s="15">
-        <v>0.784076</v>
+        <v>0.78007798652959948</v>
       </c>
       <c r="E64">
         <v>738008372</v>
@@ -17601,7 +17598,7 @@
         <v>55108.958837206002</v>
       </c>
       <c r="D68" s="15">
-        <v>0.24413699999999999</v>
+        <v>0.25196740232940434</v>
       </c>
       <c r="E68">
         <v>5316692624</v>
@@ -17637,7 +17634,7 @@
         <v>51799.999988895099</v>
       </c>
       <c r="D69" s="15">
-        <v>0.99457099999999998</v>
+        <v>1</v>
       </c>
       <c r="E69">
         <v>1205246686</v>
@@ -17853,7 +17850,7 @@
         <v>42270.7837374015</v>
       </c>
       <c r="D75" s="15">
-        <v>0.99952799999999997</v>
+        <v>1</v>
       </c>
       <c r="E75">
         <v>944454244</v>
@@ -17889,7 +17886,7 @@
         <v>53877.159295318401</v>
       </c>
       <c r="D76" s="15">
-        <v>0.76276699999999997</v>
+        <v>0.76612380384326129</v>
       </c>
       <c r="E76">
         <v>4611399282</v>
@@ -17925,7 +17922,7 @@
         <v>104638.928736916</v>
       </c>
       <c r="D77" s="15">
-        <v>0.28186299999999997</v>
+        <v>0.26175368245975783</v>
       </c>
       <c r="E77">
         <v>13702979328</v>

</xml_diff>

<commit_message>
added update to muni retail sales and EAV
</commit_message>
<xml_diff>
--- a/input/community_cohort_inputs.xlsx
+++ b/input/community_cohort_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cmapil-my.sharepoint.com/personal/amcadams_cmap_illinois_gov/Documents/Documents/GitHub/community-cohort-tool/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amcadams\Documents\R\cohort_sprint23\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{C36DDCD9-BD5F-4C42-986E-5A8F34BED458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EC267EA-9F5B-418B-B696-7DF9E2ED8F9D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0601AD-1F7D-4417-885C-11F87AAE5F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="60" windowWidth="21696" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="336" yWindow="612" windowWidth="17280" windowHeight="10908" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FACTORS_MUNI" sheetId="1" r:id="rId1"/>
@@ -134,7 +134,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>2020 total retail sales from IL Dept. of Revenue</t>
+          <t>2021 total retail sales from IL Dept. of Revenue</t>
         </r>
       </text>
     </comment>
@@ -157,7 +157,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>2019 total equalized assessed value from IL Dept. of Revenue</t>
+          <t>2021 total equalized assessed value from IL Dept. of Revenue</t>
         </r>
       </text>
     </comment>
@@ -2889,8 +2889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L285"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15169,7 +15169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Finalize inputs, correction to column label
</commit_message>
<xml_diff>
--- a/input/community_cohort_inputs.xlsx
+++ b/input/community_cohort_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amcadams\Documents\R\cohort_sprint23\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cmapil-my.sharepoint.com/personal/amcadams_cmap_illinois_gov/Documents/Documents/GitHub/community-cohort-tool/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0601AD-1F7D-4417-885C-11F87AAE5F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{1A0601AD-1F7D-4417-885C-11F87AAE5F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FD7D8D6-8F6E-43A6-AD74-14CDF9D7F17A}"/>
   <bookViews>
-    <workbookView xWindow="336" yWindow="612" windowWidth="17280" windowHeight="10908" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14265" yWindow="1860" windowWidth="18240" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FACTORS_MUNI" sheetId="1" r:id="rId1"/>
@@ -2587,21 +2587,21 @@
   <dxfs count="2">
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF800000"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2889,8 +2889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L285"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3012,11 +3012,11 @@
         <v>4.4444444444444446E-2</v>
       </c>
       <c r="H3" s="26">
-        <f t="shared" ref="H3:H65" si="4">E3+F3</f>
+        <f>E3+F3</f>
         <v>1687821595</v>
       </c>
       <c r="I3" s="4">
-        <f t="shared" si="0"/>
+        <f>H3/C3</f>
         <v>56507.469115136097</v>
       </c>
       <c r="J3" s="8">
@@ -3055,7 +3055,7 @@
         <v>2.2556785395792898E-2</v>
       </c>
       <c r="H4" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="H3:H65" si="4">E4+F4</f>
         <v>948787195</v>
       </c>
       <c r="I4" s="4">
@@ -15169,7 +15169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -18055,6 +18055,9 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="colorScale" priority="4">
       <colorScale>
@@ -18066,9 +18069,6 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated CCA Estimated Total Market Value (CCAO 2021)
</commit_message>
<xml_diff>
--- a/input/community_cohort_inputs.xlsx
+++ b/input/community_cohort_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cmapil-my.sharepoint.com/personal/amcadams_cmap_illinois_gov/Documents/Documents/GitHub/community-cohort-tool/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="117" documentId="13_ncr:1_{1A0601AD-1F7D-4417-885C-11F87AAE5F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62E1DADA-A6B3-4083-8808-C38712C00A06}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="13_ncr:1_{1A0601AD-1F7D-4417-885C-11F87AAE5F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC4E1846-3992-4756-A33F-26A77A312DEF}"/>
   <bookViews>
-    <workbookView xWindow="-13815" yWindow="-15930" windowWidth="22755" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14580" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FACTORS_MUNI" sheetId="1" r:id="rId1"/>
@@ -400,7 +400,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> Total market value, calculated from 2019 county assessor data. For each Chicago PIN, total market value is calculated by multiplying total assessed value by a factor, depending on the parcel's class. Factors are as follows: 10x for classes 100-399 &amp; 600-999; 5x for classes 400-499; and 4x for classes 500-599.
+          <t xml:space="preserve"> Total market value, calculated from 2021 county assessor data. For each Chicago PIN, total market value is calculated by multiplying total assessed value by a factor, depending on the parcel's class. Factors are as follows: 10x for classes 100-399 &amp; 600-999; 5x for classes 400-499; and 4x for classes 500-599.
 </t>
         </r>
         <r>
@@ -422,7 +422,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> Chicago is reassessed on a triennial basis, with the most recent assessment being done in 2018. This variable can next be updated with the 2021 assessor data.</t>
+          <t xml:space="preserve"> Chicago is reassessed on a triennial basis, with the most recent assessment being done in 2021. This variable can next be updated with the 2023 assessor data.</t>
         </r>
       </text>
     </comment>
@@ -1901,12 +1901,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2123,14 +2124,6 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -2524,7 +2517,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2548,11 +2541,12 @@
     <xf numFmtId="164" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="30" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
     <xf numFmtId="2" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="21" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2904,7 +2898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G292" sqref="G292"/>
     </sheetView>
   </sheetViews>
@@ -7532,7 +7526,7 @@
       <c r="D108">
         <v>107428</v>
       </c>
-      <c r="E108" s="27">
+      <c r="E108" s="26">
         <v>941487155.99999905</v>
       </c>
       <c r="F108">
@@ -9983,7 +9977,7 @@
       <c r="D165">
         <v>122235</v>
       </c>
-      <c r="E165" s="27">
+      <c r="E165" s="26">
         <v>989145749.99999905</v>
       </c>
       <c r="F165">
@@ -10370,7 +10364,7 @@
       <c r="D174">
         <v>75783</v>
       </c>
-      <c r="E174" s="27">
+      <c r="E174" s="26">
         <v>1854879443.99999</v>
       </c>
       <c r="F174">
@@ -14799,7 +14793,7 @@
       <c r="D277">
         <v>250001</v>
       </c>
-      <c r="E277" s="27" t="s">
+      <c r="E277" s="26" t="s">
         <v>380</v>
       </c>
       <c r="F277">
@@ -15184,8 +15178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15209,16 +15203,16 @@
       <c r="B1" s="14" t="s">
         <v>376</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="28" t="s">
         <v>379</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="25" t="s">
         <v>378</v>
       </c>
       <c r="G1" s="6" t="s">
@@ -15241,32 +15235,32 @@
       <c r="B2" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="23">
         <v>78537.735849056597</v>
       </c>
       <c r="D2" s="15">
         <v>0.80810397553516822</v>
       </c>
       <c r="E2">
-        <v>3074752230</v>
+        <v>3548280190.2389002</v>
       </c>
       <c r="F2" s="16">
         <v>47663</v>
       </c>
       <c r="G2" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E2/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F2)</f>
-        <v>35479.885595453045</v>
+        <v>29781.962918929472</v>
       </c>
       <c r="H2" s="8">
-        <f t="shared" ref="H2:H33" si="0">LN(G2)</f>
-        <v>10.476721211938415</v>
+        <f>LN(G2)</f>
+        <v>10.301658218066086</v>
       </c>
       <c r="I2" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J2" s="8">
-        <f t="shared" ref="J2:J33" si="1">LN(C2)</f>
+        <f>LN(C2)</f>
         <v>11.271334499718714</v>
       </c>
     </row>
@@ -15277,32 +15271,32 @@
       <c r="B3" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="23">
         <v>57500</v>
       </c>
       <c r="D3" s="15">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>895906079</v>
+        <v>994396260.73109198</v>
       </c>
       <c r="F3" s="16">
         <v>13867</v>
       </c>
       <c r="G3" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E3/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F3)</f>
-        <v>35512.876167382732</v>
+        <v>29183.470760991047</v>
       </c>
       <c r="H3" s="8">
-        <f t="shared" si="0"/>
-        <v>10.47765061864088</v>
+        <f>LN(G3)</f>
+        <v>10.281357758149285</v>
       </c>
       <c r="I3" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J3" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C3)</f>
         <v>10.959540226785442</v>
       </c>
     </row>
@@ -15313,32 +15307,32 @@
       <c r="B4" s="13" t="s">
         <v>301</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="23">
         <v>45246.299021729697</v>
       </c>
       <c r="D4" s="15">
         <v>0.9967602591792657</v>
       </c>
       <c r="E4">
-        <v>1114516085</v>
+        <v>1398865114</v>
       </c>
       <c r="F4" s="16">
         <v>13228</v>
       </c>
       <c r="G4" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E4/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F4)</f>
-        <v>42208.576641870066</v>
+        <v>36630.808537357385</v>
       </c>
       <c r="H4" s="8">
-        <f t="shared" si="0"/>
-        <v>10.650378717333073</v>
+        <f>LN(G4)</f>
+        <v>10.508644928621182</v>
       </c>
       <c r="I4" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J4" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C4)</f>
         <v>10.719876156208088</v>
       </c>
     </row>
@@ -15349,32 +15343,32 @@
       <c r="B5" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="23">
         <v>78059.954751131198</v>
       </c>
       <c r="D5" s="15">
         <v>0.68655409022336855</v>
       </c>
       <c r="E5">
-        <v>2369193464</v>
+        <v>2591607528.0592399</v>
       </c>
       <c r="F5" s="16">
         <v>42745</v>
       </c>
       <c r="G5" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E5/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F5)</f>
-        <v>32384.083558677303</v>
+        <v>26759.409089345005</v>
       </c>
       <c r="H5" s="8">
-        <f t="shared" si="0"/>
-        <v>10.385422332889526</v>
+        <f>LN(G5)</f>
+        <v>10.194641432135315</v>
       </c>
       <c r="I5" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J5" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C5)</f>
         <v>11.265232461066633</v>
       </c>
     </row>
@@ -15385,32 +15379,32 @@
       <c r="B6" s="13" t="s">
         <v>303</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="23">
         <v>41000</v>
       </c>
       <c r="D6" s="15">
         <v>0.96742279067694636</v>
       </c>
       <c r="E6">
-        <v>1665809795</v>
+        <v>1852067815</v>
       </c>
       <c r="F6" s="16">
         <v>46468</v>
       </c>
       <c r="G6" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E6/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F6)</f>
-        <v>25712.095929230931</v>
+        <v>22214.831291047369</v>
       </c>
       <c r="H6" s="8">
-        <f t="shared" si="0"/>
-        <v>10.154716818883173</v>
+        <f>LN(G6)</f>
+        <v>10.008515420970133</v>
       </c>
       <c r="I6" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J6" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C6)</f>
         <v>10.621327345686446</v>
       </c>
     </row>
@@ -15421,32 +15415,32 @@
       <c r="B7" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="23">
         <v>40085.768742058397</v>
       </c>
       <c r="D7" s="15">
         <v>0.92424163965326178</v>
       </c>
       <c r="E7">
-        <v>4184073209</v>
+        <v>4743250985.9707403</v>
       </c>
       <c r="F7" s="16">
         <v>100120</v>
       </c>
       <c r="G7" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E7/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F7)</f>
-        <v>27737.119877175453</v>
+        <v>23859.775398112979</v>
       </c>
       <c r="H7" s="8">
-        <f t="shared" si="0"/>
-        <v>10.230526862854036</v>
+        <f>LN(G7)</f>
+        <v>10.079949282284591</v>
       </c>
       <c r="I7" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J7" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C7)</f>
         <v>10.598776656091799</v>
       </c>
     </row>
@@ -15457,32 +15451,32 @@
       <c r="B8" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="23">
         <v>54138.727163220203</v>
       </c>
       <c r="D8" s="15">
         <v>0.34383590611122861</v>
       </c>
       <c r="E8">
-        <v>560331876</v>
+        <v>554922436</v>
       </c>
       <c r="F8" s="16">
         <v>9606</v>
       </c>
       <c r="G8" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E8/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F8)</f>
-        <v>33374.174724357901</v>
+        <v>26133.449873254835</v>
       </c>
       <c r="H8" s="8">
-        <f t="shared" si="0"/>
-        <v>10.415537668036762</v>
+        <f>LN(G8)</f>
+        <v>10.170971377096217</v>
       </c>
       <c r="I8" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J8" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C8)</f>
         <v>10.899305052792558</v>
       </c>
     </row>
@@ -15493,32 +15487,32 @@
       <c r="B9" s="13" t="s">
         <v>306</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="23">
         <v>91543.404461687605</v>
       </c>
       <c r="D9" s="15">
         <v>0.70753233858289433</v>
       </c>
       <c r="E9">
-        <v>3203486966</v>
+        <v>3863916690.1880798</v>
       </c>
       <c r="F9" s="16">
         <v>36374</v>
       </c>
       <c r="G9" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E9/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F9)</f>
-        <v>43509.215177410093</v>
+        <v>36735.192125354428</v>
       </c>
       <c r="H9" s="8">
-        <f t="shared" si="0"/>
-        <v>10.680728037800035</v>
+        <f>LN(G9)</f>
+        <v>10.511490488076211</v>
       </c>
       <c r="I9" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J9" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C9)</f>
         <v>11.424568504489276</v>
       </c>
     </row>
@@ -15529,32 +15523,32 @@
       <c r="B10" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="23">
         <v>62476.238119059497</v>
       </c>
       <c r="D10" s="15">
         <v>0.94340468021916124</v>
       </c>
       <c r="E10">
-        <v>3801400914</v>
+        <v>3965235780.5862598</v>
       </c>
       <c r="F10" s="16">
         <v>73991</v>
       </c>
       <c r="G10" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E10/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F10)</f>
-        <v>31003.969523183128</v>
+        <v>25219.502230169608</v>
       </c>
       <c r="H10" s="8">
-        <f t="shared" si="0"/>
-        <v>10.341870524404632</v>
+        <f>LN(G10)</f>
+        <v>10.135372872217454</v>
       </c>
       <c r="I10" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J10" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C10)</f>
         <v>11.042541573338868</v>
       </c>
     </row>
@@ -15565,32 +15559,32 @@
       <c r="B11" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="23">
         <v>131169.757489301</v>
       </c>
       <c r="D11" s="15">
         <v>5.192989464223299E-3</v>
       </c>
       <c r="E11">
-        <v>2218940535</v>
+        <v>2206100566</v>
       </c>
       <c r="F11" s="16">
         <v>19781</v>
       </c>
       <c r="G11" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E11/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F11)</f>
-        <v>51723.943708196741</v>
+        <v>37894.449282783746</v>
       </c>
       <c r="H11" s="8">
-        <f t="shared" si="0"/>
-        <v>10.853676081104052</v>
+        <f>LN(G11)</f>
+        <v>10.542559923426021</v>
       </c>
       <c r="I11" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J11" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C11)</f>
         <v>11.784247621980015</v>
       </c>
     </row>
@@ -15601,32 +15595,32 @@
       <c r="B12" s="13" t="s">
         <v>309</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="23">
         <v>72159.103528127205</v>
       </c>
       <c r="D12" s="15">
         <v>0.78081419500326388</v>
       </c>
       <c r="E12">
-        <v>2925010709</v>
+        <v>3425149601.8145499</v>
       </c>
       <c r="F12" s="16">
         <v>33186</v>
       </c>
       <c r="G12" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E12/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F12)</f>
-        <v>43532.766966510564</v>
+        <v>36075.195438752475</v>
       </c>
       <c r="H12" s="8">
-        <f t="shared" si="0"/>
-        <v>10.681269197114084</v>
+        <f>LN(G12)</f>
+        <v>10.493360801195033</v>
       </c>
       <c r="I12" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J12" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C12)</f>
         <v>11.186628731268636</v>
       </c>
     </row>
@@ -15637,32 +15631,32 @@
       <c r="B13" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="23">
         <v>52144.588045234203</v>
       </c>
       <c r="D13" s="15">
         <v>1</v>
       </c>
       <c r="E13">
-        <v>1633121018</v>
+        <v>1780426102.36166</v>
       </c>
       <c r="F13" s="16">
         <v>42243</v>
       </c>
       <c r="G13" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E13/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F13)</f>
-        <v>26670.284110813485</v>
+        <v>22715.91864694142</v>
       </c>
       <c r="H13" s="8">
-        <f t="shared" si="0"/>
-        <v>10.191305269943221</v>
+        <f>LN(G13)</f>
+        <v>10.030821219680002</v>
       </c>
       <c r="I13" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J13" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C13)</f>
         <v>10.861775678346413</v>
       </c>
     </row>
@@ -15673,32 +15667,32 @@
       <c r="B14" s="13" t="s">
         <v>311</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="23">
         <v>46710.526315789401</v>
       </c>
       <c r="D14" s="15">
         <v>1</v>
       </c>
       <c r="E14">
-        <v>161181904</v>
+        <v>154979128</v>
       </c>
       <c r="F14" s="16">
         <v>2246</v>
       </c>
       <c r="G14" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E14/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F14)</f>
-        <v>37951.924926460051</v>
+        <v>28591.184047535768</v>
       </c>
       <c r="H14" s="8">
-        <f t="shared" si="0"/>
-        <v>10.544075504237293</v>
+        <f>LN(G14)</f>
+        <v>10.26085369920296</v>
       </c>
       <c r="I14" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J14" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C14)</f>
         <v>10.751724821165267</v>
       </c>
     </row>
@@ -15709,32 +15703,32 @@
       <c r="B15" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="23">
         <v>68435.550935550898</v>
       </c>
       <c r="D15" s="15">
         <v>0.31242359413202936</v>
       </c>
       <c r="E15">
-        <v>758982916</v>
+        <v>801655546</v>
       </c>
       <c r="F15" s="16">
         <v>12087</v>
       </c>
       <c r="G15" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E15/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F15)</f>
-        <v>34894.763550041658</v>
+        <v>28005.18938199283</v>
       </c>
       <c r="H15" s="8">
-        <f t="shared" si="0"/>
-        <v>10.460092055387076</v>
+        <f>LN(G15)</f>
+        <v>10.24014510705609</v>
       </c>
       <c r="I15" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J15" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C15)</f>
         <v>11.133647719106873</v>
       </c>
     </row>
@@ -15745,32 +15739,32 @@
       <c r="B16" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16" s="23">
         <v>39348.449964329702</v>
       </c>
       <c r="D16" s="15">
         <v>0.69205298013245031</v>
       </c>
       <c r="E16">
-        <v>1528169814</v>
+        <v>1517860263.90818</v>
       </c>
       <c r="F16" s="16">
         <v>31382</v>
       </c>
       <c r="G16" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E16/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F16)</f>
-        <v>30090.368571303748</v>
+        <v>24076.707312769591</v>
       </c>
       <c r="H16" s="8">
-        <f t="shared" si="0"/>
-        <v>10.311960418512308</v>
+        <f>LN(G16)</f>
+        <v>10.089000150570135</v>
       </c>
       <c r="I16" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J16" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C16)</f>
         <v>10.58021186207427</v>
       </c>
     </row>
@@ -15781,32 +15775,32 @@
       <c r="B17" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="C17" s="24">
+      <c r="C17" s="23">
         <v>43293.492695883098</v>
       </c>
       <c r="D17" s="15">
         <v>1</v>
       </c>
       <c r="E17">
-        <v>1620176100</v>
+        <v>1912350686</v>
       </c>
       <c r="F17" s="16">
         <v>52464</v>
       </c>
       <c r="G17" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E17/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F17)</f>
-        <v>24019.410311776341</v>
+        <v>21469.650112295898</v>
       </c>
       <c r="H17" s="8">
-        <f t="shared" si="0"/>
-        <v>10.086617545448206</v>
+        <f>LN(G17)</f>
+        <v>9.9743955941539113</v>
       </c>
       <c r="I17" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J17" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C17)</f>
         <v>10.675757618537041</v>
       </c>
     </row>
@@ -15817,32 +15811,32 @@
       <c r="B18" s="13" t="s">
         <v>315</v>
       </c>
-      <c r="C18" s="24">
+      <c r="C18" s="23">
         <v>73778.040141676494</v>
       </c>
       <c r="D18" s="15">
         <v>0.29334368487721163</v>
       </c>
       <c r="E18">
-        <v>1642346506</v>
+        <v>1740504096.6638999</v>
       </c>
       <c r="F18" s="16">
         <v>24728</v>
       </c>
       <c r="G18" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E18/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F18)</f>
-        <v>36129.516327302983</v>
+        <v>28893.901446860826</v>
       </c>
       <c r="H18" s="8">
-        <f t="shared" si="0"/>
-        <v>10.494865437041367</v>
+        <f>LN(G18)</f>
+        <v>10.27138582923215</v>
       </c>
       <c r="I18" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J18" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C18)</f>
         <v>11.208816407253209</v>
       </c>
     </row>
@@ -15853,32 +15847,32 @@
       <c r="B19" s="13" t="s">
         <v>316</v>
       </c>
-      <c r="C19" s="24">
+      <c r="C19" s="23">
         <v>43527.777777777701</v>
       </c>
       <c r="D19" s="15">
         <v>0.58316494997782264</v>
       </c>
       <c r="E19">
-        <v>1098142533</v>
+        <v>1457390874</v>
       </c>
       <c r="F19" s="16">
         <v>21355</v>
       </c>
       <c r="G19" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E19/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F19)</f>
-        <v>31019.875624668406</v>
+        <v>28425.701498510003</v>
       </c>
       <c r="H19" s="8">
-        <f t="shared" si="0"/>
-        <v>10.342383427201808</v>
+        <f>LN(G19)</f>
+        <v>10.25504899724157</v>
       </c>
       <c r="I19" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J19" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C19)</f>
         <v>10.681154582882046</v>
       </c>
     </row>
@@ -15889,32 +15883,32 @@
       <c r="B20" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="C20" s="24">
+      <c r="C20" s="23">
         <v>84541.036717062598</v>
       </c>
       <c r="D20" s="15">
         <v>0.41284446195564001</v>
       </c>
       <c r="E20">
-        <v>3618848543</v>
+        <v>4228655447.0969</v>
       </c>
       <c r="F20" s="16">
         <v>42574</v>
       </c>
       <c r="G20" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E20/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F20)</f>
-        <v>42463.171338933091</v>
+        <v>35225.061560690148</v>
       </c>
       <c r="H20" s="8">
-        <f t="shared" si="0"/>
-        <v>10.656392422504192</v>
+        <f>LN(G20)</f>
+        <v>10.469513084407374</v>
       </c>
       <c r="I20" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J20" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C20)</f>
         <v>11.34499233708158</v>
       </c>
     </row>
@@ -15925,32 +15919,32 @@
       <c r="B21" s="13" t="s">
         <v>318</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C21" s="23">
         <v>31762.4020887728</v>
       </c>
       <c r="D21" s="15">
         <v>1</v>
       </c>
       <c r="E21">
-        <v>821709626</v>
+        <v>934575156.70661795</v>
       </c>
       <c r="F21" s="16">
         <v>19901</v>
       </c>
       <c r="G21" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E21/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F21)</f>
-        <v>27566.477596877055</v>
+        <v>23769.104741285177</v>
       </c>
       <c r="H21" s="8">
-        <f t="shared" si="0"/>
-        <v>10.224355733682078</v>
+        <f>LN(G21)</f>
+        <v>10.076141896257711</v>
       </c>
       <c r="I21" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J21" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C21)</f>
         <v>10.366038545019112</v>
       </c>
     </row>
@@ -15961,32 +15955,32 @@
       <c r="B22" s="13" t="s">
         <v>319</v>
       </c>
-      <c r="C22" s="24">
+      <c r="C22" s="23">
         <v>61897.597539120899</v>
       </c>
       <c r="D22" s="15">
         <v>1</v>
       </c>
       <c r="E22">
-        <v>743673578</v>
+        <v>717220175.04682505</v>
       </c>
       <c r="F22" s="16">
         <v>23870</v>
       </c>
       <c r="G22" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E22/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F22)</f>
-        <v>24112.612149672183</v>
+        <v>20068.64706722321</v>
       </c>
       <c r="H22" s="8">
-        <f t="shared" si="0"/>
-        <v>10.09049030830414</v>
+        <f>LN(G22)</f>
+        <v>9.9069140288167965</v>
       </c>
       <c r="I22" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J22" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C22)</f>
         <v>11.033236645950517</v>
       </c>
     </row>
@@ -15997,32 +15991,32 @@
       <c r="B23" s="13" t="s">
         <v>320</v>
       </c>
-      <c r="C23" s="24">
+      <c r="C23" s="23">
         <v>67795.667447306798</v>
       </c>
       <c r="D23" s="15">
         <v>0.155925820662214</v>
       </c>
       <c r="E23">
-        <v>5392909908</v>
+        <v>5719026262</v>
       </c>
       <c r="F23" s="16">
         <v>56099</v>
       </c>
       <c r="G23" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E23/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F23)</f>
-        <v>46256.445410382308</v>
+        <v>35798.347341622932</v>
       </c>
       <c r="H23" s="8">
-        <f t="shared" si="0"/>
-        <v>10.74195609345532</v>
+        <f>LN(G23)</f>
+        <v>10.4856570076814</v>
       </c>
       <c r="I23" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J23" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C23)</f>
         <v>11.124253569929543</v>
       </c>
     </row>
@@ -16033,32 +16027,32 @@
       <c r="B24" s="13" t="s">
         <v>321</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24" s="23">
         <v>120023.58490566</v>
       </c>
       <c r="D24" s="15">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>1597380076</v>
+        <v>1738199600</v>
       </c>
       <c r="F24" s="16">
         <v>11402</v>
       </c>
       <c r="G24" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E24/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F24)</f>
-        <v>61239.345822148985</v>
+        <v>46846.950603594269</v>
       </c>
       <c r="H24" s="8">
-        <f t="shared" si="0"/>
-        <v>11.022545167515823</v>
+        <f>LN(G24)</f>
+        <v>10.754641197044362</v>
       </c>
       <c r="I24" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J24" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C24)</f>
         <v>11.695443543333054</v>
       </c>
     </row>
@@ -16069,32 +16063,32 @@
       <c r="B25" s="13" t="s">
         <v>322</v>
       </c>
-      <c r="C25" s="24">
+      <c r="C25" s="23">
         <v>27791.811846689801</v>
       </c>
       <c r="D25" s="15">
         <v>1</v>
       </c>
       <c r="E25">
-        <v>708798902</v>
+        <v>586459514</v>
       </c>
       <c r="F25" s="16">
         <v>21378</v>
       </c>
       <c r="G25" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E25/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F25)</f>
-        <v>24794.330628674819</v>
+        <v>19496.747283112865</v>
       </c>
       <c r="H25" s="8">
-        <f t="shared" si="0"/>
-        <v>10.118370302336801</v>
+        <f>LN(G25)</f>
+        <v>9.8780029246439582</v>
       </c>
       <c r="I25" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J25" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C25)</f>
         <v>10.23249671840507</v>
       </c>
     </row>
@@ -16105,32 +16099,32 @@
       <c r="B26" s="13" t="s">
         <v>323</v>
       </c>
-      <c r="C26" s="24">
+      <c r="C26" s="23">
         <v>139045.698924731</v>
       </c>
       <c r="D26" s="15">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>3069909495</v>
+        <v>3334593535</v>
       </c>
       <c r="F26" s="16">
         <v>19855</v>
       </c>
       <c r="G26" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E26/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F26)</f>
-        <v>66187.686594569153</v>
+        <v>50238.080062177505</v>
       </c>
       <c r="H26" s="8">
-        <f t="shared" si="0"/>
-        <v>11.100249721521193</v>
+        <f>LN(G26)</f>
+        <v>10.824528585088956</v>
       </c>
       <c r="I26" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J26" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C26)</f>
         <v>11.842557927322733</v>
       </c>
     </row>
@@ -16141,32 +16135,32 @@
       <c r="B27" s="13" t="s">
         <v>324</v>
       </c>
-      <c r="C27" s="24">
+      <c r="C27" s="23">
         <v>15358.6872957909</v>
       </c>
       <c r="D27" s="15">
         <v>1</v>
       </c>
       <c r="E27">
-        <v>121410304</v>
+        <v>108407276</v>
       </c>
       <c r="F27" s="16">
         <v>2219</v>
       </c>
       <c r="G27" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E27/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F27)</f>
-        <v>32141.355002918332</v>
+        <v>24183.227088594656</v>
       </c>
       <c r="H27" s="8">
-        <f t="shared" si="0"/>
-        <v>10.377898797796671</v>
+        <f>LN(G27)</f>
+        <v>10.093414576330424</v>
       </c>
       <c r="I27" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J27" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C27)</f>
         <v>9.6394365405359217</v>
       </c>
     </row>
@@ -16177,32 +16171,32 @@
       <c r="B28" s="13" t="s">
         <v>325</v>
       </c>
-      <c r="C28" s="24">
+      <c r="C28" s="23">
         <v>50111.867704280099</v>
       </c>
       <c r="D28" s="15">
         <v>1</v>
       </c>
       <c r="E28">
-        <v>1117201156</v>
+        <v>1259700999.6398001</v>
       </c>
       <c r="F28" s="16">
         <v>34788</v>
       </c>
       <c r="G28" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E28/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F28)</f>
-        <v>24439.571293511079</v>
+        <v>21417.158705556936</v>
       </c>
       <c r="H28" s="8">
-        <f t="shared" si="0"/>
-        <v>10.103958871949649</v>
+        <f>LN(G28)</f>
+        <v>9.9719476884039793</v>
       </c>
       <c r="I28" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J28" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C28)</f>
         <v>10.822013139346193</v>
       </c>
     </row>
@@ -16213,32 +16207,32 @@
       <c r="B29" s="13" t="s">
         <v>326</v>
       </c>
-      <c r="C29" s="24">
+      <c r="C29" s="23">
         <v>90373.672230652504</v>
       </c>
       <c r="D29" s="15">
         <v>0.44061627021078476</v>
       </c>
       <c r="E29">
-        <v>2820115348</v>
+        <v>2929880472</v>
       </c>
       <c r="F29" s="16">
         <v>36401</v>
       </c>
       <c r="G29" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E29/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F29)</f>
-        <v>39897.727140216411</v>
+        <v>31104.216173608947</v>
       </c>
       <c r="H29" s="8">
-        <f t="shared" si="0"/>
-        <v>10.594074637351099</v>
+        <f>LN(G29)</f>
+        <v>10.345098657262023</v>
       </c>
       <c r="I29" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J29" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C29)</f>
         <v>11.411708267576127</v>
       </c>
     </row>
@@ -16249,32 +16243,32 @@
       <c r="B30" s="13" t="s">
         <v>327</v>
       </c>
-      <c r="C30" s="24">
+      <c r="C30" s="23">
         <v>43047.619047619002</v>
       </c>
       <c r="D30" s="15">
         <v>0.9041847980804425</v>
       </c>
       <c r="E30">
-        <v>1238226238</v>
+        <v>1473809152</v>
       </c>
       <c r="F30" s="16">
         <v>24813</v>
       </c>
       <c r="G30" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E30/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F30)</f>
-        <v>30501.564344800536</v>
+        <v>26489.692790960624</v>
       </c>
       <c r="H30" s="8">
-        <f t="shared" si="0"/>
-        <v>10.325533251273676</v>
+        <f>LN(G30)</f>
+        <v>10.184510985028638</v>
       </c>
       <c r="I30" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J30" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C30)</f>
         <v>10.670062201650889</v>
       </c>
     </row>
@@ -16285,32 +16279,32 @@
       <c r="B31" s="13" t="s">
         <v>328</v>
       </c>
-      <c r="C31" s="24">
+      <c r="C31" s="23">
         <v>39907.834101382403</v>
       </c>
       <c r="D31" s="15">
         <v>0.96847891709828093</v>
       </c>
       <c r="E31">
-        <v>1334281723</v>
+        <v>1151954740</v>
       </c>
       <c r="F31" s="16">
         <v>28991</v>
       </c>
       <c r="G31" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E31/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F31)</f>
-        <v>29179.8492839705</v>
+        <v>22188.154718559199</v>
       </c>
       <c r="H31" s="8">
-        <f t="shared" si="0"/>
-        <v>10.281233657017875</v>
+        <f>LN(G31)</f>
+        <v>10.007313854224511</v>
       </c>
       <c r="I31" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J31" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C31)</f>
         <v>10.594327926998156</v>
       </c>
     </row>
@@ -16321,32 +16315,32 @@
       <c r="B32" s="13" t="s">
         <v>329</v>
       </c>
-      <c r="C32" s="24">
+      <c r="C32" s="23">
         <v>58647.459696833597</v>
       </c>
       <c r="D32" s="15">
         <v>1</v>
       </c>
       <c r="E32">
-        <v>573792429</v>
+        <v>555427497.29508102</v>
       </c>
       <c r="F32" s="16">
         <v>9097</v>
       </c>
       <c r="G32" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E32/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F32)</f>
-        <v>34990.725574429503</v>
+        <v>26852.74541380454</v>
       </c>
       <c r="H32" s="8">
-        <f t="shared" si="0"/>
-        <v>10.462838321769468</v>
+        <f>LN(G32)</f>
+        <v>10.198123344758416</v>
       </c>
       <c r="I32" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J32" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C32)</f>
         <v>10.979299540216626</v>
       </c>
     </row>
@@ -16357,32 +16351,32 @@
       <c r="B33" s="13" t="s">
         <v>330</v>
       </c>
-      <c r="C33" s="24">
+      <c r="C33" s="23">
         <v>66072.905894519106</v>
       </c>
       <c r="D33" s="15">
         <v>1</v>
       </c>
       <c r="E33">
-        <v>1069026926</v>
+        <v>1280582613.6588299</v>
       </c>
       <c r="F33" s="16">
         <v>23157</v>
       </c>
       <c r="G33" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E33/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F33)</f>
-        <v>29227.667034084145</v>
+        <v>25593.444046410092</v>
       </c>
       <c r="H33" s="8">
-        <f t="shared" si="0"/>
-        <v>10.282871040827748</v>
+        <f>LN(G33)</f>
+        <v>10.150091505733409</v>
       </c>
       <c r="I33" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J33" s="8">
-        <f t="shared" si="1"/>
+        <f>LN(C33)</f>
         <v>11.098514046113948</v>
       </c>
     </row>
@@ -16393,32 +16387,32 @@
       <c r="B34" s="13" t="s">
         <v>331</v>
       </c>
-      <c r="C34" s="24">
+      <c r="C34" s="23">
         <v>51104.505632040004</v>
       </c>
       <c r="D34" s="15">
         <v>1</v>
       </c>
       <c r="E34">
-        <v>2411252436</v>
+        <v>3039736669.3952899</v>
       </c>
       <c r="F34" s="16">
         <v>55416</v>
       </c>
       <c r="G34" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E34/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F34)</f>
-        <v>28323.718616743325</v>
+        <v>25495.656998544615</v>
       </c>
       <c r="H34" s="8">
-        <f t="shared" ref="H34:H65" si="2">LN(G34)</f>
-        <v>10.25145484627603</v>
+        <f>LN(G34)</f>
+        <v>10.146263402858914</v>
       </c>
       <c r="I34" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J34" s="8">
-        <f t="shared" ref="J34:J65" si="3">LN(C34)</f>
+        <f>LN(C34)</f>
         <v>10.841627945143156</v>
       </c>
     </row>
@@ -16429,32 +16423,32 @@
       <c r="B35" s="13" t="s">
         <v>332</v>
       </c>
-      <c r="C35" s="24">
+      <c r="C35" s="23">
         <v>61004.2735042735</v>
       </c>
       <c r="D35" s="15">
         <v>0.24035850081477458</v>
       </c>
       <c r="E35">
-        <v>2586665620</v>
+        <v>3571513320</v>
       </c>
       <c r="F35" s="16">
         <v>29559</v>
       </c>
       <c r="G35" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E35/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F35)</f>
-        <v>43317.610239364578</v>
+        <v>39929.153202477828</v>
       </c>
       <c r="H35" s="8">
-        <f t="shared" si="2"/>
-        <v>10.676314534296973</v>
+        <f>LN(G35)</f>
+        <v>10.594861992782002</v>
       </c>
       <c r="I35" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J35" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C35)</f>
         <v>11.018699198148646</v>
       </c>
     </row>
@@ -16465,32 +16459,32 @@
       <c r="B36" s="13" t="s">
         <v>333</v>
       </c>
-      <c r="C36" s="24">
+      <c r="C36" s="23">
         <v>86849.049964813501</v>
       </c>
       <c r="D36" s="15">
         <v>0.60032730073161344</v>
       </c>
       <c r="E36">
-        <v>4794964392</v>
+        <v>5614957192.4309101</v>
       </c>
       <c r="F36" s="16">
         <v>53584</v>
       </c>
       <c r="G36" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E36/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F36)</f>
-        <v>43991.172339754034</v>
+        <v>36420.264743786283</v>
       </c>
       <c r="H36" s="8">
-        <f t="shared" si="2"/>
-        <v>10.691744264129825</v>
+        <f>LN(G36)</f>
+        <v>10.502880622442062</v>
       </c>
       <c r="I36" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J36" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C36)</f>
         <v>11.371926832804741</v>
       </c>
     </row>
@@ -16501,32 +16495,32 @@
       <c r="B37" s="13" t="s">
         <v>334</v>
       </c>
-      <c r="C37" s="24">
+      <c r="C37" s="23">
         <v>90740.4692082111</v>
       </c>
       <c r="D37" s="15">
         <v>0.37648764113518463</v>
       </c>
       <c r="E37">
-        <v>2558287960</v>
+        <v>2760477311.1213899</v>
       </c>
       <c r="F37" s="16">
         <v>27032</v>
       </c>
       <c r="G37" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E37/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F37)</f>
-        <v>45747.714443684927</v>
+        <v>35836.332789086635</v>
       </c>
       <c r="H37" s="8">
-        <f t="shared" si="2"/>
-        <v>10.730897111940665</v>
+        <f>LN(G37)</f>
+        <v>10.486717540120567</v>
       </c>
       <c r="I37" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J37" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C37)</f>
         <v>11.415758724112797</v>
       </c>
     </row>
@@ -16537,32 +16531,32 @@
       <c r="B38" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="C38" s="24">
+      <c r="C38" s="23">
         <v>58051.948051947998</v>
       </c>
       <c r="D38" s="15">
         <v>0.72729650554509306</v>
       </c>
       <c r="E38">
-        <v>1467645796</v>
+        <v>1816301258</v>
       </c>
       <c r="F38" s="16">
         <v>18637</v>
       </c>
       <c r="G38" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E38/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F38)</f>
-        <v>40332.401361954202</v>
+        <v>34816.365618341588</v>
       </c>
       <c r="H38" s="8">
-        <f t="shared" si="2"/>
-        <v>10.604910428915396</v>
+        <f>LN(G38)</f>
+        <v>10.457842831606408</v>
       </c>
       <c r="I38" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J38" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C38)</f>
         <v>10.969093544736067</v>
       </c>
     </row>
@@ -16573,32 +16567,32 @@
       <c r="B39" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="C39" s="24">
+      <c r="C39" s="23">
         <v>100624.647755025</v>
       </c>
       <c r="D39" s="15">
         <v>1.3333333333333334E-2</v>
       </c>
       <c r="E39">
-        <v>17020108368</v>
+        <v>20148584267.721901</v>
       </c>
       <c r="F39" s="16">
         <v>101739</v>
       </c>
       <c r="G39" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E39/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F39)</f>
-        <v>70507.419822619879</v>
+        <v>56822.087243243906</v>
       </c>
       <c r="H39" s="8">
-        <f t="shared" si="2"/>
-        <v>11.16347322897334</v>
+        <f>LN(G39)</f>
+        <v>10.947680389039085</v>
       </c>
       <c r="I39" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J39" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C39)</f>
         <v>11.519152514143558</v>
       </c>
     </row>
@@ -16609,32 +16603,32 @@
       <c r="B40" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="C40" s="24">
+      <c r="C40" s="23">
         <v>134277.48885586901</v>
       </c>
       <c r="D40" s="15">
         <v>0</v>
       </c>
       <c r="E40">
-        <v>17349311390</v>
+        <v>20868022993.062698</v>
       </c>
       <c r="F40" s="16">
         <v>69099</v>
       </c>
       <c r="G40" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E40/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F40)</f>
-        <v>99061.727292085692</v>
+        <v>79566.128920131596</v>
       </c>
       <c r="H40" s="8">
-        <f t="shared" si="2"/>
-        <v>11.503498442817239</v>
+        <f>LN(G40)</f>
+        <v>11.284343765196068</v>
       </c>
       <c r="I40" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J40" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C40)</f>
         <v>11.807663750113845</v>
       </c>
     </row>
@@ -16645,32 +16639,32 @@
       <c r="B41" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="C41" s="24">
+      <c r="C41" s="23">
         <v>90568.923327895594</v>
       </c>
       <c r="D41" s="15">
         <v>0.25798883785252136</v>
       </c>
       <c r="E41">
-        <v>4664155763</v>
+        <v>5335063217</v>
       </c>
       <c r="F41" s="16">
         <v>42271</v>
       </c>
       <c r="G41" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E41/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F41)</f>
-        <v>51098.252778997849</v>
+        <v>41107.127198575428</v>
       </c>
       <c r="H41" s="8">
-        <f t="shared" si="2"/>
-        <v>10.841505583415406</v>
+        <f>LN(G41)</f>
+        <v>10.623936796607902</v>
       </c>
       <c r="I41" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J41" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C41)</f>
         <v>11.413866423563936</v>
       </c>
     </row>
@@ -16681,32 +16675,32 @@
       <c r="B42" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="C42" s="24">
+      <c r="C42" s="23">
         <v>97759.226713532495</v>
       </c>
       <c r="D42" s="15">
         <v>0.59259052536105494</v>
       </c>
       <c r="E42">
-        <v>8491098449</v>
+        <v>10349284631.224199</v>
       </c>
       <c r="F42" s="16">
         <v>71252</v>
       </c>
       <c r="G42" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E42/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F42)</f>
-        <v>54107.679918731454</v>
+        <v>45272.22336589529</v>
       </c>
       <c r="H42" s="8">
-        <f t="shared" si="2"/>
-        <v>10.898731412591887</v>
+        <f>LN(G42)</f>
+        <v>10.720448952674284</v>
       </c>
       <c r="I42" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J42" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C42)</f>
         <v>11.490262864324347</v>
       </c>
     </row>
@@ -16717,32 +16711,32 @@
       <c r="B43" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="C43" s="24">
+      <c r="C43" s="23">
         <v>69810.4508196721</v>
       </c>
       <c r="D43" s="15">
         <v>0.95294954223578565</v>
       </c>
       <c r="E43">
-        <v>2348097084</v>
+        <v>3355586836.6333699</v>
       </c>
       <c r="F43" s="16">
         <v>34237</v>
       </c>
       <c r="G43" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E43/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F43)</f>
-        <v>36868.068082443686</v>
+        <v>34937.524265830849</v>
       </c>
       <c r="H43" s="8">
-        <f t="shared" si="2"/>
-        <v>10.515101091765958</v>
+        <f>LN(G43)</f>
+        <v>10.461316724446935</v>
       </c>
       <c r="I43" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J43" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C43)</f>
         <v>11.153539002752964</v>
       </c>
     </row>
@@ -16753,32 +16747,32 @@
       <c r="B44" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="C44" s="24">
+      <c r="C44" s="23">
         <v>70410.677618069807</v>
       </c>
       <c r="D44" s="15">
         <v>1</v>
       </c>
       <c r="E44">
-        <v>1055302140</v>
+        <v>1238142773.8199301</v>
       </c>
       <c r="F44" s="16">
         <v>15479</v>
       </c>
       <c r="G44" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E44/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F44)</f>
-        <v>36729.284558447158</v>
+        <v>30994.727023960724</v>
       </c>
       <c r="H44" s="8">
-        <f t="shared" si="2"/>
-        <v>10.511329660226162</v>
+        <f>LN(G44)</f>
+        <v>10.341572372998051</v>
       </c>
       <c r="I44" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J44" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C44)</f>
         <v>11.162100201356512</v>
       </c>
     </row>
@@ -16789,32 +16783,32 @@
       <c r="B45" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="C45" s="24">
+      <c r="C45" s="23">
         <v>69038.461538461503</v>
       </c>
       <c r="D45" s="15">
         <v>1</v>
       </c>
       <c r="E45">
-        <v>899492032</v>
+        <v>947789398</v>
       </c>
       <c r="F45" s="16">
         <v>13765</v>
       </c>
       <c r="G45" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E45/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F45)</f>
-        <v>35764.811773635658</v>
+        <v>28558.967006281608</v>
       </c>
       <c r="H45" s="8">
-        <f t="shared" si="2"/>
-        <v>10.484719777663702</v>
+        <f>LN(G45)</f>
+        <v>10.259726246551555</v>
       </c>
       <c r="I45" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J45" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C45)</f>
         <v>11.142419041883034</v>
       </c>
     </row>
@@ -16825,32 +16819,32 @@
       <c r="B46" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="C46" s="24">
+      <c r="C46" s="23">
         <v>71682.5636538135</v>
       </c>
       <c r="D46" s="15">
         <v>0.31365052393089776</v>
       </c>
       <c r="E46">
-        <v>1562522182</v>
+        <v>1505913598.3160801</v>
       </c>
       <c r="F46" s="16">
         <v>20724</v>
       </c>
       <c r="G46" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E46/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F46)</f>
-        <v>39189.955460509082</v>
+        <v>29392.546054372368</v>
       </c>
       <c r="H46" s="8">
-        <f t="shared" si="2"/>
-        <v>10.576175754691604</v>
+        <f>LN(G46)</f>
+        <v>10.288496385615632</v>
       </c>
       <c r="I46" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J46" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C46)</f>
         <v>11.180002812268926</v>
       </c>
     </row>
@@ -16861,32 +16855,32 @@
       <c r="B47" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="C47" s="24">
+      <c r="C47" s="23">
         <v>113327.73512476</v>
       </c>
       <c r="D47" s="15">
         <v>0.82639038007300836</v>
       </c>
       <c r="E47">
-        <v>1694398438</v>
+        <v>1628720074</v>
       </c>
       <c r="F47" s="16">
         <v>19121</v>
       </c>
       <c r="G47" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E47/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F47)</f>
-        <v>43694.519126894898</v>
+        <v>32130.420204227077</v>
       </c>
       <c r="H47" s="8">
-        <f t="shared" si="2"/>
-        <v>10.684977952780693</v>
+        <f>LN(G47)</f>
+        <v>10.377558530276083</v>
       </c>
       <c r="I47" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J47" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C47)</f>
         <v>11.638039210746214</v>
       </c>
     </row>
@@ -16897,32 +16891,32 @@
       <c r="B48" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="C48" s="24">
+      <c r="C48" s="23">
         <v>121561.582444753</v>
       </c>
       <c r="D48" s="15">
         <v>6.7775239142594396E-2</v>
       </c>
       <c r="E48">
-        <v>41340193588</v>
+        <v>132811651780.245</v>
       </c>
       <c r="F48" s="16">
         <v>101208</v>
       </c>
       <c r="G48" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E48/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F48)</f>
-        <v>152699.0817404163</v>
+        <v>300588.37309242727</v>
       </c>
       <c r="H48" s="8">
-        <f t="shared" si="2"/>
-        <v>11.936224477700865</v>
+        <f>LN(G48)</f>
+        <v>12.613497076552385</v>
       </c>
       <c r="I48" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J48" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C48)</f>
         <v>11.708176264754101</v>
       </c>
     </row>
@@ -16933,32 +16927,32 @@
       <c r="B49" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="C49" s="24">
+      <c r="C49" s="23">
         <v>124558.359621451</v>
       </c>
       <c r="D49" s="15">
         <v>0</v>
       </c>
       <c r="E49">
-        <v>6401850717</v>
+        <v>7669949196.5560703</v>
       </c>
       <c r="F49" s="16">
         <v>28216</v>
       </c>
       <c r="G49" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E49/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F49)</f>
-        <v>90817.266475636628</v>
+        <v>72965.182927549846</v>
       </c>
       <c r="H49" s="8">
-        <f t="shared" si="2"/>
-        <v>11.416604705934684</v>
+        <f>LN(G49)</f>
+        <v>11.197737660157566</v>
       </c>
       <c r="I49" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J49" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C49)</f>
         <v>11.732529637036537</v>
       </c>
     </row>
@@ -16969,32 +16963,32 @@
       <c r="B50" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="C50" s="24">
+      <c r="C50" s="23">
         <v>106954.91556091599</v>
       </c>
       <c r="D50" s="15">
         <v>0.44102178812922616</v>
       </c>
       <c r="E50">
-        <v>15217346858</v>
+        <v>22690599560.388</v>
       </c>
       <c r="F50" s="16">
         <v>65581</v>
       </c>
       <c r="G50" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E50/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F50)</f>
-        <v>92572.945245311334</v>
+        <v>89190.500021186512</v>
       </c>
       <c r="H50" s="8">
-        <f t="shared" si="2"/>
-        <v>11.435752209967692</v>
+        <f>LN(G50)</f>
+        <v>11.398529810891723</v>
       </c>
       <c r="I50" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J50" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C50)</f>
         <v>11.58016267475325</v>
       </c>
     </row>
@@ -17005,32 +16999,32 @@
       <c r="B51" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="C51" s="24">
+      <c r="C51" s="23">
         <v>40959.373548967102</v>
       </c>
       <c r="D51" s="15">
         <v>1</v>
       </c>
       <c r="E51">
-        <v>1571602882</v>
+        <v>1744139059.0571401</v>
       </c>
       <c r="F51" s="16">
         <v>40971</v>
       </c>
       <c r="G51" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E51/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F51)</f>
-        <v>26567.620222055826</v>
+        <v>22808.426731448846</v>
       </c>
       <c r="H51" s="8">
-        <f t="shared" si="2"/>
-        <v>10.187448468391626</v>
+        <f>LN(G51)</f>
+        <v>10.034885340144283</v>
       </c>
       <c r="I51" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J51" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C51)</f>
         <v>10.620335965381761</v>
       </c>
     </row>
@@ -17041,32 +17035,32 @@
       <c r="B52" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="C52" s="24">
+      <c r="C52" s="23">
         <v>148585.304054054</v>
       </c>
       <c r="D52" s="15">
         <v>0</v>
       </c>
       <c r="E52">
-        <v>6605127507</v>
+        <v>7458343008.5430002</v>
       </c>
       <c r="F52" s="16">
         <v>35814</v>
       </c>
       <c r="G52" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E52/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F52)</f>
-        <v>76347.556281666024</v>
+        <v>59055.859830313871</v>
       </c>
       <c r="H52" s="8">
-        <f t="shared" si="2"/>
-        <v>11.243051303345631</v>
+        <f>LN(G52)</f>
+        <v>10.986239051762389</v>
       </c>
       <c r="I52" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J52" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C52)</f>
         <v>11.908914510372936</v>
       </c>
     </row>
@@ -17077,32 +17071,32 @@
       <c r="B53" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="C53" s="24">
+      <c r="C53" s="23">
         <v>33334.428383705599</v>
       </c>
       <c r="D53" s="15">
         <v>1</v>
       </c>
       <c r="E53">
-        <v>1146743608</v>
+        <v>1255679042.0029199</v>
       </c>
       <c r="F53" s="16">
         <v>30409</v>
       </c>
       <c r="G53" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E53/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F53)</f>
-        <v>26346.701240104183</v>
+        <v>22529.030770653291</v>
       </c>
       <c r="H53" s="8">
-        <f t="shared" si="2"/>
-        <v>10.179098356003697</v>
+        <f>LN(G53)</f>
+        <v>10.022560013000405</v>
       </c>
       <c r="I53" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J53" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C53)</f>
         <v>10.414346027273687</v>
       </c>
     </row>
@@ -17113,32 +17107,32 @@
       <c r="B54" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="C54" s="24">
+      <c r="C54" s="23">
         <v>74648.760330578501</v>
       </c>
       <c r="D54" s="15">
         <v>0.63061677772082692</v>
       </c>
       <c r="E54">
-        <v>1617997584</v>
+        <v>1966649200.72945</v>
       </c>
       <c r="F54" s="16">
         <v>19398</v>
       </c>
       <c r="G54" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E54/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F54)</f>
-        <v>41921.020355515582</v>
+        <v>35675.586686472605</v>
       </c>
       <c r="H54" s="8">
-        <f t="shared" si="2"/>
-        <v>10.643542659240577</v>
+        <f>LN(G54)</f>
+        <v>10.48222188752089</v>
       </c>
       <c r="I54" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J54" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C54)</f>
         <v>11.220549196407191</v>
       </c>
     </row>
@@ -17149,32 +17143,32 @@
       <c r="B55" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="C55" s="24">
+      <c r="C55" s="23">
         <v>107121.65728431899</v>
       </c>
       <c r="D55" s="15">
         <v>0.3766284625225178</v>
       </c>
       <c r="E55">
-        <v>4482429240</v>
+        <v>4738453822</v>
       </c>
       <c r="F55" s="16">
         <v>39641</v>
       </c>
       <c r="G55" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E55/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F55)</f>
-        <v>52030.740790506723</v>
+        <v>39646.399143461444</v>
       </c>
       <c r="H55" s="8">
-        <f t="shared" si="2"/>
-        <v>10.859589991940187</v>
+        <f>LN(G55)</f>
+        <v>10.58775540688503</v>
       </c>
       <c r="I55" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J55" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C55)</f>
         <v>11.581720451532894</v>
       </c>
     </row>
@@ -17185,32 +17179,32 @@
       <c r="B56" s="13" t="s">
         <v>354</v>
       </c>
-      <c r="C56" s="24">
+      <c r="C56" s="23">
         <v>27693.3701657458</v>
       </c>
       <c r="D56" s="15">
         <v>1</v>
       </c>
       <c r="E56">
-        <v>331716553</v>
+        <v>420233996</v>
       </c>
       <c r="F56" s="16">
         <v>6977</v>
       </c>
       <c r="G56" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E56/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F56)</f>
-        <v>29697.960312098698</v>
+        <v>26672.301145177298</v>
       </c>
       <c r="H56" s="8">
-        <f t="shared" si="2"/>
-        <v>10.298833646072149</v>
+        <f>LN(G56)</f>
+        <v>10.191380895612847</v>
       </c>
       <c r="I56" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J56" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C56)</f>
         <v>10.228948319331135</v>
       </c>
     </row>
@@ -17221,32 +17215,32 @@
       <c r="B57" s="13" t="s">
         <v>353</v>
       </c>
-      <c r="C57" s="24">
+      <c r="C57" s="23">
         <v>69948.321735570993</v>
       </c>
       <c r="D57" s="15">
         <v>0.47652407214189896</v>
       </c>
       <c r="E57">
-        <v>2007253376</v>
+        <v>1697988043.6924701</v>
       </c>
       <c r="F57" s="16">
         <v>13997</v>
       </c>
       <c r="G57" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E57/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F57)</f>
-        <v>62367.205750488654</v>
+        <v>40035.098278045916</v>
       </c>
       <c r="H57" s="8">
-        <f t="shared" si="2"/>
-        <v>11.040794867337933</v>
+        <f>LN(G57)</f>
+        <v>10.597511805306917</v>
       </c>
       <c r="I57" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J57" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C57)</f>
         <v>11.15551198746229</v>
       </c>
     </row>
@@ -17257,32 +17251,32 @@
       <c r="B58" s="13" t="s">
         <v>355</v>
       </c>
-      <c r="C58" s="24">
+      <c r="C58" s="23">
         <v>85473.405959628304</v>
       </c>
       <c r="D58" s="15">
         <v>0.48509996826404317</v>
       </c>
       <c r="E58">
-        <v>4938927987</v>
+        <v>5574661088</v>
       </c>
       <c r="F58" s="16">
         <v>64213</v>
       </c>
       <c r="G58" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E58/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F58)</f>
-        <v>39707.290461090946</v>
+        <v>32488.229724070618</v>
       </c>
       <c r="H58" s="8">
-        <f t="shared" si="2"/>
-        <v>10.589290088634149</v>
+        <f>LN(G58)</f>
+        <v>10.388633140384924</v>
       </c>
       <c r="I58" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J58" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C58)</f>
         <v>11.355960565133584</v>
       </c>
     </row>
@@ -17293,32 +17287,32 @@
       <c r="B59" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="C59" s="24">
+      <c r="C59" s="23">
         <v>54755.244755244697</v>
       </c>
       <c r="D59" s="15">
         <v>0.48020527859237538</v>
       </c>
       <c r="E59">
-        <v>474600206</v>
+        <v>463034211.20127797</v>
       </c>
       <c r="F59" s="16">
         <v>6856</v>
       </c>
       <c r="G59" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E59/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F59)</f>
-        <v>37086.332914669983</v>
+        <v>28270.630949512713</v>
       </c>
       <c r="H59" s="8">
-        <f t="shared" si="2"/>
-        <v>10.521003795675758</v>
+        <f>LN(G59)</f>
+        <v>10.249578769133757</v>
       </c>
       <c r="I59" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J59" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C59)</f>
         <v>10.910628437707077</v>
       </c>
     </row>
@@ -17329,32 +17323,32 @@
       <c r="B60" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="C60" s="24">
+      <c r="C60" s="23">
         <v>21129.032258064501</v>
       </c>
       <c r="D60" s="15">
         <v>1</v>
       </c>
-      <c r="E60">
-        <v>112665634</v>
+      <c r="E60" s="27">
+        <v>88633152</v>
       </c>
       <c r="F60" s="16">
         <v>7817</v>
       </c>
       <c r="G60" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E60/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F60)</f>
-        <v>18406.923214624792</v>
+        <v>15975.675396810533</v>
       </c>
       <c r="H60" s="8">
-        <f t="shared" si="2"/>
-        <v>9.8204821344927993</v>
+        <f>LN(G60)</f>
+        <v>9.6788225567126283</v>
       </c>
       <c r="I60" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J60" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C60)</f>
         <v>9.9584033101322422</v>
       </c>
     </row>
@@ -17365,32 +17359,32 @@
       <c r="B61" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="C61" s="24">
+      <c r="C61" s="23">
         <v>57590.882862088802</v>
       </c>
       <c r="D61" s="15">
         <v>0.65371755231178541</v>
       </c>
       <c r="E61">
-        <v>3078363644</v>
+        <v>3945507288</v>
       </c>
       <c r="F61" s="16">
         <v>55711</v>
       </c>
       <c r="G61" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E61/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F61)</f>
-        <v>32326.055160299322</v>
+        <v>28989.071852351441</v>
       </c>
       <c r="H61" s="8">
-        <f t="shared" si="2"/>
-        <v>10.383628845343949</v>
+        <f>LN(G61)</f>
+        <v>10.274674205271799</v>
       </c>
       <c r="I61" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J61" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C61)</f>
         <v>10.961119550511514</v>
       </c>
     </row>
@@ -17401,32 +17395,32 @@
       <c r="B62" s="13" t="s">
         <v>358</v>
       </c>
-      <c r="C62" s="24">
+      <c r="C62" s="23">
         <v>49808.153477218199</v>
       </c>
       <c r="D62" s="15">
         <v>0.94860366859027201</v>
       </c>
       <c r="E62">
-        <v>1470290440</v>
+        <v>1467654352.7150199</v>
       </c>
       <c r="F62" s="16">
         <v>37610</v>
       </c>
       <c r="G62" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E62/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F62)</f>
-        <v>26817.819647503842</v>
+        <v>22032.401491644319</v>
       </c>
       <c r="H62" s="8">
-        <f t="shared" si="2"/>
-        <v>10.19682185776305</v>
+        <f>LN(G62)</f>
+        <v>10.000269443916245</v>
       </c>
       <c r="I62" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J62" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C62)</f>
         <v>10.815933974053493</v>
       </c>
     </row>
@@ -17437,32 +17431,32 @@
       <c r="B63" s="13" t="s">
         <v>359</v>
       </c>
-      <c r="C63" s="24">
+      <c r="C63" s="23">
         <v>43935.950413223101</v>
       </c>
       <c r="D63" s="15">
         <v>1</v>
       </c>
       <c r="E63">
-        <v>1001855568</v>
+        <v>886136027.60169101</v>
       </c>
       <c r="F63" s="16">
         <v>30315</v>
       </c>
       <c r="G63" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E63/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F63)</f>
-        <v>24757.746406189581</v>
+        <v>19890.128188207571</v>
       </c>
       <c r="H63" s="8">
-        <f t="shared" si="2"/>
-        <v>10.116893705135572</v>
+        <f>LN(G63)</f>
+        <v>9.8979788166843417</v>
       </c>
       <c r="I63" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J63" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C63)</f>
         <v>10.690488179953238</v>
       </c>
     </row>
@@ -17473,32 +17467,32 @@
       <c r="B64" s="13" t="s">
         <v>360</v>
       </c>
-      <c r="C64" s="24">
+      <c r="C64" s="23">
         <v>34814.241486068102</v>
       </c>
       <c r="D64" s="15">
         <v>0.78007798652959948</v>
       </c>
       <c r="E64">
-        <v>738008372</v>
+        <v>632440233.59475005</v>
       </c>
       <c r="F64" s="16">
         <v>15218</v>
       </c>
       <c r="G64" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E64/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F64)</f>
-        <v>30022.212827599207</v>
+        <v>22587.157447590638</v>
       </c>
       <c r="H64" s="8">
-        <f t="shared" si="2"/>
-        <v>10.309692814249662</v>
+        <f>LN(G64)</f>
+        <v>10.025136769211192</v>
       </c>
       <c r="I64" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J64" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C64)</f>
         <v>10.457781820152896</v>
       </c>
     </row>
@@ -17509,32 +17503,32 @@
       <c r="B65" s="13" t="s">
         <v>361</v>
       </c>
-      <c r="C65" s="24">
+      <c r="C65" s="23">
         <v>42009.868421052597</v>
       </c>
       <c r="D65" s="15">
         <v>1</v>
       </c>
       <c r="E65">
-        <v>1811622658</v>
+        <v>2214326519.5912199</v>
       </c>
       <c r="F65" s="16">
         <v>69708</v>
       </c>
       <c r="G65" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E65/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F65)</f>
-        <v>22351.917694388405</v>
+        <v>20444.684613386424</v>
       </c>
       <c r="H65" s="8">
-        <f t="shared" si="2"/>
-        <v>10.014667399241771</v>
+        <f>LN(G65)</f>
+        <v>9.925478206579804</v>
       </c>
       <c r="I65" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J65" s="8">
-        <f t="shared" si="3"/>
+        <f>LN(C65)</f>
         <v>10.645659832072177</v>
       </c>
     </row>
@@ -17545,32 +17539,32 @@
       <c r="B66" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="C66" s="24">
+      <c r="C66" s="23">
         <v>39649.467190128998</v>
       </c>
       <c r="D66" s="15">
         <v>1</v>
       </c>
       <c r="E66">
-        <v>2151988838</v>
+        <v>2059404538</v>
       </c>
       <c r="F66" s="16">
         <v>55754</v>
       </c>
       <c r="G66" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E66/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F66)</f>
-        <v>26649.076446053557</v>
+        <v>21576.111253465962</v>
       </c>
       <c r="H66" s="8">
-        <f t="shared" ref="H66:H78" si="4">LN(G66)</f>
-        <v>10.190509774061169</v>
+        <f>LN(G66)</f>
+        <v>9.9793420211589776</v>
       </c>
       <c r="I66" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J66" s="8">
-        <f t="shared" ref="J66:J78" si="5">LN(C66)</f>
+        <f>LN(C66)</f>
         <v>10.587832789144938</v>
       </c>
     </row>
@@ -17581,32 +17575,32 @@
       <c r="B67" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="C67" s="24">
+      <c r="C67" s="23">
         <v>120174.618023074</v>
       </c>
       <c r="D67" s="15">
         <v>0</v>
       </c>
       <c r="E67">
-        <v>29138897152</v>
+        <v>60869319139.509003</v>
       </c>
       <c r="F67" s="16">
         <v>41671</v>
       </c>
       <c r="G67" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E67/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F67)</f>
-        <v>251800.13722547694</v>
+        <v>333065.25063794554</v>
       </c>
       <c r="H67" s="8">
-        <f t="shared" si="4"/>
-        <v>12.436390945570301</v>
+        <f>LN(G67)</f>
+        <v>12.716093697629004</v>
       </c>
       <c r="I67" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J67" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C67)</f>
         <v>11.696701114251381</v>
       </c>
     </row>
@@ -17617,32 +17611,32 @@
       <c r="B68" s="13" t="s">
         <v>364</v>
       </c>
-      <c r="C68" s="24">
+      <c r="C68" s="23">
         <v>66870.910172516305</v>
       </c>
       <c r="D68" s="15">
         <v>0.25196740232940434</v>
       </c>
       <c r="E68">
-        <v>5316692624</v>
+        <v>6215659728</v>
       </c>
       <c r="F68" s="16">
         <v>57464</v>
       </c>
       <c r="G68" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E68/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F68)</f>
-        <v>45026.217787680507</v>
+        <v>37159.338945202151</v>
       </c>
       <c r="H68" s="8">
-        <f t="shared" si="4"/>
-        <v>10.715000216600783</v>
+        <f>LN(G68)</f>
+        <v>10.52297040335087</v>
       </c>
       <c r="I68" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J68" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C68)</f>
         <v>11.110519326029364</v>
       </c>
     </row>
@@ -17653,32 +17647,32 @@
       <c r="B69" s="13" t="s">
         <v>365</v>
       </c>
-      <c r="C69" s="24">
+      <c r="C69" s="23">
         <v>66796.875</v>
       </c>
       <c r="D69" s="15">
         <v>1</v>
       </c>
       <c r="E69">
-        <v>1205246686</v>
+        <v>1274341977.2748699</v>
       </c>
       <c r="F69" s="16">
         <v>26456</v>
       </c>
       <c r="G69" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E69/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F69)</f>
-        <v>29020.578538805948</v>
+        <v>24033.198874881611</v>
       </c>
       <c r="H69" s="8">
-        <f t="shared" si="4"/>
-        <v>10.275760462104587</v>
+        <f>LN(G69)</f>
+        <v>10.08719143992416</v>
       </c>
       <c r="I69" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J69" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C69)</f>
         <v>11.109411576993326</v>
       </c>
     </row>
@@ -17689,32 +17683,32 @@
       <c r="B70" s="13" t="s">
         <v>366</v>
       </c>
-      <c r="C70" s="24">
+      <c r="C70" s="23">
         <v>26013.8888888888</v>
       </c>
       <c r="D70" s="15">
         <v>1</v>
       </c>
       <c r="E70">
-        <v>425011356</v>
+        <v>474204750</v>
       </c>
       <c r="F70" s="16">
         <v>12366</v>
       </c>
       <c r="G70" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E70/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F70)</f>
-        <v>25207.994823081179</v>
+        <v>21884.61384983642</v>
       </c>
       <c r="H70" s="8">
-        <f t="shared" si="4"/>
-        <v>10.134916478069</v>
+        <f>LN(G70)</f>
+        <v>9.9935391049564863</v>
       </c>
       <c r="I70" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J70" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C70)</f>
         <v>10.166385862410166</v>
       </c>
     </row>
@@ -17725,32 +17719,32 @@
       <c r="B71" s="13" t="s">
         <v>367</v>
       </c>
-      <c r="C71" s="24">
+      <c r="C71" s="23">
         <v>64441.176470588201</v>
       </c>
       <c r="D71" s="15">
         <v>1</v>
       </c>
       <c r="E71">
-        <v>886766612</v>
+        <v>943420954</v>
       </c>
       <c r="F71" s="16">
         <v>18366</v>
       </c>
       <c r="G71" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E71/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F71)</f>
-        <v>29949.726645664043</v>
+        <v>24733.163421129382</v>
       </c>
       <c r="H71" s="8">
-        <f t="shared" si="4"/>
-        <v>10.30727547647904</v>
+        <f>LN(G71)</f>
+        <v>10.115900270698107</v>
       </c>
       <c r="I71" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J71" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C71)</f>
         <v>11.073508093961442</v>
       </c>
     </row>
@@ -17761,32 +17755,32 @@
       <c r="B72" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="C72" s="24">
+      <c r="C72" s="23">
         <v>29233.695652173901</v>
       </c>
       <c r="D72" s="15">
         <v>1</v>
       </c>
       <c r="E72">
-        <v>808873876</v>
+        <v>627711081.28356099</v>
       </c>
       <c r="F72" s="16">
         <v>25772</v>
       </c>
       <c r="G72" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E72/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F72)</f>
-        <v>24191.201853396356</v>
+        <v>18823.672719654594</v>
       </c>
       <c r="H72" s="8">
-        <f t="shared" si="4"/>
-        <v>10.09374428626389</v>
+        <f>LN(G72)</f>
+        <v>9.8428705439223627</v>
       </c>
       <c r="I72" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J72" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C72)</f>
         <v>10.283077283646394</v>
       </c>
     </row>
@@ -17797,32 +17791,32 @@
       <c r="B73" s="13" t="s">
         <v>369</v>
       </c>
-      <c r="C73" s="24">
+      <c r="C73" s="23">
         <v>36360.294117646998</v>
       </c>
       <c r="D73" s="15">
         <v>1</v>
       </c>
       <c r="E73">
-        <v>610156830</v>
+        <v>532283575.13797301</v>
       </c>
       <c r="F73" s="16">
         <v>16374</v>
       </c>
       <c r="G73" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E73/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F73)</f>
-        <v>26194.398482589455</v>
+        <v>20607.040770706662</v>
       </c>
       <c r="H73" s="8">
-        <f t="shared" si="4"/>
-        <v>10.173300868516609</v>
+        <f>LN(G73)</f>
+        <v>9.9333880813682498</v>
       </c>
       <c r="I73" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J73" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C73)</f>
         <v>10.501232637302897</v>
       </c>
     </row>
@@ -17833,32 +17827,32 @@
       <c r="B74" s="13" t="s">
         <v>370</v>
       </c>
-      <c r="C74" s="24">
+      <c r="C74" s="23">
         <v>69646.581691772793</v>
       </c>
       <c r="D74" s="15">
         <v>1</v>
       </c>
       <c r="E74">
-        <v>1610667516</v>
+        <v>1662849170</v>
       </c>
       <c r="F74" s="16">
         <v>32594</v>
       </c>
       <c r="G74" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E74/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F74)</f>
-        <v>30335.854192189108</v>
+        <v>24656.424357756732</v>
       </c>
       <c r="H74" s="8">
-        <f t="shared" si="4"/>
-        <v>10.320085598614831</v>
+        <f>LN(G74)</f>
+        <v>10.112792768547282</v>
       </c>
       <c r="I74" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J74" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C74)</f>
         <v>11.151188899637063</v>
       </c>
     </row>
@@ -17869,32 +17863,32 @@
       <c r="B75" s="13" t="s">
         <v>371</v>
       </c>
-      <c r="C75" s="24">
+      <c r="C75" s="23">
         <v>46860.632183907997</v>
       </c>
       <c r="D75" s="15">
         <v>1</v>
       </c>
       <c r="E75">
-        <v>944454244</v>
+        <v>894063121.09593594</v>
       </c>
       <c r="F75" s="16">
         <v>25449</v>
       </c>
       <c r="G75" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E75/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F75)</f>
-        <v>26142.55772344819</v>
+        <v>21181.048170526352</v>
       </c>
       <c r="H75" s="8">
-        <f t="shared" si="4"/>
-        <v>10.17131982950122</v>
+        <f>LN(G75)</f>
+        <v>9.9608621066242797</v>
       </c>
       <c r="I75" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J75" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C75)</f>
         <v>10.754933202877913</v>
       </c>
     </row>
@@ -17905,32 +17899,32 @@
       <c r="B76" s="13" t="s">
         <v>372</v>
       </c>
-      <c r="C76" s="24">
+      <c r="C76" s="23">
         <v>68091.372912801395</v>
       </c>
       <c r="D76" s="15">
         <v>0.76612380384326129</v>
       </c>
       <c r="E76">
-        <v>4611399282</v>
+        <v>5358863377.8789196</v>
       </c>
       <c r="F76" s="16">
         <v>79265</v>
       </c>
       <c r="G76" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E76/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F76)</f>
-        <v>33321.537311986816</v>
+        <v>28285.913018486506</v>
       </c>
       <c r="H76" s="8">
-        <f t="shared" si="4"/>
-        <v>10.413959233031193</v>
+        <f>LN(G76)</f>
+        <v>10.250119186502767</v>
       </c>
       <c r="I76" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J76" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C76)</f>
         <v>11.128605801481278</v>
       </c>
     </row>
@@ -17941,32 +17935,32 @@
       <c r="B77" s="13" t="s">
         <v>373</v>
       </c>
-      <c r="C77" s="24">
+      <c r="C77" s="23">
         <v>128716.672291596</v>
       </c>
       <c r="D77" s="15">
         <v>0.26175368245975783</v>
       </c>
       <c r="E77">
-        <v>13702979328</v>
+        <v>16462631666.2216</v>
       </c>
       <c r="F77" s="16">
         <v>86482</v>
       </c>
       <c r="G77" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E77/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F77)</f>
-        <v>67493.777222656645</v>
+        <v>55141.258168912616</v>
       </c>
       <c r="H77" s="8">
-        <f t="shared" si="4"/>
-        <v>11.119790683316952</v>
+        <f>LN(G77)</f>
+        <v>10.917653502034417</v>
       </c>
       <c r="I77" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J77" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C77)</f>
         <v>11.765368929029385</v>
       </c>
     </row>
@@ -17977,36 +17971,41 @@
       <c r="B78" s="13" t="s">
         <v>374</v>
       </c>
-      <c r="C78" s="24">
+      <c r="C78" s="23">
         <v>29969.4055944055</v>
       </c>
       <c r="D78" s="15">
         <v>1</v>
       </c>
       <c r="E78">
-        <v>973565344</v>
+        <v>1087817372</v>
       </c>
       <c r="F78" s="16">
         <v>23865</v>
       </c>
       <c r="G78" s="4">
         <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E78/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F78)</f>
-        <v>27397.72466364472</v>
+        <v>23467.390959382756</v>
       </c>
       <c r="H78" s="8">
-        <f t="shared" si="4"/>
-        <v>10.218215247455207</v>
+        <f>LN(G78)</f>
+        <v>10.063367117748141</v>
       </c>
       <c r="I78" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.816845867278564</v>
       </c>
       <c r="J78" s="8">
-        <f t="shared" si="5"/>
+        <f>LN(C78)</f>
         <v>10.307932326760856</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J78" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J78">
+      <sortCondition ref="B1:B78"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
remove EDA from WEIGHTS tab, remove weight interval
</commit_message>
<xml_diff>
--- a/input/community_cohort_inputs.xlsx
+++ b/input/community_cohort_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cmapil-my.sharepoint.com/personal/amcadams_cmap_illinois_gov/Documents/Documents/GitHub/community-cohort-tool/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amcadams\GitHub\community-cohort-tool\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="13_ncr:1_{1A0601AD-1F7D-4417-885C-11F87AAE5F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC4E1846-3992-4756-A33F-26A77A312DEF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBB28C8-E4AA-4992-9DF7-674069F87587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14580" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23880" yWindow="4470" windowWidth="19140" windowHeight="10920" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FACTORS_MUNI" sheetId="1" r:id="rId1"/>
@@ -15178,7 +15178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
@@ -15252,7 +15252,7 @@
         <v>29781.962918929472</v>
       </c>
       <c r="H2" s="8">
-        <f>LN(G2)</f>
+        <f t="shared" ref="H2:H33" si="0">LN(G2)</f>
         <v>10.301658218066086</v>
       </c>
       <c r="I2" s="8">
@@ -15260,7 +15260,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J2" s="8">
-        <f>LN(C2)</f>
+        <f t="shared" ref="J2:J33" si="1">LN(C2)</f>
         <v>11.271334499718714</v>
       </c>
     </row>
@@ -15288,7 +15288,7 @@
         <v>29183.470760991047</v>
       </c>
       <c r="H3" s="8">
-        <f>LN(G3)</f>
+        <f t="shared" si="0"/>
         <v>10.281357758149285</v>
       </c>
       <c r="I3" s="8">
@@ -15296,7 +15296,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J3" s="8">
-        <f>LN(C3)</f>
+        <f t="shared" si="1"/>
         <v>10.959540226785442</v>
       </c>
     </row>
@@ -15324,7 +15324,7 @@
         <v>36630.808537357385</v>
       </c>
       <c r="H4" s="8">
-        <f>LN(G4)</f>
+        <f t="shared" si="0"/>
         <v>10.508644928621182</v>
       </c>
       <c r="I4" s="8">
@@ -15332,7 +15332,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J4" s="8">
-        <f>LN(C4)</f>
+        <f t="shared" si="1"/>
         <v>10.719876156208088</v>
       </c>
     </row>
@@ -15360,7 +15360,7 @@
         <v>26759.409089345005</v>
       </c>
       <c r="H5" s="8">
-        <f>LN(G5)</f>
+        <f t="shared" si="0"/>
         <v>10.194641432135315</v>
       </c>
       <c r="I5" s="8">
@@ -15368,7 +15368,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J5" s="8">
-        <f>LN(C5)</f>
+        <f t="shared" si="1"/>
         <v>11.265232461066633</v>
       </c>
     </row>
@@ -15396,7 +15396,7 @@
         <v>22214.831291047369</v>
       </c>
       <c r="H6" s="8">
-        <f>LN(G6)</f>
+        <f t="shared" si="0"/>
         <v>10.008515420970133</v>
       </c>
       <c r="I6" s="8">
@@ -15404,7 +15404,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J6" s="8">
-        <f>LN(C6)</f>
+        <f t="shared" si="1"/>
         <v>10.621327345686446</v>
       </c>
     </row>
@@ -15432,7 +15432,7 @@
         <v>23859.775398112979</v>
       </c>
       <c r="H7" s="8">
-        <f>LN(G7)</f>
+        <f t="shared" si="0"/>
         <v>10.079949282284591</v>
       </c>
       <c r="I7" s="8">
@@ -15440,7 +15440,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J7" s="8">
-        <f>LN(C7)</f>
+        <f t="shared" si="1"/>
         <v>10.598776656091799</v>
       </c>
     </row>
@@ -15468,7 +15468,7 @@
         <v>26133.449873254835</v>
       </c>
       <c r="H8" s="8">
-        <f>LN(G8)</f>
+        <f t="shared" si="0"/>
         <v>10.170971377096217</v>
       </c>
       <c r="I8" s="8">
@@ -15476,7 +15476,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J8" s="8">
-        <f>LN(C8)</f>
+        <f t="shared" si="1"/>
         <v>10.899305052792558</v>
       </c>
     </row>
@@ -15504,7 +15504,7 @@
         <v>36735.192125354428</v>
       </c>
       <c r="H9" s="8">
-        <f>LN(G9)</f>
+        <f t="shared" si="0"/>
         <v>10.511490488076211</v>
       </c>
       <c r="I9" s="8">
@@ -15512,7 +15512,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J9" s="8">
-        <f>LN(C9)</f>
+        <f t="shared" si="1"/>
         <v>11.424568504489276</v>
       </c>
     </row>
@@ -15540,7 +15540,7 @@
         <v>25219.502230169608</v>
       </c>
       <c r="H10" s="8">
-        <f>LN(G10)</f>
+        <f t="shared" si="0"/>
         <v>10.135372872217454</v>
       </c>
       <c r="I10" s="8">
@@ -15548,7 +15548,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J10" s="8">
-        <f>LN(C10)</f>
+        <f t="shared" si="1"/>
         <v>11.042541573338868</v>
       </c>
     </row>
@@ -15576,7 +15576,7 @@
         <v>37894.449282783746</v>
       </c>
       <c r="H11" s="8">
-        <f>LN(G11)</f>
+        <f t="shared" si="0"/>
         <v>10.542559923426021</v>
       </c>
       <c r="I11" s="8">
@@ -15584,7 +15584,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J11" s="8">
-        <f>LN(C11)</f>
+        <f t="shared" si="1"/>
         <v>11.784247621980015</v>
       </c>
     </row>
@@ -15612,7 +15612,7 @@
         <v>36075.195438752475</v>
       </c>
       <c r="H12" s="8">
-        <f>LN(G12)</f>
+        <f t="shared" si="0"/>
         <v>10.493360801195033</v>
       </c>
       <c r="I12" s="8">
@@ -15620,7 +15620,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J12" s="8">
-        <f>LN(C12)</f>
+        <f t="shared" si="1"/>
         <v>11.186628731268636</v>
       </c>
     </row>
@@ -15648,7 +15648,7 @@
         <v>22715.91864694142</v>
       </c>
       <c r="H13" s="8">
-        <f>LN(G13)</f>
+        <f t="shared" si="0"/>
         <v>10.030821219680002</v>
       </c>
       <c r="I13" s="8">
@@ -15656,7 +15656,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J13" s="8">
-        <f>LN(C13)</f>
+        <f t="shared" si="1"/>
         <v>10.861775678346413</v>
       </c>
     </row>
@@ -15684,7 +15684,7 @@
         <v>28591.184047535768</v>
       </c>
       <c r="H14" s="8">
-        <f>LN(G14)</f>
+        <f t="shared" si="0"/>
         <v>10.26085369920296</v>
       </c>
       <c r="I14" s="8">
@@ -15692,7 +15692,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J14" s="8">
-        <f>LN(C14)</f>
+        <f t="shared" si="1"/>
         <v>10.751724821165267</v>
       </c>
     </row>
@@ -15720,7 +15720,7 @@
         <v>28005.18938199283</v>
       </c>
       <c r="H15" s="8">
-        <f>LN(G15)</f>
+        <f t="shared" si="0"/>
         <v>10.24014510705609</v>
       </c>
       <c r="I15" s="8">
@@ -15728,7 +15728,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J15" s="8">
-        <f>LN(C15)</f>
+        <f t="shared" si="1"/>
         <v>11.133647719106873</v>
       </c>
     </row>
@@ -15756,7 +15756,7 @@
         <v>24076.707312769591</v>
       </c>
       <c r="H16" s="8">
-        <f>LN(G16)</f>
+        <f t="shared" si="0"/>
         <v>10.089000150570135</v>
       </c>
       <c r="I16" s="8">
@@ -15764,7 +15764,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J16" s="8">
-        <f>LN(C16)</f>
+        <f t="shared" si="1"/>
         <v>10.58021186207427</v>
       </c>
     </row>
@@ -15792,7 +15792,7 @@
         <v>21469.650112295898</v>
       </c>
       <c r="H17" s="8">
-        <f>LN(G17)</f>
+        <f t="shared" si="0"/>
         <v>9.9743955941539113</v>
       </c>
       <c r="I17" s="8">
@@ -15800,7 +15800,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J17" s="8">
-        <f>LN(C17)</f>
+        <f t="shared" si="1"/>
         <v>10.675757618537041</v>
       </c>
     </row>
@@ -15828,7 +15828,7 @@
         <v>28893.901446860826</v>
       </c>
       <c r="H18" s="8">
-        <f>LN(G18)</f>
+        <f t="shared" si="0"/>
         <v>10.27138582923215</v>
       </c>
       <c r="I18" s="8">
@@ -15836,7 +15836,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J18" s="8">
-        <f>LN(C18)</f>
+        <f t="shared" si="1"/>
         <v>11.208816407253209</v>
       </c>
     </row>
@@ -15864,7 +15864,7 @@
         <v>28425.701498510003</v>
       </c>
       <c r="H19" s="8">
-        <f>LN(G19)</f>
+        <f t="shared" si="0"/>
         <v>10.25504899724157</v>
       </c>
       <c r="I19" s="8">
@@ -15872,7 +15872,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J19" s="8">
-        <f>LN(C19)</f>
+        <f t="shared" si="1"/>
         <v>10.681154582882046</v>
       </c>
     </row>
@@ -15900,7 +15900,7 @@
         <v>35225.061560690148</v>
       </c>
       <c r="H20" s="8">
-        <f>LN(G20)</f>
+        <f t="shared" si="0"/>
         <v>10.469513084407374</v>
       </c>
       <c r="I20" s="8">
@@ -15908,7 +15908,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J20" s="8">
-        <f>LN(C20)</f>
+        <f t="shared" si="1"/>
         <v>11.34499233708158</v>
       </c>
     </row>
@@ -15936,7 +15936,7 @@
         <v>23769.104741285177</v>
       </c>
       <c r="H21" s="8">
-        <f>LN(G21)</f>
+        <f t="shared" si="0"/>
         <v>10.076141896257711</v>
       </c>
       <c r="I21" s="8">
@@ -15944,7 +15944,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J21" s="8">
-        <f>LN(C21)</f>
+        <f t="shared" si="1"/>
         <v>10.366038545019112</v>
       </c>
     </row>
@@ -15972,7 +15972,7 @@
         <v>20068.64706722321</v>
       </c>
       <c r="H22" s="8">
-        <f>LN(G22)</f>
+        <f t="shared" si="0"/>
         <v>9.9069140288167965</v>
       </c>
       <c r="I22" s="8">
@@ -15980,7 +15980,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J22" s="8">
-        <f>LN(C22)</f>
+        <f t="shared" si="1"/>
         <v>11.033236645950517</v>
       </c>
     </row>
@@ -16008,7 +16008,7 @@
         <v>35798.347341622932</v>
       </c>
       <c r="H23" s="8">
-        <f>LN(G23)</f>
+        <f t="shared" si="0"/>
         <v>10.4856570076814</v>
       </c>
       <c r="I23" s="8">
@@ -16016,7 +16016,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J23" s="8">
-        <f>LN(C23)</f>
+        <f t="shared" si="1"/>
         <v>11.124253569929543</v>
       </c>
     </row>
@@ -16044,7 +16044,7 @@
         <v>46846.950603594269</v>
       </c>
       <c r="H24" s="8">
-        <f>LN(G24)</f>
+        <f t="shared" si="0"/>
         <v>10.754641197044362</v>
       </c>
       <c r="I24" s="8">
@@ -16052,7 +16052,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J24" s="8">
-        <f>LN(C24)</f>
+        <f t="shared" si="1"/>
         <v>11.695443543333054</v>
       </c>
     </row>
@@ -16080,7 +16080,7 @@
         <v>19496.747283112865</v>
       </c>
       <c r="H25" s="8">
-        <f>LN(G25)</f>
+        <f t="shared" si="0"/>
         <v>9.8780029246439582</v>
       </c>
       <c r="I25" s="8">
@@ -16088,7 +16088,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J25" s="8">
-        <f>LN(C25)</f>
+        <f t="shared" si="1"/>
         <v>10.23249671840507</v>
       </c>
     </row>
@@ -16116,7 +16116,7 @@
         <v>50238.080062177505</v>
       </c>
       <c r="H26" s="8">
-        <f>LN(G26)</f>
+        <f t="shared" si="0"/>
         <v>10.824528585088956</v>
       </c>
       <c r="I26" s="8">
@@ -16124,7 +16124,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J26" s="8">
-        <f>LN(C26)</f>
+        <f t="shared" si="1"/>
         <v>11.842557927322733</v>
       </c>
     </row>
@@ -16152,7 +16152,7 @@
         <v>24183.227088594656</v>
       </c>
       <c r="H27" s="8">
-        <f>LN(G27)</f>
+        <f t="shared" si="0"/>
         <v>10.093414576330424</v>
       </c>
       <c r="I27" s="8">
@@ -16160,7 +16160,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J27" s="8">
-        <f>LN(C27)</f>
+        <f t="shared" si="1"/>
         <v>9.6394365405359217</v>
       </c>
     </row>
@@ -16188,7 +16188,7 @@
         <v>21417.158705556936</v>
       </c>
       <c r="H28" s="8">
-        <f>LN(G28)</f>
+        <f t="shared" si="0"/>
         <v>9.9719476884039793</v>
       </c>
       <c r="I28" s="8">
@@ -16196,7 +16196,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J28" s="8">
-        <f>LN(C28)</f>
+        <f t="shared" si="1"/>
         <v>10.822013139346193</v>
       </c>
     </row>
@@ -16224,7 +16224,7 @@
         <v>31104.216173608947</v>
       </c>
       <c r="H29" s="8">
-        <f>LN(G29)</f>
+        <f t="shared" si="0"/>
         <v>10.345098657262023</v>
       </c>
       <c r="I29" s="8">
@@ -16232,7 +16232,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J29" s="8">
-        <f>LN(C29)</f>
+        <f t="shared" si="1"/>
         <v>11.411708267576127</v>
       </c>
     </row>
@@ -16260,7 +16260,7 @@
         <v>26489.692790960624</v>
       </c>
       <c r="H30" s="8">
-        <f>LN(G30)</f>
+        <f t="shared" si="0"/>
         <v>10.184510985028638</v>
       </c>
       <c r="I30" s="8">
@@ -16268,7 +16268,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J30" s="8">
-        <f>LN(C30)</f>
+        <f t="shared" si="1"/>
         <v>10.670062201650889</v>
       </c>
     </row>
@@ -16296,7 +16296,7 @@
         <v>22188.154718559199</v>
       </c>
       <c r="H31" s="8">
-        <f>LN(G31)</f>
+        <f t="shared" si="0"/>
         <v>10.007313854224511</v>
       </c>
       <c r="I31" s="8">
@@ -16304,7 +16304,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J31" s="8">
-        <f>LN(C31)</f>
+        <f t="shared" si="1"/>
         <v>10.594327926998156</v>
       </c>
     </row>
@@ -16332,7 +16332,7 @@
         <v>26852.74541380454</v>
       </c>
       <c r="H32" s="8">
-        <f>LN(G32)</f>
+        <f t="shared" si="0"/>
         <v>10.198123344758416</v>
       </c>
       <c r="I32" s="8">
@@ -16340,7 +16340,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J32" s="8">
-        <f>LN(C32)</f>
+        <f t="shared" si="1"/>
         <v>10.979299540216626</v>
       </c>
     </row>
@@ -16368,7 +16368,7 @@
         <v>25593.444046410092</v>
       </c>
       <c r="H33" s="8">
-        <f>LN(G33)</f>
+        <f t="shared" si="0"/>
         <v>10.150091505733409</v>
       </c>
       <c r="I33" s="8">
@@ -16376,7 +16376,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J33" s="8">
-        <f>LN(C33)</f>
+        <f t="shared" si="1"/>
         <v>11.098514046113948</v>
       </c>
     </row>
@@ -16404,7 +16404,7 @@
         <v>25495.656998544615</v>
       </c>
       <c r="H34" s="8">
-        <f>LN(G34)</f>
+        <f t="shared" ref="H34:H65" si="2">LN(G34)</f>
         <v>10.146263402858914</v>
       </c>
       <c r="I34" s="8">
@@ -16412,7 +16412,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J34" s="8">
-        <f>LN(C34)</f>
+        <f t="shared" ref="J34:J65" si="3">LN(C34)</f>
         <v>10.841627945143156</v>
       </c>
     </row>
@@ -16440,7 +16440,7 @@
         <v>39929.153202477828</v>
       </c>
       <c r="H35" s="8">
-        <f>LN(G35)</f>
+        <f t="shared" si="2"/>
         <v>10.594861992782002</v>
       </c>
       <c r="I35" s="8">
@@ -16448,7 +16448,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J35" s="8">
-        <f>LN(C35)</f>
+        <f t="shared" si="3"/>
         <v>11.018699198148646</v>
       </c>
     </row>
@@ -16476,7 +16476,7 @@
         <v>36420.264743786283</v>
       </c>
       <c r="H36" s="8">
-        <f>LN(G36)</f>
+        <f t="shared" si="2"/>
         <v>10.502880622442062</v>
       </c>
       <c r="I36" s="8">
@@ -16484,7 +16484,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J36" s="8">
-        <f>LN(C36)</f>
+        <f t="shared" si="3"/>
         <v>11.371926832804741</v>
       </c>
     </row>
@@ -16512,7 +16512,7 @@
         <v>35836.332789086635</v>
       </c>
       <c r="H37" s="8">
-        <f>LN(G37)</f>
+        <f t="shared" si="2"/>
         <v>10.486717540120567</v>
       </c>
       <c r="I37" s="8">
@@ -16520,7 +16520,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J37" s="8">
-        <f>LN(C37)</f>
+        <f t="shared" si="3"/>
         <v>11.415758724112797</v>
       </c>
     </row>
@@ -16548,7 +16548,7 @@
         <v>34816.365618341588</v>
       </c>
       <c r="H38" s="8">
-        <f>LN(G38)</f>
+        <f t="shared" si="2"/>
         <v>10.457842831606408</v>
       </c>
       <c r="I38" s="8">
@@ -16556,7 +16556,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J38" s="8">
-        <f>LN(C38)</f>
+        <f t="shared" si="3"/>
         <v>10.969093544736067</v>
       </c>
     </row>
@@ -16584,7 +16584,7 @@
         <v>56822.087243243906</v>
       </c>
       <c r="H39" s="8">
-        <f>LN(G39)</f>
+        <f t="shared" si="2"/>
         <v>10.947680389039085</v>
       </c>
       <c r="I39" s="8">
@@ -16592,7 +16592,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J39" s="8">
-        <f>LN(C39)</f>
+        <f t="shared" si="3"/>
         <v>11.519152514143558</v>
       </c>
     </row>
@@ -16620,7 +16620,7 @@
         <v>79566.128920131596</v>
       </c>
       <c r="H40" s="8">
-        <f>LN(G40)</f>
+        <f t="shared" si="2"/>
         <v>11.284343765196068</v>
       </c>
       <c r="I40" s="8">
@@ -16628,7 +16628,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J40" s="8">
-        <f>LN(C40)</f>
+        <f t="shared" si="3"/>
         <v>11.807663750113845</v>
       </c>
     </row>
@@ -16656,7 +16656,7 @@
         <v>41107.127198575428</v>
       </c>
       <c r="H41" s="8">
-        <f>LN(G41)</f>
+        <f t="shared" si="2"/>
         <v>10.623936796607902</v>
       </c>
       <c r="I41" s="8">
@@ -16664,7 +16664,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J41" s="8">
-        <f>LN(C41)</f>
+        <f t="shared" si="3"/>
         <v>11.413866423563936</v>
       </c>
     </row>
@@ -16692,7 +16692,7 @@
         <v>45272.22336589529</v>
       </c>
       <c r="H42" s="8">
-        <f>LN(G42)</f>
+        <f t="shared" si="2"/>
         <v>10.720448952674284</v>
       </c>
       <c r="I42" s="8">
@@ -16700,7 +16700,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J42" s="8">
-        <f>LN(C42)</f>
+        <f t="shared" si="3"/>
         <v>11.490262864324347</v>
       </c>
     </row>
@@ -16728,7 +16728,7 @@
         <v>34937.524265830849</v>
       </c>
       <c r="H43" s="8">
-        <f>LN(G43)</f>
+        <f t="shared" si="2"/>
         <v>10.461316724446935</v>
       </c>
       <c r="I43" s="8">
@@ -16736,7 +16736,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J43" s="8">
-        <f>LN(C43)</f>
+        <f t="shared" si="3"/>
         <v>11.153539002752964</v>
       </c>
     </row>
@@ -16764,7 +16764,7 @@
         <v>30994.727023960724</v>
       </c>
       <c r="H44" s="8">
-        <f>LN(G44)</f>
+        <f t="shared" si="2"/>
         <v>10.341572372998051</v>
       </c>
       <c r="I44" s="8">
@@ -16772,7 +16772,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J44" s="8">
-        <f>LN(C44)</f>
+        <f t="shared" si="3"/>
         <v>11.162100201356512</v>
       </c>
     </row>
@@ -16800,7 +16800,7 @@
         <v>28558.967006281608</v>
       </c>
       <c r="H45" s="8">
-        <f>LN(G45)</f>
+        <f t="shared" si="2"/>
         <v>10.259726246551555</v>
       </c>
       <c r="I45" s="8">
@@ -16808,7 +16808,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J45" s="8">
-        <f>LN(C45)</f>
+        <f t="shared" si="3"/>
         <v>11.142419041883034</v>
       </c>
     </row>
@@ -16836,7 +16836,7 @@
         <v>29392.546054372368</v>
       </c>
       <c r="H46" s="8">
-        <f>LN(G46)</f>
+        <f t="shared" si="2"/>
         <v>10.288496385615632</v>
       </c>
       <c r="I46" s="8">
@@ -16844,7 +16844,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J46" s="8">
-        <f>LN(C46)</f>
+        <f t="shared" si="3"/>
         <v>11.180002812268926</v>
       </c>
     </row>
@@ -16872,7 +16872,7 @@
         <v>32130.420204227077</v>
       </c>
       <c r="H47" s="8">
-        <f>LN(G47)</f>
+        <f t="shared" si="2"/>
         <v>10.377558530276083</v>
       </c>
       <c r="I47" s="8">
@@ -16880,7 +16880,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J47" s="8">
-        <f>LN(C47)</f>
+        <f t="shared" si="3"/>
         <v>11.638039210746214</v>
       </c>
     </row>
@@ -16908,7 +16908,7 @@
         <v>300588.37309242727</v>
       </c>
       <c r="H48" s="8">
-        <f>LN(G48)</f>
+        <f t="shared" si="2"/>
         <v>12.613497076552385</v>
       </c>
       <c r="I48" s="8">
@@ -16916,7 +16916,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J48" s="8">
-        <f>LN(C48)</f>
+        <f t="shared" si="3"/>
         <v>11.708176264754101</v>
       </c>
     </row>
@@ -16944,7 +16944,7 @@
         <v>72965.182927549846</v>
       </c>
       <c r="H49" s="8">
-        <f>LN(G49)</f>
+        <f t="shared" si="2"/>
         <v>11.197737660157566</v>
       </c>
       <c r="I49" s="8">
@@ -16952,7 +16952,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J49" s="8">
-        <f>LN(C49)</f>
+        <f t="shared" si="3"/>
         <v>11.732529637036537</v>
       </c>
     </row>
@@ -16980,7 +16980,7 @@
         <v>89190.500021186512</v>
       </c>
       <c r="H50" s="8">
-        <f>LN(G50)</f>
+        <f t="shared" si="2"/>
         <v>11.398529810891723</v>
       </c>
       <c r="I50" s="8">
@@ -16988,7 +16988,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J50" s="8">
-        <f>LN(C50)</f>
+        <f t="shared" si="3"/>
         <v>11.58016267475325</v>
       </c>
     </row>
@@ -17016,7 +17016,7 @@
         <v>22808.426731448846</v>
       </c>
       <c r="H51" s="8">
-        <f>LN(G51)</f>
+        <f t="shared" si="2"/>
         <v>10.034885340144283</v>
       </c>
       <c r="I51" s="8">
@@ -17024,7 +17024,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J51" s="8">
-        <f>LN(C51)</f>
+        <f t="shared" si="3"/>
         <v>10.620335965381761</v>
       </c>
     </row>
@@ -17052,7 +17052,7 @@
         <v>59055.859830313871</v>
       </c>
       <c r="H52" s="8">
-        <f>LN(G52)</f>
+        <f t="shared" si="2"/>
         <v>10.986239051762389</v>
       </c>
       <c r="I52" s="8">
@@ -17060,7 +17060,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J52" s="8">
-        <f>LN(C52)</f>
+        <f t="shared" si="3"/>
         <v>11.908914510372936</v>
       </c>
     </row>
@@ -17088,7 +17088,7 @@
         <v>22529.030770653291</v>
       </c>
       <c r="H53" s="8">
-        <f>LN(G53)</f>
+        <f t="shared" si="2"/>
         <v>10.022560013000405</v>
       </c>
       <c r="I53" s="8">
@@ -17096,7 +17096,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J53" s="8">
-        <f>LN(C53)</f>
+        <f t="shared" si="3"/>
         <v>10.414346027273687</v>
       </c>
     </row>
@@ -17124,7 +17124,7 @@
         <v>35675.586686472605</v>
       </c>
       <c r="H54" s="8">
-        <f>LN(G54)</f>
+        <f t="shared" si="2"/>
         <v>10.48222188752089</v>
       </c>
       <c r="I54" s="8">
@@ -17132,7 +17132,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J54" s="8">
-        <f>LN(C54)</f>
+        <f t="shared" si="3"/>
         <v>11.220549196407191</v>
       </c>
     </row>
@@ -17160,7 +17160,7 @@
         <v>39646.399143461444</v>
       </c>
       <c r="H55" s="8">
-        <f>LN(G55)</f>
+        <f t="shared" si="2"/>
         <v>10.58775540688503</v>
       </c>
       <c r="I55" s="8">
@@ -17168,7 +17168,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J55" s="8">
-        <f>LN(C55)</f>
+        <f t="shared" si="3"/>
         <v>11.581720451532894</v>
       </c>
     </row>
@@ -17196,7 +17196,7 @@
         <v>26672.301145177298</v>
       </c>
       <c r="H56" s="8">
-        <f>LN(G56)</f>
+        <f t="shared" si="2"/>
         <v>10.191380895612847</v>
       </c>
       <c r="I56" s="8">
@@ -17204,7 +17204,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J56" s="8">
-        <f>LN(C56)</f>
+        <f t="shared" si="3"/>
         <v>10.228948319331135</v>
       </c>
     </row>
@@ -17232,7 +17232,7 @@
         <v>40035.098278045916</v>
       </c>
       <c r="H57" s="8">
-        <f>LN(G57)</f>
+        <f t="shared" si="2"/>
         <v>10.597511805306917</v>
       </c>
       <c r="I57" s="8">
@@ -17240,7 +17240,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J57" s="8">
-        <f>LN(C57)</f>
+        <f t="shared" si="3"/>
         <v>11.15551198746229</v>
       </c>
     </row>
@@ -17268,7 +17268,7 @@
         <v>32488.229724070618</v>
       </c>
       <c r="H58" s="8">
-        <f>LN(G58)</f>
+        <f t="shared" si="2"/>
         <v>10.388633140384924</v>
       </c>
       <c r="I58" s="8">
@@ -17276,7 +17276,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J58" s="8">
-        <f>LN(C58)</f>
+        <f t="shared" si="3"/>
         <v>11.355960565133584</v>
       </c>
     </row>
@@ -17304,7 +17304,7 @@
         <v>28270.630949512713</v>
       </c>
       <c r="H59" s="8">
-        <f>LN(G59)</f>
+        <f t="shared" si="2"/>
         <v>10.249578769133757</v>
       </c>
       <c r="I59" s="8">
@@ -17312,7 +17312,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J59" s="8">
-        <f>LN(C59)</f>
+        <f t="shared" si="3"/>
         <v>10.910628437707077</v>
       </c>
     </row>
@@ -17340,7 +17340,7 @@
         <v>15975.675396810533</v>
       </c>
       <c r="H60" s="8">
-        <f>LN(G60)</f>
+        <f t="shared" si="2"/>
         <v>9.6788225567126283</v>
       </c>
       <c r="I60" s="8">
@@ -17348,7 +17348,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J60" s="8">
-        <f>LN(C60)</f>
+        <f t="shared" si="3"/>
         <v>9.9584033101322422</v>
       </c>
     </row>
@@ -17376,7 +17376,7 @@
         <v>28989.071852351441</v>
       </c>
       <c r="H61" s="8">
-        <f>LN(G61)</f>
+        <f t="shared" si="2"/>
         <v>10.274674205271799</v>
       </c>
       <c r="I61" s="8">
@@ -17384,7 +17384,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J61" s="8">
-        <f>LN(C61)</f>
+        <f t="shared" si="3"/>
         <v>10.961119550511514</v>
       </c>
     </row>
@@ -17412,7 +17412,7 @@
         <v>22032.401491644319</v>
       </c>
       <c r="H62" s="8">
-        <f>LN(G62)</f>
+        <f t="shared" si="2"/>
         <v>10.000269443916245</v>
       </c>
       <c r="I62" s="8">
@@ -17420,7 +17420,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J62" s="8">
-        <f>LN(C62)</f>
+        <f t="shared" si="3"/>
         <v>10.815933974053493</v>
       </c>
     </row>
@@ -17448,7 +17448,7 @@
         <v>19890.128188207571</v>
       </c>
       <c r="H63" s="8">
-        <f>LN(G63)</f>
+        <f t="shared" si="2"/>
         <v>9.8979788166843417</v>
       </c>
       <c r="I63" s="8">
@@ -17456,7 +17456,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J63" s="8">
-        <f>LN(C63)</f>
+        <f t="shared" si="3"/>
         <v>10.690488179953238</v>
       </c>
     </row>
@@ -17484,7 +17484,7 @@
         <v>22587.157447590638</v>
       </c>
       <c r="H64" s="8">
-        <f>LN(G64)</f>
+        <f t="shared" si="2"/>
         <v>10.025136769211192</v>
       </c>
       <c r="I64" s="8">
@@ -17492,7 +17492,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J64" s="8">
-        <f>LN(C64)</f>
+        <f t="shared" si="3"/>
         <v>10.457781820152896</v>
       </c>
     </row>
@@ -17520,7 +17520,7 @@
         <v>20444.684613386424</v>
       </c>
       <c r="H65" s="8">
-        <f>LN(G65)</f>
+        <f t="shared" si="2"/>
         <v>9.925478206579804</v>
       </c>
       <c r="I65" s="8">
@@ -17528,7 +17528,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J65" s="8">
-        <f>LN(C65)</f>
+        <f t="shared" si="3"/>
         <v>10.645659832072177</v>
       </c>
     </row>
@@ -17556,7 +17556,7 @@
         <v>21576.111253465962</v>
       </c>
       <c r="H66" s="8">
-        <f>LN(G66)</f>
+        <f t="shared" ref="H66:H97" si="4">LN(G66)</f>
         <v>9.9793420211589776</v>
       </c>
       <c r="I66" s="8">
@@ -17564,7 +17564,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J66" s="8">
-        <f>LN(C66)</f>
+        <f t="shared" ref="J66:J78" si="5">LN(C66)</f>
         <v>10.587832789144938</v>
       </c>
     </row>
@@ -17592,7 +17592,7 @@
         <v>333065.25063794554</v>
       </c>
       <c r="H67" s="8">
-        <f>LN(G67)</f>
+        <f t="shared" si="4"/>
         <v>12.716093697629004</v>
       </c>
       <c r="I67" s="8">
@@ -17600,7 +17600,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J67" s="8">
-        <f>LN(C67)</f>
+        <f t="shared" si="5"/>
         <v>11.696701114251381</v>
       </c>
     </row>
@@ -17628,7 +17628,7 @@
         <v>37159.338945202151</v>
       </c>
       <c r="H68" s="8">
-        <f>LN(G68)</f>
+        <f t="shared" si="4"/>
         <v>10.52297040335087</v>
       </c>
       <c r="I68" s="8">
@@ -17636,7 +17636,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J68" s="8">
-        <f>LN(C68)</f>
+        <f t="shared" si="5"/>
         <v>11.110519326029364</v>
       </c>
     </row>
@@ -17664,7 +17664,7 @@
         <v>24033.198874881611</v>
       </c>
       <c r="H69" s="8">
-        <f>LN(G69)</f>
+        <f t="shared" si="4"/>
         <v>10.08719143992416</v>
       </c>
       <c r="I69" s="8">
@@ -17672,7 +17672,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J69" s="8">
-        <f>LN(C69)</f>
+        <f t="shared" si="5"/>
         <v>11.109411576993326</v>
       </c>
     </row>
@@ -17700,7 +17700,7 @@
         <v>21884.61384983642</v>
       </c>
       <c r="H70" s="8">
-        <f>LN(G70)</f>
+        <f t="shared" si="4"/>
         <v>9.9935391049564863</v>
       </c>
       <c r="I70" s="8">
@@ -17708,7 +17708,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J70" s="8">
-        <f>LN(C70)</f>
+        <f t="shared" si="5"/>
         <v>10.166385862410166</v>
       </c>
     </row>
@@ -17736,7 +17736,7 @@
         <v>24733.163421129382</v>
       </c>
       <c r="H71" s="8">
-        <f>LN(G71)</f>
+        <f t="shared" si="4"/>
         <v>10.115900270698107</v>
       </c>
       <c r="I71" s="8">
@@ -17744,7 +17744,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J71" s="8">
-        <f>LN(C71)</f>
+        <f t="shared" si="5"/>
         <v>11.073508093961442</v>
       </c>
     </row>
@@ -17772,7 +17772,7 @@
         <v>18823.672719654594</v>
       </c>
       <c r="H72" s="8">
-        <f>LN(G72)</f>
+        <f t="shared" si="4"/>
         <v>9.8428705439223627</v>
       </c>
       <c r="I72" s="8">
@@ -17780,7 +17780,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J72" s="8">
-        <f>LN(C72)</f>
+        <f t="shared" si="5"/>
         <v>10.283077283646394</v>
       </c>
     </row>
@@ -17808,7 +17808,7 @@
         <v>20607.040770706662</v>
       </c>
       <c r="H73" s="8">
-        <f>LN(G73)</f>
+        <f t="shared" si="4"/>
         <v>9.9333880813682498</v>
       </c>
       <c r="I73" s="8">
@@ -17816,7 +17816,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J73" s="8">
-        <f>LN(C73)</f>
+        <f t="shared" si="5"/>
         <v>10.501232637302897</v>
       </c>
     </row>
@@ -17844,7 +17844,7 @@
         <v>24656.424357756732</v>
       </c>
       <c r="H74" s="8">
-        <f>LN(G74)</f>
+        <f t="shared" si="4"/>
         <v>10.112792768547282</v>
       </c>
       <c r="I74" s="8">
@@ -17852,7 +17852,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J74" s="8">
-        <f>LN(C74)</f>
+        <f t="shared" si="5"/>
         <v>11.151188899637063</v>
       </c>
     </row>
@@ -17880,7 +17880,7 @@
         <v>21181.048170526352</v>
       </c>
       <c r="H75" s="8">
-        <f>LN(G75)</f>
+        <f t="shared" si="4"/>
         <v>9.9608621066242797</v>
       </c>
       <c r="I75" s="8">
@@ -17888,7 +17888,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J75" s="8">
-        <f>LN(C75)</f>
+        <f t="shared" si="5"/>
         <v>10.754933202877913</v>
       </c>
     </row>
@@ -17916,7 +17916,7 @@
         <v>28285.913018486506</v>
       </c>
       <c r="H76" s="8">
-        <f>LN(G76)</f>
+        <f t="shared" si="4"/>
         <v>10.250119186502767</v>
       </c>
       <c r="I76" s="8">
@@ -17924,7 +17924,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J76" s="8">
-        <f>LN(C76)</f>
+        <f t="shared" si="5"/>
         <v>11.128605801481278</v>
       </c>
     </row>
@@ -17952,7 +17952,7 @@
         <v>55141.258168912616</v>
       </c>
       <c r="H77" s="8">
-        <f>LN(G77)</f>
+        <f t="shared" si="4"/>
         <v>10.917653502034417</v>
       </c>
       <c r="I77" s="8">
@@ -17960,7 +17960,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J77" s="8">
-        <f>LN(C77)</f>
+        <f t="shared" si="5"/>
         <v>11.765368929029385</v>
       </c>
     </row>
@@ -17988,7 +17988,7 @@
         <v>23467.390959382756</v>
       </c>
       <c r="H78" s="8">
-        <f>LN(G78)</f>
+        <f t="shared" si="4"/>
         <v>10.063367117748141</v>
       </c>
       <c r="I78" s="8">
@@ -17996,7 +17996,7 @@
         <v>14.816845867278564</v>
       </c>
       <c r="J78" s="8">
-        <f>LN(C78)</f>
+        <f t="shared" si="5"/>
         <v>10.307932326760856</v>
       </c>
     </row>
@@ -18014,9 +18014,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -18057,15 +18059,6 @@
       </c>
       <c r="B4" s="2">
         <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <f>FACTORS_MUNI!G1</f>
-        <v>PCT_EDA_POP</v>
-      </c>
-      <c r="B5" s="2">
-        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove duplicate GEOG column
</commit_message>
<xml_diff>
--- a/input/community_cohort_inputs.xlsx
+++ b/input/community_cohort_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amcadams\GitHub\community-cohort-tool\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9572D62-A8EA-4B4E-9819-3D682E7FC63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47715D48-2FEC-4A66-B564-182B09793966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="COHORTS" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FACTORS_CCA!$A$1:$K$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FACTORS_CCA!$A$1:$J$78</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FACTORS_MUNI!$A$1:$L$285</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -335,7 +335,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{8F055FF2-A436-4A9F-8700-C75FCCAE51E3}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{8F055FF2-A436-4A9F-8700-C75FCCAE51E3}">
       <text>
         <r>
           <rPr>
@@ -358,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -381,7 +381,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -426,7 +426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{464A655B-67F8-474B-A0ED-226DC95AAAD8}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{464A655B-67F8-474B-A0ED-226DC95AAAD8}">
       <text>
         <r>
           <rPr>
@@ -506,7 +506,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -548,7 +548,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -571,7 +571,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -633,7 +633,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -752,7 +752,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="380">
   <si>
     <t>GEOID</t>
   </si>
@@ -1892,9 +1892,6 @@
   </si>
   <si>
     <t>TOT_MARKET_VAL</t>
-  </si>
-  <si>
-    <t>GEOG</t>
   </si>
 </sst>
 </file>
@@ -2913,7 +2910,7 @@
   <dimension ref="A1:L285"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14004,11 +14001,11 @@
         <v>12051912</v>
       </c>
       <c r="I258" s="4">
-        <f t="shared" ref="I258:I321" si="21">H258/C258</f>
+        <f t="shared" ref="I258:I285" si="21">H258/C258</f>
         <v>38877.135483870967</v>
       </c>
       <c r="J258" s="8">
-        <f t="shared" ref="J258:J321" si="22">LN(I258)</f>
+        <f t="shared" ref="J258:J285" si="22">LN(I258)</f>
         <v>10.568161580033815</v>
       </c>
       <c r="K258" s="8">
@@ -15195,3068 +15192,2833 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K78"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="17" customWidth="1"/>
-    <col min="8" max="8" width="19" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" style="8"/>
-    <col min="11" max="11" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="17" customWidth="1"/>
+    <col min="7" max="7" width="19" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="8"/>
+    <col min="10" max="10" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>375</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>376</v>
       </c>
-      <c r="C1" t="s">
-        <v>380</v>
-      </c>
-      <c r="D1" s="28" t="s">
+      <c r="C1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="D1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="E1" s="24" t="s">
         <v>379</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="F1" s="30" t="s">
         <v>378</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="H1" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="I1" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="7" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>14</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="C2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D2" s="21">
+      <c r="C2" s="21">
         <v>82249.644043663895</v>
       </c>
-      <c r="E2" s="15">
+      <c r="D2" s="15">
         <v>0.80810397553516822</v>
       </c>
-      <c r="F2">
+      <c r="E2">
         <v>3548280190.2389002</v>
       </c>
-      <c r="G2" s="16">
+      <c r="F2" s="16">
         <v>46620</v>
       </c>
-      <c r="H2" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F2/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G2)</f>
+      <c r="G2" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E2/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F2)</f>
         <v>31409.718328004918</v>
       </c>
+      <c r="H2" s="8">
+        <f t="shared" ref="H2:H33" si="0">LN(G2)</f>
+        <v>10.354872624902701</v>
+      </c>
       <c r="I2" s="8">
-        <f>LN(H2)</f>
-        <v>10.354872624902701</v>
-      </c>
-      <c r="J2" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K2" s="8">
-        <f>LN(D2)</f>
+      <c r="J2" s="8">
+        <f t="shared" ref="J2:J33" si="1">LN(C2)</f>
         <v>11.317514340881644</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>57</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="C3" t="s">
-        <v>300</v>
-      </c>
-      <c r="D3" s="21">
+      <c r="C3" s="21">
         <v>67397.727272727207</v>
       </c>
-      <c r="E3" s="15">
+      <c r="D3" s="15">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="E3">
         <v>994396260.73109198</v>
       </c>
-      <c r="G3" s="16">
+      <c r="F3" s="16">
         <v>14021</v>
       </c>
-      <c r="H3" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F3/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G3)</f>
+      <c r="G3" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E3/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F3)</f>
         <v>30242.247077515967</v>
       </c>
+      <c r="H3" s="8">
+        <f t="shared" si="0"/>
+        <v>10.316995135651672</v>
+      </c>
       <c r="I3" s="8">
-        <f>LN(H3)</f>
-        <v>10.316995135651672</v>
-      </c>
-      <c r="J3" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K3" s="8">
-        <f>LN(D3)</f>
+      <c r="J3" s="8">
+        <f t="shared" si="1"/>
         <v>11.118366576342655</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>34</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>301</v>
       </c>
-      <c r="C4" t="s">
-        <v>301</v>
-      </c>
-      <c r="D4" s="21">
+      <c r="C4" s="21">
         <v>43488.409088993503</v>
       </c>
-      <c r="E4" s="15">
+      <c r="D4" s="15">
         <v>0.9967602591792657</v>
       </c>
-      <c r="F4">
+      <c r="E4">
         <v>1398865114</v>
       </c>
-      <c r="G4" s="16">
+      <c r="F4" s="16">
         <v>14239.409836065501</v>
       </c>
-      <c r="H4" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F4/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G4)</f>
+      <c r="G4" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E4/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F4)</f>
         <v>36388.581210501259</v>
       </c>
+      <c r="H4" s="8">
+        <f t="shared" si="0"/>
+        <v>10.502010301401544</v>
+      </c>
       <c r="I4" s="8">
-        <f>LN(H4)</f>
-        <v>10.502010301401544</v>
-      </c>
-      <c r="J4" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K4" s="8">
-        <f>LN(D4)</f>
+      <c r="J4" s="8">
+        <f t="shared" si="1"/>
         <v>10.680249723846321</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>70</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="C5" t="s">
-        <v>302</v>
-      </c>
-      <c r="D5" s="21">
+      <c r="C5" s="21">
         <v>80909.6858638743</v>
       </c>
-      <c r="E5" s="15">
+      <c r="D5" s="15">
         <v>0.68655409022336855</v>
       </c>
-      <c r="F5">
+      <c r="E5">
         <v>2591607528.0592399</v>
       </c>
-      <c r="G5" s="16">
+      <c r="F5" s="16">
         <v>42079</v>
       </c>
-      <c r="H5" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F5/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G5)</f>
+      <c r="G5" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E5/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F5)</f>
         <v>28142.362588518004</v>
       </c>
+      <c r="H5" s="8">
+        <f t="shared" si="0"/>
+        <v>10.245031285513583</v>
+      </c>
       <c r="I5" s="8">
-        <f>LN(H5)</f>
-        <v>10.245031285513583</v>
-      </c>
-      <c r="J5" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K5" s="8">
-        <f>LN(D5)</f>
+      <c r="J5" s="8">
+        <f t="shared" si="1"/>
         <v>11.301088822256643</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>71</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>303</v>
       </c>
-      <c r="C6" t="s">
-        <v>303</v>
-      </c>
-      <c r="D6" s="21">
+      <c r="C6" s="21">
         <v>45489.510489510401</v>
       </c>
-      <c r="E6" s="15">
+      <c r="D6" s="15">
         <v>0.96742279067694636</v>
       </c>
-      <c r="F6">
+      <c r="E6">
         <v>1852067815</v>
       </c>
-      <c r="G6" s="16">
+      <c r="F6" s="16">
         <v>45049</v>
       </c>
-      <c r="H6" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F6/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G6)</f>
+      <c r="G6" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E6/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F6)</f>
         <v>23535.085994762754</v>
       </c>
+      <c r="H6" s="8">
+        <f t="shared" si="0"/>
+        <v>10.06624760773818</v>
+      </c>
       <c r="I6" s="8">
-        <f>LN(H6)</f>
-        <v>10.06624760773818</v>
-      </c>
-      <c r="J6" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K6" s="8">
-        <f>LN(D6)</f>
+      <c r="J6" s="8">
+        <f t="shared" si="1"/>
         <v>10.725237039668833</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>25</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="C7" t="s">
-        <v>304</v>
-      </c>
-      <c r="D7" s="21">
+      <c r="C7" s="21">
         <v>44883.241758241697</v>
       </c>
-      <c r="E7" s="15">
+      <c r="D7" s="15">
         <v>0.92424163965326178</v>
       </c>
-      <c r="F7">
+      <c r="E7">
         <v>4743250985.9707403</v>
       </c>
-      <c r="G7" s="16">
+      <c r="F7" s="16">
         <v>98882</v>
       </c>
-      <c r="H7" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F7/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G7)</f>
+      <c r="G7" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E7/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F7)</f>
         <v>25077.798592763364</v>
       </c>
+      <c r="H7" s="8">
+        <f t="shared" si="0"/>
+        <v>10.129738215486212</v>
+      </c>
       <c r="I7" s="8">
-        <f>LN(H7)</f>
-        <v>10.129738215486212</v>
-      </c>
-      <c r="J7" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K7" s="8">
-        <f>LN(D7)</f>
+      <c r="J7" s="8">
+        <f t="shared" si="1"/>
         <v>10.711819769277872</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>45</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="C8" t="s">
-        <v>305</v>
-      </c>
-      <c r="D8" s="21">
+      <c r="C8" s="21">
         <v>56018.7492653109</v>
       </c>
-      <c r="E8" s="15">
+      <c r="D8" s="15">
         <v>0.34383590611122861</v>
       </c>
-      <c r="F8">
+      <c r="E8">
         <v>554922436</v>
       </c>
-      <c r="G8" s="16">
+      <c r="F8" s="16">
         <v>9447.3256185155606</v>
       </c>
-      <c r="H8" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F8/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G8)</f>
+      <c r="G8" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E8/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F8)</f>
         <v>27500.995838759416</v>
       </c>
+      <c r="H8" s="8">
+        <f t="shared" si="0"/>
+        <v>10.221977495317537</v>
+      </c>
       <c r="I8" s="8">
-        <f>LN(H8)</f>
-        <v>10.221977495317537</v>
-      </c>
-      <c r="J8" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K8" s="8">
-        <f>LN(D8)</f>
+      <c r="J8" s="8">
+        <f t="shared" si="1"/>
         <v>10.933441721990615</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>21</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>306</v>
       </c>
-      <c r="C9" t="s">
-        <v>306</v>
-      </c>
-      <c r="D9" s="21">
+      <c r="C9" s="21">
         <v>92644.817073170707</v>
       </c>
-      <c r="E9" s="15">
+      <c r="D9" s="15">
         <v>0.70753233858289433</v>
       </c>
-      <c r="F9">
+      <c r="E9">
         <v>3863916690.1880798</v>
       </c>
-      <c r="G9" s="16">
+      <c r="F9" s="16">
         <v>35489</v>
       </c>
-      <c r="H9" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F9/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G9)</f>
+      <c r="G9" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E9/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F9)</f>
         <v>38782.012296273424</v>
       </c>
+      <c r="H9" s="8">
+        <f t="shared" si="0"/>
+        <v>10.565711817503868</v>
+      </c>
       <c r="I9" s="8">
-        <f>LN(H9)</f>
-        <v>10.565711817503868</v>
-      </c>
-      <c r="J9" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K9" s="8">
-        <f>LN(D9)</f>
+      <c r="J9" s="8">
+        <f t="shared" si="1"/>
         <v>11.436528289222371</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>19</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="C10" t="s">
-        <v>307</v>
-      </c>
-      <c r="D10" s="21">
+      <c r="C10" s="21">
         <v>67004.008016032007</v>
       </c>
-      <c r="E10" s="15">
+      <c r="D10" s="15">
         <v>0.94340468021916124</v>
       </c>
-      <c r="F10">
+      <c r="E10">
         <v>3965235780.5862598</v>
       </c>
-      <c r="G10" s="16">
+      <c r="F10" s="16">
         <v>72918</v>
       </c>
-      <c r="H10" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F10/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G10)</f>
+      <c r="G10" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E10/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F10)</f>
         <v>26520.178310414311</v>
       </c>
+      <c r="H10" s="8">
+        <f t="shared" si="0"/>
+        <v>10.185661167897644</v>
+      </c>
       <c r="I10" s="8">
-        <f>LN(H10)</f>
-        <v>10.185661167897644</v>
-      </c>
-      <c r="J10" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K10" s="8">
-        <f>LN(D10)</f>
+      <c r="J10" s="8">
+        <f t="shared" si="1"/>
         <v>11.112507717718696</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>72</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="C11" t="s">
-        <v>308</v>
-      </c>
-      <c r="D11" s="21">
+      <c r="C11" s="21">
         <v>127056.18892508101</v>
       </c>
-      <c r="E11" s="15">
+      <c r="D11" s="15">
         <v>5.192989464223299E-3</v>
       </c>
-      <c r="F11">
+      <c r="E11">
         <v>2206100566</v>
       </c>
-      <c r="G11" s="16">
+      <c r="F11" s="16">
         <v>19570</v>
       </c>
-      <c r="H11" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F11/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G11)</f>
+      <c r="G11" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E11/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F11)</f>
         <v>39648.764614042069</v>
       </c>
+      <c r="H11" s="8">
+        <f t="shared" si="0"/>
+        <v>10.58781506930249</v>
+      </c>
       <c r="I11" s="8">
-        <f>LN(H11)</f>
-        <v>10.58781506930249</v>
-      </c>
-      <c r="J11" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K11" s="8">
-        <f>LN(D11)</f>
+      <c r="J11" s="8">
+        <f t="shared" si="1"/>
         <v>11.75238470007729</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>60</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>309</v>
       </c>
-      <c r="C12" t="s">
-        <v>309</v>
-      </c>
-      <c r="D12" s="21">
+      <c r="C12" s="21">
         <v>73225.565411586897</v>
       </c>
-      <c r="E12" s="15">
+      <c r="D12" s="15">
         <v>0.78081419500326388</v>
       </c>
-      <c r="F12">
+      <c r="E12">
         <v>3425149601.8145499</v>
       </c>
-      <c r="G12" s="16">
+      <c r="F12" s="16">
         <v>33090.590163934401</v>
       </c>
-      <c r="H12" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F12/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G12)</f>
+      <c r="G12" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E12/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F12)</f>
         <v>37574.169434156749</v>
       </c>
+      <c r="H12" s="8">
+        <f t="shared" si="0"/>
+        <v>10.534072110162814</v>
+      </c>
       <c r="I12" s="8">
-        <f>LN(H12)</f>
-        <v>10.534072110162814</v>
-      </c>
-      <c r="J12" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K12" s="8">
-        <f>LN(D12)</f>
+      <c r="J12" s="8">
+        <f t="shared" si="1"/>
         <v>11.201299893230983</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>58</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="C13" t="s">
-        <v>310</v>
-      </c>
-      <c r="D13" s="21">
+      <c r="C13" s="21">
         <v>58095.813204508799</v>
       </c>
-      <c r="E13" s="15">
+      <c r="D13" s="15">
         <v>1</v>
       </c>
-      <c r="F13">
+      <c r="E13">
         <v>1780426102.36166</v>
       </c>
-      <c r="G13" s="16">
+      <c r="F13" s="16">
         <v>42062</v>
       </c>
-      <c r="H13" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F13/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G13)</f>
+      <c r="G13" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E13/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F13)</f>
         <v>23808.757071808206</v>
       </c>
+      <c r="H13" s="8">
+        <f t="shared" si="0"/>
+        <v>10.077808736178323</v>
+      </c>
       <c r="I13" s="8">
-        <f>LN(H13)</f>
-        <v>10.077808736178323</v>
-      </c>
-      <c r="J13" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K13" s="8">
-        <f>LN(D13)</f>
+      <c r="J13" s="8">
+        <f t="shared" si="1"/>
         <v>10.96984887835889</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>47</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>311</v>
       </c>
-      <c r="C14" t="s">
-        <v>311</v>
-      </c>
-      <c r="D14" s="21">
+      <c r="C14" s="21">
         <v>48227.848101265801</v>
       </c>
-      <c r="E14" s="15">
+      <c r="D14" s="15">
         <v>1</v>
       </c>
-      <c r="F14">
+      <c r="E14">
         <v>154979128</v>
       </c>
-      <c r="G14" s="16">
+      <c r="F14" s="16">
         <v>2148</v>
       </c>
-      <c r="H14" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F14/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G14)</f>
+      <c r="G14" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E14/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F14)</f>
         <v>30518.661763710654</v>
       </c>
+      <c r="H14" s="8">
+        <f t="shared" si="0"/>
+        <v>10.326093636590084</v>
+      </c>
       <c r="I14" s="8">
-        <f>LN(H14)</f>
-        <v>10.326093636590084</v>
-      </c>
-      <c r="J14" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K14" s="8">
-        <f>LN(D14)</f>
+      <c r="J14" s="8">
+        <f t="shared" si="1"/>
         <v>10.783691894635862</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>48</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="C15" t="s">
-        <v>312</v>
-      </c>
-      <c r="D15" s="21">
+      <c r="C15" s="21">
         <v>68354.922279792707</v>
       </c>
-      <c r="E15" s="15">
+      <c r="D15" s="15">
         <v>0.31242359413202936</v>
       </c>
-      <c r="F15">
+      <c r="E15">
         <v>801655546</v>
       </c>
-      <c r="G15" s="16">
+      <c r="F15" s="16">
         <v>11645</v>
       </c>
-      <c r="H15" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F15/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G15)</f>
+      <c r="G15" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E15/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F15)</f>
         <v>29774.08067147473</v>
       </c>
+      <c r="H15" s="8">
+        <f t="shared" si="0"/>
+        <v>10.301393517893759</v>
+      </c>
       <c r="I15" s="8">
-        <f>LN(H15)</f>
-        <v>10.301393517893759</v>
-      </c>
-      <c r="J15" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K15" s="8">
-        <f>LN(D15)</f>
+      <c r="J15" s="8">
+        <f t="shared" si="1"/>
         <v>11.132468855357073</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>44</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="C16" t="s">
-        <v>313</v>
-      </c>
-      <c r="D16" s="21">
+      <c r="C16" s="21">
         <v>42086.313106280497</v>
       </c>
-      <c r="E16" s="15">
+      <c r="D16" s="15">
         <v>0.69205298013245031</v>
       </c>
-      <c r="F16">
+      <c r="E16">
         <v>1517860263.90818</v>
       </c>
-      <c r="G16" s="16">
+      <c r="F16" s="16">
         <v>30782.674381484401</v>
       </c>
-      <c r="H16" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F16/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G16)</f>
+      <c r="G16" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E16/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F16)</f>
         <v>25379.323942000032</v>
       </c>
+      <c r="H16" s="8">
+        <f t="shared" si="0"/>
+        <v>10.141690103482549</v>
+      </c>
       <c r="I16" s="8">
-        <f>LN(H16)</f>
-        <v>10.141690103482549</v>
-      </c>
-      <c r="J16" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K16" s="8">
-        <f>LN(D16)</f>
+      <c r="J16" s="8">
+        <f t="shared" si="1"/>
         <v>10.647477862448708</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>66</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="C17" t="s">
-        <v>314</v>
-      </c>
-      <c r="D17" s="21">
+      <c r="C17" s="21">
         <v>48783.255086071898</v>
       </c>
-      <c r="E17" s="15">
+      <c r="D17" s="15">
         <v>1</v>
       </c>
-      <c r="F17">
+      <c r="E17">
         <v>1912350686</v>
       </c>
-      <c r="G17" s="16">
+      <c r="F17" s="16">
         <v>53460</v>
       </c>
-      <c r="H17" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F17/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G17)</f>
+      <c r="G17" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E17/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F17)</f>
         <v>22333.434269431677</v>
       </c>
+      <c r="H17" s="8">
+        <f t="shared" si="0"/>
+        <v>10.013840129221572</v>
+      </c>
       <c r="I17" s="8">
-        <f>LN(H17)</f>
-        <v>10.013840129221572</v>
-      </c>
-      <c r="J17" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K17" s="8">
-        <f>LN(D17)</f>
+      <c r="J17" s="8">
+        <f t="shared" si="1"/>
         <v>10.795142399475342</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>64</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>315</v>
       </c>
-      <c r="C18" t="s">
-        <v>315</v>
-      </c>
-      <c r="D18" s="21">
+      <c r="C18" s="21">
         <v>78378.3783783783</v>
       </c>
-      <c r="E18" s="15">
+      <c r="D18" s="15">
         <v>0.29334368487721163</v>
       </c>
-      <c r="F18">
+      <c r="E18">
         <v>1740504096.6638999</v>
       </c>
-      <c r="G18" s="16">
+      <c r="F18" s="16">
         <v>24924</v>
       </c>
-      <c r="H18" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F18/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G18)</f>
+      <c r="G18" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E18/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F18)</f>
         <v>29997.117189969555</v>
       </c>
+      <c r="H18" s="8">
+        <f t="shared" si="0"/>
+        <v>10.308856562359319</v>
+      </c>
       <c r="I18" s="8">
-        <f>LN(H18)</f>
-        <v>10.308856562359319</v>
-      </c>
-      <c r="J18" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K18" s="8">
-        <f>LN(D18)</f>
+      <c r="J18" s="8">
+        <f t="shared" si="1"/>
         <v>11.269303382312478</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>35</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>316</v>
       </c>
-      <c r="C19" t="s">
-        <v>316</v>
-      </c>
-      <c r="D19" s="21">
+      <c r="C19" s="21">
         <v>47426.253687315599</v>
       </c>
-      <c r="E19" s="15">
+      <c r="D19" s="15">
         <v>0.58316494997782264</v>
       </c>
-      <c r="F19">
+      <c r="E19">
         <v>1457390874</v>
       </c>
-      <c r="G19" s="16">
+      <c r="F19" s="16">
         <v>21756</v>
       </c>
-      <c r="H19" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F19/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G19)</f>
+      <c r="G19" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E19/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F19)</f>
         <v>29357.114809416205</v>
       </c>
+      <c r="H19" s="8">
+        <f t="shared" si="0"/>
+        <v>10.287290208465642</v>
+      </c>
       <c r="I19" s="8">
-        <f>LN(H19)</f>
-        <v>10.287290208465642</v>
-      </c>
-      <c r="J19" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K19" s="8">
-        <f>LN(D19)</f>
+      <c r="J19" s="8">
+        <f t="shared" si="1"/>
         <v>10.766931229610705</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>17</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="C20" t="s">
-        <v>317</v>
-      </c>
-      <c r="D20" s="21">
+      <c r="C20" s="21">
         <v>84684.420459877903</v>
       </c>
-      <c r="E20" s="15">
+      <c r="D20" s="15">
         <v>0.41284446195564001</v>
       </c>
-      <c r="F20">
+      <c r="E20">
         <v>4228655447.0969</v>
       </c>
-      <c r="G20" s="16">
+      <c r="F20" s="16">
         <v>41816</v>
       </c>
-      <c r="H20" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F20/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G20)</f>
+      <c r="G20" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E20/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F20)</f>
         <v>37038.00198014186</v>
       </c>
+      <c r="H20" s="8">
+        <f t="shared" si="0"/>
+        <v>10.51969974508439</v>
+      </c>
       <c r="I20" s="8">
-        <f>LN(H20)</f>
-        <v>10.51969974508439</v>
-      </c>
-      <c r="J20" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K20" s="8">
-        <f>LN(D20)</f>
+      <c r="J20" s="8">
+        <f t="shared" si="1"/>
         <v>11.346686925821588</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>27</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>318</v>
       </c>
-      <c r="C21" t="s">
-        <v>318</v>
-      </c>
-      <c r="D21" s="21">
+      <c r="C21" s="21">
         <v>36811.342592592497</v>
       </c>
-      <c r="E21" s="15">
+      <c r="D21" s="15">
         <v>1</v>
       </c>
-      <c r="F21">
+      <c r="E21">
         <v>934575156.70661795</v>
       </c>
-      <c r="G21" s="16">
+      <c r="F21" s="16">
         <v>20526</v>
       </c>
-      <c r="H21" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F21/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G21)</f>
+      <c r="G21" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E21/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F21)</f>
         <v>24529.357871872904</v>
       </c>
+      <c r="H21" s="8">
+        <f t="shared" si="0"/>
+        <v>10.107625959652379</v>
+      </c>
       <c r="I21" s="8">
-        <f>LN(H21)</f>
-        <v>10.107625959652379</v>
-      </c>
-      <c r="J21" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K21" s="8">
-        <f>LN(D21)</f>
+      <c r="J21" s="8">
+        <f t="shared" si="1"/>
         <v>10.513561299290984</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>52</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>319</v>
       </c>
-      <c r="C22" t="s">
-        <v>319</v>
-      </c>
-      <c r="D22" s="21">
+      <c r="C22" s="21">
         <v>62060.629019958797</v>
       </c>
-      <c r="E22" s="15">
+      <c r="D22" s="15">
         <v>1</v>
       </c>
-      <c r="F22">
+      <c r="E22">
         <v>717220175.04682505</v>
       </c>
-      <c r="G22" s="16">
+      <c r="F22" s="16">
         <v>22722.1703585748</v>
       </c>
-      <c r="H22" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F22/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G22)</f>
+      <c r="G22" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E22/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F22)</f>
         <v>21386.895110500951</v>
       </c>
+      <c r="H22" s="8">
+        <f t="shared" si="0"/>
+        <v>9.9705336354159684</v>
+      </c>
       <c r="I22" s="8">
-        <f>LN(H22)</f>
-        <v>9.9705336354159684</v>
-      </c>
-      <c r="J22" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K22" s="8">
-        <f>LN(D22)</f>
+      <c r="J22" s="8">
+        <f t="shared" si="1"/>
         <v>11.035867073625495</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>77</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>320</v>
       </c>
-      <c r="C23" t="s">
-        <v>320</v>
-      </c>
-      <c r="D23" s="21">
+      <c r="C23" s="21">
         <v>70188.4240894338</v>
       </c>
-      <c r="E23" s="15">
+      <c r="D23" s="15">
         <v>0.155925820662214</v>
       </c>
-      <c r="F23">
+      <c r="E23">
         <v>5719026262</v>
       </c>
-      <c r="G23" s="16">
+      <c r="F23" s="16">
         <v>56146</v>
       </c>
-      <c r="H23" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F23/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G23)</f>
+      <c r="G23" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E23/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F23)</f>
         <v>37203.288659213562</v>
       </c>
+      <c r="H23" s="8">
+        <f t="shared" si="0"/>
+        <v>10.524152441171331</v>
+      </c>
       <c r="I23" s="8">
-        <f>LN(H23)</f>
-        <v>10.524152441171331</v>
-      </c>
-      <c r="J23" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K23" s="8">
-        <f>LN(D23)</f>
+      <c r="J23" s="8">
+        <f t="shared" si="1"/>
         <v>11.158938677405651</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>9</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>321</v>
       </c>
-      <c r="C24" t="s">
-        <v>321</v>
-      </c>
-      <c r="D24" s="21">
+      <c r="C24" s="21">
         <v>133209.74576271101</v>
       </c>
-      <c r="E24" s="15">
+      <c r="D24" s="15">
         <v>0</v>
       </c>
-      <c r="F24">
+      <c r="E24">
         <v>1738199600</v>
       </c>
-      <c r="G24" s="16">
+      <c r="F24" s="16">
         <v>11203</v>
       </c>
-      <c r="H24" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F24/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G24)</f>
+      <c r="G24" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E24/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F24)</f>
         <v>49194.639062819566</v>
       </c>
+      <c r="H24" s="8">
+        <f t="shared" si="0"/>
+        <v>10.80353993440578</v>
+      </c>
       <c r="I24" s="8">
-        <f>LN(H24)</f>
-        <v>10.80353993440578</v>
-      </c>
-      <c r="J24" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K24" s="8">
-        <f>LN(D24)</f>
+      <c r="J24" s="8">
+        <f t="shared" si="1"/>
         <v>11.799680200798615</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>68</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>322</v>
       </c>
-      <c r="C25" t="s">
-        <v>322</v>
-      </c>
-      <c r="D25" s="21">
+      <c r="C25" s="21">
         <v>29726.962457337799</v>
       </c>
-      <c r="E25" s="15">
+      <c r="D25" s="15">
         <v>1</v>
       </c>
-      <c r="F25">
+      <c r="E25">
         <v>586459514</v>
       </c>
-      <c r="G25" s="16">
+      <c r="F25" s="16">
         <v>21411</v>
       </c>
-      <c r="H25" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F25/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G25)</f>
+      <c r="G25" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E25/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F25)</f>
         <v>20447.700044881512</v>
       </c>
+      <c r="H25" s="8">
+        <f t="shared" si="0"/>
+        <v>9.9256256879030751</v>
+      </c>
       <c r="I25" s="8">
-        <f>LN(H25)</f>
-        <v>9.9256256879030751</v>
-      </c>
-      <c r="J25" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K25" s="8">
-        <f>LN(D25)</f>
+      <c r="J25" s="8">
+        <f t="shared" si="1"/>
         <v>10.299809739811616</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>12</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>323</v>
       </c>
-      <c r="C26" t="s">
-        <v>323</v>
-      </c>
-      <c r="D26" s="21">
+      <c r="C26" s="21">
         <v>138253.012048192</v>
       </c>
-      <c r="E26" s="15">
+      <c r="D26" s="15">
         <v>0</v>
       </c>
-      <c r="F26">
+      <c r="E26">
         <v>3334593535</v>
       </c>
-      <c r="G26" s="16">
+      <c r="F26" s="16">
         <v>19517</v>
       </c>
-      <c r="H26" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F26/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G26)</f>
+      <c r="G26" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E26/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F26)</f>
         <v>52727.364271892111</v>
       </c>
+      <c r="H26" s="8">
+        <f t="shared" si="0"/>
+        <v>10.872889845913782</v>
+      </c>
       <c r="I26" s="8">
-        <f>LN(H26)</f>
-        <v>10.872889845913782</v>
-      </c>
-      <c r="J26" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K26" s="8">
-        <f>LN(D26)</f>
+      <c r="J26" s="8">
+        <f t="shared" si="1"/>
         <v>11.836840706114279</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>37</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>324</v>
       </c>
-      <c r="C27" t="s">
-        <v>324</v>
-      </c>
-      <c r="D27" s="21">
+      <c r="C27" s="21">
         <v>17297.863710113499</v>
       </c>
-      <c r="E27" s="15">
+      <c r="D27" s="15">
         <v>1</v>
       </c>
-      <c r="F27">
+      <c r="E27">
         <v>108407276</v>
       </c>
-      <c r="G27" s="16">
+      <c r="F27" s="16">
         <v>2221.3373493975901</v>
       </c>
-      <c r="H27" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F27/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G27)</f>
+      <c r="G27" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E27/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F27)</f>
         <v>25265.427318453832</v>
       </c>
+      <c r="H27" s="8">
+        <f t="shared" si="0"/>
+        <v>10.137192231038503</v>
+      </c>
       <c r="I27" s="8">
-        <f>LN(H27)</f>
-        <v>10.137192231038503</v>
-      </c>
-      <c r="J27" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K27" s="8">
-        <f>LN(D27)</f>
+      <c r="J27" s="8">
+        <f t="shared" si="1"/>
         <v>9.7583382878964375</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>63</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>325</v>
       </c>
-      <c r="C28" t="s">
-        <v>325</v>
-      </c>
-      <c r="D28" s="21">
+      <c r="C28" s="21">
         <v>57446.236559139703</v>
       </c>
-      <c r="E28" s="15">
+      <c r="D28" s="15">
         <v>1</v>
       </c>
-      <c r="F28">
+      <c r="E28">
         <v>1259700999.6398001</v>
       </c>
-      <c r="G28" s="16">
+      <c r="F28" s="16">
         <v>35691</v>
       </c>
-      <c r="H28" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F28/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G28)</f>
+      <c r="G28" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E28/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F28)</f>
         <v>22226.11436746793</v>
       </c>
+      <c r="H28" s="8">
+        <f t="shared" si="0"/>
+        <v>10.009023199393647</v>
+      </c>
       <c r="I28" s="8">
-        <f>LN(H28)</f>
-        <v>10.009023199393647</v>
-      </c>
-      <c r="J28" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K28" s="8">
-        <f>LN(D28)</f>
+      <c r="J28" s="8">
+        <f t="shared" si="1"/>
         <v>10.958604773022182</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>56</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>326</v>
       </c>
-      <c r="C29" t="s">
-        <v>326</v>
-      </c>
-      <c r="D29" s="21">
+      <c r="C29" s="21">
         <v>91762.204142011804</v>
       </c>
-      <c r="E29" s="15">
+      <c r="D29" s="15">
         <v>0.44061627021078476</v>
       </c>
-      <c r="F29">
+      <c r="E29">
         <v>2929880472</v>
       </c>
-      <c r="G29" s="16">
+      <c r="F29" s="16">
         <v>36426</v>
       </c>
-      <c r="H29" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F29/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G29)</f>
+      <c r="G29" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E29/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F29)</f>
         <v>32382.411295784575</v>
       </c>
+      <c r="H29" s="8">
+        <f t="shared" si="0"/>
+        <v>10.385370693136691</v>
+      </c>
       <c r="I29" s="8">
-        <f>LN(H29)</f>
-        <v>10.385370693136691</v>
-      </c>
-      <c r="J29" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K29" s="8">
-        <f>LN(D29)</f>
+      <c r="J29" s="8">
+        <f t="shared" si="1"/>
         <v>11.426955772242874</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>38</v>
       </c>
       <c r="B30" s="13" t="s">
         <v>327</v>
       </c>
-      <c r="C30" t="s">
-        <v>327</v>
-      </c>
-      <c r="D30" s="21">
+      <c r="C30" s="21">
         <v>49092.409240923997</v>
       </c>
-      <c r="E30" s="15">
+      <c r="D30" s="15">
         <v>0.9041847980804425</v>
       </c>
-      <c r="F30">
+      <c r="E30">
         <v>1473809152</v>
       </c>
-      <c r="G30" s="16">
+      <c r="F30" s="16">
         <v>26345</v>
       </c>
-      <c r="H30" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F30/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G30)</f>
+      <c r="G30" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E30/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F30)</f>
         <v>26871.913675206713</v>
       </c>
+      <c r="H30" s="8">
+        <f t="shared" si="0"/>
+        <v>10.198836918843039</v>
+      </c>
       <c r="I30" s="8">
-        <f>LN(H30)</f>
-        <v>10.198836918843039</v>
-      </c>
-      <c r="J30" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K30" s="8">
-        <f>LN(D30)</f>
+      <c r="J30" s="8">
+        <f t="shared" si="1"/>
         <v>10.801459703886596</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>69</v>
       </c>
       <c r="B31" s="13" t="s">
         <v>328</v>
       </c>
-      <c r="C31" t="s">
-        <v>328</v>
-      </c>
-      <c r="D31" s="21">
+      <c r="C31" s="21">
         <v>40337.982832618</v>
       </c>
-      <c r="E31" s="15">
+      <c r="D31" s="15">
         <v>0.96847891709828093</v>
       </c>
-      <c r="F31">
+      <c r="E31">
         <v>1151954740</v>
       </c>
-      <c r="G31" s="16">
+      <c r="F31" s="16">
         <v>29563</v>
       </c>
-      <c r="H31" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F31/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G31)</f>
+      <c r="G31" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E31/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F31)</f>
         <v>23052.191703863249</v>
       </c>
+      <c r="H31" s="8">
+        <f t="shared" si="0"/>
+        <v>10.045516128670826</v>
+      </c>
       <c r="I31" s="8">
-        <f>LN(H31)</f>
-        <v>10.045516128670826</v>
-      </c>
-      <c r="J31" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K31" s="8">
-        <f>LN(D31)</f>
+      <c r="J31" s="8">
+        <f t="shared" si="1"/>
         <v>10.605048806108673</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>55</v>
       </c>
       <c r="B32" s="13" t="s">
         <v>329</v>
       </c>
-      <c r="C32" t="s">
-        <v>329</v>
-      </c>
-      <c r="D32" s="21">
+      <c r="C32" s="21">
         <v>59478.403277097597</v>
       </c>
-      <c r="E32" s="15">
+      <c r="D32" s="15">
         <v>1</v>
       </c>
-      <c r="F32">
+      <c r="E32">
         <v>555427497.29508102</v>
       </c>
-      <c r="G32" s="16">
+      <c r="F32" s="16">
         <v>9041.8296414252</v>
       </c>
-      <c r="H32" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F32/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G32)</f>
+      <c r="G32" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E32/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F32)</f>
         <v>28106.265200815742</v>
       </c>
+      <c r="H32" s="8">
+        <f t="shared" si="0"/>
+        <v>10.243747791352876</v>
+      </c>
       <c r="I32" s="8">
-        <f>LN(H32)</f>
-        <v>10.243747791352876</v>
-      </c>
-      <c r="J32" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K32" s="8">
-        <f>LN(D32)</f>
+      <c r="J32" s="8">
+        <f t="shared" si="1"/>
         <v>10.993368555511305</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>20</v>
       </c>
       <c r="B33" s="13" t="s">
         <v>330</v>
       </c>
-      <c r="C33" t="s">
-        <v>330</v>
-      </c>
-      <c r="D33" s="21">
+      <c r="C33" s="21">
         <v>67039.106145251397</v>
       </c>
-      <c r="E33" s="15">
+      <c r="D33" s="15">
         <v>1</v>
       </c>
-      <c r="F33">
+      <c r="E33">
         <v>1280582613.6588299</v>
       </c>
-      <c r="G33" s="16">
+      <c r="F33" s="16">
         <v>22776</v>
       </c>
-      <c r="H33" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F33/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G33)</f>
+      <c r="G33" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E33/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F33)</f>
         <v>26935.461951011763</v>
       </c>
+      <c r="H33" s="8">
+        <f t="shared" si="0"/>
+        <v>10.201198985552741</v>
+      </c>
       <c r="I33" s="8">
-        <f>LN(H33)</f>
-        <v>10.201198985552741</v>
-      </c>
-      <c r="J33" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K33" s="8">
-        <f>LN(D33)</f>
+      <c r="J33" s="8">
+        <f t="shared" si="1"/>
         <v>11.113031401911519</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>23</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>331</v>
       </c>
-      <c r="C34" t="s">
-        <v>331</v>
-      </c>
-      <c r="D34" s="21">
+      <c r="C34" s="21">
         <v>53567.685589519599</v>
       </c>
-      <c r="E34" s="15">
+      <c r="D34" s="15">
         <v>1</v>
       </c>
-      <c r="F34">
+      <c r="E34">
         <v>3039736669.3952899</v>
       </c>
-      <c r="G34" s="16">
+      <c r="F34" s="16">
         <v>55598</v>
       </c>
-      <c r="H34" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F34/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G34)</f>
+      <c r="G34" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E34/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F34)</f>
         <v>26586.352440357754</v>
       </c>
+      <c r="H34" s="8">
+        <f t="shared" ref="H34:H65" si="2">LN(G34)</f>
+        <v>10.188153296954351</v>
+      </c>
       <c r="I34" s="8">
-        <f>LN(H34)</f>
-        <v>10.188153296954351</v>
-      </c>
-      <c r="J34" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K34" s="8">
-        <f>LN(D34)</f>
+      <c r="J34" s="8">
+        <f t="shared" ref="J34:J65" si="3">LN(C34)</f>
         <v>10.888701284460648</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>41</v>
       </c>
       <c r="B35" s="13" t="s">
         <v>332</v>
       </c>
-      <c r="C35" t="s">
-        <v>332</v>
-      </c>
-      <c r="D35" s="21">
+      <c r="C35" s="21">
         <v>68166.243654822305</v>
       </c>
-      <c r="E35" s="15">
+      <c r="D35" s="15">
         <v>0.24035850081477458</v>
       </c>
-      <c r="F35">
+      <c r="E35">
         <v>3571513320</v>
       </c>
-      <c r="G35" s="16">
+      <c r="F35" s="16">
         <v>29591</v>
       </c>
-      <c r="H35" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F35/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G35)</f>
+      <c r="G35" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E35/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F35)</f>
         <v>41441.391602862379</v>
       </c>
+      <c r="H35" s="8">
+        <f t="shared" si="2"/>
+        <v>10.632035457519684</v>
+      </c>
       <c r="I35" s="8">
-        <f>LN(H35)</f>
-        <v>10.632035457519684</v>
-      </c>
-      <c r="J35" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K35" s="8">
-        <f>LN(D35)</f>
+      <c r="J35" s="8">
+        <f t="shared" si="3"/>
         <v>11.1297047602249</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>16</v>
       </c>
       <c r="B36" s="13" t="s">
         <v>333</v>
       </c>
-      <c r="C36" t="s">
-        <v>333</v>
-      </c>
-      <c r="D36" s="21">
+      <c r="C36" s="21">
         <v>88437.625350982693</v>
       </c>
-      <c r="E36" s="15">
+      <c r="D36" s="15">
         <v>0.60032730073161344</v>
       </c>
-      <c r="F36">
+      <c r="E36">
         <v>5614957192.4309101</v>
       </c>
-      <c r="G36" s="16">
+      <c r="F36" s="16">
         <v>53832</v>
       </c>
-      <c r="H36" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F36/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G36)</f>
+      <c r="G36" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E36/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F36)</f>
         <v>37753.478110499855</v>
       </c>
+      <c r="H36" s="8">
+        <f t="shared" si="2"/>
+        <v>10.538832885810447</v>
+      </c>
       <c r="I36" s="8">
-        <f>LN(H36)</f>
-        <v>10.538832885810447</v>
-      </c>
-      <c r="J36" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K36" s="8">
-        <f>LN(D36)</f>
+      <c r="J36" s="8">
+        <f t="shared" si="3"/>
         <v>11.39005278421496</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>11</v>
       </c>
       <c r="B37" s="13" t="s">
         <v>334</v>
       </c>
-      <c r="C37" t="s">
-        <v>334</v>
-      </c>
-      <c r="D37" s="21">
+      <c r="C37" s="21">
         <v>93706.014075495797</v>
       </c>
-      <c r="E37" s="15">
+      <c r="D37" s="15">
         <v>0.37648764113518463</v>
       </c>
-      <c r="F37">
+      <c r="E37">
         <v>2760477311.1213899</v>
       </c>
-      <c r="G37" s="16">
+      <c r="F37" s="16">
         <v>26643</v>
       </c>
-      <c r="H37" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F37/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G37)</f>
+      <c r="G37" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E37/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F37)</f>
         <v>37597.026520689338</v>
       </c>
+      <c r="H37" s="8">
+        <f t="shared" si="2"/>
+        <v>10.534680244354288</v>
+      </c>
       <c r="I37" s="8">
-        <f>LN(H37)</f>
-        <v>10.534680244354288</v>
-      </c>
-      <c r="J37" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K37" s="8">
-        <f>LN(D37)</f>
+      <c r="J37" s="8">
+        <f t="shared" si="3"/>
         <v>11.447917650537072</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>39</v>
       </c>
       <c r="B38" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="C38" t="s">
-        <v>335</v>
-      </c>
-      <c r="D38" s="21">
+      <c r="C38" s="21">
         <v>61078.052550231798</v>
       </c>
-      <c r="E38" s="15">
+      <c r="D38" s="15">
         <v>0.72729650554509306</v>
       </c>
-      <c r="F38">
+      <c r="E38">
         <v>1816301258</v>
       </c>
-      <c r="G38" s="16">
+      <c r="F38" s="16">
         <v>18138</v>
       </c>
-      <c r="H38" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F38/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G38)</f>
+      <c r="G38" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E38/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F38)</f>
         <v>36815.838005803249</v>
       </c>
+      <c r="H38" s="8">
+        <f t="shared" si="2"/>
+        <v>10.513683412162338</v>
+      </c>
       <c r="I38" s="8">
-        <f>LN(H38)</f>
-        <v>10.513683412162338</v>
-      </c>
-      <c r="J38" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K38" s="8">
-        <f>LN(D38)</f>
+      <c r="J38" s="8">
+        <f t="shared" si="3"/>
         <v>11.019907875232786</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>6</v>
       </c>
       <c r="B39" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="C39" t="s">
-        <v>336</v>
-      </c>
-      <c r="D39" s="21">
+      <c r="C39" s="21">
         <v>104135.30619226801</v>
       </c>
-      <c r="E39" s="15">
+      <c r="D39" s="15">
         <v>1.3333333333333334E-2</v>
       </c>
-      <c r="F39">
+      <c r="E39">
         <v>20148584267.721901</v>
       </c>
-      <c r="G39" s="16">
+      <c r="F39" s="16">
         <v>101163</v>
       </c>
-      <c r="H39" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F39/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G39)</f>
+      <c r="G39" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E39/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F39)</f>
         <v>59097.932415462063</v>
       </c>
+      <c r="H39" s="8">
+        <f t="shared" si="2"/>
+        <v>10.986951218272269</v>
+      </c>
       <c r="I39" s="8">
-        <f>LN(H39)</f>
-        <v>10.986951218272269</v>
-      </c>
-      <c r="J39" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K39" s="8">
-        <f>LN(D39)</f>
+      <c r="J39" s="8">
+        <f t="shared" si="3"/>
         <v>11.553446353608431</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>7</v>
       </c>
       <c r="B40" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="C40" t="s">
-        <v>337</v>
-      </c>
-      <c r="D40" s="21">
+      <c r="C40" s="21">
         <v>137504.774637127</v>
       </c>
-      <c r="E40" s="15">
+      <c r="D40" s="15">
         <v>0</v>
       </c>
-      <c r="F40">
+      <c r="E40">
         <v>20868022993.062698</v>
       </c>
-      <c r="G40" s="16">
+      <c r="F40" s="16">
         <v>67831</v>
       </c>
-      <c r="H40" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F40/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G40)</f>
+      <c r="G40" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E40/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F40)</f>
         <v>83505.41670596943</v>
       </c>
+      <c r="H40" s="8">
+        <f t="shared" si="2"/>
+        <v>11.332666779465105</v>
+      </c>
       <c r="I40" s="8">
-        <f>LN(H40)</f>
-        <v>11.332666779465105</v>
-      </c>
-      <c r="J40" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K40" s="8">
-        <f>LN(D40)</f>
+      <c r="J40" s="8">
+        <f t="shared" si="3"/>
         <v>11.831413920119529</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4</v>
       </c>
       <c r="B41" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="C41" t="s">
-        <v>338</v>
-      </c>
-      <c r="D41" s="21">
+      <c r="C41" s="21">
         <v>93605.664488017399</v>
       </c>
-      <c r="E41" s="15">
+      <c r="D41" s="15">
         <v>0.25798883785252136</v>
       </c>
-      <c r="F41">
+      <c r="E41">
         <v>5335063217</v>
       </c>
-      <c r="G41" s="16">
+      <c r="F41" s="16">
         <v>41673</v>
       </c>
-      <c r="H41" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F41/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G41)</f>
+      <c r="G41" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E41/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F41)</f>
         <v>43089.768798536563</v>
       </c>
+      <c r="H41" s="8">
+        <f t="shared" si="2"/>
+        <v>10.671040865047486</v>
+      </c>
       <c r="I41" s="8">
-        <f>LN(H41)</f>
-        <v>10.671040865047486</v>
-      </c>
-      <c r="J41" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K41" s="8">
-        <f>LN(D41)</f>
+      <c r="J41" s="8">
+        <f t="shared" si="3"/>
         <v>11.446846178668915</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>22</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="C42" t="s">
-        <v>339</v>
-      </c>
-      <c r="D42" s="21">
+      <c r="C42" s="21">
         <v>103469.03669724699</v>
       </c>
-      <c r="E42" s="15">
+      <c r="D42" s="15">
         <v>0.59259052536105494</v>
       </c>
-      <c r="F42">
+      <c r="E42">
         <v>10349284631.224199</v>
       </c>
-      <c r="G42" s="16">
+      <c r="F42" s="16">
         <v>70869</v>
       </c>
-      <c r="H42" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F42/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G42)</f>
+      <c r="G42" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E42/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F42)</f>
         <v>47142.456397381306</v>
       </c>
+      <c r="H42" s="8">
+        <f t="shared" si="2"/>
+        <v>10.76092928368961</v>
+      </c>
       <c r="I42" s="8">
-        <f>LN(H42)</f>
-        <v>10.76092928368961</v>
-      </c>
-      <c r="J42" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K42" s="8">
-        <f>LN(D42)</f>
+      <c r="J42" s="8">
+        <f t="shared" si="3"/>
         <v>11.54702768458414</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>31</v>
       </c>
       <c r="B43" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="C43" t="s">
-        <v>340</v>
-      </c>
-      <c r="D43" s="21">
+      <c r="C43" s="21">
         <v>71734.657039711194</v>
       </c>
-      <c r="E43" s="15">
+      <c r="D43" s="15">
         <v>0.95294954223578565</v>
       </c>
-      <c r="F43">
+      <c r="E43">
         <v>3355586836.6333699</v>
       </c>
-      <c r="G43" s="16">
+      <c r="F43" s="16">
         <v>33279</v>
       </c>
-      <c r="H43" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F43/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G43)</f>
+      <c r="G43" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E43/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F43)</f>
         <v>36972.001320973308</v>
       </c>
+      <c r="H43" s="8">
+        <f t="shared" si="2"/>
+        <v>10.517916184113687</v>
+      </c>
       <c r="I43" s="8">
-        <f>LN(H43)</f>
-        <v>10.517916184113687</v>
-      </c>
-      <c r="J43" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K43" s="8">
-        <f>LN(D43)</f>
+      <c r="J43" s="8">
+        <f t="shared" si="3"/>
         <v>11.180729271587225</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>59</v>
       </c>
       <c r="B44" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="C44" t="s">
-        <v>341</v>
-      </c>
-      <c r="D44" s="21">
+      <c r="C44" s="21">
         <v>76145.662847790503</v>
       </c>
-      <c r="E44" s="15">
+      <c r="D44" s="15">
         <v>1</v>
       </c>
-      <c r="F44">
+      <c r="E44">
         <v>1238142773.8199301</v>
       </c>
-      <c r="G44" s="16">
+      <c r="F44" s="16">
         <v>15443</v>
       </c>
-      <c r="H44" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F44/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G44)</f>
+      <c r="G44" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E44/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F44)</f>
         <v>32324.191921799607</v>
       </c>
+      <c r="H44" s="8">
+        <f t="shared" si="2"/>
+        <v>10.383571204775373</v>
+      </c>
       <c r="I44" s="8">
-        <f>LN(H44)</f>
-        <v>10.383571204775373</v>
-      </c>
-      <c r="J44" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K44" s="8">
-        <f>LN(D44)</f>
+      <c r="J44" s="8">
+        <f t="shared" si="3"/>
         <v>11.240403401320993</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>18</v>
       </c>
       <c r="B45" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="C45" t="s">
-        <v>342</v>
-      </c>
-      <c r="D45" s="21">
+      <c r="C45" s="21">
         <v>78841.145833333299</v>
       </c>
-      <c r="E45" s="15">
+      <c r="D45" s="15">
         <v>1</v>
       </c>
-      <c r="F45">
+      <c r="E45">
         <v>947789398</v>
       </c>
-      <c r="G45" s="16">
+      <c r="F45" s="16">
         <v>14084</v>
       </c>
-      <c r="H45" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F45/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G45)</f>
+      <c r="G45" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E45/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F45)</f>
         <v>29426.296045943549</v>
       </c>
+      <c r="H45" s="8">
+        <f t="shared" si="2"/>
+        <v>10.28964397689999</v>
+      </c>
       <c r="I45" s="8">
-        <f>LN(H45)</f>
-        <v>10.28964397689999</v>
-      </c>
-      <c r="J45" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K45" s="8">
-        <f>LN(D45)</f>
+      <c r="J45" s="8">
+        <f t="shared" si="3"/>
         <v>11.275190294815703</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>75</v>
       </c>
       <c r="B46" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="C46" t="s">
-        <v>343</v>
-      </c>
-      <c r="D46" s="21">
+      <c r="C46" s="21">
         <v>73828.004598938307</v>
       </c>
-      <c r="E46" s="15">
+      <c r="D46" s="15">
         <v>0.31365052393089776</v>
       </c>
-      <c r="F46">
+      <c r="E46">
         <v>1505913598.3160801</v>
       </c>
-      <c r="G46" s="16">
+      <c r="F46" s="16">
         <v>21324.521514629902</v>
       </c>
-      <c r="H46" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F46/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G46)</f>
+      <c r="G46" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E46/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F46)</f>
         <v>30174.060396291829</v>
       </c>
+      <c r="H46" s="8">
+        <f t="shared" si="2"/>
+        <v>10.314737906998461</v>
+      </c>
       <c r="I46" s="8">
-        <f>LN(H46)</f>
-        <v>10.314737906998461</v>
-      </c>
-      <c r="J46" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K46" s="8">
-        <f>LN(D46)</f>
+      <c r="J46" s="8">
+        <f t="shared" si="3"/>
         <v>11.209493404719783</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>74</v>
       </c>
       <c r="B47" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="C47" t="s">
-        <v>344</v>
-      </c>
-      <c r="D47" s="21">
+      <c r="C47" s="21">
         <v>115749.730312837</v>
       </c>
-      <c r="E47" s="15">
+      <c r="D47" s="15">
         <v>0.82639038007300836</v>
       </c>
-      <c r="F47">
+      <c r="E47">
         <v>1628720074</v>
       </c>
-      <c r="G47" s="16">
+      <c r="F47" s="16">
         <v>18553</v>
       </c>
-      <c r="H47" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F47/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G47)</f>
+      <c r="G47" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E47/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F47)</f>
         <v>34036.982458760191</v>
       </c>
+      <c r="H47" s="8">
+        <f t="shared" si="2"/>
+        <v>10.435202931835502</v>
+      </c>
       <c r="I47" s="8">
-        <f>LN(H47)</f>
-        <v>10.435202931835502</v>
-      </c>
-      <c r="J47" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K47" s="8">
-        <f>LN(D47)</f>
+      <c r="J47" s="8">
+        <f t="shared" si="3"/>
         <v>11.659185642035071</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>8</v>
       </c>
       <c r="B48" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="C48" t="s">
-        <v>345</v>
-      </c>
-      <c r="D48" s="21">
+      <c r="C48" s="21">
         <v>122603.164187809</v>
       </c>
-      <c r="E48" s="15">
+      <c r="D48" s="15">
         <v>6.7775239142594396E-2</v>
       </c>
-      <c r="F48">
+      <c r="E48">
         <v>132811651780.245</v>
       </c>
-      <c r="G48" s="16">
+      <c r="F48" s="16">
         <v>104712</v>
       </c>
-      <c r="H48" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F48/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G48)</f>
+      <c r="G48" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E48/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F48)</f>
         <v>299663.77758122637</v>
       </c>
+      <c r="H48" s="8">
+        <f t="shared" si="2"/>
+        <v>12.610416383742153</v>
+      </c>
       <c r="I48" s="8">
-        <f>LN(H48)</f>
-        <v>12.610416383742153</v>
-      </c>
-      <c r="J48" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K48" s="8">
-        <f>LN(D48)</f>
+      <c r="J48" s="8">
+        <f t="shared" si="3"/>
         <v>11.716708111187163</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>33</v>
       </c>
       <c r="B49" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="C49" t="s">
-        <v>346</v>
-      </c>
-      <c r="D49" s="21">
+      <c r="C49" s="21">
         <v>124966.99669966901</v>
       </c>
-      <c r="E49" s="15">
+      <c r="D49" s="15">
         <v>0</v>
       </c>
-      <c r="F49">
+      <c r="E49">
         <v>7669949196.5560703</v>
       </c>
-      <c r="G49" s="16">
+      <c r="F49" s="16">
         <v>29174</v>
       </c>
-      <c r="H49" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F49/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G49)</f>
+      <c r="G49" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E49/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F49)</f>
         <v>73438.091279841756</v>
       </c>
+      <c r="H49" s="8">
+        <f t="shared" si="2"/>
+        <v>11.204198034758388</v>
+      </c>
       <c r="I49" s="8">
-        <f>LN(H49)</f>
-        <v>11.204198034758388</v>
-      </c>
-      <c r="J49" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K49" s="8">
-        <f>LN(D49)</f>
+      <c r="J49" s="8">
+        <f t="shared" si="3"/>
         <v>11.735804955020683</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>28</v>
       </c>
       <c r="B50" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="C50" t="s">
-        <v>347</v>
-      </c>
-      <c r="D50" s="21">
+      <c r="C50" s="21">
         <v>110651.05653912001</v>
       </c>
-      <c r="E50" s="15">
+      <c r="D50" s="15">
         <v>0.44102178812922616</v>
       </c>
-      <c r="F50">
+      <c r="E50">
         <v>22690599560.388</v>
       </c>
-      <c r="G50" s="16">
+      <c r="F50" s="16">
         <v>66084</v>
       </c>
-      <c r="H50" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F50/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G50)</f>
+      <c r="G50" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E50/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F50)</f>
         <v>91540.762834040361</v>
       </c>
+      <c r="H50" s="8">
+        <f t="shared" si="2"/>
+        <v>11.424539647513969</v>
+      </c>
       <c r="I50" s="8">
-        <f>LN(H50)</f>
-        <v>11.424539647513969</v>
-      </c>
-      <c r="J50" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K50" s="8">
-        <f>LN(D50)</f>
+      <c r="J50" s="8">
+        <f t="shared" si="3"/>
         <v>11.614136893911875</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>61</v>
       </c>
       <c r="B51" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="C51" t="s">
-        <v>348</v>
-      </c>
-      <c r="D51" s="21">
+      <c r="C51" s="21">
         <v>49405.207811411601</v>
       </c>
-      <c r="E51" s="15">
+      <c r="D51" s="15">
         <v>1</v>
       </c>
-      <c r="F51">
+      <c r="E51">
         <v>1744139059.0571401</v>
       </c>
-      <c r="G51" s="16">
+      <c r="F51" s="16">
         <v>41789.662650602397</v>
       </c>
-      <c r="H51" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F51/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G51)</f>
+      <c r="G51" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E51/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F51)</f>
         <v>23675.45001650937</v>
       </c>
+      <c r="H51" s="8">
+        <f t="shared" si="2"/>
+        <v>10.072193925962724</v>
+      </c>
       <c r="I51" s="8">
-        <f>LN(H51)</f>
-        <v>10.072193925962724</v>
-      </c>
-      <c r="J51" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K51" s="8">
-        <f>LN(D51)</f>
+      <c r="J51" s="8">
+        <f t="shared" si="3"/>
         <v>10.807811118903217</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>5</v>
       </c>
       <c r="B52" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="C52" t="s">
-        <v>349</v>
-      </c>
-      <c r="D52" s="21">
+      <c r="C52" s="21">
         <v>145156.86274509801</v>
       </c>
-      <c r="E52" s="15">
+      <c r="D52" s="15">
         <v>0</v>
       </c>
-      <c r="F52">
+      <c r="E52">
         <v>7458343008.5430002</v>
       </c>
-      <c r="G52" s="16">
+      <c r="F52" s="16">
         <v>35408</v>
       </c>
-      <c r="H52" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F52/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G52)</f>
+      <c r="G52" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E52/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F52)</f>
         <v>61678.804804845866</v>
       </c>
+      <c r="H52" s="8">
+        <f t="shared" si="2"/>
+        <v>11.029695630696125</v>
+      </c>
       <c r="I52" s="8">
-        <f>LN(H52)</f>
-        <v>11.029695630696125</v>
-      </c>
-      <c r="J52" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K52" s="8">
-        <f>LN(D52)</f>
+      <c r="J52" s="8">
+        <f t="shared" si="3"/>
         <v>11.88557024870091</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>29</v>
       </c>
       <c r="B53" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="C53" t="s">
-        <v>350</v>
-      </c>
-      <c r="D53" s="21">
+      <c r="C53" s="21">
         <v>37247.422680412303</v>
       </c>
-      <c r="E53" s="15">
+      <c r="D53" s="15">
         <v>1</v>
       </c>
-      <c r="F53">
+      <c r="E53">
         <v>1255679042.0029199</v>
       </c>
-      <c r="G53" s="16">
+      <c r="F53" s="16">
         <v>31244</v>
       </c>
-      <c r="H53" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F53/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G53)</f>
+      <c r="G53" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E53/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F53)</f>
         <v>23327.444863672274</v>
       </c>
+      <c r="H53" s="8">
+        <f t="shared" si="2"/>
+        <v>10.057385837529015</v>
+      </c>
       <c r="I53" s="8">
-        <f>LN(H53)</f>
-        <v>10.057385837529015</v>
-      </c>
-      <c r="J53" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K53" s="8">
-        <f>LN(D53)</f>
+      <c r="J53" s="8">
+        <f t="shared" si="3"/>
         <v>10.525338031626392</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>13</v>
       </c>
       <c r="B54" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="C54" t="s">
-        <v>351</v>
-      </c>
-      <c r="D54" s="21">
+      <c r="C54" s="21">
         <v>77368.4210526315</v>
       </c>
-      <c r="E54" s="15">
+      <c r="D54" s="15">
         <v>0.63061677772082692</v>
       </c>
-      <c r="F54">
+      <c r="E54">
         <v>1966649200.72945</v>
       </c>
-      <c r="G54" s="16">
+      <c r="F54" s="16">
         <v>18742</v>
       </c>
-      <c r="H54" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F54/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G54)</f>
+      <c r="G54" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E54/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F54)</f>
         <v>37894.673358517743</v>
       </c>
+      <c r="H54" s="8">
+        <f t="shared" si="2"/>
+        <v>10.542565836563057</v>
+      </c>
       <c r="I54" s="8">
-        <f>LN(H54)</f>
-        <v>10.542565836563057</v>
-      </c>
-      <c r="J54" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K54" s="8">
-        <f>LN(D54)</f>
+      <c r="J54" s="8">
+        <f t="shared" si="3"/>
         <v>11.256333979588478</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>10</v>
       </c>
       <c r="B55" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="C55" t="s">
-        <v>352</v>
-      </c>
-      <c r="D55" s="21">
+      <c r="C55" s="21">
         <v>108893.84609789299</v>
       </c>
-      <c r="E55" s="15">
+      <c r="D55" s="15">
         <v>0.3766284625225178</v>
       </c>
-      <c r="F55">
+      <c r="E55">
         <v>4738453822</v>
       </c>
-      <c r="G55" s="16">
+      <c r="F55" s="16">
         <v>38895.286774334301</v>
       </c>
-      <c r="H55" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F55/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G55)</f>
+      <c r="G55" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E55/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F55)</f>
         <v>41695.637175424461</v>
       </c>
+      <c r="H55" s="8">
+        <f t="shared" si="2"/>
+        <v>10.63815177822287</v>
+      </c>
       <c r="I55" s="8">
-        <f>LN(H55)</f>
-        <v>10.63815177822287</v>
-      </c>
-      <c r="J55" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K55" s="8">
-        <f>LN(D55)</f>
+      <c r="J55" s="8">
+        <f t="shared" si="3"/>
         <v>11.598128797663099</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>36</v>
       </c>
       <c r="B56" s="13" t="s">
         <v>354</v>
       </c>
-      <c r="C56" t="s">
-        <v>354</v>
-      </c>
-      <c r="D56" s="21">
+      <c r="C56" s="21">
         <v>29959.677419354801</v>
       </c>
-      <c r="E56" s="15">
+      <c r="D56" s="15">
         <v>1</v>
       </c>
-      <c r="F56">
+      <c r="E56">
         <v>420233996</v>
       </c>
-      <c r="G56" s="16">
+      <c r="F56" s="16">
         <v>6946</v>
       </c>
-      <c r="H56" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F56/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G56)</f>
+      <c r="G56" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E56/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F56)</f>
         <v>27897.348650118838</v>
       </c>
+      <c r="H56" s="8">
+        <f t="shared" si="2"/>
+        <v>10.236286932832087</v>
+      </c>
       <c r="I56" s="8">
-        <f>LN(H56)</f>
-        <v>10.236286932832087</v>
-      </c>
-      <c r="J56" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K56" s="8">
-        <f>LN(D56)</f>
+      <c r="J56" s="8">
+        <f t="shared" si="3"/>
         <v>10.307607670528958</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>76</v>
       </c>
       <c r="B57" s="13" t="s">
         <v>353</v>
       </c>
-      <c r="C57" t="s">
-        <v>353</v>
-      </c>
-      <c r="D57" s="21">
+      <c r="C57" s="21">
         <v>75645.5643481882</v>
       </c>
-      <c r="E57" s="15">
+      <c r="D57" s="15">
         <v>0.47652407214189896</v>
       </c>
-      <c r="F57">
+      <c r="E57">
         <v>1697988043.6924701</v>
       </c>
-      <c r="G57" s="16">
+      <c r="F57" s="16">
         <v>14004.4055644729</v>
       </c>
-      <c r="H57" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F57/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G57)</f>
+      <c r="G57" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E57/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F57)</f>
         <v>41565.31568749671</v>
       </c>
+      <c r="H57" s="8">
+        <f t="shared" si="2"/>
+        <v>10.635021340968144</v>
+      </c>
       <c r="I57" s="8">
-        <f>LN(H57)</f>
-        <v>10.635021340968144</v>
-      </c>
-      <c r="J57" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K57" s="8">
-        <f>LN(D57)</f>
+      <c r="J57" s="8">
+        <f t="shared" si="3"/>
         <v>11.233814083633467</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>15</v>
       </c>
       <c r="B58" s="13" t="s">
         <v>355</v>
       </c>
-      <c r="C58" t="s">
-        <v>355</v>
-      </c>
-      <c r="D58" s="21">
+      <c r="C58" s="21">
         <v>89490.830115830104</v>
       </c>
-      <c r="E58" s="15">
+      <c r="D58" s="15">
         <v>0.48509996826404317</v>
       </c>
-      <c r="F58">
+      <c r="E58">
         <v>5574661088</v>
       </c>
-      <c r="G58" s="16">
+      <c r="F58" s="16">
         <v>61793</v>
       </c>
-      <c r="H58" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F58/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G58)</f>
+      <c r="G58" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E58/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F58)</f>
         <v>34583.207084717913</v>
       </c>
+      <c r="H58" s="8">
+        <f t="shared" si="2"/>
+        <v>10.451123498855798</v>
+      </c>
       <c r="I58" s="8">
-        <f>LN(H58)</f>
-        <v>10.451123498855798</v>
-      </c>
-      <c r="J58" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K58" s="8">
-        <f>LN(D58)</f>
+      <c r="J58" s="8">
+        <f t="shared" si="3"/>
         <v>11.401891442207521</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>50</v>
       </c>
       <c r="B59" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="C59" t="s">
-        <v>356</v>
-      </c>
-      <c r="D59" s="21">
+      <c r="C59" s="21">
         <v>54685.314685314603</v>
       </c>
-      <c r="E59" s="15">
+      <c r="D59" s="15">
         <v>0.48020527859237538</v>
       </c>
-      <c r="F59">
+      <c r="E59">
         <v>463034211.20127797</v>
       </c>
-      <c r="G59" s="16">
+      <c r="F59" s="16">
         <v>6741</v>
       </c>
-      <c r="H59" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F59/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G59)</f>
+      <c r="G59" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E59/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F59)</f>
         <v>29739.895581347035</v>
       </c>
+      <c r="H59" s="8">
+        <f t="shared" si="2"/>
+        <v>10.300244708957109</v>
+      </c>
       <c r="I59" s="8">
-        <f>LN(H59)</f>
-        <v>10.300244708957109</v>
-      </c>
-      <c r="J59" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K59" s="8">
-        <f>LN(D59)</f>
+      <c r="J59" s="8">
+        <f t="shared" si="3"/>
         <v>10.909350482261585</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>54</v>
       </c>
       <c r="B60" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="C60" t="s">
-        <v>225</v>
-      </c>
-      <c r="D60" s="21">
+      <c r="C60" s="21">
         <v>20515.625</v>
       </c>
-      <c r="E60" s="15">
+      <c r="D60" s="15">
         <v>1</v>
       </c>
-      <c r="F60" s="23">
+      <c r="E60" s="23">
         <v>88633152</v>
       </c>
-      <c r="G60" s="16">
+      <c r="F60" s="16">
         <v>7536</v>
       </c>
-      <c r="H60" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F60/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G60)</f>
+      <c r="G60" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E60/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F60)</f>
         <v>16931.116399161918</v>
       </c>
+      <c r="H60" s="8">
+        <f t="shared" si="2"/>
+        <v>9.7369084150181848</v>
+      </c>
       <c r="I60" s="8">
-        <f>LN(H60)</f>
-        <v>9.7369084150181848</v>
-      </c>
-      <c r="J60" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K60" s="8">
-        <f>LN(D60)</f>
+      <c r="J60" s="8">
+        <f t="shared" si="3"/>
         <v>9.9289420699252613</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>1</v>
       </c>
       <c r="B61" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="C61" t="s">
-        <v>357</v>
-      </c>
-      <c r="D61" s="21">
+      <c r="C61" s="21">
         <v>59553.862894450402</v>
       </c>
-      <c r="E61" s="15">
+      <c r="D61" s="15">
         <v>0.65371755231178541</v>
       </c>
-      <c r="F61">
+      <c r="E61">
         <v>3945507288</v>
       </c>
-      <c r="G61" s="16">
+      <c r="F61" s="16">
         <v>54388</v>
       </c>
-      <c r="H61" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F61/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G61)</f>
+      <c r="G61" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E61/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F61)</f>
         <v>30607.149197741561</v>
       </c>
+      <c r="H61" s="8">
+        <f t="shared" si="2"/>
+        <v>10.328988894565443</v>
+      </c>
       <c r="I61" s="8">
-        <f>LN(H61)</f>
-        <v>10.328988894565443</v>
-      </c>
-      <c r="J61" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K61" s="8">
-        <f>LN(D61)</f>
+      <c r="J61" s="8">
+        <f t="shared" si="3"/>
         <v>10.994636440764411</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>49</v>
       </c>
       <c r="B62" s="13" t="s">
         <v>358</v>
       </c>
-      <c r="C62" t="s">
-        <v>358</v>
-      </c>
-      <c r="D62" s="21">
+      <c r="C62" s="21">
         <v>50453.639082751703</v>
       </c>
-      <c r="E62" s="15">
+      <c r="D62" s="15">
         <v>0.94860366859027201</v>
       </c>
-      <c r="F62">
+      <c r="E62">
         <v>1467654352.7150199</v>
       </c>
-      <c r="G62" s="16">
+      <c r="F62" s="16">
         <v>36700</v>
       </c>
-      <c r="H62" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F62/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G62)</f>
+      <c r="G62" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E62/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F62)</f>
         <v>23282.700517448069</v>
       </c>
+      <c r="H62" s="8">
+        <f t="shared" si="2"/>
+        <v>10.055465896726302</v>
+      </c>
       <c r="I62" s="8">
-        <f>LN(H62)</f>
-        <v>10.055465896726302</v>
-      </c>
-      <c r="J62" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K62" s="8">
-        <f>LN(D62)</f>
+      <c r="J62" s="8">
+        <f t="shared" si="3"/>
         <v>10.828810155643202</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>46</v>
       </c>
       <c r="B63" s="13" t="s">
         <v>359</v>
       </c>
-      <c r="C63" t="s">
-        <v>359</v>
-      </c>
-      <c r="D63" s="21">
+      <c r="C63" s="21">
         <v>42455.673758865203</v>
       </c>
-      <c r="E63" s="15">
+      <c r="D63" s="15">
         <v>1</v>
       </c>
-      <c r="F63">
+      <c r="E63">
         <v>886136027.60169101</v>
       </c>
-      <c r="G63" s="16">
+      <c r="F63" s="16">
         <v>29381</v>
       </c>
-      <c r="H63" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F63/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G63)</f>
+      <c r="G63" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E63/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F63)</f>
         <v>21070.859960264315</v>
       </c>
+      <c r="H63" s="8">
+        <f t="shared" si="2"/>
+        <v>9.9556463204059895</v>
+      </c>
       <c r="I63" s="8">
-        <f>LN(H63)</f>
-        <v>9.9556463204059895</v>
-      </c>
-      <c r="J63" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K63" s="8">
-        <f>LN(D63)</f>
+      <c r="J63" s="8">
+        <f t="shared" si="3"/>
         <v>10.656215840260787</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>51</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>360</v>
       </c>
-      <c r="C64" t="s">
-        <v>360</v>
-      </c>
-      <c r="D64" s="21">
+      <c r="C64" s="21">
         <v>37095.3757225433</v>
       </c>
-      <c r="E64" s="15">
+      <c r="D64" s="15">
         <v>0.78007798652959948</v>
       </c>
-      <c r="F64">
+      <c r="E64">
         <v>632440233.59475005</v>
       </c>
-      <c r="G64" s="16">
+      <c r="F64" s="16">
         <v>14210</v>
       </c>
-      <c r="H64" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F64/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G64)</f>
+      <c r="G64" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E64/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F64)</f>
         <v>24298.826820173505</v>
       </c>
+      <c r="H64" s="8">
+        <f t="shared" si="2"/>
+        <v>10.098183349157965</v>
+      </c>
       <c r="I64" s="8">
-        <f>LN(H64)</f>
-        <v>10.098183349157965</v>
-      </c>
-      <c r="J64" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K64" s="8">
-        <f>LN(D64)</f>
+      <c r="J64" s="8">
+        <f t="shared" si="3"/>
         <v>10.521247597229651</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>30</v>
       </c>
       <c r="B65" s="13" t="s">
         <v>361</v>
       </c>
-      <c r="C65" t="s">
-        <v>361</v>
-      </c>
-      <c r="D65" s="21">
+      <c r="C65" s="21">
         <v>47515.090543259503</v>
       </c>
-      <c r="E65" s="15">
+      <c r="D65" s="15">
         <v>1</v>
       </c>
-      <c r="F65">
+      <c r="E65">
         <v>2214326519.5912199</v>
       </c>
-      <c r="G65" s="16">
+      <c r="F65" s="16">
         <v>68798</v>
       </c>
-      <c r="H65" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F65/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G65)</f>
+      <c r="G65" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E65/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F65)</f>
         <v>21526.651511210828</v>
       </c>
+      <c r="H65" s="8">
+        <f t="shared" si="2"/>
+        <v>9.9770470516122032</v>
+      </c>
       <c r="I65" s="8">
-        <f>LN(H65)</f>
-        <v>9.9770470516122032</v>
-      </c>
-      <c r="J65" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K65" s="8">
-        <f>LN(D65)</f>
+      <c r="J65" s="8">
+        <f t="shared" si="3"/>
         <v>10.768802635215724</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>43</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="C66" t="s">
-        <v>362</v>
-      </c>
-      <c r="D66" s="21">
+      <c r="C66" s="21">
         <v>40124.821683309499</v>
       </c>
-      <c r="E66" s="15">
+      <c r="D66" s="15">
         <v>1</v>
       </c>
-      <c r="F66">
+      <c r="E66">
         <v>2059404538</v>
       </c>
-      <c r="G66" s="16">
+      <c r="F66" s="16">
         <v>54345</v>
       </c>
-      <c r="H66" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F66/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G66)</f>
+      <c r="G66" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E66/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F66)</f>
         <v>22811.198096572451</v>
       </c>
+      <c r="H66" s="8">
+        <f t="shared" ref="H66:H97" si="4">LN(G66)</f>
+        <v>10.035006838957019</v>
+      </c>
       <c r="I66" s="8">
-        <f>LN(H66)</f>
-        <v>10.035006838957019</v>
-      </c>
-      <c r="J66" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K66" s="8">
-        <f>LN(D66)</f>
+      <c r="J66" s="8">
+        <f t="shared" ref="J66:J78" si="5">LN(C66)</f>
         <v>10.599750416392773</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>32</v>
       </c>
       <c r="B67" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="C67" t="s">
-        <v>363</v>
-      </c>
-      <c r="D67" s="21">
+      <c r="C67" s="21">
         <v>119836.78593848</v>
       </c>
-      <c r="E67" s="15">
+      <c r="D67" s="15">
         <v>0</v>
       </c>
-      <c r="F67">
+      <c r="E67">
         <v>60869319139.509003</v>
       </c>
-      <c r="G67" s="16">
+      <c r="F67" s="16">
         <v>42181</v>
       </c>
-      <c r="H67" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F67/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G67)</f>
+      <c r="G67" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E67/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F67)</f>
         <v>338970.99372603663</v>
       </c>
+      <c r="H67" s="8">
+        <f t="shared" si="4"/>
+        <v>12.73366981847178</v>
+      </c>
       <c r="I67" s="8">
-        <f>LN(H67)</f>
-        <v>12.73366981847178</v>
-      </c>
-      <c r="J67" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K67" s="8">
-        <f>LN(D67)</f>
+      <c r="J67" s="8">
+        <f t="shared" si="5"/>
         <v>11.69388597878592</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>3</v>
       </c>
       <c r="B68" s="13" t="s">
         <v>364</v>
       </c>
-      <c r="C68" t="s">
-        <v>364</v>
-      </c>
-      <c r="D68" s="21">
+      <c r="C68" s="21">
         <v>68444.460944460894</v>
       </c>
-      <c r="E68" s="15">
+      <c r="D68" s="15">
         <v>0.25196740232940434</v>
       </c>
-      <c r="F68">
+      <c r="E68">
         <v>6215659728</v>
       </c>
-      <c r="G68" s="16">
+      <c r="F68" s="16">
         <v>57331</v>
       </c>
-      <c r="H68" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F68/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G68)</f>
+      <c r="G68" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E68/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F68)</f>
         <v>38678.652309958939</v>
       </c>
+      <c r="H68" s="8">
+        <f t="shared" si="4"/>
+        <v>10.563043106921942</v>
+      </c>
       <c r="I68" s="8">
-        <f>LN(H68)</f>
-        <v>10.563043106921942</v>
-      </c>
-      <c r="J68" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K68" s="8">
-        <f>LN(D68)</f>
+      <c r="J68" s="8">
+        <f t="shared" si="5"/>
         <v>11.133777906251078</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>73</v>
       </c>
       <c r="B69" s="13" t="s">
         <v>365</v>
       </c>
-      <c r="C69" t="s">
-        <v>365</v>
-      </c>
-      <c r="D69" s="21">
+      <c r="C69" s="21">
         <v>69526.209677419305</v>
       </c>
-      <c r="E69" s="15">
+      <c r="D69" s="15">
         <v>1</v>
       </c>
-      <c r="F69">
+      <c r="E69">
         <v>1274341977.2748699</v>
       </c>
-      <c r="G69" s="16">
+      <c r="F69" s="16">
         <v>25312</v>
       </c>
-      <c r="H69" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F69/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G69)</f>
+      <c r="G69" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E69/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F69)</f>
         <v>25612.525981619146</v>
       </c>
+      <c r="H69" s="8">
+        <f t="shared" si="4"/>
+        <v>10.150836806958321</v>
+      </c>
       <c r="I69" s="8">
-        <f>LN(H69)</f>
-        <v>10.150836806958321</v>
-      </c>
-      <c r="J69" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K69" s="8">
-        <f>LN(D69)</f>
+      <c r="J69" s="8">
+        <f t="shared" si="5"/>
         <v>11.1494590781226</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>40</v>
       </c>
       <c r="B70" s="13" t="s">
         <v>366</v>
       </c>
-      <c r="C70" t="s">
-        <v>366</v>
-      </c>
-      <c r="D70" s="21">
+      <c r="C70" s="21">
         <v>27868.589743589699</v>
       </c>
-      <c r="E70" s="15">
+      <c r="D70" s="15">
         <v>1</v>
       </c>
-      <c r="F70">
+      <c r="E70">
         <v>474204750</v>
       </c>
-      <c r="G70" s="16">
+      <c r="F70" s="16">
         <v>13111</v>
       </c>
-      <c r="H70" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F70/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G70)</f>
+      <c r="G70" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E70/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F70)</f>
         <v>22422.724926194216</v>
       </c>
+      <c r="H70" s="8">
+        <f t="shared" si="4"/>
+        <v>10.017830229213747</v>
+      </c>
       <c r="I70" s="8">
-        <f>LN(H70)</f>
-        <v>10.017830229213747</v>
-      </c>
-      <c r="J70" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K70" s="8">
-        <f>LN(D70)</f>
+      <c r="J70" s="8">
+        <f t="shared" si="5"/>
         <v>10.235255517961036</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>62</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>367</v>
       </c>
-      <c r="C71" t="s">
-        <v>367</v>
-      </c>
-      <c r="D71" s="21">
+      <c r="C71" s="21">
         <v>70782.051282051194</v>
       </c>
-      <c r="E71" s="15">
+      <c r="D71" s="15">
         <v>1</v>
       </c>
-      <c r="F71">
+      <c r="E71">
         <v>943420954</v>
       </c>
-      <c r="G71" s="16">
+      <c r="F71" s="16">
         <v>18568</v>
       </c>
-      <c r="H71" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F71/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G71)</f>
+      <c r="G71" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E71/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F71)</f>
         <v>25716.836147528946</v>
       </c>
+      <c r="H71" s="8">
+        <f t="shared" si="4"/>
+        <v>10.154901159413688</v>
+      </c>
       <c r="I71" s="8">
-        <f>LN(H71)</f>
-        <v>10.154901159413688</v>
-      </c>
-      <c r="J71" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K71" s="8">
-        <f>LN(D71)</f>
+      <c r="J71" s="8">
+        <f t="shared" si="5"/>
         <v>11.167360734576588</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>67</v>
       </c>
       <c r="B72" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="C72" t="s">
-        <v>368</v>
-      </c>
-      <c r="D72" s="21">
+      <c r="C72" s="21">
         <v>34376.068376068302</v>
       </c>
-      <c r="E72" s="15">
+      <c r="D72" s="15">
         <v>1</v>
       </c>
-      <c r="F72">
+      <c r="E72">
         <v>627711081.28356099</v>
       </c>
-      <c r="G72" s="16">
+      <c r="F72" s="16">
         <v>26729</v>
       </c>
-      <c r="H72" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F72/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G72)</f>
+      <c r="G72" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E72/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F72)</f>
         <v>19568.783190635524</v>
       </c>
+      <c r="H72" s="8">
+        <f t="shared" si="4"/>
+        <v>9.8816908811772972</v>
+      </c>
       <c r="I72" s="8">
-        <f>LN(H72)</f>
-        <v>9.8816908811772972</v>
-      </c>
-      <c r="J72" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K72" s="8">
-        <f>LN(D72)</f>
+      <c r="J72" s="8">
+        <f t="shared" si="5"/>
         <v>10.445115914516975</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>26</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>369</v>
       </c>
-      <c r="C73" t="s">
-        <v>369</v>
-      </c>
-      <c r="D73" s="21">
+      <c r="C73" s="21">
         <v>38178.571428571398</v>
       </c>
-      <c r="E73" s="15">
+      <c r="D73" s="15">
         <v>1</v>
       </c>
-      <c r="F73">
+      <c r="E73">
         <v>532283575.13797301</v>
       </c>
-      <c r="G73" s="16">
+      <c r="F73" s="16">
         <v>15619</v>
       </c>
-      <c r="H73" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F73/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G73)</f>
+      <c r="G73" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E73/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F73)</f>
         <v>21952.648464852929</v>
       </c>
+      <c r="H73" s="8">
+        <f t="shared" si="4"/>
+        <v>9.9966430702156295</v>
+      </c>
       <c r="I73" s="8">
-        <f>LN(H73)</f>
-        <v>9.9966430702156295</v>
-      </c>
-      <c r="J73" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K73" s="8">
-        <f>LN(D73)</f>
+      <c r="J73" s="8">
+        <f t="shared" si="5"/>
         <v>10.550029679831978</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>65</v>
       </c>
       <c r="B74" s="13" t="s">
         <v>370</v>
       </c>
-      <c r="C74" t="s">
-        <v>370</v>
-      </c>
-      <c r="D74" s="21">
+      <c r="C74" s="21">
         <v>73411.6022099447</v>
       </c>
-      <c r="E74" s="15">
+      <c r="D74" s="15">
         <v>1</v>
       </c>
-      <c r="F74">
+      <c r="E74">
         <v>1662849170</v>
       </c>
-      <c r="G74" s="16">
+      <c r="F74" s="16">
         <v>32649</v>
       </c>
-      <c r="H74" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F74/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G74)</f>
+      <c r="G74" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E74/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F74)</f>
         <v>25744.31322674387</v>
       </c>
+      <c r="H74" s="8">
+        <f t="shared" si="4"/>
+        <v>10.155969036138565</v>
+      </c>
       <c r="I74" s="8">
-        <f>LN(H74)</f>
-        <v>10.155969036138565</v>
-      </c>
-      <c r="J74" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K74" s="8">
-        <f>LN(D74)</f>
+      <c r="J74" s="8">
+        <f t="shared" si="5"/>
         <v>11.203837270366513</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>53</v>
       </c>
       <c r="B75" s="13" t="s">
         <v>371</v>
       </c>
-      <c r="C75" t="s">
-        <v>371</v>
-      </c>
-      <c r="D75" s="21">
+      <c r="C75" s="21">
         <v>50429.6875</v>
       </c>
-      <c r="E75" s="15">
+      <c r="D75" s="15">
         <v>1</v>
       </c>
-      <c r="F75">
+      <c r="E75">
         <v>894063121.09593594</v>
       </c>
-      <c r="G75" s="16">
+      <c r="F75" s="16">
         <v>24470</v>
       </c>
-      <c r="H75" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F75/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G75)</f>
+      <c r="G75" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E75/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F75)</f>
         <v>22505.670263120184</v>
       </c>
+      <c r="H75" s="8">
+        <f t="shared" si="4"/>
+        <v>10.021522568137129</v>
+      </c>
       <c r="I75" s="8">
-        <f>LN(H75)</f>
-        <v>10.021522568137129</v>
-      </c>
-      <c r="J75" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K75" s="8">
-        <f>LN(D75)</f>
+      <c r="J75" s="8">
+        <f t="shared" si="5"/>
         <v>10.828335318343262</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2</v>
       </c>
       <c r="B76" s="13" t="s">
         <v>372</v>
       </c>
-      <c r="C76" t="s">
-        <v>372</v>
-      </c>
-      <c r="D76" s="21">
+      <c r="C76" s="21">
         <v>71524.771024146496</v>
       </c>
-      <c r="E76" s="15">
+      <c r="D76" s="15">
         <v>0.76612380384326129</v>
       </c>
-      <c r="F76">
+      <c r="E76">
         <v>5358863377.8789196</v>
       </c>
-      <c r="G76" s="16">
+      <c r="F76" s="16">
         <v>78227</v>
       </c>
-      <c r="H76" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F76/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G76)</f>
+      <c r="G76" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E76/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F76)</f>
         <v>29698.217919367875</v>
       </c>
+      <c r="H76" s="8">
+        <f t="shared" si="4"/>
+        <v>10.29884232027567</v>
+      </c>
       <c r="I76" s="8">
-        <f>LN(H76)</f>
-        <v>10.29884232027567</v>
-      </c>
-      <c r="J76" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K76" s="8">
-        <f>LN(D76)</f>
+      <c r="J76" s="8">
+        <f t="shared" si="5"/>
         <v>11.177799116573047</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>24</v>
       </c>
       <c r="B77" s="13" t="s">
         <v>373</v>
       </c>
-      <c r="C77" t="s">
-        <v>373</v>
-      </c>
-      <c r="D77" s="21">
+      <c r="C77" s="21">
         <v>134321.966058277</v>
       </c>
-      <c r="E77" s="15">
+      <c r="D77" s="15">
         <v>0.26175368245975783</v>
       </c>
-      <c r="F77">
+      <c r="E77">
         <v>16462631666.2216</v>
       </c>
-      <c r="G77" s="16">
+      <c r="F77" s="16">
         <v>86598</v>
       </c>
-      <c r="H77" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F77/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G77)</f>
+      <c r="G77" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E77/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F77)</f>
         <v>57058.210252934921</v>
       </c>
+      <c r="H77" s="8">
+        <f t="shared" si="4"/>
+        <v>10.951827258221149</v>
+      </c>
       <c r="I77" s="8">
-        <f>LN(H77)</f>
-        <v>10.951827258221149</v>
-      </c>
-      <c r="J77" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K77" s="8">
-        <f>LN(D77)</f>
+      <c r="J77" s="8">
+        <f t="shared" si="5"/>
         <v>11.807994928766673</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>42</v>
       </c>
       <c r="B78" s="13" t="s">
         <v>374</v>
       </c>
-      <c r="C78" t="s">
-        <v>374</v>
-      </c>
-      <c r="D78" s="21">
+      <c r="C78" s="21">
         <v>35029.850746268603</v>
       </c>
-      <c r="E78" s="15">
+      <c r="D78" s="15">
         <v>1</v>
       </c>
-      <c r="F78">
+      <c r="E78">
         <v>1087817372</v>
       </c>
-      <c r="G78" s="16">
+      <c r="F78" s="16">
         <v>23956</v>
       </c>
-      <c r="H78" s="4">
-        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(F78/SUM(F$2:F$78)*FACTORS_MUNI!$F$42/G78)</f>
+      <c r="G78" s="4">
+        <f>(FACTORS_MUNI!$E$42/FACTORS_MUNI!$C$42)+(E78/SUM(E$2:E$78)*FACTORS_MUNI!$F$42/F78)</f>
         <v>24501.837821469911</v>
       </c>
+      <c r="H78" s="8">
+        <f t="shared" si="4"/>
+        <v>10.106503406840696</v>
+      </c>
       <c r="I78" s="8">
-        <f>LN(H78)</f>
-        <v>10.106503406840696</v>
-      </c>
-      <c r="J78" s="8">
         <f>FACTORS_MUNI!$K$42</f>
         <v>14.81159091933654</v>
       </c>
-      <c r="K78" s="8">
-        <f>LN(D78)</f>
+      <c r="J78" s="8">
+        <f t="shared" si="5"/>
         <v>10.463955855442192</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K78" xr:uid="{00000000-0001-0000-0100-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K78">
+  <autoFilter ref="A1:J78" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J78">
       <sortCondition ref="B1:B78"/>
     </sortState>
   </autoFilter>
@@ -18336,7 +18098,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="18"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18345,8 +18107,8 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="15" id="{A36205D5-D3BC-40FB-8028-6B3A6753CC9E}">
-            <xm:f>AND(ISNA(HLOOKUP(A2, FACTORS_CCA!$D$1:$XFD$1, 1, FALSE)), A2&lt;&gt;"")</xm:f>
+          <x14:cfRule type="expression" priority="17" id="{A36205D5-D3BC-40FB-8028-6B3A6753CC9E}">
+            <xm:f>AND(ISNA(HLOOKUP(A2, FACTORS_CCA!$C$1:$XFD$1, 1, FALSE)), A2&lt;&gt;"")</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF800000"/>

</xml_diff>

<commit_message>
modify PCT POP EDA/DA factor for muni and CCA
changing factor from % POP in EDA or DA to % POP in DA alone
</commit_message>
<xml_diff>
--- a/input/community_cohort_inputs.xlsx
+++ b/input/community_cohort_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amcadams\GitHub\community-cohort-tool\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47715D48-2FEC-4A66-B564-182B09793966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83DD2BA-29A2-4EBF-BCD0-21C7380AB117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15690" yWindow="-15420" windowWidth="24720" windowHeight="14430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FACTORS_MUNI" sheetId="1" r:id="rId1"/>
@@ -161,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{37C7737E-3758-43A8-AE1D-AFE76001D2BC}">
       <text>
         <r>
           <rPr>
@@ -358,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{4068B7E3-F99F-4C68-8235-67F35C13E64E}">
       <text>
         <r>
           <rPr>
@@ -377,7 +377,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> Percent of population living in an EDA or disinvested area, calculated from 2020 Census block centroids and EDA/disinvested layer</t>
+          <t xml:space="preserve"> Percent of population living in an disinvested area, calculated from 2020 Census block centroids and ON TO 2050 disinvested areas layer</t>
         </r>
       </text>
     </comment>
@@ -772,9 +772,6 @@
     <t>TOT_EAV</t>
   </si>
   <si>
-    <t>PCT_EDA_POP</t>
-  </si>
-  <si>
     <t>TAX_BASE</t>
   </si>
   <si>
@@ -1892,6 +1889,9 @@
   </si>
   <si>
     <t>TOT_MARKET_VAL</t>
+  </si>
+  <si>
+    <t>PCT_DA_POP</t>
   </si>
 </sst>
 </file>
@@ -2556,8 +2556,8 @@
     <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="21" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="21" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="21" fillId="34" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2909,8 +2909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L285"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2920,7 +2920,7 @@
     <col min="3" max="3" width="8" style="10" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" style="11" customWidth="1"/>
     <col min="5" max="6" width="12" style="11" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" style="9" customWidth="1"/>
     <col min="8" max="8" width="13.109375" style="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.6640625" style="8" bestFit="1" customWidth="1"/>
@@ -2948,22 +2948,22 @@
         <v>5</v>
       </c>
       <c r="G1" s="18" t="s">
+        <v>379</v>
+      </c>
+      <c r="H1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="L1" s="7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -2971,7 +2971,7 @@
         <v>1700243</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>35470</v>
@@ -2986,7 +2986,7 @@
         <v>1530498318</v>
       </c>
       <c r="G2" s="9">
-        <v>0.5683715198028122</v>
+        <v>0</v>
       </c>
       <c r="H2" s="20">
         <f t="shared" ref="H2:H65" si="0">E2+F2</f>
@@ -3014,7 +3014,7 @@
         <v>1700685</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>29904</v>
@@ -3057,7 +3057,7 @@
         <v>1701010</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>18650</v>
@@ -3072,7 +3072,7 @@
         <v>835589144</v>
       </c>
       <c r="G4" s="9">
-        <v>2.2556785395792898E-2</v>
+        <v>0</v>
       </c>
       <c r="H4" s="20">
         <f t="shared" si="0"/>
@@ -3100,7 +3100,7 @@
         <v>1701595</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>14751</v>
@@ -3143,7 +3143,7 @@
         <v>1702154</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>76220</v>
@@ -3158,7 +3158,7 @@
         <v>3846327521</v>
       </c>
       <c r="G6" s="9">
-        <v>0.17019413976002884</v>
+        <v>0.11417941191616458</v>
       </c>
       <c r="H6" s="20">
         <f t="shared" si="0"/>
@@ -3186,7 +3186,7 @@
         <v>1703012</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>179867</v>
@@ -3201,7 +3201,7 @@
         <v>5231224008</v>
       </c>
       <c r="G7" s="9">
-        <v>0.62980359140809339</v>
+        <v>0.4095667490113104</v>
       </c>
       <c r="H7" s="20">
         <f t="shared" si="0"/>
@@ -3229,7 +3229,7 @@
         <v>1703610</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>1125</v>
@@ -3272,7 +3272,7 @@
         <v>1703844</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>11049</v>
@@ -3315,7 +3315,7 @@
         <v>1703883</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>3923</v>
@@ -3358,7 +3358,7 @@
         <v>1704013</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11">
         <v>40531</v>
@@ -3373,7 +3373,7 @@
         <v>1509188932</v>
       </c>
       <c r="G11" s="9">
-        <v>0.18829826055224425</v>
+        <v>0.14733000851477923</v>
       </c>
       <c r="H11" s="20">
         <f t="shared" si="0"/>
@@ -3401,7 +3401,7 @@
         <v>1704078</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>26730</v>
@@ -3444,7 +3444,7 @@
         <v>1704303</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>13988</v>
@@ -3459,7 +3459,7 @@
         <v>286693852</v>
       </c>
       <c r="G13" s="9">
-        <v>9.1725735139308026E-2</v>
+        <v>7.3268299529791567E-2</v>
       </c>
       <c r="H13" s="20">
         <f t="shared" si="0"/>
@@ -3487,7 +3487,7 @@
         <v>1704572</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>594</v>
@@ -3502,7 +3502,7 @@
         <v>657214482</v>
       </c>
       <c r="G14" s="9">
-        <v>2.3255813953488372E-2</v>
+        <v>0</v>
       </c>
       <c r="H14" s="20">
         <f t="shared" si="0"/>
@@ -3530,7 +3530,7 @@
         <v>1704585</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <v>4837</v>
@@ -3573,7 +3573,7 @@
         <v>1704975</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16">
         <v>18373</v>
@@ -3588,7 +3588,7 @@
         <v>309346201</v>
       </c>
       <c r="G16" s="9">
-        <v>0.83186971100111773</v>
+        <v>0.53861301825536223</v>
       </c>
       <c r="H16" s="20">
         <f t="shared" si="0"/>
@@ -3616,7 +3616,7 @@
         <v>1705248</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17">
         <v>18576</v>
@@ -3631,7 +3631,7 @@
         <v>740546705</v>
       </c>
       <c r="G17" s="9">
-        <v>0.25663105299526923</v>
+        <v>0</v>
       </c>
       <c r="H17" s="20">
         <f t="shared" si="0"/>
@@ -3659,7 +3659,7 @@
         <v>1705404</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18">
         <v>5222</v>
@@ -3702,7 +3702,7 @@
         <v>1705573</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19">
         <v>55888</v>
@@ -3717,7 +3717,7 @@
         <v>1058995569</v>
       </c>
       <c r="G19" s="9">
-        <v>0.72496069868995638</v>
+        <v>0.64953711790393009</v>
       </c>
       <c r="H19" s="20">
         <f t="shared" si="0"/>
@@ -3745,7 +3745,7 @@
         <v>1705976</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20">
         <v>1208</v>
@@ -3788,7 +3788,7 @@
         <v>1706587</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21">
         <v>22388</v>
@@ -3803,7 +3803,7 @@
         <v>1046744575</v>
       </c>
       <c r="G21" s="9">
-        <v>0.12523456348851755</v>
+        <v>0</v>
       </c>
       <c r="H21" s="20">
         <f t="shared" si="0"/>
@@ -3831,7 +3831,7 @@
         <v>1706704</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22">
         <v>23416</v>
@@ -3846,7 +3846,7 @@
         <v>344449342</v>
       </c>
       <c r="G22" s="9">
-        <v>1</v>
+        <v>0.43111091408812841</v>
       </c>
       <c r="H22" s="20">
         <f t="shared" si="0"/>
@@ -3874,7 +3874,7 @@
         <v>1707133</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23">
         <v>73813</v>
@@ -3889,7 +3889,7 @@
         <v>2805344734</v>
       </c>
       <c r="G23" s="9">
-        <v>0.25710884445767163</v>
+        <v>0.124252590568437</v>
       </c>
       <c r="H23" s="20">
         <f t="shared" si="0"/>
@@ -3917,7 +3917,7 @@
         <v>1707640</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24">
         <v>890</v>
@@ -3960,7 +3960,7 @@
         <v>1707770</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25">
         <v>6175</v>
@@ -4003,7 +4003,7 @@
         <v>1708225</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26">
         <v>16721</v>
@@ -4018,7 +4018,7 @@
         <v>611862921</v>
       </c>
       <c r="G26" s="9">
-        <v>0.30275444881658542</v>
+        <v>0</v>
       </c>
       <c r="H26" s="20">
         <f t="shared" si="0"/>
@@ -4046,7 +4046,7 @@
         <v>1708446</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27">
         <v>7898</v>
@@ -4089,7 +4089,7 @@
         <v>1708576</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28">
         <v>19235</v>
@@ -4132,7 +4132,7 @@
         <v>1709447</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29">
         <v>42824</v>
@@ -4147,7 +4147,7 @@
         <v>1912208695</v>
       </c>
       <c r="G29" s="9">
-        <v>4.30435990002777E-3</v>
+        <v>4.1655095806720352E-3</v>
       </c>
       <c r="H29" s="20">
         <f t="shared" si="0"/>
@@ -4175,7 +4175,7 @@
         <v>1709531</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C30">
         <v>1121</v>
@@ -4218,7 +4218,7 @@
         <v>1709642</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31">
         <v>28822</v>
@@ -4233,7 +4233,7 @@
         <v>677412001</v>
       </c>
       <c r="G31" s="9">
-        <v>0.6628961581575461</v>
+        <v>0.19579469411325112</v>
       </c>
       <c r="H31" s="20">
         <f t="shared" si="0"/>
@@ -4261,7 +4261,7 @@
         <v>1709759</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C32">
         <v>479</v>
@@ -4304,7 +4304,7 @@
         <v>1709798</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C33">
         <v>3978</v>
@@ -4319,7 +4319,7 @@
         <v>67587939</v>
       </c>
       <c r="G33" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" s="20">
         <f t="shared" si="0"/>
@@ -4347,7 +4347,7 @@
         <v>1709980</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34">
         <v>11119</v>
@@ -4390,7 +4390,7 @@
         <v>1710487</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C35">
         <v>35253</v>
@@ -4405,7 +4405,7 @@
         <v>459527750</v>
       </c>
       <c r="G35" s="9">
-        <v>1</v>
+        <v>0.40934698748369552</v>
       </c>
       <c r="H35" s="20">
         <f t="shared" si="0"/>
@@ -4433,7 +4433,7 @@
         <v>1710513</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C36">
         <v>6836</v>
@@ -4448,7 +4448,7 @@
         <v>99930455</v>
       </c>
       <c r="G36" s="9">
-        <v>0.54448398576512458</v>
+        <v>0.40854092526690389</v>
       </c>
       <c r="H36" s="20">
         <f t="shared" si="0"/>
@@ -4476,7 +4476,7 @@
         <v>1710906</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C37">
         <v>10724</v>
@@ -4519,7 +4519,7 @@
         <v>1711332</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38">
         <v>39427</v>
@@ -4534,7 +4534,7 @@
         <v>1562972232</v>
       </c>
       <c r="G38" s="9">
-        <v>0.16685903547950018</v>
+        <v>0</v>
       </c>
       <c r="H38" s="20">
         <f t="shared" si="0"/>
@@ -4562,7 +4562,7 @@
         <v>1711358</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39">
         <v>37544</v>
@@ -4577,7 +4577,7 @@
         <v>804200060</v>
       </c>
       <c r="G39" s="9">
-        <v>0.72645657267725039</v>
+        <v>0.42089882315772847</v>
       </c>
       <c r="H39" s="20">
         <f t="shared" si="0"/>
@@ -4605,7 +4605,7 @@
         <v>1711592</v>
       </c>
       <c r="B40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C40">
         <v>17875</v>
@@ -4648,7 +4648,7 @@
         <v>1712476</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C41">
         <v>13854</v>
@@ -4691,7 +4691,7 @@
         <v>1714000</v>
       </c>
       <c r="B42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C42">
         <v>2707648</v>
@@ -4706,7 +4706,7 @@
         <v>99651574461</v>
       </c>
       <c r="G42" s="9">
-        <v>0.62405129937940307</v>
+        <v>0.30133542674960712</v>
       </c>
       <c r="H42" s="20">
         <f t="shared" si="0"/>
@@ -4734,7 +4734,7 @@
         <v>1714026</v>
       </c>
       <c r="B43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43">
         <v>26938</v>
@@ -4749,7 +4749,7 @@
         <v>436860152</v>
       </c>
       <c r="G43" s="9">
-        <v>0.77678311499272201</v>
+        <v>0.61677583697234351</v>
       </c>
       <c r="H43" s="20">
         <f t="shared" si="0"/>
@@ -4777,7 +4777,7 @@
         <v>1714065</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C44">
         <v>14147</v>
@@ -4792,7 +4792,7 @@
         <v>388087052</v>
       </c>
       <c r="G44" s="9">
-        <v>0.57756530173907017</v>
+        <v>0</v>
       </c>
       <c r="H44" s="20">
         <f t="shared" si="0"/>
@@ -4820,7 +4820,7 @@
         <v>1714351</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C45">
         <v>83223</v>
@@ -4835,7 +4835,7 @@
         <v>1071067761</v>
       </c>
       <c r="G45" s="9">
-        <v>1</v>
+        <v>0.77353755218839426</v>
       </c>
       <c r="H45" s="20">
         <f t="shared" si="0"/>
@@ -4863,7 +4863,7 @@
         <v>1714572</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46">
         <v>8642</v>
@@ -4906,7 +4906,7 @@
         <v>1715170</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C47">
         <v>5145</v>
@@ -4949,7 +4949,7 @@
         <v>1716691</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C48">
         <v>16419</v>
@@ -4964,7 +4964,7 @@
         <v>297853210</v>
       </c>
       <c r="G48" s="9">
-        <v>0.43540983606557376</v>
+        <v>0.11678092399403875</v>
       </c>
       <c r="H48" s="20">
         <f t="shared" si="0"/>
@@ -4992,7 +4992,7 @@
         <v>1716873</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C49">
         <v>6294</v>
@@ -5035,7 +5035,7 @@
         <v>1717458</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C50">
         <v>19754</v>
@@ -5078,7 +5078,7 @@
         <v>1717497</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C51">
         <v>10622</v>
@@ -5093,7 +5093,7 @@
         <v>422508589</v>
       </c>
       <c r="G51" s="9">
-        <v>0.14049510437834842</v>
+        <v>0</v>
       </c>
       <c r="H51" s="20">
         <f t="shared" si="0"/>
@@ -5121,7 +5121,7 @@
         <v>1717523</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C52">
         <v>8382</v>
@@ -5164,7 +5164,7 @@
         <v>1717887</v>
       </c>
       <c r="B53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C53">
         <v>40436</v>
@@ -5207,7 +5207,7 @@
         <v>1718628</v>
       </c>
       <c r="B54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C54">
         <v>21855</v>
@@ -5250,7 +5250,7 @@
         <v>1719083</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C55">
         <v>3711</v>
@@ -5293,7 +5293,7 @@
         <v>1718992</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C56">
         <v>19185</v>
@@ -5336,7 +5336,7 @@
         <v>1719642</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C57">
         <v>59408</v>
@@ -5351,7 +5351,7 @@
         <v>2815046596</v>
       </c>
       <c r="G57" s="9">
-        <v>0.14597445405850845</v>
+        <v>1.03831891223733E-2</v>
       </c>
       <c r="H57" s="20">
         <f t="shared" si="0"/>
@@ -5379,7 +5379,7 @@
         <v>1719837</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C58">
         <v>2900</v>
@@ -5422,7 +5422,7 @@
         <v>1720149</v>
       </c>
       <c r="B59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C59">
         <v>2962</v>
@@ -5437,7 +5437,7 @@
         <v>41233715</v>
       </c>
       <c r="G59" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H59" s="20">
         <f t="shared" si="0"/>
@@ -5465,7 +5465,7 @@
         <v>1720292</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C60">
         <v>20979</v>
@@ -5480,7 +5480,7 @@
         <v>300510446</v>
       </c>
       <c r="G60" s="9">
-        <v>1</v>
+        <v>0.60491925697750393</v>
       </c>
       <c r="H60" s="20">
         <f t="shared" si="0"/>
@@ -5508,7 +5508,7 @@
         <v>1720591</v>
       </c>
       <c r="B61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C61">
         <v>49867</v>
@@ -5551,7 +5551,7 @@
         <v>1721696</v>
       </c>
       <c r="B62" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C62">
         <v>3156</v>
@@ -5566,7 +5566,7 @@
         <v>132226120</v>
       </c>
       <c r="G62" s="9">
-        <v>6.9796954314720813E-3</v>
+        <v>0</v>
       </c>
       <c r="H62" s="20">
         <f t="shared" si="0"/>
@@ -5594,7 +5594,7 @@
         <v>1721904</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C63">
         <v>1122</v>
@@ -5637,7 +5637,7 @@
         <v>1722931</v>
       </c>
       <c r="B64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C64">
         <v>6054</v>
@@ -5680,7 +5680,7 @@
         <v>1723074</v>
       </c>
       <c r="B65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C65">
         <v>114106</v>
@@ -5695,7 +5695,7 @@
         <v>3548670387</v>
       </c>
       <c r="G65" s="9">
-        <v>0.5655287159072101</v>
+        <v>0.35435595006838155</v>
       </c>
       <c r="H65" s="20">
         <f t="shared" si="0"/>
@@ -5723,7 +5723,7 @@
         <v>1723256</v>
       </c>
       <c r="B66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C66">
         <v>32132</v>
@@ -5766,7 +5766,7 @@
         <v>1723620</v>
       </c>
       <c r="B67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C67">
         <v>45538</v>
@@ -5809,7 +5809,7 @@
         <v>1723724</v>
       </c>
       <c r="B68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C68">
         <v>23982</v>
@@ -5852,7 +5852,7 @@
         <v>1723945</v>
       </c>
       <c r="B69" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C69">
         <v>2141</v>
@@ -5895,7 +5895,7 @@
         <v>1724582</v>
       </c>
       <c r="B70" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C70">
         <v>76552</v>
@@ -5910,7 +5910,7 @@
         <v>3845100807</v>
       </c>
       <c r="G70" s="9">
-        <v>7.9656894123671745E-2</v>
+        <v>0</v>
       </c>
       <c r="H70" s="20">
         <f t="shared" si="5"/>
@@ -5938,7 +5938,7 @@
         <v>1724634</v>
       </c>
       <c r="B71" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C71">
         <v>19498</v>
@@ -5981,7 +5981,7 @@
         <v>1726571</v>
       </c>
       <c r="B72" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C72">
         <v>9666</v>
@@ -6024,7 +6024,7 @@
         <v>1726710</v>
       </c>
       <c r="B73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C73">
         <v>1587</v>
@@ -6039,7 +6039,7 @@
         <v>18987009</v>
       </c>
       <c r="G73" s="9">
-        <v>1</v>
+        <v>1.26861555432984E-2</v>
       </c>
       <c r="H73" s="20">
         <f t="shared" si="5"/>
@@ -6067,7 +6067,7 @@
         <v>1726935</v>
       </c>
       <c r="B74" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C74">
         <v>14000</v>
@@ -6110,7 +6110,7 @@
         <v>1726987</v>
       </c>
       <c r="B75" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C75">
         <v>1022</v>
@@ -6153,7 +6153,7 @@
         <v>1727442</v>
       </c>
       <c r="B76" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C76">
         <v>10872</v>
@@ -6196,7 +6196,7 @@
         <v>1727533</v>
       </c>
       <c r="B77" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C77">
         <v>4501</v>
@@ -6239,7 +6239,7 @@
         <v>1727624</v>
       </c>
       <c r="B78" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C78">
         <v>20417</v>
@@ -6282,7 +6282,7 @@
         <v>1727702</v>
       </c>
       <c r="B79" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C79">
         <v>18233</v>
@@ -6297,7 +6297,7 @@
         <v>1152489115</v>
       </c>
       <c r="G79" s="9">
-        <v>7.0179238641901773E-2</v>
+        <v>0</v>
       </c>
       <c r="H79" s="20">
         <f t="shared" si="5"/>
@@ -6325,7 +6325,7 @@
         <v>1728872</v>
       </c>
       <c r="B80" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C80">
         <v>21299</v>
@@ -6368,7 +6368,7 @@
         <v>1729171</v>
       </c>
       <c r="B81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C81">
         <v>8389</v>
@@ -6411,7 +6411,7 @@
         <v>1729756</v>
       </c>
       <c r="B82" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C82">
         <v>28270</v>
@@ -6426,7 +6426,7 @@
         <v>1712572298</v>
       </c>
       <c r="G82" s="9">
-        <v>8.7741801289606874E-2</v>
+        <v>0</v>
       </c>
       <c r="H82" s="20">
         <f t="shared" si="5"/>
@@ -6454,7 +6454,7 @@
         <v>1729652</v>
       </c>
       <c r="B83" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C83">
         <v>8715</v>
@@ -6497,7 +6497,7 @@
         <v>1729730</v>
       </c>
       <c r="B84" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C84">
         <v>32864</v>
@@ -6512,7 +6512,7 @@
         <v>937886760</v>
       </c>
       <c r="G84" s="9">
-        <v>0.32653122739329637</v>
+        <v>0</v>
       </c>
       <c r="H84" s="20">
         <f t="shared" si="5"/>
@@ -6540,7 +6540,7 @@
         <v>1729938</v>
       </c>
       <c r="B85" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C85">
         <v>47682</v>
@@ -6555,7 +6555,7 @@
         <v>3893390163</v>
       </c>
       <c r="G85" s="9">
-        <v>7.2703007904732581E-2</v>
+        <v>0</v>
       </c>
       <c r="H85" s="20">
         <f t="shared" si="5"/>
@@ -6583,7 +6583,7 @@
         <v>1730029</v>
       </c>
       <c r="B86" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C86">
         <v>8620</v>
@@ -6626,7 +6626,7 @@
         <v>1730120</v>
       </c>
       <c r="B87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C87">
         <v>538</v>
@@ -6669,7 +6669,7 @@
         <v>1730328</v>
       </c>
       <c r="B88" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C88">
         <v>548</v>
@@ -6712,7 +6712,7 @@
         <v>1731121</v>
       </c>
       <c r="B89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C89">
         <v>20707</v>
@@ -6727,7 +6727,7 @@
         <v>727564291</v>
       </c>
       <c r="G89" s="9">
-        <v>0.1706042921686747</v>
+        <v>0.16862763554216867</v>
       </c>
       <c r="H89" s="20">
         <f t="shared" si="5"/>
@@ -6755,7 +6755,7 @@
         <v>1731446</v>
       </c>
       <c r="B90" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C90">
         <v>4085</v>
@@ -6798,7 +6798,7 @@
         <v>1731667</v>
       </c>
       <c r="B91" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C91">
         <v>559</v>
@@ -6841,7 +6841,7 @@
         <v>1732018</v>
       </c>
       <c r="B92" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C92">
         <v>30486</v>
@@ -6856,7 +6856,7 @@
         <v>1325717325</v>
       </c>
       <c r="G92" s="9">
-        <v>8.7930697583534162E-4</v>
+        <v>0</v>
       </c>
       <c r="H92" s="20">
         <f t="shared" si="5"/>
@@ -6884,7 +6884,7 @@
         <v>1732200</v>
       </c>
       <c r="B93" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C93">
         <v>3524</v>
@@ -6899,7 +6899,7 @@
         <v>88103851</v>
       </c>
       <c r="G93" s="9">
-        <v>0.40862944162436549</v>
+        <v>0.40439932318104904</v>
       </c>
       <c r="H93" s="20">
         <f t="shared" si="5"/>
@@ -6927,7 +6927,7 @@
         <v>1732525</v>
       </c>
       <c r="B94" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C94">
         <v>8351</v>
@@ -6970,7 +6970,7 @@
         <v>1732746</v>
       </c>
       <c r="B95" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C95">
         <v>36850</v>
@@ -6985,7 +6985,7 @@
         <v>874979819</v>
       </c>
       <c r="G95" s="9">
-        <v>0.43509474246063518</v>
+        <v>0.19661062183079797</v>
       </c>
       <c r="H95" s="20">
         <f t="shared" si="5"/>
@@ -7013,7 +7013,7 @@
         <v>1733331</v>
       </c>
       <c r="B96" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C96">
         <v>9875</v>
@@ -7028,7 +7028,7 @@
         <v>168040274</v>
       </c>
       <c r="G96" s="9">
-        <v>0.81856584644629848</v>
+        <v>0</v>
       </c>
       <c r="H96" s="20">
         <f t="shared" si="5"/>
@@ -7056,7 +7056,7 @@
         <v>1733383</v>
       </c>
       <c r="B97" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C97">
         <v>19831</v>
@@ -7071,7 +7071,7 @@
         <v>257717248</v>
       </c>
       <c r="G97" s="9">
-        <v>1</v>
+        <v>0.53690218460932893</v>
       </c>
       <c r="H97" s="20">
         <f t="shared" si="5"/>
@@ -7099,7 +7099,7 @@
         <v>1733435</v>
       </c>
       <c r="B98" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C98">
         <v>8851</v>
@@ -7142,7 +7142,7 @@
         <v>1733630</v>
       </c>
       <c r="B99" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C99">
         <v>9145</v>
@@ -7185,7 +7185,7 @@
         <v>1733695</v>
       </c>
       <c r="B100" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C100">
         <v>13493</v>
@@ -7200,7 +7200,7 @@
         <v>222154507</v>
       </c>
       <c r="G100" s="9">
-        <v>0.61717232102824693</v>
+        <v>0.2873262591540876</v>
       </c>
       <c r="H100" s="20">
         <f t="shared" si="5"/>
@@ -7228,7 +7228,7 @@
         <v>1733851</v>
       </c>
       <c r="B101" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C101">
         <v>1458</v>
@@ -7271,7 +7271,7 @@
         <v>1734514</v>
       </c>
       <c r="B102" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C102">
         <v>14718</v>
@@ -7286,7 +7286,7 @@
         <v>398322791</v>
       </c>
       <c r="G102" s="9">
-        <v>0.34036539124439846</v>
+        <v>0</v>
       </c>
       <c r="H102" s="20">
         <f t="shared" si="5"/>
@@ -7314,7 +7314,7 @@
         <v>1734722</v>
       </c>
       <c r="B103" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C103">
         <v>30229</v>
@@ -7329,7 +7329,7 @@
         <v>2580489664</v>
       </c>
       <c r="G103" s="9">
-        <v>1.193001060445387E-2</v>
+        <v>0</v>
       </c>
       <c r="H103" s="20">
         <f t="shared" si="5"/>
@@ -7357,7 +7357,7 @@
         <v>1734865</v>
       </c>
       <c r="B104" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C104">
         <v>5243</v>
@@ -7372,7 +7372,7 @@
         <v>166254157</v>
       </c>
       <c r="G104" s="9">
-        <v>0.98561292865589278</v>
+        <v>0</v>
       </c>
       <c r="H104" s="20">
         <f t="shared" si="5"/>
@@ -7400,7 +7400,7 @@
         <v>1735086</v>
       </c>
       <c r="B105" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C105">
         <v>8133</v>
@@ -7443,7 +7443,7 @@
         <v>1735307</v>
       </c>
       <c r="B106" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C106">
         <v>17155</v>
@@ -7486,7 +7486,7 @@
         <v>1735385</v>
       </c>
       <c r="B107" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C107">
         <v>1766</v>
@@ -7529,7 +7529,7 @@
         <v>1735411</v>
       </c>
       <c r="B108" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C108">
         <v>51186</v>
@@ -7544,7 +7544,7 @@
         <v>1991155078</v>
       </c>
       <c r="G108" s="9">
-        <v>9.9961926518180089E-2</v>
+        <v>3.0515895678659814E-2</v>
       </c>
       <c r="H108" s="20">
         <f t="shared" si="5"/>
@@ -7572,7 +7572,7 @@
         <v>1735515</v>
       </c>
       <c r="B109" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C109">
         <v>662</v>
@@ -7615,7 +7615,7 @@
         <v>1735835</v>
       </c>
       <c r="B110" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C110">
         <v>24516</v>
@@ -7658,7 +7658,7 @@
         <v>1735866</v>
       </c>
       <c r="B111" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C111">
         <v>4244</v>
@@ -7701,7 +7701,7 @@
         <v>1735879</v>
       </c>
       <c r="B112" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C112">
         <v>19471</v>
@@ -7716,7 +7716,7 @@
         <v>522253881</v>
       </c>
       <c r="G112" s="9">
-        <v>0.34896984020962851</v>
+        <v>0.23973693675178545</v>
       </c>
       <c r="H112" s="20">
         <f t="shared" si="5"/>
@@ -7744,7 +7744,7 @@
         <v>1736750</v>
       </c>
       <c r="B113" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C113">
         <v>27859</v>
@@ -7787,7 +7787,7 @@
         <v>1737218</v>
       </c>
       <c r="B114" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C114">
         <v>892</v>
@@ -7830,7 +7830,7 @@
         <v>1737257</v>
       </c>
       <c r="B115" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C115">
         <v>3992</v>
@@ -7873,7 +7873,7 @@
         <v>1737608</v>
       </c>
       <c r="B116" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C116">
         <v>7541</v>
@@ -7916,7 +7916,7 @@
         <v>1737894</v>
       </c>
       <c r="B117" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C117">
         <v>8023</v>
@@ -7959,7 +7959,7 @@
         <v>1737907</v>
       </c>
       <c r="B118" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C118">
         <v>9525</v>
@@ -8002,7 +8002,7 @@
         <v>1738479</v>
       </c>
       <c r="B119" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C119">
         <v>6374</v>
@@ -8045,7 +8045,7 @@
         <v>1738570</v>
       </c>
       <c r="B120" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C120">
         <v>149785</v>
@@ -8060,7 +8060,7 @@
         <v>4252403083</v>
       </c>
       <c r="G120" s="9">
-        <v>0.38476476769396523</v>
+        <v>0.3251885449781195</v>
       </c>
       <c r="H120" s="20">
         <f t="shared" si="5"/>
@@ -8088,7 +8088,7 @@
         <v>1738830</v>
       </c>
       <c r="B121" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C121">
         <v>12372</v>
@@ -8103,7 +8103,7 @@
         <v>217385463</v>
       </c>
       <c r="G121" s="9">
-        <v>0.54738095238095241</v>
+        <v>0</v>
       </c>
       <c r="H121" s="20">
         <f t="shared" si="5"/>
@@ -8131,7 +8131,7 @@
         <v>1738895</v>
       </c>
       <c r="B122" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C122">
         <v>615</v>
@@ -8174,7 +8174,7 @@
         <v>1739519</v>
       </c>
       <c r="B123" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C123">
         <v>2543</v>
@@ -8217,7 +8217,7 @@
         <v>1739883</v>
       </c>
       <c r="B124" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C124">
         <v>4189</v>
@@ -8260,7 +8260,7 @@
         <v>1740767</v>
       </c>
       <c r="B125" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C125">
         <v>15999</v>
@@ -8303,7 +8303,7 @@
         <v>1740793</v>
       </c>
       <c r="B126" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C126">
         <v>13227</v>
@@ -8346,7 +8346,7 @@
         <v>1740884</v>
       </c>
       <c r="B127" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C127">
         <v>5400</v>
@@ -8389,7 +8389,7 @@
         <v>1740910</v>
       </c>
       <c r="B128" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C128">
         <v>5834</v>
@@ -8432,7 +8432,7 @@
         <v>1741105</v>
       </c>
       <c r="B129" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C129">
         <v>19190</v>
@@ -8475,7 +8475,7 @@
         <v>1741183</v>
       </c>
       <c r="B130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C130">
         <v>28853</v>
@@ -8518,7 +8518,7 @@
         <v>1741586</v>
       </c>
       <c r="B131" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C131">
         <v>8707</v>
@@ -8561,7 +8561,7 @@
         <v>1741742</v>
       </c>
       <c r="B132" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C132">
         <v>19727</v>
@@ -8604,7 +8604,7 @@
         <v>1741326</v>
       </c>
       <c r="B133" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C133">
         <v>5878</v>
@@ -8647,7 +8647,7 @@
         <v>1741651</v>
       </c>
       <c r="B134" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C134">
         <v>4699</v>
@@ -8690,7 +8690,7 @@
         <v>1742028</v>
       </c>
       <c r="B135" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C135">
         <v>28415</v>
@@ -8705,7 +8705,7 @@
         <v>523192427</v>
       </c>
       <c r="G135" s="9">
-        <v>0.5263103590590178</v>
+        <v>0.15242811941119824</v>
       </c>
       <c r="H135" s="20">
         <f t="shared" si="10"/>
@@ -8733,7 +8733,7 @@
         <v>1742795</v>
       </c>
       <c r="B136" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C136">
         <v>17643</v>
@@ -8776,7 +8776,7 @@
         <v>1743250</v>
       </c>
       <c r="B137" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C137">
         <v>20493</v>
@@ -8819,7 +8819,7 @@
         <v>1743406</v>
       </c>
       <c r="B138" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C138">
         <v>1432</v>
@@ -8862,7 +8862,7 @@
         <v>1743666</v>
       </c>
       <c r="B139" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C139">
         <v>7937</v>
@@ -8905,7 +8905,7 @@
         <v>1743744</v>
       </c>
       <c r="B140" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C140">
         <v>13179</v>
@@ -8948,7 +8948,7 @@
         <v>1743770</v>
       </c>
       <c r="B141" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C141">
         <v>14365</v>
@@ -8991,7 +8991,7 @@
         <v>1743900</v>
       </c>
       <c r="B142" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C142">
         <v>300</v>
@@ -9034,7 +9034,7 @@
         <v>1743939</v>
       </c>
       <c r="B143" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C143">
         <v>23413</v>
@@ -9077,7 +9077,7 @@
         <v>1744225</v>
       </c>
       <c r="B144" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C144">
         <v>26228</v>
@@ -9092,7 +9092,7 @@
         <v>1020180913</v>
       </c>
       <c r="G144" s="9">
-        <v>9.1591936843718868E-3</v>
+        <v>0</v>
       </c>
       <c r="H144" s="20">
         <f t="shared" si="10"/>
@@ -9120,7 +9120,7 @@
         <v>1744407</v>
       </c>
       <c r="B145" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C145">
         <v>43722</v>
@@ -9135,7 +9135,7 @@
         <v>1881677101</v>
       </c>
       <c r="G145" s="9">
-        <v>0.3023653206223581</v>
+        <v>0.28480528824534579</v>
       </c>
       <c r="H145" s="20">
         <f t="shared" si="10"/>
@@ -9163,7 +9163,7 @@
         <v>1744524</v>
       </c>
       <c r="B146" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C146">
         <v>8266</v>
@@ -9206,7 +9206,7 @@
         <v>1745421</v>
       </c>
       <c r="B147" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C147">
         <v>9047</v>
@@ -9221,7 +9221,7 @@
         <v>214273069</v>
       </c>
       <c r="G147" s="9">
-        <v>1</v>
+        <v>3.0057042562527423E-2</v>
       </c>
       <c r="H147" s="20">
         <f t="shared" si="10"/>
@@ -9249,7 +9249,7 @@
         <v>1745434</v>
       </c>
       <c r="B148" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C148">
         <v>10391</v>
@@ -9264,7 +9264,7 @@
         <v>248897323</v>
       </c>
       <c r="G148" s="9">
-        <v>0.56891929370435423</v>
+        <v>0</v>
       </c>
       <c r="H148" s="20">
         <f t="shared" si="10"/>
@@ -9292,7 +9292,7 @@
         <v>1746357</v>
       </c>
       <c r="B149" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C149">
         <v>10315</v>
@@ -9335,7 +9335,7 @@
         <v>1746604</v>
       </c>
       <c r="B150" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C150">
         <v>1939</v>
@@ -9378,7 +9378,7 @@
         <v>1746786</v>
       </c>
       <c r="B151" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C151">
         <v>7123</v>
@@ -9421,7 +9421,7 @@
         <v>1747007</v>
       </c>
       <c r="B152" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C152">
         <v>11434</v>
@@ -9436,7 +9436,7 @@
         <v>180335648</v>
       </c>
       <c r="G152" s="9">
-        <v>1</v>
+        <v>2.6412829088414372E-2</v>
       </c>
       <c r="H152" s="20">
         <f t="shared" si="10"/>
@@ -9464,7 +9464,7 @@
         <v>1747540</v>
       </c>
       <c r="B153" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C153">
         <v>18681</v>
@@ -9507,7 +9507,7 @@
         <v>1747774</v>
       </c>
       <c r="B154" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C154">
         <v>23173</v>
@@ -9550,7 +9550,7 @@
         <v>1745564</v>
       </c>
       <c r="B155" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C155">
         <v>299</v>
@@ -9593,7 +9593,7 @@
         <v>1745616</v>
       </c>
       <c r="B156" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C156">
         <v>1087</v>
@@ -9636,7 +9636,7 @@
         <v>1745694</v>
       </c>
       <c r="B157" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C157">
         <v>27774</v>
@@ -9679,7 +9679,7 @@
         <v>1748242</v>
       </c>
       <c r="B158" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C158">
         <v>24513</v>
@@ -9694,7 +9694,7 @@
         <v>927968751</v>
       </c>
       <c r="G158" s="9">
-        <v>0.80085497660913052</v>
+        <v>0.18809485400871109</v>
       </c>
       <c r="H158" s="20">
         <f t="shared" si="10"/>
@@ -9722,7 +9722,7 @@
         <v>1748554</v>
       </c>
       <c r="B159" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C159">
         <v>2144</v>
@@ -9765,7 +9765,7 @@
         <v>1748671</v>
       </c>
       <c r="B160" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C160">
         <v>665</v>
@@ -9808,7 +9808,7 @@
         <v>1748892</v>
       </c>
       <c r="B161" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C161">
         <v>14024</v>
@@ -9851,7 +9851,7 @@
         <v>1749100</v>
       </c>
       <c r="B162" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C162">
         <v>298</v>
@@ -9894,7 +9894,7 @@
         <v>1749308</v>
       </c>
       <c r="B163" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C163">
         <v>675</v>
@@ -9937,7 +9937,7 @@
         <v>1749607</v>
       </c>
       <c r="B164" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C164">
         <v>12632</v>
@@ -9980,7 +9980,7 @@
         <v>1749854</v>
       </c>
       <c r="B165" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C165">
         <v>19906</v>
@@ -10023,7 +10023,7 @@
         <v>1749945</v>
       </c>
       <c r="B166" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C166">
         <v>5104</v>
@@ -10066,7 +10066,7 @@
         <v>1750218</v>
       </c>
       <c r="B167" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C167">
         <v>21205</v>
@@ -10081,7 +10081,7 @@
         <v>645150390</v>
       </c>
       <c r="G167" s="9">
-        <v>7.4375678610206303E-2</v>
+        <v>0</v>
       </c>
       <c r="H167" s="20">
         <f t="shared" si="10"/>
@@ -10109,7 +10109,7 @@
         <v>1750647</v>
       </c>
       <c r="B168" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C168">
         <v>24687</v>
@@ -10152,7 +10152,7 @@
         <v>1751089</v>
       </c>
       <c r="B169" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C169">
         <v>55648</v>
@@ -10167,7 +10167,7 @@
         <v>2207217374</v>
       </c>
       <c r="G169" s="9">
-        <v>0.32104411454302401</v>
+        <v>8.720889326672765E-2</v>
       </c>
       <c r="H169" s="20">
         <f t="shared" si="10"/>
@@ -10195,7 +10195,7 @@
         <v>1751349</v>
       </c>
       <c r="B170" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C170">
         <v>31632</v>
@@ -10210,7 +10210,7 @@
         <v>1094312128</v>
       </c>
       <c r="G170" s="9">
-        <v>0.17908745247148289</v>
+        <v>0</v>
       </c>
       <c r="H170" s="20">
         <f t="shared" si="10"/>
@@ -10238,7 +10238,7 @@
         <v>1751622</v>
       </c>
       <c r="B171" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C171">
         <v>149424</v>
@@ -10253,7 +10253,7 @@
         <v>8845723206</v>
       </c>
       <c r="G171" s="9">
-        <v>0.16067272970442692</v>
+        <v>0.11856359502474255</v>
       </c>
       <c r="H171" s="20">
         <f t="shared" si="10"/>
@@ -10281,7 +10281,7 @@
         <v>1752584</v>
       </c>
       <c r="B172" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C172">
         <v>27456</v>
@@ -10296,7 +10296,7 @@
         <v>1186300561</v>
       </c>
       <c r="G172" s="9">
-        <v>7.4924671125156175E-2</v>
+        <v>7.477768795472918E-2</v>
       </c>
       <c r="H172" s="20">
         <f t="shared" si="10"/>
@@ -10324,7 +10324,7 @@
         <v>1752103</v>
       </c>
       <c r="B173" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C173">
         <v>1152</v>
@@ -10367,7 +10367,7 @@
         <v>1753000</v>
       </c>
       <c r="B174" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C174">
         <v>30262</v>
@@ -10382,7 +10382,7 @@
         <v>1619625927</v>
       </c>
       <c r="G174" s="9">
-        <v>0.32767210144927539</v>
+        <v>0.13114648033126294</v>
       </c>
       <c r="H174" s="20">
         <f t="shared" si="10"/>
@@ -10410,7 +10410,7 @@
         <v>1753377</v>
       </c>
       <c r="B175" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C175">
         <v>15177</v>
@@ -10453,7 +10453,7 @@
         <v>1753442</v>
       </c>
       <c r="B176" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C176">
         <v>18375</v>
@@ -10468,7 +10468,7 @@
         <v>705859131</v>
       </c>
       <c r="G176" s="9">
-        <v>1.965938338535677E-2</v>
+        <v>0</v>
       </c>
       <c r="H176" s="20">
         <f t="shared" si="10"/>
@@ -10496,7 +10496,7 @@
         <v>1753455</v>
       </c>
       <c r="B177" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C177">
         <v>3113</v>
@@ -10539,7 +10539,7 @@
         <v>1753559</v>
       </c>
       <c r="B178" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C178">
         <v>30772</v>
@@ -10554,7 +10554,7 @@
         <v>258913043</v>
       </c>
       <c r="G178" s="9">
-        <v>0.58269124483890888</v>
+        <v>0.20790662895412726</v>
       </c>
       <c r="H178" s="20">
         <f t="shared" si="10"/>
@@ -10582,7 +10582,7 @@
         <v>1754144</v>
       </c>
       <c r="B179" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C179">
         <v>7495</v>
@@ -10625,7 +10625,7 @@
         <v>1753481</v>
       </c>
       <c r="B180" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C180">
         <v>34642</v>
@@ -10640,7 +10640,7 @@
         <v>3206339539</v>
       </c>
       <c r="G180" s="9">
-        <v>1.371302027142127E-2</v>
+        <v>0</v>
       </c>
       <c r="H180" s="20">
         <f t="shared" si="10"/>
@@ -10668,7 +10668,7 @@
         <v>1753663</v>
       </c>
       <c r="B181" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C181">
         <v>5683</v>
@@ -10711,7 +10711,7 @@
         <v>1753871</v>
       </c>
       <c r="B182" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C182">
         <v>12547</v>
@@ -10726,7 +10726,7 @@
         <v>590411689</v>
       </c>
       <c r="G182" s="9">
-        <v>0.20973520249221184</v>
+        <v>0</v>
       </c>
       <c r="H182" s="20">
         <f t="shared" si="10"/>
@@ -10754,7 +10754,7 @@
         <v>1754534</v>
       </c>
       <c r="B183" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C183">
         <v>8028</v>
@@ -10797,7 +10797,7 @@
         <v>1754638</v>
       </c>
       <c r="B184" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C184">
         <v>26888</v>
@@ -10812,7 +10812,7 @@
         <v>648100850</v>
       </c>
       <c r="G184" s="9">
-        <v>7.4568745905815567E-2</v>
+        <v>7.32949996360725E-2</v>
       </c>
       <c r="H184" s="20">
         <f t="shared" si="10"/>
@@ -10840,7 +10840,7 @@
         <v>1754820</v>
       </c>
       <c r="B185" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C185">
         <v>57098</v>
@@ -10855,7 +10855,7 @@
         <v>1633123906</v>
       </c>
       <c r="G185" s="9">
-        <v>0.36803056783523524</v>
+        <v>0.28835543675679381</v>
       </c>
       <c r="H185" s="20">
         <f t="shared" si="10"/>
@@ -10883,7 +10883,7 @@
         <v>1754885</v>
       </c>
       <c r="B186" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C186">
         <v>53315</v>
@@ -10926,7 +10926,7 @@
         <v>1754560</v>
       </c>
       <c r="B187" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C187">
         <v>2714</v>
@@ -10941,7 +10941,7 @@
         <v>308975314</v>
       </c>
       <c r="G187" s="9">
-        <v>0.5136314067611778</v>
+        <v>0</v>
       </c>
       <c r="H187" s="20">
         <f t="shared" si="10"/>
@@ -10969,7 +10969,7 @@
         <v>1755041</v>
       </c>
       <c r="B188" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C188">
         <v>2454</v>
@@ -11012,7 +11012,7 @@
         <v>1755639</v>
       </c>
       <c r="B189" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C189">
         <v>131</v>
@@ -11055,7 +11055,7 @@
         <v>1755938</v>
       </c>
       <c r="B190" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C190">
         <v>4636</v>
@@ -11098,7 +11098,7 @@
         <v>1756627</v>
       </c>
       <c r="B191" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C191">
         <v>6758</v>
@@ -11141,7 +11141,7 @@
         <v>1756640</v>
       </c>
       <c r="B192" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C192">
         <v>57961</v>
@@ -11184,7 +11184,7 @@
         <v>1756887</v>
       </c>
       <c r="B193" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C193">
         <v>35463</v>
@@ -11227,7 +11227,7 @@
         <v>1757225</v>
       </c>
       <c r="B194" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C194">
         <v>66548</v>
@@ -11242,7 +11242,7 @@
         <v>2334196490</v>
       </c>
       <c r="G194" s="9">
-        <v>0.18455852035106321</v>
+        <v>8.3907639747894211E-2</v>
       </c>
       <c r="H194" s="20">
         <f t="shared" ref="H194:H257" si="15">E194+F194</f>
@@ -11270,7 +11270,7 @@
         <v>1757381</v>
       </c>
       <c r="B195" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C195">
         <v>11817</v>
@@ -11313,7 +11313,7 @@
         <v>1757394</v>
       </c>
       <c r="B196" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C196">
         <v>18139</v>
@@ -11328,7 +11328,7 @@
         <v>519539384</v>
       </c>
       <c r="G196" s="9">
-        <v>0.39136535348084189</v>
+        <v>0</v>
       </c>
       <c r="H196" s="20">
         <f t="shared" si="15"/>
@@ -11356,7 +11356,7 @@
         <v>1757407</v>
       </c>
       <c r="B197" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C197">
         <v>4832</v>
@@ -11399,7 +11399,7 @@
         <v>1757654</v>
       </c>
       <c r="B198" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C198">
         <v>7631</v>
@@ -11414,7 +11414,7 @@
         <v>62844558</v>
       </c>
       <c r="G198" s="9">
-        <v>0.79746353836398221</v>
+        <v>0.16296766011414077</v>
       </c>
       <c r="H198" s="20">
         <f t="shared" si="15"/>
@@ -11442,7 +11442,7 @@
         <v>1757732</v>
       </c>
       <c r="B199" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C199">
         <v>20898</v>
@@ -11485,7 +11485,7 @@
         <v>1757875</v>
       </c>
       <c r="B200" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C200">
         <v>39241</v>
@@ -11500,7 +11500,7 @@
         <v>2045142443</v>
       </c>
       <c r="G200" s="9">
-        <v>1.7525721202340125E-2</v>
+        <v>0</v>
       </c>
       <c r="H200" s="20">
         <f t="shared" si="15"/>
@@ -11528,7 +11528,7 @@
         <v>1759052</v>
       </c>
       <c r="B201" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C201">
         <v>4462</v>
@@ -11571,7 +11571,7 @@
         <v>1759572</v>
       </c>
       <c r="B202" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C202">
         <v>1284</v>
@@ -11586,7 +11586,7 @@
         <v>5731998</v>
       </c>
       <c r="G202" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H202" s="20">
         <f t="shared" si="15"/>
@@ -11614,7 +11614,7 @@
         <v>1759988</v>
       </c>
       <c r="B203" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C203">
         <v>10576</v>
@@ -11657,7 +11657,7 @@
         <v>1760287</v>
       </c>
       <c r="B204" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C204">
         <v>45705</v>
@@ -11700,7 +11700,7 @@
         <v>1760352</v>
       </c>
       <c r="B205" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C205">
         <v>11626</v>
@@ -11743,7 +11743,7 @@
         <v>1760391</v>
       </c>
       <c r="B206" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C206">
         <v>200</v>
@@ -11786,7 +11786,7 @@
         <v>1761216</v>
       </c>
       <c r="B207" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C207">
         <v>1574</v>
@@ -11829,7 +11829,7 @@
         <v>1761314</v>
       </c>
       <c r="B208" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C208">
         <v>5331</v>
@@ -11844,7 +11844,7 @@
         <v>71889963</v>
       </c>
       <c r="G208" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H208" s="20">
         <f t="shared" si="15"/>
@@ -11872,7 +11872,7 @@
         <v>1761678</v>
       </c>
       <c r="B209" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C209">
         <v>1992</v>
@@ -11915,7 +11915,7 @@
         <v>1762016</v>
       </c>
       <c r="B210" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C210">
         <v>15681</v>
@@ -11930,7 +11930,7 @@
         <v>529334333</v>
       </c>
       <c r="G210" s="9">
-        <v>0.28926391829617637</v>
+        <v>0.17580022418732097</v>
       </c>
       <c r="H210" s="20">
         <f t="shared" si="15"/>
@@ -11958,7 +11958,7 @@
         <v>1763641</v>
       </c>
       <c r="B211" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C211">
         <v>2530</v>
@@ -12001,7 +12001,7 @@
         <v>1763706</v>
       </c>
       <c r="B212" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C212">
         <v>12576</v>
@@ -12016,7 +12016,7 @@
         <v>218936786</v>
       </c>
       <c r="G212" s="9">
-        <v>0.32790606653620352</v>
+        <v>0</v>
       </c>
       <c r="H212" s="20">
         <f t="shared" si="15"/>
@@ -12044,7 +12044,7 @@
         <v>1764135</v>
       </c>
       <c r="B213" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C213">
         <v>778</v>
@@ -12087,7 +12087,7 @@
         <v>1764304</v>
       </c>
       <c r="B214" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C214">
         <v>11489</v>
@@ -12130,7 +12130,7 @@
         <v>1764343</v>
       </c>
       <c r="B215" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C215">
         <v>10482</v>
@@ -12145,7 +12145,7 @@
         <v>283755806</v>
       </c>
       <c r="G215" s="9">
-        <v>0.63164342254052019</v>
+        <v>0</v>
       </c>
       <c r="H215" s="20">
         <f t="shared" si="15"/>
@@ -12173,7 +12173,7 @@
         <v>1764278</v>
       </c>
       <c r="B216" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C216">
         <v>10515</v>
@@ -12188,7 +12188,7 @@
         <v>127888284</v>
       </c>
       <c r="G216" s="9">
-        <v>1</v>
+        <v>0.8597955547219357</v>
       </c>
       <c r="H216" s="20">
         <f t="shared" si="15"/>
@@ -12216,7 +12216,7 @@
         <v>1764421</v>
       </c>
       <c r="B217" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C217">
         <v>9079</v>
@@ -12259,7 +12259,7 @@
         <v>1764538</v>
       </c>
       <c r="B218" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C218">
         <v>3988</v>
@@ -12302,7 +12302,7 @@
         <v>1764616</v>
       </c>
       <c r="B219" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C219">
         <v>4956</v>
@@ -12317,7 +12317,7 @@
         <v>62698876</v>
       </c>
       <c r="G219" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H219" s="20">
         <f t="shared" si="15"/>
@@ -12345,7 +12345,7 @@
         <v>1764902</v>
       </c>
       <c r="B220" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C220">
         <v>2598</v>
@@ -12388,7 +12388,7 @@
         <v>1765338</v>
       </c>
       <c r="B221" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C221">
         <v>23981</v>
@@ -12403,7 +12403,7 @@
         <v>1012827838</v>
       </c>
       <c r="G221" s="9">
-        <v>5.37603305785124E-2</v>
+        <v>0</v>
       </c>
       <c r="H221" s="20">
         <f t="shared" si="15"/>
@@ -12431,7 +12431,7 @@
         <v>1765442</v>
       </c>
       <c r="B222" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C222">
         <v>40996</v>
@@ -12446,7 +12446,7 @@
         <v>1580427628</v>
       </c>
       <c r="G222" s="9">
-        <v>0.3603592303639967</v>
+        <v>0.18014198630308809</v>
       </c>
       <c r="H222" s="20">
         <f t="shared" si="15"/>
@@ -12474,7 +12474,7 @@
         <v>1765806</v>
       </c>
       <c r="B223" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C223">
         <v>22731</v>
@@ -12517,7 +12517,7 @@
         <v>1765819</v>
       </c>
       <c r="B224" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C224">
         <v>4145</v>
@@ -12532,7 +12532,7 @@
         <v>795542779</v>
       </c>
       <c r="G224" s="9">
-        <v>0.35804655870445345</v>
+        <v>0</v>
       </c>
       <c r="H224" s="20">
         <f t="shared" si="15"/>
@@ -12560,7 +12560,7 @@
         <v>1766027</v>
       </c>
       <c r="B225" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C225">
         <v>18588</v>
@@ -12575,7 +12575,7 @@
         <v>418572083</v>
       </c>
       <c r="G225" s="9">
-        <v>0.53351850862667594</v>
+        <v>2.5265744351263286E-2</v>
       </c>
       <c r="H225" s="20">
         <f t="shared" si="15"/>
@@ -12603,7 +12603,7 @@
         <v>1766040</v>
       </c>
       <c r="B226" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C226">
         <v>27081</v>
@@ -12618,7 +12618,7 @@
         <v>498096977</v>
       </c>
       <c r="G226" s="9">
-        <v>0.63518273888154997</v>
+        <v>0.29784969910465287</v>
       </c>
       <c r="H226" s="20">
         <f t="shared" si="15"/>
@@ -12646,7 +12646,7 @@
         <v>1766053</v>
       </c>
       <c r="B227" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C227">
         <v>2585</v>
@@ -12661,7 +12661,7 @@
         <v>52230828</v>
       </c>
       <c r="G227" s="9">
-        <v>0.41952707856598015</v>
+        <v>0</v>
       </c>
       <c r="H227" s="20">
         <f t="shared" si="15"/>
@@ -12689,7 +12689,7 @@
         <v>1766066</v>
       </c>
       <c r="B228" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C228">
         <v>7833</v>
@@ -12704,7 +12704,7 @@
         <v>99880265</v>
       </c>
       <c r="G228" s="9">
-        <v>0.71015625000000004</v>
+        <v>0.52604166666666663</v>
       </c>
       <c r="H228" s="20">
         <f t="shared" si="15"/>
@@ -12732,7 +12732,7 @@
         <v>1767548</v>
       </c>
       <c r="B229" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C229">
         <v>7121</v>
@@ -12775,7 +12775,7 @@
         <v>1767769</v>
       </c>
       <c r="B230" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C230">
         <v>9724</v>
@@ -12790,7 +12790,7 @@
         <v>103639257</v>
       </c>
       <c r="G230" s="9">
-        <v>1</v>
+        <v>0.404495514565064</v>
       </c>
       <c r="H230" s="20">
         <f t="shared" si="15"/>
@@ -12818,7 +12818,7 @@
         <v>1768003</v>
       </c>
       <c r="B231" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C231">
         <v>76780</v>
@@ -12833,7 +12833,7 @@
         <v>4215556094</v>
       </c>
       <c r="G231" s="9">
-        <v>0.18863610380701956</v>
+        <v>0.13722800198163179</v>
       </c>
       <c r="H231" s="20">
         <f t="shared" si="15"/>
@@ -12861,7 +12861,7 @@
         <v>1768081</v>
       </c>
       <c r="B232" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C232">
         <v>11454</v>
@@ -12904,7 +12904,7 @@
         <v>1769758</v>
       </c>
       <c r="B233" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C233">
         <v>18218</v>
@@ -12947,7 +12947,7 @@
         <v>1770122</v>
       </c>
       <c r="B234" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C234">
         <v>66427</v>
@@ -12962,7 +12962,7 @@
         <v>3223728231</v>
       </c>
       <c r="G234" s="9">
-        <v>9.7531847133757968E-2</v>
+        <v>1.1043288511441377E-2</v>
       </c>
       <c r="H234" s="20">
         <f t="shared" si="15"/>
@@ -12990,7 +12990,7 @@
         <v>1770161</v>
       </c>
       <c r="B235" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C235">
         <v>3165</v>
@@ -13033,7 +13033,7 @@
         <v>1770564</v>
       </c>
       <c r="B236" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C236">
         <v>5004</v>
@@ -13076,7 +13076,7 @@
         <v>1770629</v>
       </c>
       <c r="B237" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C237">
         <v>3934</v>
@@ -13091,7 +13091,7 @@
         <v>92153924</v>
       </c>
       <c r="G237" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H237" s="20">
         <f t="shared" si="15"/>
@@ -13119,7 +13119,7 @@
         <v>1770720</v>
       </c>
       <c r="B238" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C238">
         <v>23984</v>
@@ -13162,7 +13162,7 @@
         <v>1770850</v>
       </c>
       <c r="B239" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C239">
         <v>21016</v>
@@ -13177,7 +13177,7 @@
         <v>552042373</v>
       </c>
       <c r="G239" s="9">
-        <v>0.53640810621942703</v>
+        <v>0.48912182622874445</v>
       </c>
       <c r="H239" s="20">
         <f t="shared" si="15"/>
@@ -13205,7 +13205,7 @@
         <v>1772052</v>
       </c>
       <c r="B240" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C240">
         <v>5866</v>
@@ -13248,7 +13248,7 @@
         <v>1766703</v>
       </c>
       <c r="B241" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C241">
         <v>32733</v>
@@ -13291,7 +13291,7 @@
         <v>1772520</v>
       </c>
       <c r="B242" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C242">
         <v>9449</v>
@@ -13306,7 +13306,7 @@
         <v>141711315</v>
       </c>
       <c r="G242" s="9">
-        <v>0.23069699499165275</v>
+        <v>0.11769616026711185</v>
       </c>
       <c r="H242" s="20">
         <f t="shared" si="15"/>
@@ -13334,7 +13334,7 @@
         <v>1772676</v>
       </c>
       <c r="B243" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C243">
         <v>6957</v>
@@ -13349,7 +13349,7 @@
         <v>156724408</v>
       </c>
       <c r="G243" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H243" s="20">
         <f t="shared" si="15"/>
@@ -13377,7 +13377,7 @@
         <v>1772923</v>
       </c>
       <c r="B244" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C244">
         <v>4504</v>
@@ -13392,7 +13392,7 @@
         <v>65792626</v>
       </c>
       <c r="G244" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H244" s="20">
         <f t="shared" si="15"/>
@@ -13420,7 +13420,7 @@
         <v>1773157</v>
       </c>
       <c r="B245" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C245">
         <v>39055</v>
@@ -13435,7 +13435,7 @@
         <v>1050907889</v>
       </c>
       <c r="G245" s="9">
-        <v>0.26090911387927329</v>
+        <v>0.14215327083912374</v>
       </c>
       <c r="H245" s="20">
         <f t="shared" si="15"/>
@@ -13463,7 +13463,7 @@
         <v>1773391</v>
       </c>
       <c r="B246" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C246">
         <v>9233</v>
@@ -13506,7 +13506,7 @@
         <v>1773638</v>
       </c>
       <c r="B247" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C247">
         <v>10896</v>
@@ -13521,7 +13521,7 @@
         <v>226100815</v>
       </c>
       <c r="G247" s="9">
-        <v>0.99847683899292183</v>
+        <v>0</v>
       </c>
       <c r="H247" s="20">
         <f t="shared" si="15"/>
@@ -13549,7 +13549,7 @@
         <v>1774275</v>
       </c>
       <c r="B248" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C248">
         <v>113</v>
@@ -13592,7 +13592,7 @@
         <v>1775081</v>
       </c>
       <c r="B249" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C249">
         <v>1203</v>
@@ -13635,7 +13635,7 @@
         <v>1775185</v>
       </c>
       <c r="B250" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C250">
         <v>1876</v>
@@ -13678,7 +13678,7 @@
         <v>1775484</v>
       </c>
       <c r="B251" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C251">
         <v>55007</v>
@@ -13721,7 +13721,7 @@
         <v>1775874</v>
       </c>
       <c r="B252" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C252">
         <v>1148</v>
@@ -13764,7 +13764,7 @@
         <v>1776160</v>
       </c>
       <c r="B253" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C253">
         <v>584</v>
@@ -13807,7 +13807,7 @@
         <v>1776706</v>
       </c>
       <c r="B254" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C254">
         <v>753</v>
@@ -13850,7 +13850,7 @@
         <v>1776935</v>
       </c>
       <c r="B255" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C255">
         <v>7109</v>
@@ -13865,7 +13865,7 @@
         <v>161495345</v>
       </c>
       <c r="G255" s="9">
-        <v>0.4489853044086774</v>
+        <v>0.40461861441567532</v>
       </c>
       <c r="H255" s="20">
         <f t="shared" si="15"/>
@@ -13893,7 +13893,7 @@
         <v>1777694</v>
       </c>
       <c r="B256" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C256">
         <v>26772</v>
@@ -13936,7 +13936,7 @@
         <v>1777993</v>
       </c>
       <c r="B257" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C257">
         <v>22456</v>
@@ -13951,7 +13951,7 @@
         <v>756281549</v>
       </c>
       <c r="G257" s="9">
-        <v>0.23321205587746485</v>
+        <v>0.21061851502492926</v>
       </c>
       <c r="H257" s="20">
         <f t="shared" si="15"/>
@@ -13979,7 +13979,7 @@
         <v>1778175</v>
       </c>
       <c r="B258" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C258">
         <v>310</v>
@@ -14022,7 +14022,7 @@
         <v>1778227</v>
       </c>
       <c r="B259" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C259">
         <v>6398</v>
@@ -14065,7 +14065,7 @@
         <v>1778370</v>
       </c>
       <c r="B260" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C260">
         <v>3535</v>
@@ -14108,7 +14108,7 @@
         <v>1778929</v>
       </c>
       <c r="B261" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C261">
         <v>14232</v>
@@ -14151,7 +14151,7 @@
         <v>1779267</v>
       </c>
       <c r="B262" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C262">
         <v>14010</v>
@@ -14166,7 +14166,7 @@
         <v>470942002</v>
       </c>
       <c r="G262" s="9">
-        <v>0.17963646691280885</v>
+        <v>0</v>
       </c>
       <c r="H262" s="20">
         <f t="shared" si="20"/>
@@ -14194,7 +14194,7 @@
         <v>1779293</v>
       </c>
       <c r="B263" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C263">
         <v>88919</v>
@@ -14209,7 +14209,7 @@
         <v>1623202327</v>
       </c>
       <c r="G263" s="9">
-        <v>0.84672137571231854</v>
+        <v>0.54947884596007657</v>
       </c>
       <c r="H263" s="20">
         <f t="shared" si="20"/>
@@ -14237,7 +14237,7 @@
         <v>1779397</v>
       </c>
       <c r="B264" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C264">
         <v>2284</v>
@@ -14280,7 +14280,7 @@
         <v>1780060</v>
       </c>
       <c r="B265" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C265">
         <v>25434</v>
@@ -14295,7 +14295,7 @@
         <v>960829476</v>
       </c>
       <c r="G265" s="9">
-        <v>0.25650035137034433</v>
+        <v>0.14054813773717498</v>
       </c>
       <c r="H265" s="20">
         <f t="shared" si="20"/>
@@ -14323,7 +14323,7 @@
         <v>1780125</v>
       </c>
       <c r="B266" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C266">
         <v>7867</v>
@@ -14366,7 +14366,7 @@
         <v>1780047</v>
       </c>
       <c r="B267" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C267">
         <v>16524</v>
@@ -14409,7 +14409,7 @@
         <v>1780242</v>
       </c>
       <c r="B268" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C268">
         <v>13353</v>
@@ -14452,7 +14452,7 @@
         <v>1780645</v>
       </c>
       <c r="B269" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C269">
         <v>24201</v>
@@ -14495,7 +14495,7 @@
         <v>1781048</v>
       </c>
       <c r="B270" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C270">
         <v>53453</v>
@@ -14538,7 +14538,7 @@
         <v>1781087</v>
       </c>
       <c r="B271" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C271">
         <v>38495</v>
@@ -14553,7 +14553,7 @@
         <v>1308243839</v>
       </c>
       <c r="G271" s="9">
-        <v>0.57822520888162099</v>
+        <v>7.2923320642869924E-2</v>
       </c>
       <c r="H271" s="20">
         <f t="shared" si="20"/>
@@ -14581,7 +14581,7 @@
         <v>1782049</v>
       </c>
       <c r="B272" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C272">
         <v>5871</v>
@@ -14624,7 +14624,7 @@
         <v>1781919</v>
       </c>
       <c r="B273" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C273">
         <v>9138</v>
@@ -14667,7 +14667,7 @@
         <v>1782075</v>
       </c>
       <c r="B274" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C274">
         <v>27550</v>
@@ -14710,7 +14710,7 @@
         <v>1782101</v>
       </c>
       <c r="B275" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C275">
         <v>5507</v>
@@ -14753,7 +14753,7 @@
         <v>1782400</v>
       </c>
       <c r="B276" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C276">
         <v>9982</v>
@@ -14796,7 +14796,7 @@
         <v>1782530</v>
       </c>
       <c r="B277" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C277">
         <v>12508</v>
@@ -14839,7 +14839,7 @@
         <v>1782686</v>
       </c>
       <c r="B278" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C278">
         <v>6663</v>
@@ -14882,7 +14882,7 @@
         <v>1782855</v>
       </c>
       <c r="B279" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C279">
         <v>4141</v>
@@ -14925,7 +14925,7 @@
         <v>1782985</v>
       </c>
       <c r="B280" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C280">
         <v>13926</v>
@@ -14940,7 +14940,7 @@
         <v>700653204</v>
       </c>
       <c r="G280" s="9">
-        <v>5.6308878104481874E-2</v>
+        <v>0</v>
       </c>
       <c r="H280" s="20">
         <f t="shared" si="20"/>
@@ -14968,7 +14968,7 @@
         <v>1783245</v>
       </c>
       <c r="B281" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C281">
         <v>33889</v>
@@ -15011,7 +15011,7 @@
         <v>1783349</v>
       </c>
       <c r="B282" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C282">
         <v>26316</v>
@@ -15054,7 +15054,7 @@
         <v>1783518</v>
       </c>
       <c r="B283" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C283">
         <v>10731</v>
@@ -15097,7 +15097,7 @@
         <v>1784038</v>
       </c>
       <c r="B284" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C284">
         <v>22350</v>
@@ -15140,7 +15140,7 @@
         <v>1784220</v>
       </c>
       <c r="B285" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C285">
         <v>24466</v>
@@ -15194,8 +15194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15214,34 +15214,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>375</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>376</v>
       </c>
       <c r="C1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="29" t="s">
-        <v>6</v>
+      <c r="D1" s="30" t="s">
+        <v>379</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>379</v>
-      </c>
-      <c r="F1" s="30" t="s">
         <v>378</v>
       </c>
+      <c r="F1" s="29" t="s">
+        <v>377</v>
+      </c>
       <c r="G1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="J1" s="7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -15249,13 +15249,13 @@
         <v>14</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C2" s="21">
         <v>82249.644043663895</v>
       </c>
       <c r="D2" s="15">
-        <v>0.80810397553516822</v>
+        <v>0.1205471526572444</v>
       </c>
       <c r="E2">
         <v>3548280190.2389002</v>
@@ -15285,13 +15285,13 @@
         <v>57</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C3" s="21">
         <v>67397.727272727207</v>
       </c>
       <c r="D3" s="15">
-        <v>1</v>
+        <v>9.270216962524655E-2</v>
       </c>
       <c r="E3">
         <v>994396260.73109198</v>
@@ -15321,13 +15321,13 @@
         <v>34</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C4" s="21">
         <v>43488.409088993503</v>
       </c>
       <c r="D4" s="15">
-        <v>0.9967602591792657</v>
+        <v>0.21713462922966162</v>
       </c>
       <c r="E4">
         <v>1398865114</v>
@@ -15357,13 +15357,13 @@
         <v>70</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C5" s="21">
         <v>80909.6858638743</v>
       </c>
       <c r="D5" s="15">
-        <v>0.68655409022336855</v>
+        <v>0.30595162781643875</v>
       </c>
       <c r="E5">
         <v>2591607528.0592399</v>
@@ -15393,13 +15393,13 @@
         <v>71</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C6" s="21">
         <v>45489.510489510401</v>
       </c>
       <c r="D6" s="15">
-        <v>0.96742279067694636</v>
+        <v>0.59438923303177504</v>
       </c>
       <c r="E6">
         <v>1852067815</v>
@@ -15429,13 +15429,13 @@
         <v>25</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C7" s="21">
         <v>44883.241758241697</v>
       </c>
       <c r="D7" s="15">
-        <v>0.92424163965326178</v>
+        <v>0.49213417981088892</v>
       </c>
       <c r="E7">
         <v>4743250985.9707403</v>
@@ -15465,13 +15465,13 @@
         <v>45</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C8" s="21">
         <v>56018.7492653109</v>
       </c>
       <c r="D8" s="15">
-        <v>0.34383590611122861</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>554922436</v>
@@ -15501,13 +15501,13 @@
         <v>21</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C9" s="21">
         <v>92644.817073170707</v>
       </c>
       <c r="D9" s="15">
-        <v>0.70753233858289433</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>3863916690.1880798</v>
@@ -15537,13 +15537,13 @@
         <v>19</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C10" s="21">
         <v>67004.008016032007</v>
       </c>
       <c r="D10" s="15">
-        <v>0.94340468021916124</v>
+        <v>0.4069716831378975</v>
       </c>
       <c r="E10">
         <v>3965235780.5862598</v>
@@ -15573,13 +15573,13 @@
         <v>72</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C11" s="21">
         <v>127056.18892508101</v>
       </c>
       <c r="D11" s="15">
-        <v>5.192989464223299E-3</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>2206100566</v>
@@ -15609,13 +15609,13 @@
         <v>60</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C12" s="21">
         <v>73225.565411586897</v>
       </c>
       <c r="D12" s="15">
-        <v>0.78081419500326388</v>
+        <v>7.6879710402943446E-2</v>
       </c>
       <c r="E12">
         <v>3425149601.8145499</v>
@@ -15645,13 +15645,13 @@
         <v>58</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C13" s="21">
         <v>58095.813204508799</v>
       </c>
       <c r="D13" s="15">
-        <v>1</v>
+        <v>0.4090515614942401</v>
       </c>
       <c r="E13">
         <v>1780426102.36166</v>
@@ -15681,13 +15681,13 @@
         <v>47</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C14" s="21">
         <v>48227.848101265801</v>
       </c>
       <c r="D14" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>154979128</v>
@@ -15717,13 +15717,13 @@
         <v>48</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C15" s="21">
         <v>68354.922279792707</v>
       </c>
       <c r="D15" s="15">
-        <v>0.31242359413202936</v>
+        <v>8.4275672371638147E-2</v>
       </c>
       <c r="E15">
         <v>801655546</v>
@@ -15753,13 +15753,13 @@
         <v>44</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C16" s="21">
         <v>42086.313106280497</v>
       </c>
       <c r="D16" s="15">
-        <v>0.69205298013245031</v>
+        <v>0.5042573320719016</v>
       </c>
       <c r="E16">
         <v>1517860263.90818</v>
@@ -15789,13 +15789,13 @@
         <v>66</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C17" s="21">
         <v>48783.255086071898</v>
       </c>
       <c r="D17" s="15">
-        <v>1</v>
+        <v>0.75820207040818155</v>
       </c>
       <c r="E17">
         <v>1912350686</v>
@@ -15825,13 +15825,13 @@
         <v>64</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C18" s="21">
         <v>78378.3783783783</v>
       </c>
       <c r="D18" s="15">
-        <v>0.29334368487721163</v>
+        <v>5.3610100927552813E-2</v>
       </c>
       <c r="E18">
         <v>1740504096.6638999</v>
@@ -15861,13 +15861,13 @@
         <v>35</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C19" s="21">
         <v>47426.253687315599</v>
       </c>
       <c r="D19" s="15">
-        <v>0.58316494997782264</v>
+        <v>0.243556256468385</v>
       </c>
       <c r="E19">
         <v>1457390874</v>
@@ -15897,13 +15897,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C20" s="21">
         <v>84684.420459877903</v>
       </c>
       <c r="D20" s="15">
-        <v>0.41284446195564001</v>
+        <v>0.25343592833800727</v>
       </c>
       <c r="E20">
         <v>4228655447.0969</v>
@@ -15933,13 +15933,13 @@
         <v>27</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C21" s="21">
         <v>36811.342592592497</v>
       </c>
       <c r="D21" s="15">
-        <v>1</v>
+        <v>0.68962585034013602</v>
       </c>
       <c r="E21">
         <v>934575156.70661795</v>
@@ -15969,13 +15969,13 @@
         <v>52</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C22" s="21">
         <v>62060.629019958797</v>
       </c>
       <c r="D22" s="15">
-        <v>1</v>
+        <v>0.99935555146381883</v>
       </c>
       <c r="E22">
         <v>717220175.04682505</v>
@@ -16005,13 +16005,13 @@
         <v>77</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C23" s="21">
         <v>70188.4240894338</v>
       </c>
       <c r="D23" s="15">
-        <v>0.155925820662214</v>
+        <v>1.7550092368907203E-2</v>
       </c>
       <c r="E23">
         <v>5719026262</v>
@@ -16041,7 +16041,7 @@
         <v>9</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C24" s="21">
         <v>133209.74576271101</v>
@@ -16077,13 +16077,13 @@
         <v>68</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C25" s="21">
         <v>29726.962457337799</v>
       </c>
       <c r="D25" s="15">
-        <v>1</v>
+        <v>0.9463662850342649</v>
       </c>
       <c r="E25">
         <v>586459514</v>
@@ -16113,7 +16113,7 @@
         <v>12</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C26" s="21">
         <v>138253.012048192</v>
@@ -16149,13 +16149,13 @@
         <v>37</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C27" s="21">
         <v>17297.863710113499</v>
       </c>
       <c r="D27" s="15">
-        <v>1</v>
+        <v>0.9668874172185431</v>
       </c>
       <c r="E27">
         <v>108407276</v>
@@ -16185,13 +16185,13 @@
         <v>63</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C28" s="21">
         <v>57446.236559139703</v>
       </c>
       <c r="D28" s="15">
-        <v>1</v>
+        <v>0.91780475467880629</v>
       </c>
       <c r="E28">
         <v>1259700999.6398001</v>
@@ -16221,13 +16221,13 @@
         <v>56</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C29" s="21">
         <v>91762.204142011804</v>
       </c>
       <c r="D29" s="15">
-        <v>0.44061627021078476</v>
+        <v>0.20226304353960325</v>
       </c>
       <c r="E29">
         <v>2929880472</v>
@@ -16257,13 +16257,13 @@
         <v>38</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C30" s="21">
         <v>49092.409240923997</v>
       </c>
       <c r="D30" s="15">
-        <v>0.9041847980804425</v>
+        <v>0.40599455040871935</v>
       </c>
       <c r="E30">
         <v>1473809152</v>
@@ -16293,13 +16293,13 @@
         <v>69</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C31" s="21">
         <v>40337.982832618</v>
       </c>
       <c r="D31" s="15">
-        <v>0.96847891709828093</v>
+        <v>0.51663436179339706</v>
       </c>
       <c r="E31">
         <v>1151954740</v>
@@ -16329,13 +16329,13 @@
         <v>55</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C32" s="21">
         <v>59478.403277097597</v>
       </c>
       <c r="D32" s="15">
-        <v>1</v>
+        <v>5.2857285329610051E-3</v>
       </c>
       <c r="E32">
         <v>555427497.29508102</v>
@@ -16365,13 +16365,13 @@
         <v>20</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C33" s="21">
         <v>67039.106145251397</v>
       </c>
       <c r="D33" s="15">
-        <v>1</v>
+        <v>0.23929847892943229</v>
       </c>
       <c r="E33">
         <v>1280582613.6588299</v>
@@ -16401,13 +16401,13 @@
         <v>23</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C34" s="21">
         <v>53567.685589519599</v>
       </c>
       <c r="D34" s="15">
-        <v>1</v>
+        <v>0.45625403858580266</v>
       </c>
       <c r="E34">
         <v>3039736669.3952899</v>
@@ -16437,13 +16437,13 @@
         <v>41</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C35" s="21">
         <v>68166.243654822305</v>
       </c>
       <c r="D35" s="15">
-        <v>0.24035850081477458</v>
+        <v>9.919880499728409E-2</v>
       </c>
       <c r="E35">
         <v>3571513320</v>
@@ -16473,13 +16473,13 @@
         <v>16</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C36" s="21">
         <v>88437.625350982693</v>
       </c>
       <c r="D36" s="15">
-        <v>0.60032730073161344</v>
+        <v>0</v>
       </c>
       <c r="E36">
         <v>5614957192.4309101</v>
@@ -16509,7 +16509,7 @@
         <v>11</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C37" s="21">
         <v>93706.014075495797</v>
@@ -16545,13 +16545,13 @@
         <v>39</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C38" s="21">
         <v>61078.052550231798</v>
       </c>
       <c r="D38" s="15">
-        <v>0.72729650554509306</v>
+        <v>0.62879263444235201</v>
       </c>
       <c r="E38">
         <v>1816301258</v>
@@ -16581,13 +16581,13 @@
         <v>6</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C39" s="21">
         <v>104135.30619226801</v>
       </c>
       <c r="D39" s="15">
-        <v>1.3333333333333334E-2</v>
+        <v>0</v>
       </c>
       <c r="E39">
         <v>20148584267.721901</v>
@@ -16617,7 +16617,7 @@
         <v>7</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C40" s="21">
         <v>137504.774637127</v>
@@ -16653,13 +16653,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C41" s="21">
         <v>93605.664488017399</v>
       </c>
       <c r="D41" s="15">
-        <v>0.25798883785252136</v>
+        <v>0</v>
       </c>
       <c r="E41">
         <v>5335063217</v>
@@ -16689,13 +16689,13 @@
         <v>22</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C42" s="21">
         <v>103469.03669724699</v>
       </c>
       <c r="D42" s="15">
-        <v>0.59259052536105494</v>
+        <v>6.2987511337472962E-2</v>
       </c>
       <c r="E42">
         <v>10349284631.224199</v>
@@ -16725,13 +16725,13 @@
         <v>31</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C43" s="21">
         <v>71734.657039711194</v>
       </c>
       <c r="D43" s="15">
-        <v>0.95294954223578565</v>
+        <v>0.31566472104530235</v>
       </c>
       <c r="E43">
         <v>3355586836.6333699</v>
@@ -16761,13 +16761,13 @@
         <v>59</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C44" s="21">
         <v>76145.662847790503</v>
       </c>
       <c r="D44" s="15">
-        <v>1</v>
+        <v>0.21836337373610501</v>
       </c>
       <c r="E44">
         <v>1238142773.8199301</v>
@@ -16797,13 +16797,13 @@
         <v>18</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C45" s="21">
         <v>78841.145833333299</v>
       </c>
       <c r="D45" s="15">
-        <v>1</v>
+        <v>0.46219012568571627</v>
       </c>
       <c r="E45">
         <v>947789398</v>
@@ -16833,7 +16833,7 @@
         <v>75</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C46" s="21">
         <v>73828.004598938307</v>
@@ -16869,7 +16869,7 @@
         <v>74</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C47" s="21">
         <v>115749.730312837</v>
@@ -16905,13 +16905,13 @@
         <v>8</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C48" s="21">
         <v>122603.164187809</v>
       </c>
       <c r="D48" s="15">
-        <v>6.7775239142594396E-2</v>
+        <v>0</v>
       </c>
       <c r="E48">
         <v>132811651780.245</v>
@@ -16941,7 +16941,7 @@
         <v>33</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C49" s="21">
         <v>124966.99669966901</v>
@@ -16977,13 +16977,13 @@
         <v>28</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C50" s="21">
         <v>110651.05653912001</v>
       </c>
       <c r="D50" s="15">
-        <v>0.44102178812922616</v>
+        <v>0.1626522885638102</v>
       </c>
       <c r="E50">
         <v>22690599560.388</v>
@@ -17013,13 +17013,13 @@
         <v>61</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C51" s="21">
         <v>49405.207811411601</v>
       </c>
       <c r="D51" s="15">
-        <v>1</v>
+        <v>0.44576877234803336</v>
       </c>
       <c r="E51">
         <v>1744139059.0571401</v>
@@ -17049,7 +17049,7 @@
         <v>5</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C52" s="21">
         <v>145156.86274509801</v>
@@ -17085,13 +17085,13 @@
         <v>29</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C53" s="21">
         <v>37247.422680412303</v>
       </c>
       <c r="D53" s="15">
-        <v>1</v>
+        <v>0.6732482611944588</v>
       </c>
       <c r="E53">
         <v>1255679042.0029199</v>
@@ -17121,13 +17121,13 @@
         <v>13</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C54" s="21">
         <v>77368.4210526315</v>
       </c>
       <c r="D54" s="15">
-        <v>0.63061677772082692</v>
+        <v>0</v>
       </c>
       <c r="E54">
         <v>1966649200.72945</v>
@@ -17157,7 +17157,7 @@
         <v>10</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C55" s="21">
         <v>108893.84609789299</v>
@@ -17193,7 +17193,7 @@
         <v>36</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C56" s="21">
         <v>29959.677419354801</v>
@@ -17229,13 +17229,13 @@
         <v>76</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C57" s="21">
         <v>75645.5643481882</v>
       </c>
       <c r="D57" s="15">
-        <v>0.47652407214189896</v>
+        <v>0</v>
       </c>
       <c r="E57">
         <v>1697988043.6924701</v>
@@ -17265,13 +17265,13 @@
         <v>15</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C58" s="21">
         <v>89490.830115830104</v>
       </c>
       <c r="D58" s="15">
-        <v>0.48509996826404317</v>
+        <v>0.22267534116153603</v>
       </c>
       <c r="E58">
         <v>5574661088</v>
@@ -17301,7 +17301,7 @@
         <v>50</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C59" s="21">
         <v>54685.314685314603</v>
@@ -17337,7 +17337,7 @@
         <v>54</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C60" s="21">
         <v>20515.625</v>
@@ -17373,13 +17373,13 @@
         <v>1</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C61" s="21">
         <v>59553.862894450402</v>
       </c>
       <c r="D61" s="15">
-        <v>0.65371755231178541</v>
+        <v>0.29557057596893649</v>
       </c>
       <c r="E61">
         <v>3945507288</v>
@@ -17409,13 +17409,13 @@
         <v>49</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C62" s="21">
         <v>50453.639082751703</v>
       </c>
       <c r="D62" s="15">
-        <v>0.94860366859027201</v>
+        <v>0.64146228359439406</v>
       </c>
       <c r="E62">
         <v>1467654352.7150199</v>
@@ -17445,13 +17445,13 @@
         <v>46</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C63" s="21">
         <v>42455.673758865203</v>
       </c>
       <c r="D63" s="15">
-        <v>1</v>
+        <v>0.63666666666666671</v>
       </c>
       <c r="E63">
         <v>886136027.60169101</v>
@@ -17481,13 +17481,13 @@
         <v>51</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C64" s="21">
         <v>37095.3757225433</v>
       </c>
       <c r="D64" s="15">
-        <v>0.78007798652959948</v>
+        <v>0</v>
       </c>
       <c r="E64">
         <v>632440233.59475005</v>
@@ -17517,13 +17517,13 @@
         <v>30</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C65" s="21">
         <v>47515.090543259503</v>
       </c>
       <c r="D65" s="15">
-        <v>1</v>
+        <v>0.61087690303785769</v>
       </c>
       <c r="E65">
         <v>2214326519.5912199</v>
@@ -17553,13 +17553,13 @@
         <v>43</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C66" s="21">
         <v>40124.821683309499</v>
       </c>
       <c r="D66" s="15">
-        <v>1</v>
+        <v>0.46788089900131552</v>
       </c>
       <c r="E66">
         <v>2059404538</v>
@@ -17572,7 +17572,7 @@
         <v>22811.198096572451</v>
       </c>
       <c r="H66" s="8">
-        <f t="shared" ref="H66:H97" si="4">LN(G66)</f>
+        <f t="shared" ref="H66:H78" si="4">LN(G66)</f>
         <v>10.035006838957019</v>
       </c>
       <c r="I66" s="8">
@@ -17589,7 +17589,7 @@
         <v>32</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C67" s="21">
         <v>119836.78593848</v>
@@ -17625,13 +17625,13 @@
         <v>3</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C68" s="21">
         <v>68444.460944460894</v>
       </c>
       <c r="D68" s="15">
-        <v>0.25196740232940434</v>
+        <v>0</v>
       </c>
       <c r="E68">
         <v>6215659728</v>
@@ -17661,13 +17661,13 @@
         <v>73</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C69" s="21">
         <v>69526.209677419305</v>
       </c>
       <c r="D69" s="15">
-        <v>1</v>
+        <v>0.75599441452224214</v>
       </c>
       <c r="E69">
         <v>1274341977.2748699</v>
@@ -17697,13 +17697,13 @@
         <v>40</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C70" s="21">
         <v>27868.589743589699</v>
       </c>
       <c r="D70" s="15">
-        <v>1</v>
+        <v>0.67443141575509558</v>
       </c>
       <c r="E70">
         <v>474204750</v>
@@ -17733,13 +17733,13 @@
         <v>62</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C71" s="21">
         <v>70782.051282051194</v>
       </c>
       <c r="D71" s="15">
-        <v>1</v>
+        <v>0.75171251495052738</v>
       </c>
       <c r="E71">
         <v>943420954</v>
@@ -17769,13 +17769,13 @@
         <v>67</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C72" s="21">
         <v>34376.068376068302</v>
       </c>
       <c r="D72" s="15">
-        <v>1</v>
+        <v>0.67517792694033119</v>
       </c>
       <c r="E72">
         <v>627711081.28356099</v>
@@ -17805,13 +17805,13 @@
         <v>26</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C73" s="21">
         <v>38178.571428571398</v>
       </c>
       <c r="D73" s="15">
-        <v>1</v>
+        <v>0.64332013996443527</v>
       </c>
       <c r="E73">
         <v>532283575.13797301</v>
@@ -17841,13 +17841,13 @@
         <v>65</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C74" s="21">
         <v>73411.6022099447</v>
       </c>
       <c r="D74" s="15">
-        <v>1</v>
+        <v>0.66009149783138255</v>
       </c>
       <c r="E74">
         <v>1662849170</v>
@@ -17877,13 +17877,13 @@
         <v>53</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C75" s="21">
         <v>50429.6875</v>
       </c>
       <c r="D75" s="15">
-        <v>1</v>
+        <v>0.89373276126264178</v>
       </c>
       <c r="E75">
         <v>894063121.09593594</v>
@@ -17913,13 +17913,13 @@
         <v>2</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C76" s="21">
         <v>71524.771024146496</v>
       </c>
       <c r="D76" s="15">
-        <v>0.76612380384326129</v>
+        <v>5.750628873732528E-2</v>
       </c>
       <c r="E76">
         <v>5358863377.8789196</v>
@@ -17949,13 +17949,13 @@
         <v>24</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C77" s="21">
         <v>134321.966058277</v>
       </c>
       <c r="D77" s="15">
-        <v>0.26175368245975783</v>
+        <v>1.2781809275355716E-2</v>
       </c>
       <c r="E77">
         <v>16462631666.2216</v>
@@ -17985,13 +17985,13 @@
         <v>42</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C78" s="21">
         <v>35029.850746268603</v>
       </c>
       <c r="D78" s="15">
-        <v>1</v>
+        <v>0.64528147389969293</v>
       </c>
       <c r="E78">
         <v>1087817372</v>
@@ -18032,7 +18032,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -18042,10 +18044,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -18078,13 +18080,16 @@
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>FACTORS_MUNI!G1</f>
-        <v>PCT_EDA_POP</v>
+        <v>PCT_DA_POP</v>
       </c>
       <c r="B5" s="2">
         <v>-1</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="18"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="colorScale" priority="4">
       <colorScale>
@@ -18096,9 +18101,6 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="18"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18142,7 +18144,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -18152,10 +18156,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>